<commit_message>
AssetsCatalog: update assets. Constants: add letterboxOverlay ZPosition. CutsceneIntro: add letterbox, update heights of objects to fit within the letterbox (flying dragon, princess abduction, princess closeup zoom).
</commit_message>
<xml_diff>
--- a/JSON/AssetsCatalog.xlsx
+++ b/JSON/AssetsCatalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B99ED31-BC5B-8645-8A25-628EE8CB253F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7E1724-712F-B143-9013-E65D87AC7FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36000" yWindow="-2400" windowWidth="51200" windowHeight="24180" xr2:uid="{E84333C6-E3B6-FB42-AB04-827399F33810}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$236</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$239</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2003" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="577">
   <si>
     <t>Filename</t>
   </si>
@@ -1752,6 +1752,24 @@
   </si>
   <si>
     <t>Source</t>
+  </si>
+  <si>
+    <t>playerTextures/princess2</t>
+  </si>
+  <si>
+    <t>Princess2Idle (1…16)</t>
+  </si>
+  <si>
+    <t>https://www.freepik.com/free-vector/heart-gem-rank-medal-game-badge-gold_39709541.htm#page=2&amp;query=gold%20badge%20sprite&amp;position=49&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d</t>
+  </si>
+  <si>
+    <t>Free vector heart gem rank medal game badge in gold</t>
+  </si>
+  <si>
+    <t>https://www.freepik.com/free-vector/golden-award-badges-game-avatar-frames_27472607.htm#page=4&amp;query=gold%20badge%20sprite&amp;position=9&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d</t>
+  </si>
+  <si>
+    <t>Free vector golden award badges game avatar frames</t>
   </si>
 </sst>
 </file>
@@ -2158,13 +2176,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}">
-  <dimension ref="A1:L236"/>
+  <dimension ref="A1:L239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="K106" sqref="K106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5251,7 +5269,7 @@
         <v>4</v>
       </c>
       <c r="B103" t="s">
-        <v>240</v>
+        <v>571</v>
       </c>
       <c r="C103" t="s">
         <v>238</v>
@@ -5272,10 +5290,10 @@
         <v>174</v>
       </c>
       <c r="K103" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="L103" s="6" t="s">
-        <v>124</v>
+        <v>195</v>
+      </c>
+      <c r="L103" s="7" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.2">
@@ -5283,10 +5301,10 @@
         <v>4</v>
       </c>
       <c r="B104" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C104" t="s">
-        <v>244</v>
+        <v>572</v>
       </c>
       <c r="D104" t="s">
         <v>6</v>
@@ -5298,16 +5316,19 @@
         <v>0</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="I104" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
+      </c>
+      <c r="J104" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="K104" s="3" t="s">
-        <v>224</v>
+        <v>126</v>
       </c>
       <c r="L104" s="6" t="s">
-        <v>223</v>
+        <v>124</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.2">
@@ -5315,10 +5336,10 @@
         <v>4</v>
       </c>
       <c r="B105" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C105" t="s">
-        <v>244</v>
+        <v>572</v>
       </c>
       <c r="D105" t="s">
         <v>6</v>
@@ -5330,19 +5351,16 @@
         <v>0</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>234</v>
+        <v>36</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="J105" s="3" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
       <c r="K105" s="3" t="s">
-        <v>236</v>
+        <v>574</v>
       </c>
       <c r="L105" s="6" t="s">
-        <v>233</v>
+        <v>573</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.2">
@@ -5350,10 +5368,10 @@
         <v>4</v>
       </c>
       <c r="B106" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C106" t="s">
-        <v>244</v>
+        <v>572</v>
       </c>
       <c r="D106" t="s">
         <v>6</v>
@@ -5365,19 +5383,16 @@
         <v>0</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>125</v>
+        <v>36</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J106" s="3" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>126</v>
+        <v>576</v>
       </c>
       <c r="L106" s="6" t="s">
-        <v>124</v>
+        <v>575</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.2">
@@ -5400,19 +5415,16 @@
         <v>0</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>125</v>
+        <v>36</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J107" s="3" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="K107" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="L107" s="7" t="s">
-        <v>196</v>
+        <v>224</v>
+      </c>
+      <c r="L107" s="6" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.2">
@@ -5423,7 +5435,7 @@
         <v>243</v>
       </c>
       <c r="C108" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D108" t="s">
         <v>6</v>
@@ -5435,16 +5447,19 @@
         <v>0</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>36</v>
+        <v>234</v>
       </c>
       <c r="I108" s="3" t="s">
-        <v>135</v>
+        <v>235</v>
+      </c>
+      <c r="J108" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="K108" s="3" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="L108" s="6" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.2">
@@ -5455,7 +5470,7 @@
         <v>243</v>
       </c>
       <c r="C109" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D109" t="s">
         <v>6</v>
@@ -5490,7 +5505,7 @@
         <v>243</v>
       </c>
       <c r="C110" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D110" t="s">
         <v>6</v>
@@ -5502,16 +5517,19 @@
         <v>0</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
+      </c>
+      <c r="J110" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="K110" s="3" t="s">
-        <v>229</v>
+        <v>195</v>
       </c>
       <c r="L110" s="7" t="s">
-        <v>230</v>
+        <v>196</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.2">
@@ -5522,7 +5540,7 @@
         <v>243</v>
       </c>
       <c r="C111" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D111" t="s">
         <v>6</v>
@@ -5534,19 +5552,16 @@
         <v>0</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>125</v>
+        <v>36</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J111" s="3" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="K111" s="3" t="s">
-        <v>126</v>
+        <v>224</v>
       </c>
       <c r="L111" s="6" t="s">
-        <v>124</v>
+        <v>223</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.2">
@@ -5557,7 +5572,7 @@
         <v>243</v>
       </c>
       <c r="C112" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D112" t="s">
         <v>6</v>
@@ -5578,10 +5593,10 @@
         <v>174</v>
       </c>
       <c r="K112" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="L112" s="7" t="s">
-        <v>196</v>
+        <v>126</v>
+      </c>
+      <c r="L112" s="6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.2">
@@ -5607,13 +5622,13 @@
         <v>36</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="K113" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L113" s="6" t="s">
-        <v>87</v>
+        <v>229</v>
+      </c>
+      <c r="L113" s="7" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.2">
@@ -5624,7 +5639,7 @@
         <v>243</v>
       </c>
       <c r="C114" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D114" t="s">
         <v>6</v>
@@ -5636,16 +5651,19 @@
         <v>0</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
+      </c>
+      <c r="J114" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="K114" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="L114" s="7" t="s">
-        <v>230</v>
+        <v>126</v>
+      </c>
+      <c r="L114" s="6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.2">
@@ -5656,7 +5674,7 @@
         <v>243</v>
       </c>
       <c r="C115" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D115" t="s">
         <v>6</v>
@@ -5677,10 +5695,10 @@
         <v>174</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="L115" s="6" t="s">
-        <v>124</v>
+        <v>195</v>
+      </c>
+      <c r="L115" s="7" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.2">
@@ -5691,7 +5709,7 @@
         <v>243</v>
       </c>
       <c r="C116" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D116" t="s">
         <v>6</v>
@@ -5703,19 +5721,16 @@
         <v>0</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>125</v>
+        <v>36</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J116" s="3" t="s">
-        <v>174</v>
+        <v>88</v>
       </c>
       <c r="K116" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="L116" s="7" t="s">
-        <v>196</v>
+        <v>95</v>
+      </c>
+      <c r="L116" s="6" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.2">
@@ -5741,13 +5756,13 @@
         <v>36</v>
       </c>
       <c r="I117" s="3" t="s">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="K117" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="L117" s="6" t="s">
-        <v>106</v>
+        <v>229</v>
+      </c>
+      <c r="L117" s="7" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.2">
@@ -5758,7 +5773,7 @@
         <v>243</v>
       </c>
       <c r="C118" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D118" t="s">
         <v>6</v>
@@ -5770,16 +5785,19 @@
         <v>0</v>
       </c>
       <c r="H118" s="3" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
+      </c>
+      <c r="J118" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="K118" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="L118" s="7" t="s">
-        <v>230</v>
+        <v>126</v>
+      </c>
+      <c r="L118" s="6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.2">
@@ -5790,7 +5808,7 @@
         <v>243</v>
       </c>
       <c r="C119" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D119" t="s">
         <v>6</v>
@@ -5811,10 +5829,10 @@
         <v>174</v>
       </c>
       <c r="K119" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="L119" s="6" t="s">
-        <v>124</v>
+        <v>195</v>
+      </c>
+      <c r="L119" s="7" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.2">
@@ -5825,7 +5843,7 @@
         <v>243</v>
       </c>
       <c r="C120" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D120" t="s">
         <v>6</v>
@@ -5837,19 +5855,16 @@
         <v>0</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>125</v>
+        <v>36</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J120" s="3" t="s">
-        <v>174</v>
+        <v>93</v>
       </c>
       <c r="K120" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="L120" s="7" t="s">
-        <v>196</v>
+        <v>107</v>
+      </c>
+      <c r="L120" s="6" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.2">
@@ -5860,7 +5875,7 @@
         <v>243</v>
       </c>
       <c r="C121" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D121" t="s">
         <v>6</v>
@@ -5878,10 +5893,10 @@
         <v>135</v>
       </c>
       <c r="K121" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="L121" s="6" t="s">
-        <v>223</v>
+        <v>229</v>
+      </c>
+      <c r="L121" s="7" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.2">
@@ -5892,7 +5907,7 @@
         <v>243</v>
       </c>
       <c r="C122" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D122" t="s">
         <v>6</v>
@@ -5927,7 +5942,7 @@
         <v>243</v>
       </c>
       <c r="C123" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D123" t="s">
         <v>6</v>
@@ -5939,16 +5954,19 @@
         <v>0</v>
       </c>
       <c r="H123" s="3" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="I123" s="3" t="s">
-        <v>88</v>
+        <v>125</v>
+      </c>
+      <c r="J123" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="K123" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L123" s="6" t="s">
-        <v>87</v>
+        <v>195</v>
+      </c>
+      <c r="L123" s="7" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.2">
@@ -5956,28 +5974,31 @@
         <v>4</v>
       </c>
       <c r="B124" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C124" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D124" t="s">
         <v>6</v>
       </c>
+      <c r="E124" t="s">
+        <v>174</v>
+      </c>
       <c r="F124" s="3">
         <v>0</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>111</v>
+        <v>36</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>257</v>
+        <v>135</v>
       </c>
       <c r="K124" s="3" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="L124" s="6" t="s">
-        <v>256</v>
+        <v>223</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.2">
@@ -5985,28 +6006,34 @@
         <v>4</v>
       </c>
       <c r="B125" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C125" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D125" t="s">
         <v>6</v>
       </c>
+      <c r="E125" t="s">
+        <v>174</v>
+      </c>
       <c r="F125" s="3">
         <v>0</v>
       </c>
       <c r="H125" s="3" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="I125" s="3" t="s">
-        <v>260</v>
+        <v>125</v>
+      </c>
+      <c r="J125" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="K125" s="3" t="s">
-        <v>261</v>
+        <v>126</v>
       </c>
       <c r="L125" s="6" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.2">
@@ -6014,28 +6041,31 @@
         <v>4</v>
       </c>
       <c r="B126" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C126" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D126" t="s">
         <v>6</v>
       </c>
+      <c r="E126" t="s">
+        <v>174</v>
+      </c>
       <c r="F126" s="3">
         <v>0</v>
       </c>
       <c r="H126" s="3" t="s">
-        <v>111</v>
+        <v>36</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>257</v>
+        <v>88</v>
       </c>
       <c r="K126" s="3" t="s">
-        <v>301</v>
+        <v>95</v>
       </c>
       <c r="L126" s="6" t="s">
-        <v>300</v>
+        <v>87</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.2">
@@ -6046,7 +6076,7 @@
         <v>250</v>
       </c>
       <c r="C127" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D127" t="s">
         <v>6</v>
@@ -6058,13 +6088,13 @@
         <v>111</v>
       </c>
       <c r="I127" s="3" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="K127" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="L127" s="6" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.2">
@@ -6075,7 +6105,7 @@
         <v>250</v>
       </c>
       <c r="C128" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D128" t="s">
         <v>6</v>
@@ -6087,13 +6117,13 @@
         <v>111</v>
       </c>
       <c r="I128" s="3" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="K128" s="3" t="s">
-        <v>303</v>
+        <v>261</v>
       </c>
       <c r="L128" s="6" t="s">
-        <v>302</v>
+        <v>259</v>
       </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.2">
@@ -6101,10 +6131,10 @@
         <v>4</v>
       </c>
       <c r="B129" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="C129" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="D129" t="s">
         <v>6</v>
@@ -6113,16 +6143,16 @@
         <v>0</v>
       </c>
       <c r="H129" s="3" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="I129" s="3" t="s">
-        <v>135</v>
+        <v>257</v>
       </c>
       <c r="K129" s="3" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="L129" s="6" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.2">
@@ -6130,10 +6160,10 @@
         <v>4</v>
       </c>
       <c r="B130" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="C130" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="D130" t="s">
         <v>6</v>
@@ -6142,16 +6172,16 @@
         <v>0</v>
       </c>
       <c r="H130" s="3" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="I130" s="3" t="s">
-        <v>135</v>
+        <v>264</v>
       </c>
       <c r="K130" s="3" t="s">
-        <v>290</v>
+        <v>263</v>
       </c>
       <c r="L130" s="6" t="s">
-        <v>289</v>
+        <v>262</v>
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.2">
@@ -6159,10 +6189,10 @@
         <v>4</v>
       </c>
       <c r="B131" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="C131" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="D131" t="s">
         <v>6</v>
@@ -6171,16 +6201,16 @@
         <v>0</v>
       </c>
       <c r="H131" s="3" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="I131" s="3" t="s">
-        <v>135</v>
+        <v>257</v>
       </c>
       <c r="K131" s="3" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="L131" s="6" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.2">
@@ -6191,7 +6221,7 @@
         <v>265</v>
       </c>
       <c r="C132" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D132" t="s">
         <v>6</v>
@@ -6203,13 +6233,13 @@
         <v>36</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>36</v>
+        <v>135</v>
       </c>
       <c r="K132" s="3" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="L132" s="6" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.2">
@@ -6220,7 +6250,7 @@
         <v>265</v>
       </c>
       <c r="C133" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D133" t="s">
         <v>6</v>
@@ -6232,13 +6262,13 @@
         <v>36</v>
       </c>
       <c r="I133" s="3" t="s">
-        <v>36</v>
+        <v>135</v>
       </c>
       <c r="K133" s="3" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="L133" s="6" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.2">
@@ -6249,20 +6279,26 @@
         <v>265</v>
       </c>
       <c r="C134" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D134" t="s">
         <v>6</v>
       </c>
-      <c r="F134" s="8">
-        <v>0</v>
-      </c>
-      <c r="G134" s="8"/>
-      <c r="H134" s="8"/>
-      <c r="I134" s="8"/>
-      <c r="J134" s="8"/>
-      <c r="K134" s="8"/>
-      <c r="L134" s="9"/>
+      <c r="F134" s="3">
+        <v>0</v>
+      </c>
+      <c r="H134" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K134" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="L134" s="6" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
@@ -6272,20 +6308,26 @@
         <v>265</v>
       </c>
       <c r="C135" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D135" t="s">
         <v>6</v>
       </c>
-      <c r="F135" s="8">
-        <v>0</v>
-      </c>
-      <c r="G135" s="8"/>
-      <c r="H135" s="8"/>
-      <c r="I135" s="8"/>
-      <c r="J135" s="8"/>
-      <c r="K135" s="8"/>
-      <c r="L135" s="9"/>
+      <c r="F135" s="3">
+        <v>0</v>
+      </c>
+      <c r="H135" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I135" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K135" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="L135" s="6" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
@@ -6295,7 +6337,7 @@
         <v>265</v>
       </c>
       <c r="C136" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D136" t="s">
         <v>6</v>
@@ -6307,13 +6349,13 @@
         <v>36</v>
       </c>
       <c r="I136" s="3" t="s">
-        <v>93</v>
+        <v>36</v>
       </c>
       <c r="K136" s="3" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="L136" s="6" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.2">
@@ -6324,26 +6366,20 @@
         <v>265</v>
       </c>
       <c r="C137" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D137" t="s">
         <v>6</v>
       </c>
-      <c r="F137" s="3">
-        <v>0</v>
-      </c>
-      <c r="H137" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I137" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K137" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="L137" s="6" t="s">
-        <v>295</v>
-      </c>
+      <c r="F137" s="8">
+        <v>0</v>
+      </c>
+      <c r="G137" s="8"/>
+      <c r="H137" s="8"/>
+      <c r="I137" s="8"/>
+      <c r="J137" s="8"/>
+      <c r="K137" s="8"/>
+      <c r="L137" s="9"/>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
@@ -6353,26 +6389,20 @@
         <v>265</v>
       </c>
       <c r="C138" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D138" t="s">
         <v>6</v>
       </c>
-      <c r="F138" s="3">
-        <v>0</v>
-      </c>
-      <c r="H138" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I138" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K138" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="L138" s="6" t="s">
-        <v>289</v>
-      </c>
+      <c r="F138" s="8">
+        <v>0</v>
+      </c>
+      <c r="G138" s="8"/>
+      <c r="H138" s="8"/>
+      <c r="I138" s="8"/>
+      <c r="J138" s="8"/>
+      <c r="K138" s="8"/>
+      <c r="L138" s="9"/>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
@@ -6382,7 +6412,7 @@
         <v>265</v>
       </c>
       <c r="C139" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D139" t="s">
         <v>6</v>
@@ -6394,13 +6424,13 @@
         <v>36</v>
       </c>
       <c r="I139" s="3" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="K139" s="3" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="L139" s="6" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.2">
@@ -6411,7 +6441,7 @@
         <v>265</v>
       </c>
       <c r="C140" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="D140" t="s">
         <v>6</v>
@@ -6426,10 +6456,10 @@
         <v>135</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="L140" s="6" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.2">
@@ -6440,20 +6470,26 @@
         <v>265</v>
       </c>
       <c r="C141" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D141" t="s">
         <v>6</v>
       </c>
-      <c r="F141" s="8">
-        <v>0</v>
-      </c>
-      <c r="G141" s="8"/>
-      <c r="H141" s="8"/>
-      <c r="I141" s="8"/>
-      <c r="J141" s="8"/>
-      <c r="K141" s="8"/>
-      <c r="L141" s="9"/>
+      <c r="F141" s="3">
+        <v>0</v>
+      </c>
+      <c r="H141" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I141" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K141" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="L141" s="6" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
@@ -6463,20 +6499,26 @@
         <v>265</v>
       </c>
       <c r="C142" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D142" t="s">
         <v>6</v>
       </c>
-      <c r="F142" s="8">
-        <v>0</v>
-      </c>
-      <c r="G142" s="8"/>
-      <c r="H142" s="8"/>
-      <c r="I142" s="8"/>
-      <c r="J142" s="8"/>
-      <c r="K142" s="8"/>
-      <c r="L142" s="9"/>
+      <c r="F142" s="3">
+        <v>0</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I142" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K142" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="L142" s="6" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
@@ -6486,20 +6528,26 @@
         <v>265</v>
       </c>
       <c r="C143" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="D143" t="s">
         <v>6</v>
       </c>
-      <c r="F143" s="8">
-        <v>0</v>
-      </c>
-      <c r="G143" s="8"/>
-      <c r="H143" s="8"/>
-      <c r="I143" s="8"/>
-      <c r="J143" s="8"/>
-      <c r="K143" s="8"/>
-      <c r="L143" s="9"/>
+      <c r="F143" s="3">
+        <v>0</v>
+      </c>
+      <c r="H143" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I143" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K143" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="L143" s="6" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
@@ -6509,7 +6557,7 @@
         <v>265</v>
       </c>
       <c r="C144" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D144" t="s">
         <v>6</v>
@@ -6532,26 +6580,20 @@
         <v>265</v>
       </c>
       <c r="C145" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D145" t="s">
         <v>6</v>
       </c>
-      <c r="F145" s="3">
-        <v>0</v>
-      </c>
-      <c r="H145" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I145" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K145" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="L145" s="6" t="s">
-        <v>291</v>
-      </c>
+      <c r="F145" s="8">
+        <v>0</v>
+      </c>
+      <c r="G145" s="8"/>
+      <c r="H145" s="8"/>
+      <c r="I145" s="8"/>
+      <c r="J145" s="8"/>
+      <c r="K145" s="8"/>
+      <c r="L145" s="9"/>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
@@ -6561,26 +6603,20 @@
         <v>265</v>
       </c>
       <c r="C146" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D146" t="s">
         <v>6</v>
       </c>
-      <c r="F146" s="3">
-        <v>0</v>
-      </c>
-      <c r="H146" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I146" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K146" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="L146" s="6" t="s">
-        <v>291</v>
-      </c>
+      <c r="F146" s="8">
+        <v>0</v>
+      </c>
+      <c r="G146" s="8"/>
+      <c r="H146" s="8"/>
+      <c r="I146" s="8"/>
+      <c r="J146" s="8"/>
+      <c r="K146" s="8"/>
+      <c r="L146" s="9"/>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
@@ -6590,26 +6626,20 @@
         <v>265</v>
       </c>
       <c r="C147" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D147" t="s">
         <v>6</v>
       </c>
-      <c r="F147" s="3">
-        <v>0</v>
-      </c>
-      <c r="H147" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I147" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K147" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="L147" s="6" t="s">
-        <v>291</v>
-      </c>
+      <c r="F147" s="8">
+        <v>0</v>
+      </c>
+      <c r="G147" s="8"/>
+      <c r="H147" s="8"/>
+      <c r="I147" s="8"/>
+      <c r="J147" s="8"/>
+      <c r="K147" s="8"/>
+      <c r="L147" s="9"/>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
@@ -6619,20 +6649,26 @@
         <v>265</v>
       </c>
       <c r="C148" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D148" t="s">
         <v>6</v>
       </c>
-      <c r="F148" s="8">
-        <v>0</v>
-      </c>
-      <c r="G148" s="8"/>
-      <c r="H148" s="8"/>
-      <c r="I148" s="8"/>
-      <c r="J148" s="8"/>
-      <c r="K148" s="8"/>
-      <c r="L148" s="9"/>
+      <c r="F148" s="3">
+        <v>0</v>
+      </c>
+      <c r="H148" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K148" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="L148" s="6" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
@@ -6642,7 +6678,7 @@
         <v>265</v>
       </c>
       <c r="C149" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D149" t="s">
         <v>6</v>
@@ -6671,7 +6707,7 @@
         <v>265</v>
       </c>
       <c r="C150" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D150" t="s">
         <v>6</v>
@@ -6700,174 +6736,170 @@
         <v>265</v>
       </c>
       <c r="C151" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D151" t="s">
         <v>6</v>
       </c>
-      <c r="F151" s="3">
-        <v>0</v>
-      </c>
-      <c r="H151" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I151" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K151" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="L151" s="6" t="s">
-        <v>291</v>
-      </c>
+      <c r="F151" s="8">
+        <v>0</v>
+      </c>
+      <c r="G151" s="8"/>
+      <c r="H151" s="8"/>
+      <c r="I151" s="8"/>
+      <c r="J151" s="8"/>
+      <c r="K151" s="8"/>
+      <c r="L151" s="9"/>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>404</v>
+        <v>4</v>
       </c>
       <c r="B152" t="s">
-        <v>408</v>
+        <v>265</v>
       </c>
       <c r="C152" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="D152" t="s">
-        <v>388</v>
+        <v>6</v>
       </c>
       <c r="F152" s="3">
-        <v>19</v>
-      </c>
-      <c r="G152" s="3" t="s">
-        <v>174</v>
+        <v>0</v>
       </c>
       <c r="H152" s="3" t="s">
-        <v>391</v>
+        <v>36</v>
       </c>
       <c r="I152" s="3" t="s">
-        <v>409</v>
+        <v>135</v>
       </c>
       <c r="K152" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="L152" s="7" t="s">
-        <v>411</v>
+        <v>292</v>
+      </c>
+      <c r="L152" s="6" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>404</v>
+        <v>4</v>
       </c>
       <c r="B153" t="s">
-        <v>408</v>
+        <v>265</v>
       </c>
       <c r="C153" t="s">
-        <v>305</v>
+        <v>287</v>
       </c>
       <c r="D153" t="s">
-        <v>388</v>
+        <v>6</v>
       </c>
       <c r="F153" s="3">
         <v>0</v>
       </c>
-      <c r="G153" s="3" t="s">
-        <v>174</v>
-      </c>
       <c r="H153" s="3" t="s">
-        <v>391</v>
+        <v>36</v>
       </c>
       <c r="I153" s="3" t="s">
-        <v>409</v>
+        <v>135</v>
       </c>
       <c r="K153" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="L153" s="7" t="s">
-        <v>411</v>
+        <v>292</v>
+      </c>
+      <c r="L153" s="6" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>389</v>
+        <v>4</v>
       </c>
       <c r="B154" t="s">
-        <v>408</v>
+        <v>265</v>
       </c>
       <c r="C154" t="s">
-        <v>306</v>
+        <v>288</v>
       </c>
       <c r="D154" t="s">
-        <v>388</v>
-      </c>
-      <c r="F154" s="8"/>
-      <c r="G154" s="8"/>
-      <c r="H154" s="8"/>
-      <c r="I154" s="8"/>
-      <c r="J154" s="8"/>
-      <c r="K154" s="8"/>
-      <c r="L154" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="F154" s="3">
+        <v>0</v>
+      </c>
+      <c r="H154" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I154" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K154" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="L154" s="6" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="B155" t="s">
         <v>408</v>
       </c>
       <c r="C155" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D155" t="s">
         <v>388</v>
       </c>
       <c r="F155" s="3">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H155" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I155" s="3" t="s">
-        <v>392</v>
+        <v>409</v>
       </c>
       <c r="K155" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="L155" s="6" t="s">
-        <v>400</v>
+        <v>410</v>
+      </c>
+      <c r="L155" s="7" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="B156" t="s">
         <v>408</v>
       </c>
       <c r="C156" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D156" t="s">
         <v>388</v>
       </c>
       <c r="F156" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H156" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>539</v>
+        <v>409</v>
       </c>
       <c r="K156" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="L156" s="6" t="s">
-        <v>537</v>
+        <v>410</v>
+      </c>
+      <c r="L156" s="7" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.2">
@@ -6878,29 +6910,18 @@
         <v>408</v>
       </c>
       <c r="C157" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D157" t="s">
         <v>388</v>
       </c>
-      <c r="F157" s="3">
-        <v>15</v>
-      </c>
-      <c r="G157" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="H157" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="I157" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="K157" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="L157" s="6" t="s">
-        <v>467</v>
-      </c>
+      <c r="F157" s="8"/>
+      <c r="G157" s="8"/>
+      <c r="H157" s="8"/>
+      <c r="I157" s="8"/>
+      <c r="J157" s="8"/>
+      <c r="K157" s="8"/>
+      <c r="L157" s="9"/>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
@@ -6910,28 +6931,28 @@
         <v>408</v>
       </c>
       <c r="C158" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D158" t="s">
         <v>388</v>
       </c>
       <c r="F158" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G158" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H158" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I158" s="3" t="s">
-        <v>432</v>
+        <v>392</v>
       </c>
       <c r="K158" s="3" t="s">
-        <v>468</v>
+        <v>393</v>
       </c>
       <c r="L158" s="6" t="s">
-        <v>467</v>
+        <v>400</v>
       </c>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.2">
@@ -6942,28 +6963,28 @@
         <v>408</v>
       </c>
       <c r="C159" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D159" t="s">
         <v>388</v>
       </c>
       <c r="F159" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G159" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H159" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I159" s="3" t="s">
-        <v>432</v>
+        <v>539</v>
       </c>
       <c r="K159" s="3" t="s">
-        <v>468</v>
+        <v>538</v>
       </c>
       <c r="L159" s="6" t="s">
-        <v>467</v>
+        <v>537</v>
       </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.2">
@@ -6974,13 +6995,13 @@
         <v>408</v>
       </c>
       <c r="C160" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D160" t="s">
         <v>388</v>
       </c>
       <c r="F160" s="3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G160" s="3" t="s">
         <v>174</v>
@@ -7006,7 +7027,7 @@
         <v>408</v>
       </c>
       <c r="C161" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D161" t="s">
         <v>388</v>
@@ -7038,7 +7059,7 @@
         <v>408</v>
       </c>
       <c r="C162" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D162" t="s">
         <v>388</v>
@@ -7070,28 +7091,28 @@
         <v>408</v>
       </c>
       <c r="C163" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D163" t="s">
         <v>388</v>
       </c>
       <c r="F163" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G163" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H163" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I163" s="3" t="s">
-        <v>490</v>
+        <v>432</v>
       </c>
       <c r="K163" s="3" t="s">
-        <v>489</v>
+        <v>468</v>
       </c>
       <c r="L163" s="6" t="s">
-        <v>488</v>
+        <v>467</v>
       </c>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.2">
@@ -7102,13 +7123,13 @@
         <v>408</v>
       </c>
       <c r="C164" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D164" t="s">
         <v>388</v>
       </c>
       <c r="F164" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G164" s="3" t="s">
         <v>174</v>
@@ -7120,10 +7141,10 @@
         <v>432</v>
       </c>
       <c r="K164" s="3" t="s">
-        <v>431</v>
+        <v>468</v>
       </c>
       <c r="L164" s="6" t="s">
-        <v>430</v>
+        <v>467</v>
       </c>
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.2">
@@ -7134,7 +7155,7 @@
         <v>408</v>
       </c>
       <c r="C165" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D165" t="s">
         <v>388</v>
@@ -7152,10 +7173,10 @@
         <v>432</v>
       </c>
       <c r="K165" s="3" t="s">
-        <v>431</v>
+        <v>468</v>
       </c>
       <c r="L165" s="6" t="s">
-        <v>430</v>
+        <v>467</v>
       </c>
     </row>
     <row r="166" spans="1:12" x14ac:dyDescent="0.2">
@@ -7166,28 +7187,28 @@
         <v>408</v>
       </c>
       <c r="C166" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D166" t="s">
         <v>388</v>
       </c>
       <c r="F166" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H166" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I166" s="3" t="s">
-        <v>432</v>
+        <v>490</v>
       </c>
       <c r="K166" s="3" t="s">
-        <v>431</v>
+        <v>489</v>
       </c>
       <c r="L166" s="6" t="s">
-        <v>430</v>
+        <v>488</v>
       </c>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.2">
@@ -7198,13 +7219,13 @@
         <v>408</v>
       </c>
       <c r="C167" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D167" t="s">
         <v>388</v>
       </c>
       <c r="F167" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G167" s="3" t="s">
         <v>174</v>
@@ -7230,7 +7251,7 @@
         <v>408</v>
       </c>
       <c r="C168" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D168" t="s">
         <v>388</v>
@@ -7262,13 +7283,13 @@
         <v>408</v>
       </c>
       <c r="C169" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D169" t="s">
         <v>388</v>
       </c>
       <c r="F169" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G169" s="3" t="s">
         <v>174</v>
@@ -7277,13 +7298,13 @@
         <v>391</v>
       </c>
       <c r="I169" s="3" t="s">
-        <v>463</v>
+        <v>432</v>
       </c>
       <c r="K169" s="3" t="s">
-        <v>462</v>
+        <v>431</v>
       </c>
       <c r="L169" s="6" t="s">
-        <v>461</v>
+        <v>430</v>
       </c>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.2">
@@ -7294,18 +7315,29 @@
         <v>408</v>
       </c>
       <c r="C170" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D170" t="s">
         <v>388</v>
       </c>
-      <c r="F170" s="8"/>
-      <c r="G170" s="8"/>
-      <c r="H170" s="8"/>
-      <c r="I170" s="8"/>
-      <c r="J170" s="8"/>
-      <c r="K170" s="8"/>
-      <c r="L170" s="9"/>
+      <c r="F170" s="3">
+        <v>0</v>
+      </c>
+      <c r="G170" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H170" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I170" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="K170" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="L170" s="6" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
@@ -7315,13 +7347,13 @@
         <v>408</v>
       </c>
       <c r="C171" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D171" t="s">
         <v>388</v>
       </c>
       <c r="F171" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G171" s="3" t="s">
         <v>174</v>
@@ -7330,13 +7362,13 @@
         <v>391</v>
       </c>
       <c r="I171" s="3" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="K171" s="3" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="L171" s="6" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
     </row>
     <row r="172" spans="1:12" x14ac:dyDescent="0.2">
@@ -7347,28 +7379,28 @@
         <v>408</v>
       </c>
       <c r="C172" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D172" t="s">
         <v>388</v>
       </c>
       <c r="F172" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H172" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I172" s="3" t="s">
-        <v>530</v>
+        <v>463</v>
       </c>
       <c r="K172" s="3" t="s">
-        <v>549</v>
+        <v>462</v>
       </c>
       <c r="L172" s="6" t="s">
-        <v>548</v>
+        <v>461</v>
       </c>
     </row>
     <row r="173" spans="1:12" x14ac:dyDescent="0.2">
@@ -7379,29 +7411,18 @@
         <v>408</v>
       </c>
       <c r="C173" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D173" t="s">
         <v>388</v>
       </c>
-      <c r="F173" s="3">
-        <v>5</v>
-      </c>
-      <c r="G173" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="H173" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="I173" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="K173" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="L173" s="6" t="s">
-        <v>485</v>
-      </c>
+      <c r="F173" s="8"/>
+      <c r="G173" s="8"/>
+      <c r="H173" s="8"/>
+      <c r="I173" s="8"/>
+      <c r="J173" s="8"/>
+      <c r="K173" s="8"/>
+      <c r="L173" s="9"/>
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
@@ -7411,28 +7432,28 @@
         <v>408</v>
       </c>
       <c r="C174" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D174" t="s">
         <v>388</v>
       </c>
       <c r="F174" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G174" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H174" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I174" s="3" t="s">
-        <v>487</v>
+        <v>441</v>
       </c>
       <c r="K174" s="3" t="s">
-        <v>484</v>
+        <v>440</v>
       </c>
       <c r="L174" s="6" t="s">
-        <v>483</v>
+        <v>439</v>
       </c>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.2">
@@ -7443,7 +7464,7 @@
         <v>408</v>
       </c>
       <c r="C175" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D175" t="s">
         <v>388</v>
@@ -7458,13 +7479,13 @@
         <v>391</v>
       </c>
       <c r="I175" s="3" t="s">
-        <v>544</v>
+        <v>530</v>
       </c>
       <c r="K175" s="3" t="s">
-        <v>543</v>
+        <v>549</v>
       </c>
       <c r="L175" s="6" t="s">
-        <v>542</v>
+        <v>548</v>
       </c>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.2">
@@ -7475,13 +7496,13 @@
         <v>408</v>
       </c>
       <c r="C176" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D176" t="s">
         <v>388</v>
       </c>
       <c r="F176" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G176" s="3" t="s">
         <v>435</v>
@@ -7490,13 +7511,13 @@
         <v>391</v>
       </c>
       <c r="I176" s="3" t="s">
-        <v>559</v>
+        <v>487</v>
       </c>
       <c r="K176" s="3" t="s">
-        <v>558</v>
+        <v>486</v>
       </c>
       <c r="L176" s="6" t="s">
-        <v>557</v>
+        <v>485</v>
       </c>
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.2">
@@ -7507,28 +7528,28 @@
         <v>408</v>
       </c>
       <c r="C177" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D177" t="s">
         <v>388</v>
       </c>
       <c r="F177" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G177" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H177" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I177" s="3" t="s">
-        <v>452</v>
+        <v>487</v>
       </c>
       <c r="K177" s="3" t="s">
-        <v>451</v>
+        <v>484</v>
       </c>
       <c r="L177" s="6" t="s">
-        <v>450</v>
+        <v>483</v>
       </c>
     </row>
     <row r="178" spans="1:12" x14ac:dyDescent="0.2">
@@ -7539,13 +7560,13 @@
         <v>408</v>
       </c>
       <c r="C178" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D178" t="s">
         <v>388</v>
       </c>
       <c r="F178" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G178" s="3" t="s">
         <v>435</v>
@@ -7554,45 +7575,45 @@
         <v>391</v>
       </c>
       <c r="I178" s="3" t="s">
-        <v>562</v>
+        <v>544</v>
       </c>
       <c r="K178" s="3" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="L178" s="6" t="s">
-        <v>560</v>
+        <v>542</v>
       </c>
     </row>
     <row r="179" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="B179" t="s">
         <v>408</v>
       </c>
       <c r="C179" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D179" t="s">
         <v>388</v>
       </c>
       <c r="F179" s="3">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G179" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H179" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I179" s="3" t="s">
-        <v>460</v>
+        <v>559</v>
       </c>
       <c r="K179" s="3" t="s">
-        <v>459</v>
+        <v>558</v>
       </c>
       <c r="L179" s="6" t="s">
-        <v>458</v>
+        <v>557</v>
       </c>
     </row>
     <row r="180" spans="1:12" x14ac:dyDescent="0.2">
@@ -7603,7 +7624,7 @@
         <v>408</v>
       </c>
       <c r="C180" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D180" t="s">
         <v>388</v>
@@ -7612,19 +7633,19 @@
         <v>1</v>
       </c>
       <c r="G180" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H180" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I180" s="3" t="s">
-        <v>490</v>
+        <v>452</v>
       </c>
       <c r="K180" s="3" t="s">
-        <v>501</v>
+        <v>451</v>
       </c>
       <c r="L180" s="6" t="s">
-        <v>500</v>
+        <v>450</v>
       </c>
     </row>
     <row r="181" spans="1:12" x14ac:dyDescent="0.2">
@@ -7635,13 +7656,13 @@
         <v>408</v>
       </c>
       <c r="C181" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D181" t="s">
         <v>388</v>
       </c>
       <c r="F181" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G181" s="3" t="s">
         <v>435</v>
@@ -7650,45 +7671,45 @@
         <v>391</v>
       </c>
       <c r="I181" s="3" t="s">
-        <v>490</v>
+        <v>562</v>
       </c>
       <c r="K181" s="3" t="s">
-        <v>502</v>
+        <v>561</v>
       </c>
       <c r="L181" s="6" t="s">
-        <v>503</v>
+        <v>560</v>
       </c>
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="B182" t="s">
         <v>408</v>
       </c>
       <c r="C182" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D182" t="s">
         <v>388</v>
       </c>
       <c r="F182" s="3">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H182" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I182" s="3" t="s">
-        <v>506</v>
+        <v>460</v>
       </c>
       <c r="K182" s="3" t="s">
-        <v>519</v>
+        <v>459</v>
       </c>
       <c r="L182" s="6" t="s">
-        <v>518</v>
+        <v>458</v>
       </c>
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.2">
@@ -7699,13 +7720,13 @@
         <v>408</v>
       </c>
       <c r="C183" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D183" t="s">
         <v>388</v>
       </c>
       <c r="F183" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G183" s="3" t="s">
         <v>435</v>
@@ -7714,13 +7735,13 @@
         <v>391</v>
       </c>
       <c r="I183" s="3" t="s">
-        <v>530</v>
+        <v>490</v>
       </c>
       <c r="K183" s="3" t="s">
-        <v>564</v>
+        <v>501</v>
       </c>
       <c r="L183" s="6" t="s">
-        <v>563</v>
+        <v>500</v>
       </c>
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.2">
@@ -7731,28 +7752,28 @@
         <v>408</v>
       </c>
       <c r="C184" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D184" t="s">
         <v>388</v>
       </c>
       <c r="F184" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H184" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I184" s="3" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="K184" s="3" t="s">
-        <v>481</v>
+        <v>502</v>
       </c>
       <c r="L184" s="6" t="s">
-        <v>480</v>
+        <v>503</v>
       </c>
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.2">
@@ -7763,28 +7784,28 @@
         <v>408</v>
       </c>
       <c r="C185" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D185" t="s">
         <v>388</v>
       </c>
       <c r="F185" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H185" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I185" s="3" t="s">
-        <v>477</v>
+        <v>506</v>
       </c>
       <c r="K185" s="3" t="s">
-        <v>476</v>
+        <v>519</v>
       </c>
       <c r="L185" s="6" t="s">
-        <v>475</v>
+        <v>518</v>
       </c>
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.2">
@@ -7795,28 +7816,28 @@
         <v>408</v>
       </c>
       <c r="C186" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D186" t="s">
         <v>388</v>
       </c>
       <c r="F186" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G186" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H186" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I186" s="3" t="s">
-        <v>477</v>
+        <v>530</v>
       </c>
       <c r="K186" s="3" t="s">
-        <v>476</v>
+        <v>564</v>
       </c>
       <c r="L186" s="6" t="s">
-        <v>475</v>
+        <v>563</v>
       </c>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.2">
@@ -7827,13 +7848,13 @@
         <v>408</v>
       </c>
       <c r="C187" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D187" t="s">
         <v>388</v>
       </c>
       <c r="F187" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G187" s="3" t="s">
         <v>174</v>
@@ -7842,13 +7863,13 @@
         <v>391</v>
       </c>
       <c r="I187" s="3" t="s">
-        <v>425</v>
+        <v>482</v>
       </c>
       <c r="K187" s="3" t="s">
-        <v>428</v>
+        <v>481</v>
       </c>
       <c r="L187" s="6" t="s">
-        <v>426</v>
+        <v>480</v>
       </c>
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.2">
@@ -7859,13 +7880,13 @@
         <v>408</v>
       </c>
       <c r="C188" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D188" t="s">
         <v>388</v>
       </c>
       <c r="F188" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G188" s="3" t="s">
         <v>174</v>
@@ -7874,13 +7895,13 @@
         <v>391</v>
       </c>
       <c r="I188" s="3" t="s">
-        <v>425</v>
+        <v>477</v>
       </c>
       <c r="K188" s="3" t="s">
-        <v>424</v>
+        <v>476</v>
       </c>
       <c r="L188" s="6" t="s">
-        <v>423</v>
+        <v>475</v>
       </c>
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.2">
@@ -7891,13 +7912,13 @@
         <v>408</v>
       </c>
       <c r="C189" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D189" t="s">
         <v>388</v>
       </c>
       <c r="F189" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G189" s="3" t="s">
         <v>174</v>
@@ -7906,13 +7927,13 @@
         <v>391</v>
       </c>
       <c r="I189" s="3" t="s">
-        <v>425</v>
+        <v>477</v>
       </c>
       <c r="K189" s="3" t="s">
-        <v>427</v>
+        <v>476</v>
       </c>
       <c r="L189" s="6" t="s">
-        <v>429</v>
+        <v>475</v>
       </c>
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.2">
@@ -7923,28 +7944,28 @@
         <v>408</v>
       </c>
       <c r="C190" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D190" t="s">
         <v>388</v>
       </c>
       <c r="F190" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G190" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H190" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I190" s="3" t="s">
-        <v>539</v>
+        <v>425</v>
       </c>
       <c r="K190" s="3" t="s">
-        <v>541</v>
+        <v>428</v>
       </c>
       <c r="L190" s="6" t="s">
-        <v>540</v>
+        <v>426</v>
       </c>
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.2">
@@ -7955,28 +7976,28 @@
         <v>408</v>
       </c>
       <c r="C191" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D191" t="s">
         <v>388</v>
       </c>
       <c r="F191" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G191" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H191" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I191" s="3" t="s">
-        <v>555</v>
+        <v>425</v>
       </c>
       <c r="K191" s="3" t="s">
-        <v>554</v>
+        <v>424</v>
       </c>
       <c r="L191" s="6" t="s">
-        <v>553</v>
+        <v>423</v>
       </c>
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.2">
@@ -7987,28 +8008,28 @@
         <v>408</v>
       </c>
       <c r="C192" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D192" t="s">
         <v>388</v>
       </c>
       <c r="F192" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G192" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H192" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I192" s="3" t="s">
-        <v>482</v>
+        <v>425</v>
       </c>
       <c r="K192" s="3" t="s">
-        <v>554</v>
+        <v>427</v>
       </c>
       <c r="L192" s="6" t="s">
-        <v>556</v>
+        <v>429</v>
       </c>
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.2">
@@ -8019,7 +8040,7 @@
         <v>408</v>
       </c>
       <c r="C193" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D193" t="s">
         <v>388</v>
@@ -8034,13 +8055,13 @@
         <v>391</v>
       </c>
       <c r="I193" s="3" t="s">
-        <v>516</v>
+        <v>539</v>
       </c>
       <c r="K193" s="3" t="s">
-        <v>517</v>
+        <v>541</v>
       </c>
       <c r="L193" s="6" t="s">
-        <v>515</v>
+        <v>540</v>
       </c>
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.2">
@@ -8051,13 +8072,13 @@
         <v>408</v>
       </c>
       <c r="C194" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D194" t="s">
         <v>388</v>
       </c>
       <c r="F194" s="3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G194" s="3" t="s">
         <v>435</v>
@@ -8066,13 +8087,13 @@
         <v>391</v>
       </c>
       <c r="I194" s="3" t="s">
-        <v>536</v>
+        <v>555</v>
       </c>
       <c r="K194" s="3" t="s">
-        <v>535</v>
+        <v>554</v>
       </c>
       <c r="L194" s="6" t="s">
-        <v>534</v>
+        <v>553</v>
       </c>
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.2">
@@ -8083,28 +8104,28 @@
         <v>408</v>
       </c>
       <c r="C195" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D195" t="s">
         <v>388</v>
       </c>
       <c r="F195" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G195" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H195" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I195" s="3" t="s">
-        <v>396</v>
+        <v>482</v>
       </c>
       <c r="K195" s="3" t="s">
-        <v>395</v>
+        <v>554</v>
       </c>
       <c r="L195" s="6" t="s">
-        <v>394</v>
+        <v>556</v>
       </c>
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.2">
@@ -8115,28 +8136,28 @@
         <v>408</v>
       </c>
       <c r="C196" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D196" t="s">
         <v>388</v>
       </c>
       <c r="F196" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G196" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H196" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I196" s="3" t="s">
-        <v>414</v>
+        <v>516</v>
       </c>
       <c r="K196" s="3" t="s">
-        <v>419</v>
+        <v>517</v>
       </c>
       <c r="L196" s="6" t="s">
-        <v>418</v>
+        <v>515</v>
       </c>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.2">
@@ -8147,28 +8168,28 @@
         <v>408</v>
       </c>
       <c r="C197" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D197" t="s">
         <v>388</v>
       </c>
       <c r="F197" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G197" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H197" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I197" s="3" t="s">
-        <v>397</v>
+        <v>536</v>
       </c>
       <c r="K197" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="L197" s="7" t="s">
-        <v>399</v>
+        <v>535</v>
+      </c>
+      <c r="L197" s="6" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.2">
@@ -8179,13 +8200,13 @@
         <v>408</v>
       </c>
       <c r="C198" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D198" t="s">
         <v>388</v>
       </c>
       <c r="F198" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G198" s="3" t="s">
         <v>174</v>
@@ -8194,13 +8215,13 @@
         <v>391</v>
       </c>
       <c r="I198" s="3" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="K198" s="3" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
       <c r="L198" s="6" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.2">
@@ -8211,28 +8232,28 @@
         <v>408</v>
       </c>
       <c r="C199" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D199" t="s">
         <v>388</v>
       </c>
       <c r="F199" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G199" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H199" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I199" s="3" t="s">
-        <v>567</v>
+        <v>414</v>
       </c>
       <c r="K199" s="3" t="s">
-        <v>566</v>
+        <v>419</v>
       </c>
       <c r="L199" s="6" t="s">
-        <v>565</v>
+        <v>418</v>
       </c>
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.2">
@@ -8243,7 +8264,7 @@
         <v>408</v>
       </c>
       <c r="C200" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D200" t="s">
         <v>388</v>
@@ -8252,19 +8273,19 @@
         <v>2</v>
       </c>
       <c r="G200" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H200" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I200" s="3" t="s">
-        <v>506</v>
+        <v>397</v>
       </c>
       <c r="K200" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="L200" s="6" t="s">
-        <v>507</v>
+        <v>398</v>
+      </c>
+      <c r="L200" s="7" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.2">
@@ -8275,28 +8296,28 @@
         <v>408</v>
       </c>
       <c r="C201" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D201" t="s">
         <v>388</v>
       </c>
       <c r="F201" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G201" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H201" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I201" s="3" t="s">
-        <v>552</v>
+        <v>414</v>
       </c>
       <c r="K201" s="3" t="s">
-        <v>551</v>
+        <v>413</v>
       </c>
       <c r="L201" s="6" t="s">
-        <v>550</v>
+        <v>412</v>
       </c>
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.2">
@@ -8307,13 +8328,13 @@
         <v>408</v>
       </c>
       <c r="C202" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D202" t="s">
         <v>388</v>
       </c>
       <c r="F202" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G202" s="3" t="s">
         <v>435</v>
@@ -8322,13 +8343,13 @@
         <v>391</v>
       </c>
       <c r="I202" s="3" t="s">
-        <v>552</v>
+        <v>567</v>
       </c>
       <c r="K202" s="3" t="s">
-        <v>551</v>
+        <v>566</v>
       </c>
       <c r="L202" s="6" t="s">
-        <v>550</v>
+        <v>565</v>
       </c>
     </row>
     <row r="203" spans="1:12" x14ac:dyDescent="0.2">
@@ -8339,13 +8360,13 @@
         <v>408</v>
       </c>
       <c r="C203" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D203" t="s">
         <v>388</v>
       </c>
       <c r="F203" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G203" s="3" t="s">
         <v>435</v>
@@ -8354,13 +8375,13 @@
         <v>391</v>
       </c>
       <c r="I203" s="3" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="K203" s="3" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="L203" s="6" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.2">
@@ -8371,13 +8392,13 @@
         <v>408</v>
       </c>
       <c r="C204" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D204" t="s">
         <v>388</v>
       </c>
       <c r="F204" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G204" s="3" t="s">
         <v>435</v>
@@ -8386,13 +8407,13 @@
         <v>391</v>
       </c>
       <c r="I204" s="3" t="s">
-        <v>530</v>
+        <v>552</v>
       </c>
       <c r="K204" s="3" t="s">
-        <v>529</v>
+        <v>551</v>
       </c>
       <c r="L204" s="6" t="s">
-        <v>528</v>
+        <v>550</v>
       </c>
     </row>
     <row r="205" spans="1:12" x14ac:dyDescent="0.2">
@@ -8403,13 +8424,13 @@
         <v>408</v>
       </c>
       <c r="C205" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D205" t="s">
         <v>388</v>
       </c>
       <c r="F205" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G205" s="3" t="s">
         <v>435</v>
@@ -8418,13 +8439,13 @@
         <v>391</v>
       </c>
       <c r="I205" s="3" t="s">
-        <v>527</v>
+        <v>552</v>
       </c>
       <c r="K205" s="3" t="s">
-        <v>526</v>
+        <v>551</v>
       </c>
       <c r="L205" s="6" t="s">
-        <v>525</v>
+        <v>550</v>
       </c>
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.2">
@@ -8435,13 +8456,13 @@
         <v>408</v>
       </c>
       <c r="C206" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D206" t="s">
         <v>388</v>
       </c>
       <c r="F206" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G206" s="3" t="s">
         <v>435</v>
@@ -8450,13 +8471,13 @@
         <v>391</v>
       </c>
       <c r="I206" s="3" t="s">
-        <v>547</v>
+        <v>514</v>
       </c>
       <c r="K206" s="3" t="s">
-        <v>546</v>
+        <v>513</v>
       </c>
       <c r="L206" s="6" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
     </row>
     <row r="207" spans="1:12" x14ac:dyDescent="0.2">
@@ -8467,13 +8488,13 @@
         <v>408</v>
       </c>
       <c r="C207" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D207" t="s">
         <v>388</v>
       </c>
       <c r="F207" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G207" s="3" t="s">
         <v>435</v>
@@ -8482,13 +8503,13 @@
         <v>391</v>
       </c>
       <c r="I207" s="3" t="s">
-        <v>506</v>
+        <v>530</v>
       </c>
       <c r="K207" s="3" t="s">
-        <v>505</v>
+        <v>529</v>
       </c>
       <c r="L207" s="6" t="s">
-        <v>504</v>
+        <v>528</v>
       </c>
     </row>
     <row r="208" spans="1:12" x14ac:dyDescent="0.2">
@@ -8499,13 +8520,13 @@
         <v>408</v>
       </c>
       <c r="C208" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D208" t="s">
         <v>388</v>
       </c>
       <c r="F208" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G208" s="3" t="s">
         <v>435</v>
@@ -8514,13 +8535,13 @@
         <v>391</v>
       </c>
       <c r="I208" s="3" t="s">
-        <v>506</v>
+        <v>527</v>
       </c>
       <c r="K208" s="3" t="s">
-        <v>505</v>
+        <v>526</v>
       </c>
       <c r="L208" s="6" t="s">
-        <v>504</v>
+        <v>525</v>
       </c>
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.2">
@@ -8531,13 +8552,13 @@
         <v>408</v>
       </c>
       <c r="C209" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D209" t="s">
         <v>388</v>
       </c>
       <c r="F209" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G209" s="3" t="s">
         <v>435</v>
@@ -8546,13 +8567,13 @@
         <v>391</v>
       </c>
       <c r="I209" s="3" t="s">
-        <v>506</v>
+        <v>547</v>
       </c>
       <c r="K209" s="3" t="s">
-        <v>505</v>
+        <v>546</v>
       </c>
       <c r="L209" s="6" t="s">
-        <v>504</v>
+        <v>545</v>
       </c>
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.2">
@@ -8563,13 +8584,13 @@
         <v>408</v>
       </c>
       <c r="C210" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D210" t="s">
         <v>388</v>
       </c>
       <c r="F210" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G210" s="3" t="s">
         <v>435</v>
@@ -8595,13 +8616,13 @@
         <v>408</v>
       </c>
       <c r="C211" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D211" t="s">
         <v>388</v>
       </c>
       <c r="F211" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G211" s="3" t="s">
         <v>435</v>
@@ -8610,13 +8631,13 @@
         <v>391</v>
       </c>
       <c r="I211" s="3" t="s">
-        <v>490</v>
+        <v>506</v>
       </c>
       <c r="K211" s="3" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="L211" s="6" t="s">
-        <v>493</v>
+        <v>504</v>
       </c>
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.2">
@@ -8627,13 +8648,13 @@
         <v>408</v>
       </c>
       <c r="C212" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D212" t="s">
         <v>388</v>
       </c>
       <c r="F212" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G212" s="3" t="s">
         <v>435</v>
@@ -8642,13 +8663,13 @@
         <v>391</v>
       </c>
       <c r="I212" s="3" t="s">
-        <v>490</v>
+        <v>506</v>
       </c>
       <c r="K212" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="L212" s="7" t="s">
-        <v>496</v>
+        <v>505</v>
+      </c>
+      <c r="L212" s="6" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.2">
@@ -8659,13 +8680,13 @@
         <v>408</v>
       </c>
       <c r="C213" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D213" t="s">
         <v>388</v>
       </c>
       <c r="F213" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G213" s="3" t="s">
         <v>435</v>
@@ -8674,13 +8695,13 @@
         <v>391</v>
       </c>
       <c r="I213" s="3" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="K213" s="3" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="L213" s="6" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
     </row>
     <row r="214" spans="1:12" x14ac:dyDescent="0.2">
@@ -8691,13 +8712,13 @@
         <v>408</v>
       </c>
       <c r="C214" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D214" t="s">
         <v>388</v>
       </c>
       <c r="F214" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G214" s="3" t="s">
         <v>435</v>
@@ -8709,10 +8730,10 @@
         <v>490</v>
       </c>
       <c r="K214" s="3" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="L214" s="6" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="215" spans="1:12" x14ac:dyDescent="0.2">
@@ -8723,13 +8744,13 @@
         <v>408</v>
       </c>
       <c r="C215" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D215" t="s">
         <v>388</v>
       </c>
       <c r="F215" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G215" s="3" t="s">
         <v>435</v>
@@ -8741,10 +8762,10 @@
         <v>490</v>
       </c>
       <c r="K215" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="L215" s="6" t="s">
-        <v>491</v>
+        <v>495</v>
+      </c>
+      <c r="L215" s="7" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="216" spans="1:12" x14ac:dyDescent="0.2">
@@ -8755,13 +8776,13 @@
         <v>408</v>
       </c>
       <c r="C216" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D216" t="s">
         <v>388</v>
       </c>
       <c r="F216" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G216" s="3" t="s">
         <v>435</v>
@@ -8770,13 +8791,13 @@
         <v>391</v>
       </c>
       <c r="I216" s="3" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
       <c r="K216" s="3" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="L216" s="6" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.2">
@@ -8787,7 +8808,7 @@
         <v>408</v>
       </c>
       <c r="C217" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D217" t="s">
         <v>388</v>
@@ -8802,126 +8823,126 @@
         <v>391</v>
       </c>
       <c r="I217" s="3" t="s">
-        <v>396</v>
+        <v>490</v>
       </c>
       <c r="K217" s="3" t="s">
-        <v>521</v>
+        <v>492</v>
       </c>
       <c r="L217" s="6" t="s">
-        <v>520</v>
+        <v>491</v>
       </c>
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="B218" t="s">
         <v>408</v>
       </c>
       <c r="C218" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D218" t="s">
         <v>388</v>
       </c>
       <c r="F218" s="3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G218" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H218" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I218" s="3" t="s">
-        <v>466</v>
+        <v>490</v>
       </c>
       <c r="K218" s="3" t="s">
-        <v>465</v>
+        <v>492</v>
       </c>
       <c r="L218" s="6" t="s">
-        <v>464</v>
+        <v>491</v>
       </c>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="B219" t="s">
         <v>408</v>
       </c>
       <c r="C219" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D219" t="s">
         <v>388</v>
       </c>
       <c r="F219" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G219" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H219" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I219" s="3" t="s">
-        <v>422</v>
+        <v>490</v>
       </c>
       <c r="K219" s="3" t="s">
-        <v>421</v>
+        <v>492</v>
       </c>
       <c r="L219" s="6" t="s">
-        <v>420</v>
+        <v>491</v>
       </c>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="B220" t="s">
         <v>408</v>
       </c>
       <c r="C220" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D220" t="s">
         <v>388</v>
       </c>
       <c r="F220" s="3">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G220" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H220" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>438</v>
+        <v>396</v>
       </c>
       <c r="K220" s="3" t="s">
-        <v>437</v>
+        <v>521</v>
       </c>
       <c r="L220" s="6" t="s">
-        <v>436</v>
+        <v>520</v>
       </c>
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="B221" t="s">
         <v>408</v>
       </c>
       <c r="C221" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D221" t="s">
         <v>388</v>
       </c>
       <c r="F221" s="3">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G221" s="3" t="s">
         <v>174</v>
@@ -8930,30 +8951,30 @@
         <v>391</v>
       </c>
       <c r="I221" s="3" t="s">
-        <v>449</v>
+        <v>466</v>
       </c>
       <c r="K221" s="3" t="s">
-        <v>448</v>
+        <v>465</v>
       </c>
       <c r="L221" s="6" t="s">
-        <v>447</v>
+        <v>464</v>
       </c>
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="B222" t="s">
         <v>408</v>
       </c>
       <c r="C222" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D222" t="s">
         <v>388</v>
       </c>
       <c r="F222" s="3">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G222" s="3" t="s">
         <v>174</v>
@@ -8962,30 +8983,30 @@
         <v>391</v>
       </c>
       <c r="I222" s="3" t="s">
-        <v>414</v>
+        <v>422</v>
       </c>
       <c r="K222" s="3" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="L222" s="6" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="B223" t="s">
         <v>408</v>
       </c>
       <c r="C223" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D223" t="s">
         <v>388</v>
       </c>
       <c r="F223" s="3">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G223" s="3" t="s">
         <v>174</v>
@@ -8994,13 +9015,13 @@
         <v>391</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="K223" s="3" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="L223" s="6" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.2">
@@ -9011,13 +9032,13 @@
         <v>408</v>
       </c>
       <c r="C224" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D224" t="s">
         <v>388</v>
       </c>
       <c r="F224" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G224" s="3" t="s">
         <v>174</v>
@@ -9026,13 +9047,13 @@
         <v>391</v>
       </c>
       <c r="I224" s="3" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="K224" s="3" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="L224" s="6" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
     </row>
     <row r="225" spans="1:12" x14ac:dyDescent="0.2">
@@ -9043,13 +9064,13 @@
         <v>408</v>
       </c>
       <c r="C225" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D225" t="s">
         <v>388</v>
       </c>
       <c r="F225" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G225" s="3" t="s">
         <v>174</v>
@@ -9061,10 +9082,10 @@
         <v>414</v>
       </c>
       <c r="K225" s="3" t="s">
-        <v>479</v>
+        <v>434</v>
       </c>
       <c r="L225" s="6" t="s">
-        <v>478</v>
+        <v>433</v>
       </c>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.2">
@@ -9075,28 +9096,28 @@
         <v>408</v>
       </c>
       <c r="C226" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D226" t="s">
         <v>388</v>
       </c>
       <c r="F226" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G226" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H226" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I226" s="3" t="s">
-        <v>511</v>
+        <v>449</v>
       </c>
       <c r="K226" s="3" t="s">
-        <v>510</v>
+        <v>448</v>
       </c>
       <c r="L226" s="6" t="s">
-        <v>509</v>
+        <v>447</v>
       </c>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.2">
@@ -9107,13 +9128,13 @@
         <v>408</v>
       </c>
       <c r="C227" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D227" t="s">
         <v>388</v>
       </c>
       <c r="F227" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G227" s="3" t="s">
         <v>174</v>
@@ -9122,13 +9143,13 @@
         <v>391</v>
       </c>
       <c r="I227" s="3" t="s">
-        <v>444</v>
+        <v>457</v>
       </c>
       <c r="K227" s="3" t="s">
-        <v>443</v>
+        <v>456</v>
       </c>
       <c r="L227" s="6" t="s">
-        <v>442</v>
+        <v>455</v>
       </c>
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.2">
@@ -9139,13 +9160,13 @@
         <v>408</v>
       </c>
       <c r="C228" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D228" t="s">
         <v>388</v>
       </c>
       <c r="F228" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G228" s="3" t="s">
         <v>174</v>
@@ -9154,13 +9175,13 @@
         <v>391</v>
       </c>
       <c r="I228" s="3" t="s">
-        <v>446</v>
+        <v>414</v>
       </c>
       <c r="K228" s="3" t="s">
-        <v>443</v>
+        <v>479</v>
       </c>
       <c r="L228" s="6" t="s">
-        <v>445</v>
+        <v>478</v>
       </c>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.2">
@@ -9171,7 +9192,7 @@
         <v>408</v>
       </c>
       <c r="C229" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D229" t="s">
         <v>388</v>
@@ -9180,36 +9201,36 @@
         <v>1</v>
       </c>
       <c r="G229" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H229" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I229" s="3" t="s">
-        <v>414</v>
+        <v>511</v>
       </c>
       <c r="K229" s="3" t="s">
-        <v>454</v>
+        <v>510</v>
       </c>
       <c r="L229" s="6" t="s">
-        <v>453</v>
+        <v>509</v>
       </c>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="B230" t="s">
         <v>408</v>
       </c>
       <c r="C230" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D230" t="s">
         <v>388</v>
       </c>
       <c r="F230" s="3">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="G230" s="3" t="s">
         <v>174</v>
@@ -9218,13 +9239,13 @@
         <v>391</v>
       </c>
       <c r="I230" s="3" t="s">
-        <v>417</v>
+        <v>444</v>
       </c>
       <c r="K230" s="3" t="s">
-        <v>416</v>
+        <v>443</v>
       </c>
       <c r="L230" s="6" t="s">
-        <v>415</v>
+        <v>442</v>
       </c>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.2">
@@ -9235,28 +9256,28 @@
         <v>408</v>
       </c>
       <c r="C231" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D231" t="s">
         <v>388</v>
       </c>
       <c r="F231" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G231" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H231" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I231" s="3" t="s">
-        <v>533</v>
+        <v>446</v>
       </c>
       <c r="K231" s="3" t="s">
-        <v>532</v>
-      </c>
-      <c r="L231" s="10" t="s">
-        <v>531</v>
+        <v>443</v>
+      </c>
+      <c r="L231" s="6" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.2">
@@ -9267,92 +9288,92 @@
         <v>408</v>
       </c>
       <c r="C232" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D232" t="s">
         <v>388</v>
       </c>
       <c r="F232" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G232" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H232" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I232" s="3" t="s">
-        <v>524</v>
+        <v>414</v>
       </c>
       <c r="K232" s="3" t="s">
-        <v>523</v>
+        <v>454</v>
       </c>
       <c r="L232" s="6" t="s">
-        <v>522</v>
+        <v>453</v>
       </c>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="B233" t="s">
         <v>408</v>
       </c>
       <c r="C233" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D233" t="s">
         <v>388</v>
       </c>
       <c r="F233" s="3">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G233" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H233" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I233" s="3" t="s">
-        <v>401</v>
+        <v>417</v>
       </c>
       <c r="K233" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="L233" s="7" t="s">
-        <v>403</v>
+        <v>416</v>
+      </c>
+      <c r="L233" s="6" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="B234" t="s">
         <v>408</v>
       </c>
       <c r="C234" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D234" t="s">
         <v>388</v>
       </c>
       <c r="F234" s="3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G234" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H234" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I234" s="3" t="s">
-        <v>405</v>
+        <v>533</v>
       </c>
       <c r="K234" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="L234" s="7" t="s">
-        <v>407</v>
+        <v>532</v>
+      </c>
+      <c r="L234" s="10" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.2">
@@ -9363,28 +9384,28 @@
         <v>408</v>
       </c>
       <c r="C235" t="s">
-        <v>58</v>
+        <v>384</v>
       </c>
       <c r="D235" t="s">
         <v>388</v>
       </c>
       <c r="F235" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G235" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H235" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I235" s="3" t="s">
-        <v>471</v>
+        <v>524</v>
       </c>
       <c r="K235" s="3" t="s">
-        <v>470</v>
+        <v>523</v>
       </c>
       <c r="L235" s="6" t="s">
-        <v>469</v>
+        <v>522</v>
       </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.2">
@@ -9395,32 +9416,128 @@
         <v>408</v>
       </c>
       <c r="C236" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D236" t="s">
         <v>388</v>
       </c>
       <c r="F236" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G236" s="3" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="H236" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I236" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="K236" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="L236" s="7" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>404</v>
+      </c>
+      <c r="B237" t="s">
+        <v>408</v>
+      </c>
+      <c r="C237" t="s">
+        <v>386</v>
+      </c>
+      <c r="D237" t="s">
+        <v>388</v>
+      </c>
+      <c r="F237" s="3">
+        <v>10</v>
+      </c>
+      <c r="G237" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H237" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I237" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="K237" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="L237" s="7" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>389</v>
+      </c>
+      <c r="B238" t="s">
+        <v>408</v>
+      </c>
+      <c r="C238" t="s">
+        <v>58</v>
+      </c>
+      <c r="D238" t="s">
+        <v>388</v>
+      </c>
+      <c r="F238" s="3">
+        <v>1</v>
+      </c>
+      <c r="G238" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H238" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I238" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="K238" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="L238" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>389</v>
+      </c>
+      <c r="B239" t="s">
+        <v>408</v>
+      </c>
+      <c r="C239" t="s">
+        <v>387</v>
+      </c>
+      <c r="D239" t="s">
+        <v>388</v>
+      </c>
+      <c r="F239" s="3">
+        <v>1</v>
+      </c>
+      <c r="G239" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H239" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I239" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="K236" s="3" t="s">
+      <c r="K239" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="L236" s="6" t="s">
+      <c r="L239" s="6" t="s">
         <v>472</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L236" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}"/>
+  <autoFilter ref="A1:L239" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}"/>
   <hyperlinks>
     <hyperlink ref="L3" r:id="rId1" location="query=target&amp;position=0&amp;from_view=search&amp;track=sph&amp;uuid=07a631b0-afe2-4d83-9076-a80360e62f2f" xr:uid="{6340FD26-01F6-9246-82E5-C8936FBB7B36}"/>
     <hyperlink ref="L4" r:id="rId2" location="query=spell%20book&amp;position=12&amp;from_view=keyword&amp;track=ais&amp;uuid=3aa8f740-41d0-409e-b03b-268281a69be6" xr:uid="{1A91BF66-CE85-304F-BBE7-7F8EBE53C285}"/>
@@ -9502,126 +9619,129 @@
     <hyperlink ref="L100" r:id="rId78" xr:uid="{875A91BB-08F0-9F41-AA8C-0DA91E9E3433}"/>
     <hyperlink ref="L101" r:id="rId79" xr:uid="{2358BC99-E6CB-CC40-ADFF-8AC06D23EF07}"/>
     <hyperlink ref="L102" r:id="rId80" xr:uid="{EE8601B6-0243-2A49-A9C6-75E6146D7CED}"/>
-    <hyperlink ref="L103" r:id="rId81" xr:uid="{11B6F62A-6D9A-614A-B258-D8AA048E0295}"/>
+    <hyperlink ref="L104" r:id="rId81" xr:uid="{11B6F62A-6D9A-614A-B258-D8AA048E0295}"/>
     <hyperlink ref="L80" r:id="rId82" location="&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=212ca3a5-7aff-48ca-9059-3fd4569bd97d" xr:uid="{5E0BEA94-3C14-624A-B04C-480D52071A59}"/>
-    <hyperlink ref="L104" r:id="rId83" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{62FFBF71-DDCC-FB45-B1A0-5B5743818433}"/>
-    <hyperlink ref="L105" r:id="rId84" xr:uid="{C6D42146-F620-2E4D-A1E8-6C7AB68398A0}"/>
-    <hyperlink ref="L106" r:id="rId85" xr:uid="{69D2711D-2024-4D48-B506-A5426A13437B}"/>
-    <hyperlink ref="L107" r:id="rId86" xr:uid="{D50E3661-FDF1-5C4F-B873-C0CBFBD7EF35}"/>
-    <hyperlink ref="L108" r:id="rId87" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{7D5FDD89-EC51-3648-AED9-53792D3E0C33}"/>
-    <hyperlink ref="L109" r:id="rId88" xr:uid="{152DE699-D73F-EF4E-9197-168BFA94CEA2}"/>
-    <hyperlink ref="L110" r:id="rId89" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{D0737FC4-EBDD-894D-B245-F35B45E2BB9E}"/>
-    <hyperlink ref="L111" r:id="rId90" xr:uid="{F6962BD9-CA67-934F-A5FA-A876F707D991}"/>
-    <hyperlink ref="L112" r:id="rId91" xr:uid="{9FB19C9F-53C1-C14F-B0FB-F6FFC3813A0C}"/>
-    <hyperlink ref="L113" r:id="rId92" location="page=3&amp;query=dragon%20sprite&amp;position=8&amp;from_view=search&amp;track=ais&amp;uuid=a74ae69f-43df-4e46-8d2c-551fbfc06054" xr:uid="{8CF6EC38-B466-5046-9ABB-7B436FB04B00}"/>
-    <hyperlink ref="L114" r:id="rId93" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{0A9F6B86-9F6E-BB4B-A75B-04A9E5D17C6C}"/>
-    <hyperlink ref="L115" r:id="rId94" xr:uid="{5F607910-F685-E446-84A9-7A29F560E55A}"/>
-    <hyperlink ref="L116" r:id="rId95" xr:uid="{578C63E4-A237-DE4B-B0BD-67011C0E3ADD}"/>
-    <hyperlink ref="L117" r:id="rId96" location="page=2&amp;position=43&amp;from_view=search&amp;track=ais&amp;uuid=0f4d7d50-56a5-4394-84f3-725d8c5aaddd" xr:uid="{61842379-CF7B-1241-9EBE-2870DBC6CCF0}"/>
-    <hyperlink ref="L118" r:id="rId97" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{5A8FBE05-CC1C-4445-872A-1F2B5D068722}"/>
-    <hyperlink ref="L119" r:id="rId98" xr:uid="{6C2DDDB8-2819-0F48-9FC2-13E3FD09D89C}"/>
-    <hyperlink ref="L120" r:id="rId99" xr:uid="{FA9A9087-DACC-3348-9590-AF003D7980CD}"/>
-    <hyperlink ref="L121" r:id="rId100" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{13DDFAC9-7E7A-7144-8D4D-5F7238F57C50}"/>
-    <hyperlink ref="L122" r:id="rId101" xr:uid="{536E05BD-607D-8C40-A324-92D273517532}"/>
-    <hyperlink ref="L123" r:id="rId102" location="page=3&amp;query=dragon%20sprite&amp;position=8&amp;from_view=search&amp;track=ais&amp;uuid=a74ae69f-43df-4e46-8d2c-551fbfc06054" xr:uid="{80725854-8C9E-2142-9506-1DAA5EA55E2C}"/>
-    <hyperlink ref="L124" r:id="rId103" xr:uid="{7D317CFF-0421-8240-AC77-11BBCE22AB8E}"/>
-    <hyperlink ref="L125" r:id="rId104" xr:uid="{A2D8E487-AD43-8F4E-A9DE-5869F09C0426}"/>
-    <hyperlink ref="L127" r:id="rId105" xr:uid="{D7E8C3AD-A803-064B-BE47-A4A13A516766}"/>
-    <hyperlink ref="L129" r:id="rId106" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{BDB61EDA-F818-FF45-B87D-6ADEA708FFA7}"/>
-    <hyperlink ref="L130" r:id="rId107" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{253AAE66-6702-8C4F-A846-EBF5AE2F8391}"/>
-    <hyperlink ref="L131" r:id="rId108" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{6939D314-66EF-8D4B-AFF0-C6E403A07A14}"/>
-    <hyperlink ref="L138" r:id="rId109" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{EB09046E-7A86-CA4F-8571-926934A1C16B}"/>
-    <hyperlink ref="L139" r:id="rId110" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{C5A8A89F-FAEB-664B-8EA0-ED39009C9364}"/>
-    <hyperlink ref="L140" r:id="rId111" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{B0D21C11-7039-9747-AFD6-6A560A885C1E}"/>
-    <hyperlink ref="L145" r:id="rId112" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{1565E7C7-B646-D249-BAAB-3FCB7F08DD87}"/>
-    <hyperlink ref="L146" r:id="rId113" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{A8BBBB50-0434-7448-8336-9B7ED86F56E9}"/>
-    <hyperlink ref="L147" r:id="rId114" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{C3D989D9-9B8F-A344-BCD4-784D6E9D731B}"/>
-    <hyperlink ref="L149" r:id="rId115" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{30281897-7108-FC49-9176-CC6B5A425C7A}"/>
-    <hyperlink ref="L150" r:id="rId116" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{A0297FF1-2C4C-E544-B864-7C5A962D424C}"/>
-    <hyperlink ref="L151" r:id="rId117" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{E800482C-5495-E140-9569-17E80FD691E0}"/>
-    <hyperlink ref="L132" r:id="rId118" location="query=discoball%20sprite%20purple&amp;position=5&amp;from_view=search&amp;track=ais&amp;uuid=5e15239d-0812-436d-9e99-3bbe89255301" xr:uid="{6CBD560E-8DE3-AC47-AF1D-9836CBBBCFAF}"/>
-    <hyperlink ref="L133" r:id="rId119" location="query=discoball%20sprite%20purple&amp;position=5&amp;from_view=search&amp;track=ais&amp;uuid=5e15239d-0812-436d-9e99-3bbe89255301" xr:uid="{92122264-574C-904C-AB91-F5AF6D172F32}"/>
-    <hyperlink ref="L137" r:id="rId120" location="&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=3b8eb20b-1ef9-4be4-b972-96b55e0f912c" display="https://www.freepik.com/free-vector/set-square-ui-game-frames-textured-medieval-borders-gold-silver-steel-metal-with-gems-cartoon-empty-metallic-bordering-with-gemstones-isolated-design-gui-elements-vector-illustration_24325879.htm#&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=3b8eb20b-1ef9-4be4-b972-96b55e0f912c" xr:uid="{BA52B0B4-2A86-6842-A815-4370D4A52AF0}"/>
-    <hyperlink ref="L136" r:id="rId121" location="&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=295330cb-9881-4046-9dc8-cb7e28cdaddb" xr:uid="{8F9561E6-335E-E740-8CF3-AF66A1E5C23F}"/>
+    <hyperlink ref="L107" r:id="rId83" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{62FFBF71-DDCC-FB45-B1A0-5B5743818433}"/>
+    <hyperlink ref="L108" r:id="rId84" xr:uid="{C6D42146-F620-2E4D-A1E8-6C7AB68398A0}"/>
+    <hyperlink ref="L109" r:id="rId85" xr:uid="{69D2711D-2024-4D48-B506-A5426A13437B}"/>
+    <hyperlink ref="L110" r:id="rId86" xr:uid="{D50E3661-FDF1-5C4F-B873-C0CBFBD7EF35}"/>
+    <hyperlink ref="L111" r:id="rId87" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{7D5FDD89-EC51-3648-AED9-53792D3E0C33}"/>
+    <hyperlink ref="L112" r:id="rId88" xr:uid="{152DE699-D73F-EF4E-9197-168BFA94CEA2}"/>
+    <hyperlink ref="L113" r:id="rId89" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{D0737FC4-EBDD-894D-B245-F35B45E2BB9E}"/>
+    <hyperlink ref="L114" r:id="rId90" xr:uid="{F6962BD9-CA67-934F-A5FA-A876F707D991}"/>
+    <hyperlink ref="L115" r:id="rId91" xr:uid="{9FB19C9F-53C1-C14F-B0FB-F6FFC3813A0C}"/>
+    <hyperlink ref="L116" r:id="rId92" location="page=3&amp;query=dragon%20sprite&amp;position=8&amp;from_view=search&amp;track=ais&amp;uuid=a74ae69f-43df-4e46-8d2c-551fbfc06054" xr:uid="{8CF6EC38-B466-5046-9ABB-7B436FB04B00}"/>
+    <hyperlink ref="L117" r:id="rId93" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{0A9F6B86-9F6E-BB4B-A75B-04A9E5D17C6C}"/>
+    <hyperlink ref="L118" r:id="rId94" xr:uid="{5F607910-F685-E446-84A9-7A29F560E55A}"/>
+    <hyperlink ref="L119" r:id="rId95" xr:uid="{578C63E4-A237-DE4B-B0BD-67011C0E3ADD}"/>
+    <hyperlink ref="L120" r:id="rId96" location="page=2&amp;position=43&amp;from_view=search&amp;track=ais&amp;uuid=0f4d7d50-56a5-4394-84f3-725d8c5aaddd" xr:uid="{61842379-CF7B-1241-9EBE-2870DBC6CCF0}"/>
+    <hyperlink ref="L121" r:id="rId97" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{5A8FBE05-CC1C-4445-872A-1F2B5D068722}"/>
+    <hyperlink ref="L122" r:id="rId98" xr:uid="{6C2DDDB8-2819-0F48-9FC2-13E3FD09D89C}"/>
+    <hyperlink ref="L123" r:id="rId99" xr:uid="{FA9A9087-DACC-3348-9590-AF003D7980CD}"/>
+    <hyperlink ref="L124" r:id="rId100" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{13DDFAC9-7E7A-7144-8D4D-5F7238F57C50}"/>
+    <hyperlink ref="L125" r:id="rId101" xr:uid="{536E05BD-607D-8C40-A324-92D273517532}"/>
+    <hyperlink ref="L126" r:id="rId102" location="page=3&amp;query=dragon%20sprite&amp;position=8&amp;from_view=search&amp;track=ais&amp;uuid=a74ae69f-43df-4e46-8d2c-551fbfc06054" xr:uid="{80725854-8C9E-2142-9506-1DAA5EA55E2C}"/>
+    <hyperlink ref="L127" r:id="rId103" xr:uid="{7D317CFF-0421-8240-AC77-11BBCE22AB8E}"/>
+    <hyperlink ref="L128" r:id="rId104" xr:uid="{A2D8E487-AD43-8F4E-A9DE-5869F09C0426}"/>
+    <hyperlink ref="L130" r:id="rId105" xr:uid="{D7E8C3AD-A803-064B-BE47-A4A13A516766}"/>
+    <hyperlink ref="L132" r:id="rId106" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{BDB61EDA-F818-FF45-B87D-6ADEA708FFA7}"/>
+    <hyperlink ref="L133" r:id="rId107" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{253AAE66-6702-8C4F-A846-EBF5AE2F8391}"/>
+    <hyperlink ref="L134" r:id="rId108" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{6939D314-66EF-8D4B-AFF0-C6E403A07A14}"/>
+    <hyperlink ref="L141" r:id="rId109" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{EB09046E-7A86-CA4F-8571-926934A1C16B}"/>
+    <hyperlink ref="L142" r:id="rId110" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{C5A8A89F-FAEB-664B-8EA0-ED39009C9364}"/>
+    <hyperlink ref="L143" r:id="rId111" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{B0D21C11-7039-9747-AFD6-6A560A885C1E}"/>
+    <hyperlink ref="L148" r:id="rId112" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{1565E7C7-B646-D249-BAAB-3FCB7F08DD87}"/>
+    <hyperlink ref="L149" r:id="rId113" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{A8BBBB50-0434-7448-8336-9B7ED86F56E9}"/>
+    <hyperlink ref="L150" r:id="rId114" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{C3D989D9-9B8F-A344-BCD4-784D6E9D731B}"/>
+    <hyperlink ref="L152" r:id="rId115" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{30281897-7108-FC49-9176-CC6B5A425C7A}"/>
+    <hyperlink ref="L153" r:id="rId116" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{A0297FF1-2C4C-E544-B864-7C5A962D424C}"/>
+    <hyperlink ref="L154" r:id="rId117" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{E800482C-5495-E140-9569-17E80FD691E0}"/>
+    <hyperlink ref="L135" r:id="rId118" location="query=discoball%20sprite%20purple&amp;position=5&amp;from_view=search&amp;track=ais&amp;uuid=5e15239d-0812-436d-9e99-3bbe89255301" xr:uid="{6CBD560E-8DE3-AC47-AF1D-9836CBBBCFAF}"/>
+    <hyperlink ref="L136" r:id="rId119" location="query=discoball%20sprite%20purple&amp;position=5&amp;from_view=search&amp;track=ais&amp;uuid=5e15239d-0812-436d-9e99-3bbe89255301" xr:uid="{92122264-574C-904C-AB91-F5AF6D172F32}"/>
+    <hyperlink ref="L140" r:id="rId120" location="&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=3b8eb20b-1ef9-4be4-b972-96b55e0f912c" display="https://www.freepik.com/free-vector/set-square-ui-game-frames-textured-medieval-borders-gold-silver-steel-metal-with-gems-cartoon-empty-metallic-bordering-with-gemstones-isolated-design-gui-elements-vector-illustration_24325879.htm#&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=3b8eb20b-1ef9-4be4-b972-96b55e0f912c" xr:uid="{BA52B0B4-2A86-6842-A815-4370D4A52AF0}"/>
+    <hyperlink ref="L139" r:id="rId121" location="&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=295330cb-9881-4046-9dc8-cb7e28cdaddb" xr:uid="{8F9561E6-335E-E740-8CF3-AF66A1E5C23F}"/>
     <hyperlink ref="L2" r:id="rId122" xr:uid="{9DA1D9F2-BD16-914A-B65F-BEFF391AD408}"/>
-    <hyperlink ref="L126" r:id="rId123" xr:uid="{4BFCF1BE-6310-C34B-BA09-218F6A3C75D9}"/>
-    <hyperlink ref="L128" r:id="rId124" xr:uid="{C9C421A7-64D0-5D49-9F28-B71BC19F3239}"/>
-    <hyperlink ref="L155" r:id="rId125" xr:uid="{F88953B7-468E-C34B-9347-94009F9A78D2}"/>
-    <hyperlink ref="L195" r:id="rId126" xr:uid="{1F3BBC8C-29E8-C74A-AB3F-04AE466222EF}"/>
-    <hyperlink ref="L197" r:id="rId127" xr:uid="{3C51058F-793C-D34A-8286-18AE4C8EF6CE}"/>
-    <hyperlink ref="L233" r:id="rId128" xr:uid="{A1386B57-DD43-6F4A-8F35-D9075616F763}"/>
-    <hyperlink ref="L234" r:id="rId129" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
-    <hyperlink ref="L152" r:id="rId130" xr:uid="{6A722A1D-2F7B-4242-8134-716EFF33F7D2}"/>
-    <hyperlink ref="L153" r:id="rId131" xr:uid="{547CD1A8-1967-1C46-95E3-89E39CD045C2}"/>
-    <hyperlink ref="L198" r:id="rId132" xr:uid="{5ACD6BFD-52F0-0940-AA8E-B04F1D397BC7}"/>
-    <hyperlink ref="L230" r:id="rId133" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
-    <hyperlink ref="L196" r:id="rId134" xr:uid="{2030AD8C-28A7-544B-92DC-5CBE411DE1C0}"/>
-    <hyperlink ref="L219" r:id="rId135" xr:uid="{05363CA1-BE60-3F42-B56A-1A92A0EDA166}"/>
-    <hyperlink ref="L188" r:id="rId136" xr:uid="{D4C66DCB-D6B4-EC4F-A922-B87887BE6E4A}"/>
-    <hyperlink ref="L187" r:id="rId137" xr:uid="{A05D9F8A-ED0A-4143-8920-9422DD4E0BDD}"/>
-    <hyperlink ref="L189" r:id="rId138" xr:uid="{83FA4EC1-AB5E-3B43-9476-4CA54526DF8E}"/>
-    <hyperlink ref="L168" r:id="rId139" xr:uid="{21B7C9CB-274E-C246-8989-83D9E0E7B24F}"/>
-    <hyperlink ref="L164" r:id="rId140" xr:uid="{B5B4FA15-B24C-CE46-9594-7ED28656AA43}"/>
-    <hyperlink ref="L165" r:id="rId141" xr:uid="{3AB6BE1F-95C1-A443-B12D-D7A523FAD6C5}"/>
-    <hyperlink ref="L166" r:id="rId142" xr:uid="{347BDCC2-5A0C-B249-8CA8-B72D245480FC}"/>
-    <hyperlink ref="L167" r:id="rId143" xr:uid="{E58DD28D-BD99-DF44-9E5E-B3D05F881C1F}"/>
-    <hyperlink ref="L222" r:id="rId144" xr:uid="{4F668E79-3664-0547-B3D5-B7724A9D574D}"/>
-    <hyperlink ref="L220" r:id="rId145" xr:uid="{8AB5C10C-8B45-1843-96BD-655A4FA04EFD}"/>
-    <hyperlink ref="L171" r:id="rId146" xr:uid="{EAED74E0-13EE-A046-9ADC-AC8BDE30C3E6}"/>
-    <hyperlink ref="L227" r:id="rId147" xr:uid="{3577256C-215B-134E-B541-B7B77272CD8A}"/>
-    <hyperlink ref="L228" r:id="rId148" xr:uid="{98E325FC-7F95-B44E-98EB-DE0FF53BC89D}"/>
-    <hyperlink ref="L221" r:id="rId149" xr:uid="{5CE3083F-F217-3743-B613-A7DDF354E72D}"/>
-    <hyperlink ref="L223" r:id="rId150" xr:uid="{B81B6B41-2C17-AA48-B730-D906488BA0A0}"/>
-    <hyperlink ref="L177" r:id="rId151" xr:uid="{BA0813A2-2582-7A46-A492-16A943824EE5}"/>
-    <hyperlink ref="L229" r:id="rId152" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
-    <hyperlink ref="L224" r:id="rId153" xr:uid="{C5265333-F7F0-1845-98D7-68E930F9DFAE}"/>
-    <hyperlink ref="L179" r:id="rId154" xr:uid="{C0A159CB-3986-1A46-95AD-DCEFF4247697}"/>
-    <hyperlink ref="L169" r:id="rId155" xr:uid="{37810A74-E45D-1D46-AEF5-C5FE2F414285}"/>
-    <hyperlink ref="L218" r:id="rId156" xr:uid="{D2906064-B1B8-4648-8201-BEFA97591226}"/>
-    <hyperlink ref="L157" r:id="rId157" xr:uid="{1D3CD52E-7AAD-E444-88F4-4BAE6C5B5EB7}"/>
-    <hyperlink ref="L158" r:id="rId158" xr:uid="{E6E6DA47-945D-6145-912F-08B17B7BA6AE}"/>
-    <hyperlink ref="L159" r:id="rId159" xr:uid="{006B1689-D89A-1E4A-BBC5-E9C9583907F7}"/>
-    <hyperlink ref="L160" r:id="rId160" xr:uid="{C3E773B2-D410-AF41-B197-4638485DC8EF}"/>
-    <hyperlink ref="L161" r:id="rId161" xr:uid="{A0E8A8E2-4A93-3D42-AF48-81955241A483}"/>
-    <hyperlink ref="L162" r:id="rId162" xr:uid="{1B03F18A-8745-AA4F-AA8B-88D65D3B24BC}"/>
-    <hyperlink ref="L235" r:id="rId163" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
-    <hyperlink ref="L236" r:id="rId164" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
-    <hyperlink ref="L185" r:id="rId165" xr:uid="{D6B77117-A0D5-9240-8193-0102C36CCE4C}"/>
-    <hyperlink ref="L186" r:id="rId166" xr:uid="{79FB1103-88A8-8044-9E2C-4FAEC0906E8E}"/>
-    <hyperlink ref="L225" r:id="rId167" xr:uid="{5BF1C4C9-E63A-4F42-9042-36520975FDFA}"/>
-    <hyperlink ref="L184" r:id="rId168" xr:uid="{21CDF460-9871-0547-AA6B-20304C8DD21D}"/>
-    <hyperlink ref="L174" r:id="rId169" xr:uid="{BA1EC844-435A-6C44-87FC-C12B7ECFC55B}"/>
-    <hyperlink ref="L173" r:id="rId170" xr:uid="{46D875DC-CDDD-7E4B-88DB-DFC416CF17AB}"/>
-    <hyperlink ref="L163" r:id="rId171" xr:uid="{7D2FF6AE-1C67-9D4A-A760-7E3745DD9EA6}"/>
-    <hyperlink ref="L211" r:id="rId172" xr:uid="{B5E5E388-8F37-414E-A0C6-1DC58E77628C}"/>
-    <hyperlink ref="L212" r:id="rId173" xr:uid="{D62BC330-84EA-AE41-A129-2BC1AE7C44D1}"/>
-    <hyperlink ref="L213" r:id="rId174" xr:uid="{A96B1ACF-D982-9240-BB1C-69459154AE5A}"/>
-    <hyperlink ref="L180" r:id="rId175" xr:uid="{D3BB695A-CBA9-D649-B49D-4CC8D16EFD9B}"/>
-    <hyperlink ref="L181" r:id="rId176" xr:uid="{A2922BA8-758D-3149-892C-B7B65B435332}"/>
-    <hyperlink ref="L200" r:id="rId177" xr:uid="{BDB09119-6289-4346-BC29-7A54BD393127}"/>
-    <hyperlink ref="L226" r:id="rId178" xr:uid="{5736CAF4-3646-3243-9AEB-4D82B6D0D10A}"/>
-    <hyperlink ref="L203" r:id="rId179" xr:uid="{60659D55-801C-9A4E-84CA-809884CCBE5C}"/>
-    <hyperlink ref="L193" r:id="rId180" xr:uid="{18DDC006-0939-794C-9B5D-10593F8C0973}"/>
-    <hyperlink ref="L182" r:id="rId181" xr:uid="{50EA46A5-11DD-0345-ABCA-4206D73C7606}"/>
-    <hyperlink ref="L217" r:id="rId182" xr:uid="{63DDFF3B-E62C-9445-96AD-4BB37ACCD20E}"/>
-    <hyperlink ref="L232" r:id="rId183" xr:uid="{F4FBFB75-F824-8643-A03A-0A3479747FAB}"/>
-    <hyperlink ref="L205" r:id="rId184" xr:uid="{05E34BC1-B22F-3E46-8574-E72267507402}"/>
-    <hyperlink ref="L204" r:id="rId185" xr:uid="{7125DF67-5A7E-D948-8363-A31AB1EBA44A}"/>
-    <hyperlink ref="L231" r:id="rId186" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
-    <hyperlink ref="L194" r:id="rId187" xr:uid="{CCE2D666-E296-D94C-ACE0-791CC746483B}"/>
-    <hyperlink ref="L156" r:id="rId188" xr:uid="{213D9061-74C7-4745-9991-1B8CB77BAE4C}"/>
-    <hyperlink ref="L190" r:id="rId189" xr:uid="{357D2DAE-7369-6541-B091-9DF1685B9573}"/>
-    <hyperlink ref="L175" r:id="rId190" xr:uid="{E5A2F3EE-A3B1-0842-9364-E4B6EACA9544}"/>
-    <hyperlink ref="L206" r:id="rId191" xr:uid="{E08C8BA4-5414-1947-9CA8-45FE0B846CD1}"/>
-    <hyperlink ref="L172" r:id="rId192" xr:uid="{A3B57AE0-BE24-DE4E-84B5-3ECB73F4B476}"/>
-    <hyperlink ref="L202" r:id="rId193" xr:uid="{F1A64091-5BF7-8243-B7A0-F4C13B8B0ABB}"/>
-    <hyperlink ref="L191" r:id="rId194" xr:uid="{745AEF03-3150-C54B-800A-696460474256}"/>
-    <hyperlink ref="L192" r:id="rId195" xr:uid="{9C078FBA-3B11-8049-9187-5BC86D78EA09}"/>
-    <hyperlink ref="L176" r:id="rId196" xr:uid="{BF9A6A48-C664-FA4B-A769-D87460BB9387}"/>
-    <hyperlink ref="L178" r:id="rId197" xr:uid="{11E0C06F-BBA9-B446-A3A4-5862C893161B}"/>
-    <hyperlink ref="L201" r:id="rId198" xr:uid="{D5E45024-1B58-714D-9576-1FA969BDADD9}"/>
-    <hyperlink ref="L183" r:id="rId199" xr:uid="{D160676D-AC82-D243-B9A9-56033B0A6EFE}"/>
-    <hyperlink ref="L199" r:id="rId200" xr:uid="{3DB54A74-68B7-734A-BC3C-BFE4E2E4103E}"/>
+    <hyperlink ref="L129" r:id="rId123" xr:uid="{4BFCF1BE-6310-C34B-BA09-218F6A3C75D9}"/>
+    <hyperlink ref="L131" r:id="rId124" xr:uid="{C9C421A7-64D0-5D49-9F28-B71BC19F3239}"/>
+    <hyperlink ref="L158" r:id="rId125" xr:uid="{F88953B7-468E-C34B-9347-94009F9A78D2}"/>
+    <hyperlink ref="L198" r:id="rId126" xr:uid="{1F3BBC8C-29E8-C74A-AB3F-04AE466222EF}"/>
+    <hyperlink ref="L200" r:id="rId127" xr:uid="{3C51058F-793C-D34A-8286-18AE4C8EF6CE}"/>
+    <hyperlink ref="L236" r:id="rId128" xr:uid="{A1386B57-DD43-6F4A-8F35-D9075616F763}"/>
+    <hyperlink ref="L237" r:id="rId129" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
+    <hyperlink ref="L155" r:id="rId130" xr:uid="{6A722A1D-2F7B-4242-8134-716EFF33F7D2}"/>
+    <hyperlink ref="L156" r:id="rId131" xr:uid="{547CD1A8-1967-1C46-95E3-89E39CD045C2}"/>
+    <hyperlink ref="L201" r:id="rId132" xr:uid="{5ACD6BFD-52F0-0940-AA8E-B04F1D397BC7}"/>
+    <hyperlink ref="L233" r:id="rId133" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
+    <hyperlink ref="L199" r:id="rId134" xr:uid="{2030AD8C-28A7-544B-92DC-5CBE411DE1C0}"/>
+    <hyperlink ref="L222" r:id="rId135" xr:uid="{05363CA1-BE60-3F42-B56A-1A92A0EDA166}"/>
+    <hyperlink ref="L191" r:id="rId136" xr:uid="{D4C66DCB-D6B4-EC4F-A922-B87887BE6E4A}"/>
+    <hyperlink ref="L190" r:id="rId137" xr:uid="{A05D9F8A-ED0A-4143-8920-9422DD4E0BDD}"/>
+    <hyperlink ref="L192" r:id="rId138" xr:uid="{83FA4EC1-AB5E-3B43-9476-4CA54526DF8E}"/>
+    <hyperlink ref="L171" r:id="rId139" xr:uid="{21B7C9CB-274E-C246-8989-83D9E0E7B24F}"/>
+    <hyperlink ref="L167" r:id="rId140" xr:uid="{B5B4FA15-B24C-CE46-9594-7ED28656AA43}"/>
+    <hyperlink ref="L168" r:id="rId141" xr:uid="{3AB6BE1F-95C1-A443-B12D-D7A523FAD6C5}"/>
+    <hyperlink ref="L169" r:id="rId142" xr:uid="{347BDCC2-5A0C-B249-8CA8-B72D245480FC}"/>
+    <hyperlink ref="L170" r:id="rId143" xr:uid="{E58DD28D-BD99-DF44-9E5E-B3D05F881C1F}"/>
+    <hyperlink ref="L225" r:id="rId144" xr:uid="{4F668E79-3664-0547-B3D5-B7724A9D574D}"/>
+    <hyperlink ref="L223" r:id="rId145" xr:uid="{8AB5C10C-8B45-1843-96BD-655A4FA04EFD}"/>
+    <hyperlink ref="L174" r:id="rId146" xr:uid="{EAED74E0-13EE-A046-9ADC-AC8BDE30C3E6}"/>
+    <hyperlink ref="L230" r:id="rId147" xr:uid="{3577256C-215B-134E-B541-B7B77272CD8A}"/>
+    <hyperlink ref="L231" r:id="rId148" xr:uid="{98E325FC-7F95-B44E-98EB-DE0FF53BC89D}"/>
+    <hyperlink ref="L224" r:id="rId149" xr:uid="{5CE3083F-F217-3743-B613-A7DDF354E72D}"/>
+    <hyperlink ref="L226" r:id="rId150" xr:uid="{B81B6B41-2C17-AA48-B730-D906488BA0A0}"/>
+    <hyperlink ref="L180" r:id="rId151" xr:uid="{BA0813A2-2582-7A46-A492-16A943824EE5}"/>
+    <hyperlink ref="L232" r:id="rId152" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
+    <hyperlink ref="L227" r:id="rId153" xr:uid="{C5265333-F7F0-1845-98D7-68E930F9DFAE}"/>
+    <hyperlink ref="L182" r:id="rId154" xr:uid="{C0A159CB-3986-1A46-95AD-DCEFF4247697}"/>
+    <hyperlink ref="L172" r:id="rId155" xr:uid="{37810A74-E45D-1D46-AEF5-C5FE2F414285}"/>
+    <hyperlink ref="L221" r:id="rId156" xr:uid="{D2906064-B1B8-4648-8201-BEFA97591226}"/>
+    <hyperlink ref="L160" r:id="rId157" xr:uid="{1D3CD52E-7AAD-E444-88F4-4BAE6C5B5EB7}"/>
+    <hyperlink ref="L161" r:id="rId158" xr:uid="{E6E6DA47-945D-6145-912F-08B17B7BA6AE}"/>
+    <hyperlink ref="L162" r:id="rId159" xr:uid="{006B1689-D89A-1E4A-BBC5-E9C9583907F7}"/>
+    <hyperlink ref="L163" r:id="rId160" xr:uid="{C3E773B2-D410-AF41-B197-4638485DC8EF}"/>
+    <hyperlink ref="L164" r:id="rId161" xr:uid="{A0E8A8E2-4A93-3D42-AF48-81955241A483}"/>
+    <hyperlink ref="L165" r:id="rId162" xr:uid="{1B03F18A-8745-AA4F-AA8B-88D65D3B24BC}"/>
+    <hyperlink ref="L238" r:id="rId163" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
+    <hyperlink ref="L239" r:id="rId164" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
+    <hyperlink ref="L188" r:id="rId165" xr:uid="{D6B77117-A0D5-9240-8193-0102C36CCE4C}"/>
+    <hyperlink ref="L189" r:id="rId166" xr:uid="{79FB1103-88A8-8044-9E2C-4FAEC0906E8E}"/>
+    <hyperlink ref="L228" r:id="rId167" xr:uid="{5BF1C4C9-E63A-4F42-9042-36520975FDFA}"/>
+    <hyperlink ref="L187" r:id="rId168" xr:uid="{21CDF460-9871-0547-AA6B-20304C8DD21D}"/>
+    <hyperlink ref="L177" r:id="rId169" xr:uid="{BA1EC844-435A-6C44-87FC-C12B7ECFC55B}"/>
+    <hyperlink ref="L176" r:id="rId170" xr:uid="{46D875DC-CDDD-7E4B-88DB-DFC416CF17AB}"/>
+    <hyperlink ref="L166" r:id="rId171" xr:uid="{7D2FF6AE-1C67-9D4A-A760-7E3745DD9EA6}"/>
+    <hyperlink ref="L214" r:id="rId172" xr:uid="{B5E5E388-8F37-414E-A0C6-1DC58E77628C}"/>
+    <hyperlink ref="L215" r:id="rId173" xr:uid="{D62BC330-84EA-AE41-A129-2BC1AE7C44D1}"/>
+    <hyperlink ref="L216" r:id="rId174" xr:uid="{A96B1ACF-D982-9240-BB1C-69459154AE5A}"/>
+    <hyperlink ref="L183" r:id="rId175" xr:uid="{D3BB695A-CBA9-D649-B49D-4CC8D16EFD9B}"/>
+    <hyperlink ref="L184" r:id="rId176" xr:uid="{A2922BA8-758D-3149-892C-B7B65B435332}"/>
+    <hyperlink ref="L203" r:id="rId177" xr:uid="{BDB09119-6289-4346-BC29-7A54BD393127}"/>
+    <hyperlink ref="L229" r:id="rId178" xr:uid="{5736CAF4-3646-3243-9AEB-4D82B6D0D10A}"/>
+    <hyperlink ref="L206" r:id="rId179" xr:uid="{60659D55-801C-9A4E-84CA-809884CCBE5C}"/>
+    <hyperlink ref="L196" r:id="rId180" xr:uid="{18DDC006-0939-794C-9B5D-10593F8C0973}"/>
+    <hyperlink ref="L185" r:id="rId181" xr:uid="{50EA46A5-11DD-0345-ABCA-4206D73C7606}"/>
+    <hyperlink ref="L220" r:id="rId182" xr:uid="{63DDFF3B-E62C-9445-96AD-4BB37ACCD20E}"/>
+    <hyperlink ref="L235" r:id="rId183" xr:uid="{F4FBFB75-F824-8643-A03A-0A3479747FAB}"/>
+    <hyperlink ref="L208" r:id="rId184" xr:uid="{05E34BC1-B22F-3E46-8574-E72267507402}"/>
+    <hyperlink ref="L207" r:id="rId185" xr:uid="{7125DF67-5A7E-D948-8363-A31AB1EBA44A}"/>
+    <hyperlink ref="L234" r:id="rId186" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
+    <hyperlink ref="L197" r:id="rId187" xr:uid="{CCE2D666-E296-D94C-ACE0-791CC746483B}"/>
+    <hyperlink ref="L159" r:id="rId188" xr:uid="{213D9061-74C7-4745-9991-1B8CB77BAE4C}"/>
+    <hyperlink ref="L193" r:id="rId189" xr:uid="{357D2DAE-7369-6541-B091-9DF1685B9573}"/>
+    <hyperlink ref="L178" r:id="rId190" xr:uid="{E5A2F3EE-A3B1-0842-9364-E4B6EACA9544}"/>
+    <hyperlink ref="L209" r:id="rId191" xr:uid="{E08C8BA4-5414-1947-9CA8-45FE0B846CD1}"/>
+    <hyperlink ref="L175" r:id="rId192" xr:uid="{A3B57AE0-BE24-DE4E-84B5-3ECB73F4B476}"/>
+    <hyperlink ref="L205" r:id="rId193" xr:uid="{F1A64091-5BF7-8243-B7A0-F4C13B8B0ABB}"/>
+    <hyperlink ref="L194" r:id="rId194" xr:uid="{745AEF03-3150-C54B-800A-696460474256}"/>
+    <hyperlink ref="L195" r:id="rId195" xr:uid="{9C078FBA-3B11-8049-9187-5BC86D78EA09}"/>
+    <hyperlink ref="L179" r:id="rId196" xr:uid="{BF9A6A48-C664-FA4B-A769-D87460BB9387}"/>
+    <hyperlink ref="L181" r:id="rId197" xr:uid="{11E0C06F-BBA9-B446-A3A4-5862C893161B}"/>
+    <hyperlink ref="L204" r:id="rId198" xr:uid="{D5E45024-1B58-714D-9576-1FA969BDADD9}"/>
+    <hyperlink ref="L186" r:id="rId199" xr:uid="{D160676D-AC82-D243-B9A9-56033B0A6EFE}"/>
+    <hyperlink ref="L202" r:id="rId200" xr:uid="{3DB54A74-68B7-734A-BC3C-BFE4E2E4103E}"/>
+    <hyperlink ref="L103" r:id="rId201" xr:uid="{4686296B-C235-4048-A384-BE461895E2AC}"/>
+    <hyperlink ref="L105" r:id="rId202" location="page=2&amp;query=gold%20badge%20sprite&amp;position=49&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{061AB839-ADB1-BA47-A152-68CDFE8A1979}"/>
+    <hyperlink ref="L106" r:id="rId203" location="page=4&amp;query=gold%20badge%20sprite&amp;position=9&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{138577BB-7F7D-D64A-806E-567F3970D250}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
AssetsCatalog: update audio purchases. OLD JSON FILES: moved this folder out of this project and into Documents/Work/5Play Apps/PUZL Boy Audio: purchase (new) bouldersmash, buttontap4, hammerswing, swordslash, thunderrumble. CutsceneInto: tweak dialogue, audio timing with new thunderrumble, etc.
</commit_message>
<xml_diff>
--- a/JSON/AssetsCatalog.xlsx
+++ b/JSON/AssetsCatalog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7E1724-712F-B143-9013-E65D87AC7FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E075036B-ECEB-1C4D-A5FD-4BC6DDF577C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="-2400" windowWidth="51200" windowHeight="24180" xr2:uid="{E84333C6-E3B6-FB42-AB04-827399F33810}"/>
+    <workbookView xWindow="36020" yWindow="-2400" windowWidth="51200" windowHeight="24180" xr2:uid="{E84333C6-E3B6-FB42-AB04-827399F33810}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="576">
   <si>
     <t>Filename</t>
   </si>
@@ -1244,15 +1244,6 @@
     <t>https://audiojungle.net/item/birds-singing-2/47710486</t>
   </si>
   <si>
-    <t>Alexander_Blu</t>
-  </si>
-  <si>
-    <t>Distant Low Thunder Rumbling</t>
-  </si>
-  <si>
-    <t>https://audiojungle.net/item/distant-low-thunder-rumbling/22399840</t>
-  </si>
-  <si>
     <t>music (standard license)</t>
   </si>
   <si>
@@ -1526,12 +1517,6 @@
     <t>Barefoot Male Running in Sand</t>
   </si>
   <si>
-    <t>Barefoot Female Running on Wet Sand</t>
-  </si>
-  <si>
-    <t>https://audiojungle.net/item/barefoot-female-running-on-wet-sand/10468624</t>
-  </si>
-  <si>
     <t>https://audiojungle.net/item/running-on-sand/28949683</t>
   </si>
   <si>
@@ -1607,15 +1592,6 @@
     <t>Footsteps Running on Leaves</t>
   </si>
   <si>
-    <t>https://audiojungle.net/item/gore-weap-sword_whoosh_chop_nogore_1/26830022</t>
-  </si>
-  <si>
-    <t>GORE - WEAP - Sword_Whoosh_Chop_NoGore_1</t>
-  </si>
-  <si>
-    <t>soundmorph</t>
-  </si>
-  <si>
     <t>https://audiojungle.net/item/fantasy-game-poison-2/27236653</t>
   </si>
   <si>
@@ -1652,21 +1628,6 @@
     <t>JDproduction</t>
   </si>
   <si>
-    <t>https://audiojungle.net/item/object-break-stone-medium-04/28150049</t>
-  </si>
-  <si>
-    <t>OBJECT BREAK Stone Medium 04</t>
-  </si>
-  <si>
-    <t>SmartSoundFX</t>
-  </si>
-  <si>
-    <t>https://audiojungle.net/item/weapons-medieval-hit-metal-hammer-large-03/28354688</t>
-  </si>
-  <si>
-    <t>WEAPONS MEDIEVAL Hit Metal Hammer Large 03</t>
-  </si>
-  <si>
     <t>https://audiojungle.net/item/soft-retro-bell-ingame-pause-sound/28986644</t>
   </si>
   <si>
@@ -1685,12 +1646,6 @@
     <t>BestSFX</t>
   </si>
   <si>
-    <t>https://audiojungle.net/item/dial-switch-twisting-sharp-ticking-63/32063529</t>
-  </si>
-  <si>
-    <t>Dial Switch Twisting Sharp Ticking 63</t>
-  </si>
-  <si>
     <t>https://audiojungle.net/item/running-in-mud-marsh-loop/32286579</t>
   </si>
   <si>
@@ -1770,6 +1725,48 @@
   </si>
   <si>
     <t>Free vector golden award badges game avatar frames</t>
+  </si>
+  <si>
+    <t>FX_Channel</t>
+  </si>
+  <si>
+    <t>Its Button 04</t>
+  </si>
+  <si>
+    <t>https://audiojungle.net/item/its-button-04/45861898</t>
+  </si>
+  <si>
+    <t>MusicOcean</t>
+  </si>
+  <si>
+    <t>https://audiojungle.net/item/catapult-impact/7773255</t>
+  </si>
+  <si>
+    <t>Catapult Impact</t>
+  </si>
+  <si>
+    <t>https://audiojungle.net/item/whoosh-and-metal-impact/22115839?s_rank=11</t>
+  </si>
+  <si>
+    <t>Whoosh and Metal Impact</t>
+  </si>
+  <si>
+    <t>sounddogs</t>
+  </si>
+  <si>
+    <t>Rocks Earthquakes - Rumble Earthquake Deep Debris</t>
+  </si>
+  <si>
+    <t>https://audiojungle.net/item/rocks-earthquakes-rumble-earthquake-deep-debris/46757288</t>
+  </si>
+  <si>
+    <t>AlenaLT</t>
+  </si>
+  <si>
+    <t>Sword Slash 6</t>
+  </si>
+  <si>
+    <t>https://audiojungle.net/item/sword-slash-6/19673652</t>
   </si>
 </sst>
 </file>
@@ -1849,7 +1846,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1861,6 +1858,9 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2179,10 +2179,10 @@
   <dimension ref="A1:L239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H78" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D155" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K106" sqref="K106"/>
+      <selection pane="bottomRight" activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2198,7 +2198,7 @@
     <col min="9" max="9" width="16.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.5" style="3" customWidth="1"/>
-    <col min="12" max="12" width="176.5" customWidth="1"/>
+    <col min="12" max="12" width="79" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -2224,7 +2224,7 @@
         <v>390</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>570</v>
+        <v>555</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>37</v>
@@ -4177,16 +4177,16 @@
         <v>80</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J67" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
@@ -4209,16 +4209,16 @@
         <v>80</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J68" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
@@ -4241,16 +4241,16 @@
         <v>80</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J69" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L69" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
@@ -4302,16 +4302,16 @@
         <v>80</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J71" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K71" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
@@ -4334,16 +4334,16 @@
         <v>80</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J72" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K72" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
@@ -4662,16 +4662,16 @@
         <v>216</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J83" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K83" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L83" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
@@ -4694,16 +4694,16 @@
         <v>216</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J84" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K84" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L84" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.2">
@@ -4726,16 +4726,16 @@
         <v>216</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J85" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K85" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L85" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
@@ -4758,16 +4758,16 @@
         <v>216</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J86" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K86" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L86" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.2">
@@ -4790,16 +4790,16 @@
         <v>216</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J87" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K87" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L87" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.2">
@@ -4822,16 +4822,16 @@
         <v>216</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J88" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L88" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.2">
@@ -4854,16 +4854,16 @@
         <v>216</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J89" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K89" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L89" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">
@@ -4886,16 +4886,16 @@
         <v>216</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J90" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K90" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L90" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.2">
@@ -4918,16 +4918,16 @@
         <v>216</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J91" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K91" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L91" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.2">
@@ -4950,16 +4950,16 @@
         <v>216</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J92" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K92" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L92" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.2">
@@ -4982,16 +4982,16 @@
         <v>216</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J93" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K93" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="L93" s="3" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.2">
@@ -5269,7 +5269,7 @@
         <v>4</v>
       </c>
       <c r="B103" t="s">
-        <v>571</v>
+        <v>556</v>
       </c>
       <c r="C103" t="s">
         <v>238</v>
@@ -5304,7 +5304,7 @@
         <v>240</v>
       </c>
       <c r="C104" t="s">
-        <v>572</v>
+        <v>557</v>
       </c>
       <c r="D104" t="s">
         <v>6</v>
@@ -5339,7 +5339,7 @@
         <v>240</v>
       </c>
       <c r="C105" t="s">
-        <v>572</v>
+        <v>557</v>
       </c>
       <c r="D105" t="s">
         <v>6</v>
@@ -5357,10 +5357,10 @@
         <v>135</v>
       </c>
       <c r="K105" s="3" t="s">
-        <v>574</v>
+        <v>559</v>
       </c>
       <c r="L105" s="6" t="s">
-        <v>573</v>
+        <v>558</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.2">
@@ -5371,7 +5371,7 @@
         <v>240</v>
       </c>
       <c r="C106" t="s">
-        <v>572</v>
+        <v>557</v>
       </c>
       <c r="D106" t="s">
         <v>6</v>
@@ -5389,10 +5389,10 @@
         <v>135</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>576</v>
+        <v>561</v>
       </c>
       <c r="L106" s="6" t="s">
-        <v>575</v>
+        <v>560</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.2">
@@ -6840,10 +6840,10 @@
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B155" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C155" t="s">
         <v>304</v>
@@ -6861,21 +6861,21 @@
         <v>391</v>
       </c>
       <c r="I155" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="K155" s="3" t="s">
-        <v>410</v>
+        <v>406</v>
+      </c>
+      <c r="K155" s="12" t="s">
+        <v>407</v>
       </c>
       <c r="L155" s="7" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B156" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C156" t="s">
         <v>305</v>
@@ -6893,13 +6893,13 @@
         <v>391</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="K156" s="3" t="s">
-        <v>410</v>
+        <v>406</v>
+      </c>
+      <c r="K156" s="12" t="s">
+        <v>407</v>
       </c>
       <c r="L156" s="7" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.2">
@@ -6907,7 +6907,7 @@
         <v>389</v>
       </c>
       <c r="B157" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C157" t="s">
         <v>306</v>
@@ -6928,7 +6928,7 @@
         <v>389</v>
       </c>
       <c r="B158" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C158" t="s">
         <v>307</v>
@@ -6940,7 +6940,7 @@
         <v>2</v>
       </c>
       <c r="G158" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H158" s="3" t="s">
         <v>391</v>
@@ -6948,7 +6948,7 @@
       <c r="I158" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="K158" s="3" t="s">
+      <c r="K158" s="12" t="s">
         <v>393</v>
       </c>
       <c r="L158" s="6" t="s">
@@ -6960,7 +6960,7 @@
         <v>389</v>
       </c>
       <c r="B159" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C159" t="s">
         <v>308</v>
@@ -6968,23 +6968,23 @@
       <c r="D159" t="s">
         <v>388</v>
       </c>
-      <c r="F159" s="3">
-        <v>4</v>
+      <c r="F159" s="12">
+        <v>1</v>
       </c>
       <c r="G159" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H159" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I159" s="3" t="s">
-        <v>539</v>
-      </c>
-      <c r="K159" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="L159" s="6" t="s">
-        <v>537</v>
+        <v>487</v>
+      </c>
+      <c r="K159" s="12" t="s">
+        <v>567</v>
+      </c>
+      <c r="L159" s="7" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.2">
@@ -6992,7 +6992,7 @@
         <v>389</v>
       </c>
       <c r="B160" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C160" t="s">
         <v>309</v>
@@ -7010,13 +7010,13 @@
         <v>391</v>
       </c>
       <c r="I160" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="K160" s="3" t="s">
-        <v>468</v>
+        <v>429</v>
+      </c>
+      <c r="K160" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="L160" s="6" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.2">
@@ -7024,7 +7024,7 @@
         <v>389</v>
       </c>
       <c r="B161" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C161" t="s">
         <v>310</v>
@@ -7042,13 +7042,13 @@
         <v>391</v>
       </c>
       <c r="I161" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="K161" s="3" t="s">
-        <v>468</v>
+        <v>429</v>
+      </c>
+      <c r="K161" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="L161" s="6" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.2">
@@ -7056,7 +7056,7 @@
         <v>389</v>
       </c>
       <c r="B162" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C162" t="s">
         <v>311</v>
@@ -7074,13 +7074,13 @@
         <v>391</v>
       </c>
       <c r="I162" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="K162" s="3" t="s">
-        <v>468</v>
+        <v>429</v>
+      </c>
+      <c r="K162" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="L162" s="6" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.2">
@@ -7088,7 +7088,7 @@
         <v>389</v>
       </c>
       <c r="B163" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C163" t="s">
         <v>312</v>
@@ -7106,13 +7106,13 @@
         <v>391</v>
       </c>
       <c r="I163" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="K163" s="3" t="s">
-        <v>468</v>
+        <v>429</v>
+      </c>
+      <c r="K163" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="L163" s="6" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.2">
@@ -7120,7 +7120,7 @@
         <v>389</v>
       </c>
       <c r="B164" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C164" t="s">
         <v>313</v>
@@ -7138,13 +7138,13 @@
         <v>391</v>
       </c>
       <c r="I164" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="K164" s="3" t="s">
-        <v>468</v>
+        <v>429</v>
+      </c>
+      <c r="K164" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="L164" s="6" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.2">
@@ -7152,7 +7152,7 @@
         <v>389</v>
       </c>
       <c r="B165" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C165" t="s">
         <v>314</v>
@@ -7170,13 +7170,13 @@
         <v>391</v>
       </c>
       <c r="I165" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="K165" s="3" t="s">
-        <v>468</v>
+        <v>429</v>
+      </c>
+      <c r="K165" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="L165" s="6" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="166" spans="1:12" x14ac:dyDescent="0.2">
@@ -7184,7 +7184,7 @@
         <v>389</v>
       </c>
       <c r="B166" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C166" t="s">
         <v>315</v>
@@ -7196,19 +7196,19 @@
         <v>1</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H166" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I166" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="K166" s="3" t="s">
-        <v>489</v>
+        <v>487</v>
+      </c>
+      <c r="K166" s="12" t="s">
+        <v>486</v>
       </c>
       <c r="L166" s="6" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.2">
@@ -7216,7 +7216,7 @@
         <v>389</v>
       </c>
       <c r="B167" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C167" t="s">
         <v>316</v>
@@ -7234,13 +7234,13 @@
         <v>391</v>
       </c>
       <c r="I167" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="K167" s="3" t="s">
-        <v>431</v>
+        <v>429</v>
+      </c>
+      <c r="K167" s="12" t="s">
+        <v>428</v>
       </c>
       <c r="L167" s="6" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.2">
@@ -7248,7 +7248,7 @@
         <v>389</v>
       </c>
       <c r="B168" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C168" t="s">
         <v>317</v>
@@ -7266,13 +7266,13 @@
         <v>391</v>
       </c>
       <c r="I168" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="K168" s="3" t="s">
-        <v>431</v>
+        <v>429</v>
+      </c>
+      <c r="K168" s="12" t="s">
+        <v>428</v>
       </c>
       <c r="L168" s="6" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="169" spans="1:12" x14ac:dyDescent="0.2">
@@ -7280,7 +7280,7 @@
         <v>389</v>
       </c>
       <c r="B169" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C169" t="s">
         <v>318</v>
@@ -7298,13 +7298,13 @@
         <v>391</v>
       </c>
       <c r="I169" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="K169" s="3" t="s">
-        <v>431</v>
+        <v>429</v>
+      </c>
+      <c r="K169" s="12" t="s">
+        <v>428</v>
       </c>
       <c r="L169" s="6" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.2">
@@ -7312,7 +7312,7 @@
         <v>389</v>
       </c>
       <c r="B170" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C170" t="s">
         <v>319</v>
@@ -7330,13 +7330,13 @@
         <v>391</v>
       </c>
       <c r="I170" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="K170" s="3" t="s">
-        <v>431</v>
+        <v>429</v>
+      </c>
+      <c r="K170" s="12" t="s">
+        <v>428</v>
       </c>
       <c r="L170" s="6" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.2">
@@ -7344,7 +7344,7 @@
         <v>389</v>
       </c>
       <c r="B171" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C171" t="s">
         <v>320</v>
@@ -7362,13 +7362,13 @@
         <v>391</v>
       </c>
       <c r="I171" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="K171" s="3" t="s">
-        <v>431</v>
+        <v>429</v>
+      </c>
+      <c r="K171" s="12" t="s">
+        <v>428</v>
       </c>
       <c r="L171" s="6" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="172" spans="1:12" x14ac:dyDescent="0.2">
@@ -7376,7 +7376,7 @@
         <v>389</v>
       </c>
       <c r="B172" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C172" t="s">
         <v>321</v>
@@ -7394,13 +7394,13 @@
         <v>391</v>
       </c>
       <c r="I172" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="K172" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
+      </c>
+      <c r="K172" s="12" t="s">
+        <v>459</v>
       </c>
       <c r="L172" s="6" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="173" spans="1:12" x14ac:dyDescent="0.2">
@@ -7408,7 +7408,7 @@
         <v>389</v>
       </c>
       <c r="B173" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C173" t="s">
         <v>322</v>
@@ -7429,7 +7429,7 @@
         <v>389</v>
       </c>
       <c r="B174" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C174" t="s">
         <v>323</v>
@@ -7447,13 +7447,13 @@
         <v>391</v>
       </c>
       <c r="I174" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="K174" s="3" t="s">
-        <v>440</v>
+        <v>438</v>
+      </c>
+      <c r="K174" s="12" t="s">
+        <v>437</v>
       </c>
       <c r="L174" s="6" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.2">
@@ -7461,7 +7461,7 @@
         <v>389</v>
       </c>
       <c r="B175" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C175" t="s">
         <v>324</v>
@@ -7469,23 +7469,23 @@
       <c r="D175" t="s">
         <v>388</v>
       </c>
-      <c r="F175" s="3">
-        <v>3</v>
+      <c r="F175" s="12">
+        <v>1</v>
       </c>
       <c r="G175" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H175" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I175" s="3" t="s">
-        <v>530</v>
-      </c>
-      <c r="K175" s="3" t="s">
-        <v>549</v>
-      </c>
-      <c r="L175" s="6" t="s">
-        <v>548</v>
+        <v>562</v>
+      </c>
+      <c r="K175" s="12" t="s">
+        <v>563</v>
+      </c>
+      <c r="L175" s="7" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.2">
@@ -7493,7 +7493,7 @@
         <v>389</v>
       </c>
       <c r="B176" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C176" t="s">
         <v>325</v>
@@ -7501,23 +7501,23 @@
       <c r="D176" t="s">
         <v>388</v>
       </c>
-      <c r="F176" s="3">
+      <c r="F176" s="11">
         <v>5</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H176" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I176" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="K176" s="3" t="s">
-        <v>486</v>
+        <v>484</v>
+      </c>
+      <c r="K176" s="12" t="s">
+        <v>483</v>
       </c>
       <c r="L176" s="6" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.2">
@@ -7525,7 +7525,7 @@
         <v>389</v>
       </c>
       <c r="B177" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C177" t="s">
         <v>326</v>
@@ -7537,19 +7537,19 @@
         <v>5</v>
       </c>
       <c r="G177" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H177" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I177" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="K177" s="3" t="s">
         <v>484</v>
       </c>
+      <c r="K177" s="12" t="s">
+        <v>481</v>
+      </c>
       <c r="L177" s="6" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="178" spans="1:12" x14ac:dyDescent="0.2">
@@ -7557,7 +7557,7 @@
         <v>389</v>
       </c>
       <c r="B178" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C178" t="s">
         <v>327</v>
@@ -7569,19 +7569,19 @@
         <v>3</v>
       </c>
       <c r="G178" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H178" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I178" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="K178" s="3" t="s">
-        <v>543</v>
+        <v>531</v>
+      </c>
+      <c r="K178" s="12" t="s">
+        <v>530</v>
       </c>
       <c r="L178" s="6" t="s">
-        <v>542</v>
+        <v>529</v>
       </c>
     </row>
     <row r="179" spans="1:12" x14ac:dyDescent="0.2">
@@ -7589,7 +7589,7 @@
         <v>389</v>
       </c>
       <c r="B179" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C179" t="s">
         <v>328</v>
@@ -7597,23 +7597,23 @@
       <c r="D179" t="s">
         <v>388</v>
       </c>
-      <c r="F179" s="3">
+      <c r="F179" s="12">
         <v>2</v>
       </c>
       <c r="G179" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H179" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I179" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="K179" s="3" t="s">
-        <v>558</v>
+        <v>544</v>
+      </c>
+      <c r="K179" s="12" t="s">
+        <v>543</v>
       </c>
       <c r="L179" s="6" t="s">
-        <v>557</v>
+        <v>542</v>
       </c>
     </row>
     <row r="180" spans="1:12" x14ac:dyDescent="0.2">
@@ -7621,7 +7621,7 @@
         <v>389</v>
       </c>
       <c r="B180" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C180" t="s">
         <v>329</v>
@@ -7639,13 +7639,13 @@
         <v>391</v>
       </c>
       <c r="I180" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="K180" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
+      </c>
+      <c r="K180" s="12" t="s">
+        <v>448</v>
       </c>
       <c r="L180" s="6" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="181" spans="1:12" x14ac:dyDescent="0.2">
@@ -7653,7 +7653,7 @@
         <v>389</v>
       </c>
       <c r="B181" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C181" t="s">
         <v>330</v>
@@ -7661,31 +7661,31 @@
       <c r="D181" t="s">
         <v>388</v>
       </c>
-      <c r="F181" s="3">
+      <c r="F181" s="12">
         <v>2</v>
       </c>
       <c r="G181" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H181" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I181" s="3" t="s">
-        <v>562</v>
-      </c>
-      <c r="K181" s="3" t="s">
-        <v>561</v>
+        <v>547</v>
+      </c>
+      <c r="K181" s="12" t="s">
+        <v>546</v>
       </c>
       <c r="L181" s="6" t="s">
-        <v>560</v>
+        <v>545</v>
       </c>
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B182" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C182" t="s">
         <v>331</v>
@@ -7703,13 +7703,13 @@
         <v>391</v>
       </c>
       <c r="I182" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="K182" s="3" t="s">
-        <v>459</v>
+        <v>457</v>
+      </c>
+      <c r="K182" s="12" t="s">
+        <v>456</v>
       </c>
       <c r="L182" s="6" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.2">
@@ -7717,7 +7717,7 @@
         <v>389</v>
       </c>
       <c r="B183" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C183" t="s">
         <v>332</v>
@@ -7729,19 +7729,19 @@
         <v>1</v>
       </c>
       <c r="G183" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H183" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I183" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="K183" s="3" t="s">
-        <v>501</v>
+        <v>487</v>
+      </c>
+      <c r="K183" s="12" t="s">
+        <v>496</v>
       </c>
       <c r="L183" s="6" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.2">
@@ -7749,7 +7749,7 @@
         <v>389</v>
       </c>
       <c r="B184" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C184" t="s">
         <v>333</v>
@@ -7761,19 +7761,19 @@
         <v>1</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H184" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I184" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="K184" s="3" t="s">
-        <v>502</v>
+        <v>487</v>
+      </c>
+      <c r="K184" s="12" t="s">
+        <v>497</v>
       </c>
       <c r="L184" s="6" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.2">
@@ -7781,7 +7781,7 @@
         <v>389</v>
       </c>
       <c r="B185" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C185" t="s">
         <v>334</v>
@@ -7793,19 +7793,19 @@
         <v>1</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H185" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I185" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="K185" s="3" t="s">
-        <v>519</v>
+        <v>501</v>
+      </c>
+      <c r="K185" s="12" t="s">
+        <v>514</v>
       </c>
       <c r="L185" s="6" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.2">
@@ -7813,7 +7813,7 @@
         <v>389</v>
       </c>
       <c r="B186" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C186" t="s">
         <v>335</v>
@@ -7821,23 +7821,23 @@
       <c r="D186" t="s">
         <v>388</v>
       </c>
-      <c r="F186" s="3">
+      <c r="F186" s="11">
         <v>3</v>
       </c>
       <c r="G186" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H186" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I186" s="3" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="K186" s="3" t="s">
-        <v>564</v>
+        <v>549</v>
       </c>
       <c r="L186" s="6" t="s">
-        <v>563</v>
+        <v>548</v>
       </c>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.2">
@@ -7845,7 +7845,7 @@
         <v>389</v>
       </c>
       <c r="B187" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C187" t="s">
         <v>336</v>
@@ -7863,13 +7863,13 @@
         <v>391</v>
       </c>
       <c r="I187" s="3" t="s">
-        <v>482</v>
-      </c>
-      <c r="K187" s="3" t="s">
-        <v>481</v>
+        <v>479</v>
+      </c>
+      <c r="K187" s="12" t="s">
+        <v>478</v>
       </c>
       <c r="L187" s="6" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.2">
@@ -7877,7 +7877,7 @@
         <v>389</v>
       </c>
       <c r="B188" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C188" t="s">
         <v>337</v>
@@ -7895,13 +7895,13 @@
         <v>391</v>
       </c>
       <c r="I188" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="K188" s="3" t="s">
-        <v>476</v>
+        <v>474</v>
+      </c>
+      <c r="K188" s="12" t="s">
+        <v>473</v>
       </c>
       <c r="L188" s="6" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.2">
@@ -7909,7 +7909,7 @@
         <v>389</v>
       </c>
       <c r="B189" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C189" t="s">
         <v>338</v>
@@ -7927,13 +7927,13 @@
         <v>391</v>
       </c>
       <c r="I189" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="K189" s="3" t="s">
-        <v>476</v>
+        <v>474</v>
+      </c>
+      <c r="K189" s="12" t="s">
+        <v>473</v>
       </c>
       <c r="L189" s="6" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.2">
@@ -7941,7 +7941,7 @@
         <v>389</v>
       </c>
       <c r="B190" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C190" t="s">
         <v>339</v>
@@ -7959,13 +7959,13 @@
         <v>391</v>
       </c>
       <c r="I190" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="K190" s="12" t="s">
         <v>425</v>
       </c>
-      <c r="K190" s="3" t="s">
-        <v>428</v>
-      </c>
       <c r="L190" s="6" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.2">
@@ -7973,7 +7973,7 @@
         <v>389</v>
       </c>
       <c r="B191" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C191" t="s">
         <v>340</v>
@@ -7991,13 +7991,13 @@
         <v>391</v>
       </c>
       <c r="I191" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="K191" s="3" t="s">
-        <v>424</v>
+        <v>422</v>
+      </c>
+      <c r="K191" s="12" t="s">
+        <v>421</v>
       </c>
       <c r="L191" s="6" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.2">
@@ -8005,7 +8005,7 @@
         <v>389</v>
       </c>
       <c r="B192" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C192" t="s">
         <v>341</v>
@@ -8023,13 +8023,13 @@
         <v>391</v>
       </c>
       <c r="I192" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="K192" s="3" t="s">
-        <v>427</v>
+        <v>422</v>
+      </c>
+      <c r="K192" s="12" t="s">
+        <v>424</v>
       </c>
       <c r="L192" s="6" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.2">
@@ -8037,7 +8037,7 @@
         <v>389</v>
       </c>
       <c r="B193" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C193" t="s">
         <v>342</v>
@@ -8045,23 +8045,23 @@
       <c r="D193" t="s">
         <v>388</v>
       </c>
-      <c r="F193" s="3">
-        <v>4</v>
+      <c r="F193" s="12">
+        <v>1</v>
       </c>
       <c r="G193" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H193" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I193" s="3" t="s">
-        <v>539</v>
-      </c>
-      <c r="K193" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="L193" s="6" t="s">
-        <v>540</v>
+        <v>565</v>
+      </c>
+      <c r="K193" s="12" t="s">
+        <v>569</v>
+      </c>
+      <c r="L193" s="7" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.2">
@@ -8069,7 +8069,7 @@
         <v>389</v>
       </c>
       <c r="B194" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C194" t="s">
         <v>343</v>
@@ -8077,23 +8077,23 @@
       <c r="D194" t="s">
         <v>388</v>
       </c>
-      <c r="F194" s="3">
+      <c r="F194" s="11">
         <v>2</v>
       </c>
       <c r="G194" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H194" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I194" s="3" t="s">
-        <v>555</v>
+        <v>540</v>
       </c>
       <c r="K194" s="3" t="s">
-        <v>554</v>
+        <v>539</v>
       </c>
       <c r="L194" s="6" t="s">
-        <v>553</v>
+        <v>538</v>
       </c>
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.2">
@@ -8101,7 +8101,7 @@
         <v>389</v>
       </c>
       <c r="B195" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C195" t="s">
         <v>344</v>
@@ -8109,23 +8109,23 @@
       <c r="D195" t="s">
         <v>388</v>
       </c>
-      <c r="F195" s="3">
+      <c r="F195" s="11">
         <v>3</v>
       </c>
       <c r="G195" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H195" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I195" s="3" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="K195" s="3" t="s">
-        <v>554</v>
+        <v>539</v>
       </c>
       <c r="L195" s="6" t="s">
-        <v>556</v>
+        <v>541</v>
       </c>
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.2">
@@ -8133,7 +8133,7 @@
         <v>389</v>
       </c>
       <c r="B196" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C196" t="s">
         <v>345</v>
@@ -8141,23 +8141,23 @@
       <c r="D196" t="s">
         <v>388</v>
       </c>
-      <c r="F196" s="3">
+      <c r="F196" s="11">
         <v>4</v>
       </c>
       <c r="G196" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H196" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I196" s="3" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="K196" s="3" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="L196" s="6" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.2">
@@ -8165,7 +8165,7 @@
         <v>389</v>
       </c>
       <c r="B197" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C197" t="s">
         <v>346</v>
@@ -8173,23 +8173,23 @@
       <c r="D197" t="s">
         <v>388</v>
       </c>
-      <c r="F197" s="3">
+      <c r="F197" s="11">
         <v>10</v>
       </c>
       <c r="G197" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H197" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I197" s="3" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="K197" s="3" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="L197" s="6" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.2">
@@ -8197,7 +8197,7 @@
         <v>389</v>
       </c>
       <c r="B198" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C198" t="s">
         <v>347</v>
@@ -8217,7 +8217,7 @@
       <c r="I198" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="K198" s="3" t="s">
+      <c r="K198" s="12" t="s">
         <v>395</v>
       </c>
       <c r="L198" s="6" t="s">
@@ -8229,7 +8229,7 @@
         <v>389</v>
       </c>
       <c r="B199" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C199" t="s">
         <v>348</v>
@@ -8247,13 +8247,13 @@
         <v>391</v>
       </c>
       <c r="I199" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="K199" s="3" t="s">
-        <v>419</v>
+        <v>411</v>
+      </c>
+      <c r="K199" s="12" t="s">
+        <v>416</v>
       </c>
       <c r="L199" s="6" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.2">
@@ -8261,7 +8261,7 @@
         <v>389</v>
       </c>
       <c r="B200" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C200" t="s">
         <v>349</v>
@@ -8281,7 +8281,7 @@
       <c r="I200" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="K200" s="3" t="s">
+      <c r="K200" s="12" t="s">
         <v>398</v>
       </c>
       <c r="L200" s="7" t="s">
@@ -8293,7 +8293,7 @@
         <v>389</v>
       </c>
       <c r="B201" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C201" t="s">
         <v>350</v>
@@ -8311,13 +8311,13 @@
         <v>391</v>
       </c>
       <c r="I201" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="K201" s="3" t="s">
-        <v>413</v>
+        <v>411</v>
+      </c>
+      <c r="K201" s="12" t="s">
+        <v>410</v>
       </c>
       <c r="L201" s="6" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.2">
@@ -8325,7 +8325,7 @@
         <v>389</v>
       </c>
       <c r="B202" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C202" t="s">
         <v>351</v>
@@ -8333,23 +8333,23 @@
       <c r="D202" t="s">
         <v>388</v>
       </c>
-      <c r="F202" s="3">
+      <c r="F202" s="11">
         <v>2</v>
       </c>
       <c r="G202" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H202" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I202" s="3" t="s">
-        <v>567</v>
+        <v>552</v>
       </c>
       <c r="K202" s="3" t="s">
-        <v>566</v>
+        <v>551</v>
       </c>
       <c r="L202" s="6" t="s">
-        <v>565</v>
+        <v>550</v>
       </c>
     </row>
     <row r="203" spans="1:12" x14ac:dyDescent="0.2">
@@ -8357,7 +8357,7 @@
         <v>389</v>
       </c>
       <c r="B203" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C203" t="s">
         <v>352</v>
@@ -8369,19 +8369,19 @@
         <v>2</v>
       </c>
       <c r="G203" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H203" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I203" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="K203" s="3" t="s">
-        <v>508</v>
+        <v>501</v>
+      </c>
+      <c r="K203" s="12" t="s">
+        <v>503</v>
       </c>
       <c r="L203" s="6" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.2">
@@ -8389,7 +8389,7 @@
         <v>389</v>
       </c>
       <c r="B204" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C204" t="s">
         <v>353</v>
@@ -8401,19 +8401,19 @@
         <v>2</v>
       </c>
       <c r="G204" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H204" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I204" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="K204" s="3" t="s">
-        <v>551</v>
+        <v>537</v>
+      </c>
+      <c r="K204" s="12" t="s">
+        <v>536</v>
       </c>
       <c r="L204" s="6" t="s">
-        <v>550</v>
+        <v>535</v>
       </c>
     </row>
     <row r="205" spans="1:12" x14ac:dyDescent="0.2">
@@ -8421,7 +8421,7 @@
         <v>389</v>
       </c>
       <c r="B205" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C205" t="s">
         <v>354</v>
@@ -8433,19 +8433,19 @@
         <v>0</v>
       </c>
       <c r="G205" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H205" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I205" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="K205" s="3" t="s">
-        <v>551</v>
+        <v>537</v>
+      </c>
+      <c r="K205" s="12" t="s">
+        <v>536</v>
       </c>
       <c r="L205" s="6" t="s">
-        <v>550</v>
+        <v>535</v>
       </c>
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.2">
@@ -8453,7 +8453,7 @@
         <v>389</v>
       </c>
       <c r="B206" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C206" t="s">
         <v>355</v>
@@ -8465,19 +8465,19 @@
         <v>1</v>
       </c>
       <c r="G206" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H206" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I206" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="K206" s="3" t="s">
-        <v>513</v>
+        <v>509</v>
+      </c>
+      <c r="K206" s="12" t="s">
+        <v>508</v>
       </c>
       <c r="L206" s="6" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
     </row>
     <row r="207" spans="1:12" x14ac:dyDescent="0.2">
@@ -8485,7 +8485,7 @@
         <v>389</v>
       </c>
       <c r="B207" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C207" t="s">
         <v>356</v>
@@ -8493,23 +8493,23 @@
       <c r="D207" t="s">
         <v>388</v>
       </c>
-      <c r="F207" s="3">
+      <c r="F207" s="12">
         <v>3</v>
       </c>
       <c r="G207" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H207" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I207" s="3" t="s">
-        <v>530</v>
-      </c>
-      <c r="K207" s="3" t="s">
-        <v>529</v>
+        <v>522</v>
+      </c>
+      <c r="K207" s="12" t="s">
+        <v>521</v>
       </c>
       <c r="L207" s="6" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="208" spans="1:12" x14ac:dyDescent="0.2">
@@ -8517,7 +8517,7 @@
         <v>389</v>
       </c>
       <c r="B208" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C208" t="s">
         <v>357</v>
@@ -8525,23 +8525,23 @@
       <c r="D208" t="s">
         <v>388</v>
       </c>
-      <c r="F208" s="3">
+      <c r="F208" s="12">
         <v>2</v>
       </c>
       <c r="G208" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H208" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I208" s="3" t="s">
-        <v>527</v>
-      </c>
-      <c r="K208" s="3" t="s">
-        <v>526</v>
+        <v>519</v>
+      </c>
+      <c r="K208" s="12" t="s">
+        <v>518</v>
       </c>
       <c r="L208" s="6" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.2">
@@ -8549,7 +8549,7 @@
         <v>389</v>
       </c>
       <c r="B209" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C209" t="s">
         <v>358</v>
@@ -8557,23 +8557,23 @@
       <c r="D209" t="s">
         <v>388</v>
       </c>
-      <c r="F209" s="3">
+      <c r="F209" s="12">
         <v>2</v>
       </c>
       <c r="G209" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H209" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I209" s="3" t="s">
-        <v>547</v>
-      </c>
-      <c r="K209" s="3" t="s">
-        <v>546</v>
+        <v>534</v>
+      </c>
+      <c r="K209" s="12" t="s">
+        <v>533</v>
       </c>
       <c r="L209" s="6" t="s">
-        <v>545</v>
+        <v>532</v>
       </c>
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.2">
@@ -8581,7 +8581,7 @@
         <v>389</v>
       </c>
       <c r="B210" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C210" t="s">
         <v>359</v>
@@ -8593,19 +8593,19 @@
         <v>2</v>
       </c>
       <c r="G210" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H210" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I210" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="K210" s="3" t="s">
-        <v>505</v>
+        <v>501</v>
+      </c>
+      <c r="K210" s="12" t="s">
+        <v>500</v>
       </c>
       <c r="L210" s="6" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.2">
@@ -8613,7 +8613,7 @@
         <v>389</v>
       </c>
       <c r="B211" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C211" t="s">
         <v>360</v>
@@ -8625,19 +8625,19 @@
         <v>0</v>
       </c>
       <c r="G211" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H211" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I211" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="K211" s="3" t="s">
-        <v>505</v>
+        <v>501</v>
+      </c>
+      <c r="K211" s="12" t="s">
+        <v>500</v>
       </c>
       <c r="L211" s="6" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.2">
@@ -8645,7 +8645,7 @@
         <v>389</v>
       </c>
       <c r="B212" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C212" t="s">
         <v>361</v>
@@ -8657,19 +8657,19 @@
         <v>0</v>
       </c>
       <c r="G212" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H212" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I212" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="K212" s="3" t="s">
-        <v>505</v>
+        <v>501</v>
+      </c>
+      <c r="K212" s="12" t="s">
+        <v>500</v>
       </c>
       <c r="L212" s="6" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.2">
@@ -8677,7 +8677,7 @@
         <v>389</v>
       </c>
       <c r="B213" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C213" t="s">
         <v>362</v>
@@ -8689,19 +8689,19 @@
         <v>0</v>
       </c>
       <c r="G213" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H213" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I213" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="K213" s="3" t="s">
-        <v>505</v>
+        <v>501</v>
+      </c>
+      <c r="K213" s="12" t="s">
+        <v>500</v>
       </c>
       <c r="L213" s="6" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="214" spans="1:12" x14ac:dyDescent="0.2">
@@ -8709,7 +8709,7 @@
         <v>389</v>
       </c>
       <c r="B214" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C214" t="s">
         <v>363</v>
@@ -8721,19 +8721,19 @@
         <v>2</v>
       </c>
       <c r="G214" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H214" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I214" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="K214" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="L214" s="6" t="s">
         <v>490</v>
-      </c>
-      <c r="K214" s="3" t="s">
-        <v>494</v>
-      </c>
-      <c r="L214" s="6" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="215" spans="1:12" x14ac:dyDescent="0.2">
@@ -8741,7 +8741,7 @@
         <v>389</v>
       </c>
       <c r="B215" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C215" t="s">
         <v>364</v>
@@ -8750,22 +8750,22 @@
         <v>388</v>
       </c>
       <c r="F215" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G215" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H215" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I215" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="K215" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="L215" s="6" t="s">
         <v>490</v>
-      </c>
-      <c r="K215" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="L215" s="7" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="216" spans="1:12" x14ac:dyDescent="0.2">
@@ -8773,7 +8773,7 @@
         <v>389</v>
       </c>
       <c r="B216" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C216" t="s">
         <v>365</v>
@@ -8781,23 +8781,23 @@
       <c r="D216" t="s">
         <v>388</v>
       </c>
-      <c r="F216" s="3">
+      <c r="F216" s="11">
         <v>5</v>
       </c>
       <c r="G216" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H216" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I216" s="3" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="K216" s="3" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="L216" s="6" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.2">
@@ -8805,7 +8805,7 @@
         <v>389</v>
       </c>
       <c r="B217" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C217" t="s">
         <v>366</v>
@@ -8817,19 +8817,19 @@
         <v>3</v>
       </c>
       <c r="G217" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H217" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I217" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="K217" s="3" t="s">
-        <v>492</v>
+        <v>487</v>
+      </c>
+      <c r="K217" s="12" t="s">
+        <v>489</v>
       </c>
       <c r="L217" s="6" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.2">
@@ -8837,7 +8837,7 @@
         <v>389</v>
       </c>
       <c r="B218" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C218" t="s">
         <v>367</v>
@@ -8849,19 +8849,19 @@
         <v>0</v>
       </c>
       <c r="G218" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H218" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I218" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="K218" s="3" t="s">
-        <v>492</v>
+        <v>487</v>
+      </c>
+      <c r="K218" s="12" t="s">
+        <v>489</v>
       </c>
       <c r="L218" s="6" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.2">
@@ -8869,7 +8869,7 @@
         <v>389</v>
       </c>
       <c r="B219" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C219" t="s">
         <v>368</v>
@@ -8881,19 +8881,19 @@
         <v>0</v>
       </c>
       <c r="G219" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H219" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I219" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="K219" s="3" t="s">
-        <v>492</v>
+        <v>487</v>
+      </c>
+      <c r="K219" s="12" t="s">
+        <v>489</v>
       </c>
       <c r="L219" s="6" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.2">
@@ -8901,7 +8901,7 @@
         <v>389</v>
       </c>
       <c r="B220" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C220" t="s">
         <v>369</v>
@@ -8909,11 +8909,11 @@
       <c r="D220" t="s">
         <v>388</v>
       </c>
-      <c r="F220" s="3">
+      <c r="F220" s="11">
         <v>3</v>
       </c>
       <c r="G220" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H220" s="3" t="s">
         <v>391</v>
@@ -8921,19 +8921,19 @@
       <c r="I220" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="K220" s="3" t="s">
-        <v>521</v>
+      <c r="K220" s="12" t="s">
+        <v>516</v>
       </c>
       <c r="L220" s="6" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B221" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C221" t="s">
         <v>370</v>
@@ -8951,21 +8951,21 @@
         <v>391</v>
       </c>
       <c r="I221" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="K221" s="3" t="s">
-        <v>465</v>
+        <v>463</v>
+      </c>
+      <c r="K221" s="12" t="s">
+        <v>462</v>
       </c>
       <c r="L221" s="6" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B222" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C222" t="s">
         <v>371</v>
@@ -8983,21 +8983,21 @@
         <v>391</v>
       </c>
       <c r="I222" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="K222" s="3" t="s">
-        <v>421</v>
+        <v>419</v>
+      </c>
+      <c r="K222" s="12" t="s">
+        <v>418</v>
       </c>
       <c r="L222" s="6" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B223" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C223" t="s">
         <v>372</v>
@@ -9015,13 +9015,13 @@
         <v>391</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="K223" s="3" t="s">
-        <v>437</v>
+        <v>435</v>
+      </c>
+      <c r="K223" s="12" t="s">
+        <v>434</v>
       </c>
       <c r="L223" s="6" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.2">
@@ -9029,7 +9029,7 @@
         <v>389</v>
       </c>
       <c r="B224" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C224" t="s">
         <v>373</v>
@@ -9047,13 +9047,13 @@
         <v>391</v>
       </c>
       <c r="I224" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="K224" s="3" t="s">
-        <v>448</v>
+        <v>446</v>
+      </c>
+      <c r="K224" s="12" t="s">
+        <v>445</v>
       </c>
       <c r="L224" s="6" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="225" spans="1:12" x14ac:dyDescent="0.2">
@@ -9061,7 +9061,7 @@
         <v>389</v>
       </c>
       <c r="B225" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C225" t="s">
         <v>374</v>
@@ -9079,13 +9079,13 @@
         <v>391</v>
       </c>
       <c r="I225" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="K225" s="3" t="s">
-        <v>434</v>
+        <v>411</v>
+      </c>
+      <c r="K225" s="12" t="s">
+        <v>431</v>
       </c>
       <c r="L225" s="6" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.2">
@@ -9093,7 +9093,7 @@
         <v>389</v>
       </c>
       <c r="B226" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C226" t="s">
         <v>375</v>
@@ -9111,13 +9111,13 @@
         <v>391</v>
       </c>
       <c r="I226" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="K226" s="3" t="s">
-        <v>448</v>
+        <v>446</v>
+      </c>
+      <c r="K226" s="12" t="s">
+        <v>445</v>
       </c>
       <c r="L226" s="6" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.2">
@@ -9125,7 +9125,7 @@
         <v>389</v>
       </c>
       <c r="B227" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C227" t="s">
         <v>376</v>
@@ -9143,13 +9143,13 @@
         <v>391</v>
       </c>
       <c r="I227" s="3" t="s">
-        <v>457</v>
-      </c>
-      <c r="K227" s="3" t="s">
-        <v>456</v>
+        <v>454</v>
+      </c>
+      <c r="K227" s="12" t="s">
+        <v>453</v>
       </c>
       <c r="L227" s="6" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.2">
@@ -9157,7 +9157,7 @@
         <v>389</v>
       </c>
       <c r="B228" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C228" t="s">
         <v>377</v>
@@ -9175,13 +9175,13 @@
         <v>391</v>
       </c>
       <c r="I228" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="K228" s="3" t="s">
-        <v>479</v>
+        <v>411</v>
+      </c>
+      <c r="K228" s="12" t="s">
+        <v>476</v>
       </c>
       <c r="L228" s="6" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.2">
@@ -9189,7 +9189,7 @@
         <v>389</v>
       </c>
       <c r="B229" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C229" t="s">
         <v>378</v>
@@ -9201,19 +9201,19 @@
         <v>1</v>
       </c>
       <c r="G229" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H229" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I229" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="K229" s="3" t="s">
-        <v>510</v>
+        <v>506</v>
+      </c>
+      <c r="K229" s="12" t="s">
+        <v>505</v>
       </c>
       <c r="L229" s="6" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.2">
@@ -9221,7 +9221,7 @@
         <v>389</v>
       </c>
       <c r="B230" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C230" t="s">
         <v>379</v>
@@ -9239,13 +9239,13 @@
         <v>391</v>
       </c>
       <c r="I230" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="K230" s="3" t="s">
-        <v>443</v>
+        <v>441</v>
+      </c>
+      <c r="K230" s="12" t="s">
+        <v>440</v>
       </c>
       <c r="L230" s="6" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.2">
@@ -9253,7 +9253,7 @@
         <v>389</v>
       </c>
       <c r="B231" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C231" t="s">
         <v>380</v>
@@ -9271,13 +9271,13 @@
         <v>391</v>
       </c>
       <c r="I231" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="K231" s="3" t="s">
         <v>443</v>
       </c>
+      <c r="K231" s="12" t="s">
+        <v>440</v>
+      </c>
       <c r="L231" s="6" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.2">
@@ -9285,7 +9285,7 @@
         <v>389</v>
       </c>
       <c r="B232" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C232" t="s">
         <v>381</v>
@@ -9303,21 +9303,21 @@
         <v>391</v>
       </c>
       <c r="I232" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="K232" s="3" t="s">
-        <v>454</v>
+        <v>411</v>
+      </c>
+      <c r="K232" s="12" t="s">
+        <v>451</v>
       </c>
       <c r="L232" s="6" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B233" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C233" t="s">
         <v>382</v>
@@ -9335,13 +9335,13 @@
         <v>391</v>
       </c>
       <c r="I233" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="K233" s="3" t="s">
-        <v>416</v>
+        <v>414</v>
+      </c>
+      <c r="K233" s="12" t="s">
+        <v>413</v>
       </c>
       <c r="L233" s="6" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.2">
@@ -9349,7 +9349,7 @@
         <v>389</v>
       </c>
       <c r="B234" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C234" t="s">
         <v>383</v>
@@ -9357,23 +9357,23 @@
       <c r="D234" t="s">
         <v>388</v>
       </c>
-      <c r="F234" s="3">
+      <c r="F234" s="11">
         <v>2</v>
       </c>
       <c r="G234" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H234" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I234" s="3" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="K234" s="3" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="L234" s="10" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.2">
@@ -9381,7 +9381,7 @@
         <v>389</v>
       </c>
       <c r="B235" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C235" t="s">
         <v>384</v>
@@ -9390,22 +9390,23 @@
         <v>388</v>
       </c>
       <c r="F235" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G235" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H235" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I235" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="K235" s="3" t="s">
-        <v>523</v>
+      <c r="I235" t="s">
+        <v>573</v>
+      </c>
+      <c r="J235"/>
+      <c r="K235" s="13" t="s">
+        <v>574</v>
       </c>
       <c r="L235" s="6" t="s">
-        <v>522</v>
+        <v>575</v>
       </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.2">
@@ -9413,7 +9414,7 @@
         <v>389</v>
       </c>
       <c r="B236" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C236" t="s">
         <v>385</v>
@@ -9422,30 +9423,31 @@
         <v>388</v>
       </c>
       <c r="F236" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G236" s="3" t="s">
-        <v>435</v>
+        <v>174</v>
       </c>
       <c r="H236" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I236" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="K236" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="L236" s="7" t="s">
-        <v>403</v>
+      <c r="I236" t="s">
+        <v>570</v>
+      </c>
+      <c r="J236"/>
+      <c r="K236" s="13" t="s">
+        <v>571</v>
+      </c>
+      <c r="L236" s="6" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B237" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C237" t="s">
         <v>386</v>
@@ -9463,13 +9465,13 @@
         <v>391</v>
       </c>
       <c r="I237" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="K237" s="3" t="s">
-        <v>406</v>
+        <v>402</v>
+      </c>
+      <c r="K237" s="12" t="s">
+        <v>403</v>
       </c>
       <c r="L237" s="7" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.2">
@@ -9477,7 +9479,7 @@
         <v>389</v>
       </c>
       <c r="B238" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C238" t="s">
         <v>58</v>
@@ -9495,13 +9497,13 @@
         <v>391</v>
       </c>
       <c r="I238" s="3" t="s">
-        <v>471</v>
-      </c>
-      <c r="K238" s="3" t="s">
-        <v>470</v>
+        <v>468</v>
+      </c>
+      <c r="K238" s="12" t="s">
+        <v>467</v>
       </c>
       <c r="L238" s="6" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.2">
@@ -9509,7 +9511,7 @@
         <v>389</v>
       </c>
       <c r="B239" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C239" t="s">
         <v>387</v>
@@ -9527,13 +9529,13 @@
         <v>391</v>
       </c>
       <c r="I239" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="K239" s="3" t="s">
-        <v>474</v>
+        <v>470</v>
+      </c>
+      <c r="K239" s="12" t="s">
+        <v>471</v>
       </c>
       <c r="L239" s="6" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -9666,82 +9668,82 @@
     <hyperlink ref="L158" r:id="rId125" xr:uid="{F88953B7-468E-C34B-9347-94009F9A78D2}"/>
     <hyperlink ref="L198" r:id="rId126" xr:uid="{1F3BBC8C-29E8-C74A-AB3F-04AE466222EF}"/>
     <hyperlink ref="L200" r:id="rId127" xr:uid="{3C51058F-793C-D34A-8286-18AE4C8EF6CE}"/>
-    <hyperlink ref="L236" r:id="rId128" xr:uid="{A1386B57-DD43-6F4A-8F35-D9075616F763}"/>
-    <hyperlink ref="L237" r:id="rId129" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
-    <hyperlink ref="L155" r:id="rId130" xr:uid="{6A722A1D-2F7B-4242-8134-716EFF33F7D2}"/>
-    <hyperlink ref="L156" r:id="rId131" xr:uid="{547CD1A8-1967-1C46-95E3-89E39CD045C2}"/>
-    <hyperlink ref="L201" r:id="rId132" xr:uid="{5ACD6BFD-52F0-0940-AA8E-B04F1D397BC7}"/>
-    <hyperlink ref="L233" r:id="rId133" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
-    <hyperlink ref="L199" r:id="rId134" xr:uid="{2030AD8C-28A7-544B-92DC-5CBE411DE1C0}"/>
-    <hyperlink ref="L222" r:id="rId135" xr:uid="{05363CA1-BE60-3F42-B56A-1A92A0EDA166}"/>
-    <hyperlink ref="L191" r:id="rId136" xr:uid="{D4C66DCB-D6B4-EC4F-A922-B87887BE6E4A}"/>
-    <hyperlink ref="L190" r:id="rId137" xr:uid="{A05D9F8A-ED0A-4143-8920-9422DD4E0BDD}"/>
-    <hyperlink ref="L192" r:id="rId138" xr:uid="{83FA4EC1-AB5E-3B43-9476-4CA54526DF8E}"/>
-    <hyperlink ref="L171" r:id="rId139" xr:uid="{21B7C9CB-274E-C246-8989-83D9E0E7B24F}"/>
-    <hyperlink ref="L167" r:id="rId140" xr:uid="{B5B4FA15-B24C-CE46-9594-7ED28656AA43}"/>
-    <hyperlink ref="L168" r:id="rId141" xr:uid="{3AB6BE1F-95C1-A443-B12D-D7A523FAD6C5}"/>
-    <hyperlink ref="L169" r:id="rId142" xr:uid="{347BDCC2-5A0C-B249-8CA8-B72D245480FC}"/>
-    <hyperlink ref="L170" r:id="rId143" xr:uid="{E58DD28D-BD99-DF44-9E5E-B3D05F881C1F}"/>
-    <hyperlink ref="L225" r:id="rId144" xr:uid="{4F668E79-3664-0547-B3D5-B7724A9D574D}"/>
-    <hyperlink ref="L223" r:id="rId145" xr:uid="{8AB5C10C-8B45-1843-96BD-655A4FA04EFD}"/>
-    <hyperlink ref="L174" r:id="rId146" xr:uid="{EAED74E0-13EE-A046-9ADC-AC8BDE30C3E6}"/>
-    <hyperlink ref="L230" r:id="rId147" xr:uid="{3577256C-215B-134E-B541-B7B77272CD8A}"/>
-    <hyperlink ref="L231" r:id="rId148" xr:uid="{98E325FC-7F95-B44E-98EB-DE0FF53BC89D}"/>
-    <hyperlink ref="L224" r:id="rId149" xr:uid="{5CE3083F-F217-3743-B613-A7DDF354E72D}"/>
-    <hyperlink ref="L226" r:id="rId150" xr:uid="{B81B6B41-2C17-AA48-B730-D906488BA0A0}"/>
-    <hyperlink ref="L180" r:id="rId151" xr:uid="{BA0813A2-2582-7A46-A492-16A943824EE5}"/>
-    <hyperlink ref="L232" r:id="rId152" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
-    <hyperlink ref="L227" r:id="rId153" xr:uid="{C5265333-F7F0-1845-98D7-68E930F9DFAE}"/>
-    <hyperlink ref="L182" r:id="rId154" xr:uid="{C0A159CB-3986-1A46-95AD-DCEFF4247697}"/>
-    <hyperlink ref="L172" r:id="rId155" xr:uid="{37810A74-E45D-1D46-AEF5-C5FE2F414285}"/>
-    <hyperlink ref="L221" r:id="rId156" xr:uid="{D2906064-B1B8-4648-8201-BEFA97591226}"/>
-    <hyperlink ref="L160" r:id="rId157" xr:uid="{1D3CD52E-7AAD-E444-88F4-4BAE6C5B5EB7}"/>
-    <hyperlink ref="L161" r:id="rId158" xr:uid="{E6E6DA47-945D-6145-912F-08B17B7BA6AE}"/>
-    <hyperlink ref="L162" r:id="rId159" xr:uid="{006B1689-D89A-1E4A-BBC5-E9C9583907F7}"/>
-    <hyperlink ref="L163" r:id="rId160" xr:uid="{C3E773B2-D410-AF41-B197-4638485DC8EF}"/>
-    <hyperlink ref="L164" r:id="rId161" xr:uid="{A0E8A8E2-4A93-3D42-AF48-81955241A483}"/>
-    <hyperlink ref="L165" r:id="rId162" xr:uid="{1B03F18A-8745-AA4F-AA8B-88D65D3B24BC}"/>
-    <hyperlink ref="L238" r:id="rId163" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
-    <hyperlink ref="L239" r:id="rId164" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
-    <hyperlink ref="L188" r:id="rId165" xr:uid="{D6B77117-A0D5-9240-8193-0102C36CCE4C}"/>
-    <hyperlink ref="L189" r:id="rId166" xr:uid="{79FB1103-88A8-8044-9E2C-4FAEC0906E8E}"/>
-    <hyperlink ref="L228" r:id="rId167" xr:uid="{5BF1C4C9-E63A-4F42-9042-36520975FDFA}"/>
-    <hyperlink ref="L187" r:id="rId168" xr:uid="{21CDF460-9871-0547-AA6B-20304C8DD21D}"/>
-    <hyperlink ref="L177" r:id="rId169" xr:uid="{BA1EC844-435A-6C44-87FC-C12B7ECFC55B}"/>
-    <hyperlink ref="L176" r:id="rId170" xr:uid="{46D875DC-CDDD-7E4B-88DB-DFC416CF17AB}"/>
-    <hyperlink ref="L166" r:id="rId171" xr:uid="{7D2FF6AE-1C67-9D4A-A760-7E3745DD9EA6}"/>
-    <hyperlink ref="L214" r:id="rId172" xr:uid="{B5E5E388-8F37-414E-A0C6-1DC58E77628C}"/>
-    <hyperlink ref="L215" r:id="rId173" xr:uid="{D62BC330-84EA-AE41-A129-2BC1AE7C44D1}"/>
-    <hyperlink ref="L216" r:id="rId174" xr:uid="{A96B1ACF-D982-9240-BB1C-69459154AE5A}"/>
-    <hyperlink ref="L183" r:id="rId175" xr:uid="{D3BB695A-CBA9-D649-B49D-4CC8D16EFD9B}"/>
-    <hyperlink ref="L184" r:id="rId176" xr:uid="{A2922BA8-758D-3149-892C-B7B65B435332}"/>
-    <hyperlink ref="L203" r:id="rId177" xr:uid="{BDB09119-6289-4346-BC29-7A54BD393127}"/>
-    <hyperlink ref="L229" r:id="rId178" xr:uid="{5736CAF4-3646-3243-9AEB-4D82B6D0D10A}"/>
-    <hyperlink ref="L206" r:id="rId179" xr:uid="{60659D55-801C-9A4E-84CA-809884CCBE5C}"/>
-    <hyperlink ref="L196" r:id="rId180" xr:uid="{18DDC006-0939-794C-9B5D-10593F8C0973}"/>
-    <hyperlink ref="L185" r:id="rId181" xr:uid="{50EA46A5-11DD-0345-ABCA-4206D73C7606}"/>
-    <hyperlink ref="L220" r:id="rId182" xr:uid="{63DDFF3B-E62C-9445-96AD-4BB37ACCD20E}"/>
-    <hyperlink ref="L235" r:id="rId183" xr:uid="{F4FBFB75-F824-8643-A03A-0A3479747FAB}"/>
-    <hyperlink ref="L208" r:id="rId184" xr:uid="{05E34BC1-B22F-3E46-8574-E72267507402}"/>
-    <hyperlink ref="L207" r:id="rId185" xr:uid="{7125DF67-5A7E-D948-8363-A31AB1EBA44A}"/>
-    <hyperlink ref="L234" r:id="rId186" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
-    <hyperlink ref="L197" r:id="rId187" xr:uid="{CCE2D666-E296-D94C-ACE0-791CC746483B}"/>
-    <hyperlink ref="L159" r:id="rId188" xr:uid="{213D9061-74C7-4745-9991-1B8CB77BAE4C}"/>
-    <hyperlink ref="L193" r:id="rId189" xr:uid="{357D2DAE-7369-6541-B091-9DF1685B9573}"/>
-    <hyperlink ref="L178" r:id="rId190" xr:uid="{E5A2F3EE-A3B1-0842-9364-E4B6EACA9544}"/>
-    <hyperlink ref="L209" r:id="rId191" xr:uid="{E08C8BA4-5414-1947-9CA8-45FE0B846CD1}"/>
-    <hyperlink ref="L175" r:id="rId192" xr:uid="{A3B57AE0-BE24-DE4E-84B5-3ECB73F4B476}"/>
-    <hyperlink ref="L205" r:id="rId193" xr:uid="{F1A64091-5BF7-8243-B7A0-F4C13B8B0ABB}"/>
-    <hyperlink ref="L194" r:id="rId194" xr:uid="{745AEF03-3150-C54B-800A-696460474256}"/>
-    <hyperlink ref="L195" r:id="rId195" xr:uid="{9C078FBA-3B11-8049-9187-5BC86D78EA09}"/>
-    <hyperlink ref="L179" r:id="rId196" xr:uid="{BF9A6A48-C664-FA4B-A769-D87460BB9387}"/>
-    <hyperlink ref="L181" r:id="rId197" xr:uid="{11E0C06F-BBA9-B446-A3A4-5862C893161B}"/>
-    <hyperlink ref="L204" r:id="rId198" xr:uid="{D5E45024-1B58-714D-9576-1FA969BDADD9}"/>
-    <hyperlink ref="L186" r:id="rId199" xr:uid="{D160676D-AC82-D243-B9A9-56033B0A6EFE}"/>
-    <hyperlink ref="L202" r:id="rId200" xr:uid="{3DB54A74-68B7-734A-BC3C-BFE4E2E4103E}"/>
-    <hyperlink ref="L103" r:id="rId201" xr:uid="{4686296B-C235-4048-A384-BE461895E2AC}"/>
-    <hyperlink ref="L105" r:id="rId202" location="page=2&amp;query=gold%20badge%20sprite&amp;position=49&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{061AB839-ADB1-BA47-A152-68CDFE8A1979}"/>
-    <hyperlink ref="L106" r:id="rId203" location="page=4&amp;query=gold%20badge%20sprite&amp;position=9&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{138577BB-7F7D-D64A-806E-567F3970D250}"/>
+    <hyperlink ref="L237" r:id="rId128" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
+    <hyperlink ref="L155" r:id="rId129" xr:uid="{6A722A1D-2F7B-4242-8134-716EFF33F7D2}"/>
+    <hyperlink ref="L156" r:id="rId130" xr:uid="{547CD1A8-1967-1C46-95E3-89E39CD045C2}"/>
+    <hyperlink ref="L201" r:id="rId131" xr:uid="{5ACD6BFD-52F0-0940-AA8E-B04F1D397BC7}"/>
+    <hyperlink ref="L233" r:id="rId132" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
+    <hyperlink ref="L199" r:id="rId133" xr:uid="{2030AD8C-28A7-544B-92DC-5CBE411DE1C0}"/>
+    <hyperlink ref="L222" r:id="rId134" xr:uid="{05363CA1-BE60-3F42-B56A-1A92A0EDA166}"/>
+    <hyperlink ref="L191" r:id="rId135" xr:uid="{D4C66DCB-D6B4-EC4F-A922-B87887BE6E4A}"/>
+    <hyperlink ref="L190" r:id="rId136" xr:uid="{A05D9F8A-ED0A-4143-8920-9422DD4E0BDD}"/>
+    <hyperlink ref="L192" r:id="rId137" xr:uid="{83FA4EC1-AB5E-3B43-9476-4CA54526DF8E}"/>
+    <hyperlink ref="L171" r:id="rId138" xr:uid="{21B7C9CB-274E-C246-8989-83D9E0E7B24F}"/>
+    <hyperlink ref="L167" r:id="rId139" xr:uid="{B5B4FA15-B24C-CE46-9594-7ED28656AA43}"/>
+    <hyperlink ref="L168" r:id="rId140" xr:uid="{3AB6BE1F-95C1-A443-B12D-D7A523FAD6C5}"/>
+    <hyperlink ref="L169" r:id="rId141" xr:uid="{347BDCC2-5A0C-B249-8CA8-B72D245480FC}"/>
+    <hyperlink ref="L170" r:id="rId142" xr:uid="{E58DD28D-BD99-DF44-9E5E-B3D05F881C1F}"/>
+    <hyperlink ref="L225" r:id="rId143" xr:uid="{4F668E79-3664-0547-B3D5-B7724A9D574D}"/>
+    <hyperlink ref="L223" r:id="rId144" xr:uid="{8AB5C10C-8B45-1843-96BD-655A4FA04EFD}"/>
+    <hyperlink ref="L174" r:id="rId145" xr:uid="{EAED74E0-13EE-A046-9ADC-AC8BDE30C3E6}"/>
+    <hyperlink ref="L230" r:id="rId146" xr:uid="{3577256C-215B-134E-B541-B7B77272CD8A}"/>
+    <hyperlink ref="L231" r:id="rId147" xr:uid="{98E325FC-7F95-B44E-98EB-DE0FF53BC89D}"/>
+    <hyperlink ref="L224" r:id="rId148" xr:uid="{5CE3083F-F217-3743-B613-A7DDF354E72D}"/>
+    <hyperlink ref="L226" r:id="rId149" xr:uid="{B81B6B41-2C17-AA48-B730-D906488BA0A0}"/>
+    <hyperlink ref="L180" r:id="rId150" xr:uid="{BA0813A2-2582-7A46-A492-16A943824EE5}"/>
+    <hyperlink ref="L232" r:id="rId151" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
+    <hyperlink ref="L227" r:id="rId152" xr:uid="{C5265333-F7F0-1845-98D7-68E930F9DFAE}"/>
+    <hyperlink ref="L182" r:id="rId153" xr:uid="{C0A159CB-3986-1A46-95AD-DCEFF4247697}"/>
+    <hyperlink ref="L172" r:id="rId154" xr:uid="{37810A74-E45D-1D46-AEF5-C5FE2F414285}"/>
+    <hyperlink ref="L221" r:id="rId155" xr:uid="{D2906064-B1B8-4648-8201-BEFA97591226}"/>
+    <hyperlink ref="L160" r:id="rId156" xr:uid="{1D3CD52E-7AAD-E444-88F4-4BAE6C5B5EB7}"/>
+    <hyperlink ref="L161" r:id="rId157" xr:uid="{E6E6DA47-945D-6145-912F-08B17B7BA6AE}"/>
+    <hyperlink ref="L162" r:id="rId158" xr:uid="{006B1689-D89A-1E4A-BBC5-E9C9583907F7}"/>
+    <hyperlink ref="L163" r:id="rId159" xr:uid="{C3E773B2-D410-AF41-B197-4638485DC8EF}"/>
+    <hyperlink ref="L164" r:id="rId160" xr:uid="{A0E8A8E2-4A93-3D42-AF48-81955241A483}"/>
+    <hyperlink ref="L165" r:id="rId161" xr:uid="{1B03F18A-8745-AA4F-AA8B-88D65D3B24BC}"/>
+    <hyperlink ref="L238" r:id="rId162" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
+    <hyperlink ref="L239" r:id="rId163" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
+    <hyperlink ref="L188" r:id="rId164" xr:uid="{D6B77117-A0D5-9240-8193-0102C36CCE4C}"/>
+    <hyperlink ref="L189" r:id="rId165" xr:uid="{79FB1103-88A8-8044-9E2C-4FAEC0906E8E}"/>
+    <hyperlink ref="L228" r:id="rId166" xr:uid="{5BF1C4C9-E63A-4F42-9042-36520975FDFA}"/>
+    <hyperlink ref="L187" r:id="rId167" xr:uid="{21CDF460-9871-0547-AA6B-20304C8DD21D}"/>
+    <hyperlink ref="L177" r:id="rId168" xr:uid="{BA1EC844-435A-6C44-87FC-C12B7ECFC55B}"/>
+    <hyperlink ref="L176" r:id="rId169" xr:uid="{46D875DC-CDDD-7E4B-88DB-DFC416CF17AB}"/>
+    <hyperlink ref="L166" r:id="rId170" xr:uid="{7D2FF6AE-1C67-9D4A-A760-7E3745DD9EA6}"/>
+    <hyperlink ref="L214" r:id="rId171" xr:uid="{B5E5E388-8F37-414E-A0C6-1DC58E77628C}"/>
+    <hyperlink ref="L216" r:id="rId172" xr:uid="{A96B1ACF-D982-9240-BB1C-69459154AE5A}"/>
+    <hyperlink ref="L183" r:id="rId173" xr:uid="{D3BB695A-CBA9-D649-B49D-4CC8D16EFD9B}"/>
+    <hyperlink ref="L184" r:id="rId174" xr:uid="{A2922BA8-758D-3149-892C-B7B65B435332}"/>
+    <hyperlink ref="L203" r:id="rId175" xr:uid="{BDB09119-6289-4346-BC29-7A54BD393127}"/>
+    <hyperlink ref="L229" r:id="rId176" xr:uid="{5736CAF4-3646-3243-9AEB-4D82B6D0D10A}"/>
+    <hyperlink ref="L206" r:id="rId177" xr:uid="{60659D55-801C-9A4E-84CA-809884CCBE5C}"/>
+    <hyperlink ref="L196" r:id="rId178" xr:uid="{18DDC006-0939-794C-9B5D-10593F8C0973}"/>
+    <hyperlink ref="L185" r:id="rId179" xr:uid="{50EA46A5-11DD-0345-ABCA-4206D73C7606}"/>
+    <hyperlink ref="L220" r:id="rId180" xr:uid="{63DDFF3B-E62C-9445-96AD-4BB37ACCD20E}"/>
+    <hyperlink ref="L208" r:id="rId181" xr:uid="{05E34BC1-B22F-3E46-8574-E72267507402}"/>
+    <hyperlink ref="L207" r:id="rId182" xr:uid="{7125DF67-5A7E-D948-8363-A31AB1EBA44A}"/>
+    <hyperlink ref="L234" r:id="rId183" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
+    <hyperlink ref="L197" r:id="rId184" xr:uid="{CCE2D666-E296-D94C-ACE0-791CC746483B}"/>
+    <hyperlink ref="L178" r:id="rId185" xr:uid="{E5A2F3EE-A3B1-0842-9364-E4B6EACA9544}"/>
+    <hyperlink ref="L209" r:id="rId186" xr:uid="{E08C8BA4-5414-1947-9CA8-45FE0B846CD1}"/>
+    <hyperlink ref="L205" r:id="rId187" xr:uid="{F1A64091-5BF7-8243-B7A0-F4C13B8B0ABB}"/>
+    <hyperlink ref="L194" r:id="rId188" xr:uid="{745AEF03-3150-C54B-800A-696460474256}"/>
+    <hyperlink ref="L195" r:id="rId189" xr:uid="{9C078FBA-3B11-8049-9187-5BC86D78EA09}"/>
+    <hyperlink ref="L179" r:id="rId190" xr:uid="{BF9A6A48-C664-FA4B-A769-D87460BB9387}"/>
+    <hyperlink ref="L181" r:id="rId191" xr:uid="{11E0C06F-BBA9-B446-A3A4-5862C893161B}"/>
+    <hyperlink ref="L204" r:id="rId192" xr:uid="{D5E45024-1B58-714D-9576-1FA969BDADD9}"/>
+    <hyperlink ref="L186" r:id="rId193" xr:uid="{D160676D-AC82-D243-B9A9-56033B0A6EFE}"/>
+    <hyperlink ref="L202" r:id="rId194" xr:uid="{3DB54A74-68B7-734A-BC3C-BFE4E2E4103E}"/>
+    <hyperlink ref="L103" r:id="rId195" xr:uid="{4686296B-C235-4048-A384-BE461895E2AC}"/>
+    <hyperlink ref="L105" r:id="rId196" location="page=2&amp;query=gold%20badge%20sprite&amp;position=49&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{061AB839-ADB1-BA47-A152-68CDFE8A1979}"/>
+    <hyperlink ref="L106" r:id="rId197" location="page=4&amp;query=gold%20badge%20sprite&amp;position=9&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{138577BB-7F7D-D64A-806E-567F3970D250}"/>
+    <hyperlink ref="L175" r:id="rId198" xr:uid="{927B8B79-A428-2043-9B3B-555F7877CA20}"/>
+    <hyperlink ref="L193" r:id="rId199" xr:uid="{6018233D-1425-7148-A608-3B0666055EA2}"/>
+    <hyperlink ref="L215" r:id="rId200" xr:uid="{38C9843F-1665-8F46-A66C-287455700886}"/>
+    <hyperlink ref="L235" r:id="rId201" xr:uid="{9E664F43-2A79-3744-BC57-4D11914A4B9C}"/>
+    <hyperlink ref="L236" r:id="rId202" xr:uid="{F55C22EB-ADA4-064F-8C9F-34B8DFB927E8}"/>
+    <hyperlink ref="L159" r:id="rId203" xr:uid="{A1B2F4EC-ACE1-B14D-8619-0451D719CFC0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
AssetsCatalog: update audio ChatEngine: add pause, startNewChat and endChat in ChatItem struct, to pass along to sendChat(). Can now start or end a chat mid chat, and add a pause before the start of the chat. Adds drama for LV 157. Also worked on LV157 dialogue. It's much richer! Move 150 post party dialogue to 100. Add heartbeat sound effect. GameboardSprite: change magicdoomloop to magicheartbeat. It's creepier...
</commit_message>
<xml_diff>
--- a/JSON/AssetsCatalog.xlsx
+++ b/JSON/AssetsCatalog.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E075036B-ECEB-1C4D-A5FD-4BC6DDF577C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77466430-B818-1246-82CE-732D0CDDFA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36020" yWindow="-2400" windowWidth="51200" windowHeight="24180" xr2:uid="{E84333C6-E3B6-FB42-AB04-827399F33810}"/>
+    <workbookView xWindow="38760" yWindow="1360" windowWidth="36000" windowHeight="20900" xr2:uid="{E84333C6-E3B6-FB42-AB04-827399F33810}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$239</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$246</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="588">
   <si>
     <t>Filename</t>
   </si>
@@ -1767,6 +1767,42 @@
   </si>
   <si>
     <t>https://audiojungle.net/item/sword-slash-6/19673652</t>
+  </si>
+  <si>
+    <t>movesnow1</t>
+  </si>
+  <si>
+    <t>movesnow3</t>
+  </si>
+  <si>
+    <t>movesnow2</t>
+  </si>
+  <si>
+    <t>Artyfact_SFX</t>
+  </si>
+  <si>
+    <t>Running on Crunchy Frosty Snow</t>
+  </si>
+  <si>
+    <t>https://audiojungle.net/item/running-on-crunchy-frosty-snow/3860993</t>
+  </si>
+  <si>
+    <t>waterappear</t>
+  </si>
+  <si>
+    <t>waterdrown</t>
+  </si>
+  <si>
+    <t>https://audiojungle.net/item/short-medium-plop-splash/19011833</t>
+  </si>
+  <si>
+    <t>Short Medium Plop Splash</t>
+  </si>
+  <si>
+    <t>https://audiojungle.net/item/ocean-waves-4/50172281</t>
+  </si>
+  <si>
+    <t>Ocean Waves 4</t>
   </si>
 </sst>
 </file>
@@ -1846,7 +1882,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1860,7 +1896,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1880,9 +1915,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1920,7 +1955,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2026,7 +2061,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2168,7 +2203,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2176,13 +2211,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}">
-  <dimension ref="A1:L239"/>
+  <dimension ref="A1:L246"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D155" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D214" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C159" sqref="C159"/>
+      <selection pane="bottomRight" activeCell="I243" sqref="I243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6863,7 +6898,7 @@
       <c r="I155" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="K155" s="12" t="s">
+      <c r="K155" s="3" t="s">
         <v>407</v>
       </c>
       <c r="L155" s="7" t="s">
@@ -6895,7 +6930,7 @@
       <c r="I156" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="K156" s="12" t="s">
+      <c r="K156" s="3" t="s">
         <v>407</v>
       </c>
       <c r="L156" s="7" t="s">
@@ -6948,7 +6983,7 @@
       <c r="I158" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="K158" s="12" t="s">
+      <c r="K158" s="3" t="s">
         <v>393</v>
       </c>
       <c r="L158" s="6" t="s">
@@ -6968,7 +7003,7 @@
       <c r="D159" t="s">
         <v>388</v>
       </c>
-      <c r="F159" s="12">
+      <c r="F159" s="3">
         <v>1</v>
       </c>
       <c r="G159" s="3" t="s">
@@ -6980,7 +7015,7 @@
       <c r="I159" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="K159" s="12" t="s">
+      <c r="K159" s="3" t="s">
         <v>567</v>
       </c>
       <c r="L159" s="7" t="s">
@@ -7012,7 +7047,7 @@
       <c r="I160" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="K160" s="12" t="s">
+      <c r="K160" s="3" t="s">
         <v>465</v>
       </c>
       <c r="L160" s="6" t="s">
@@ -7044,7 +7079,7 @@
       <c r="I161" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="K161" s="12" t="s">
+      <c r="K161" s="3" t="s">
         <v>465</v>
       </c>
       <c r="L161" s="6" t="s">
@@ -7076,7 +7111,7 @@
       <c r="I162" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="K162" s="12" t="s">
+      <c r="K162" s="3" t="s">
         <v>465</v>
       </c>
       <c r="L162" s="6" t="s">
@@ -7108,7 +7143,7 @@
       <c r="I163" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="K163" s="12" t="s">
+      <c r="K163" s="3" t="s">
         <v>465</v>
       </c>
       <c r="L163" s="6" t="s">
@@ -7140,7 +7175,7 @@
       <c r="I164" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="K164" s="12" t="s">
+      <c r="K164" s="3" t="s">
         <v>465</v>
       </c>
       <c r="L164" s="6" t="s">
@@ -7172,7 +7207,7 @@
       <c r="I165" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="K165" s="12" t="s">
+      <c r="K165" s="3" t="s">
         <v>465</v>
       </c>
       <c r="L165" s="6" t="s">
@@ -7204,7 +7239,7 @@
       <c r="I166" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="K166" s="12" t="s">
+      <c r="K166" s="3" t="s">
         <v>486</v>
       </c>
       <c r="L166" s="6" t="s">
@@ -7236,7 +7271,7 @@
       <c r="I167" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="K167" s="12" t="s">
+      <c r="K167" s="3" t="s">
         <v>428</v>
       </c>
       <c r="L167" s="6" t="s">
@@ -7268,7 +7303,7 @@
       <c r="I168" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="K168" s="12" t="s">
+      <c r="K168" s="3" t="s">
         <v>428</v>
       </c>
       <c r="L168" s="6" t="s">
@@ -7300,7 +7335,7 @@
       <c r="I169" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="K169" s="12" t="s">
+      <c r="K169" s="3" t="s">
         <v>428</v>
       </c>
       <c r="L169" s="6" t="s">
@@ -7332,7 +7367,7 @@
       <c r="I170" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="K170" s="12" t="s">
+      <c r="K170" s="3" t="s">
         <v>428</v>
       </c>
       <c r="L170" s="6" t="s">
@@ -7364,7 +7399,7 @@
       <c r="I171" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="K171" s="12" t="s">
+      <c r="K171" s="3" t="s">
         <v>428</v>
       </c>
       <c r="L171" s="6" t="s">
@@ -7396,7 +7431,7 @@
       <c r="I172" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="K172" s="12" t="s">
+      <c r="K172" s="3" t="s">
         <v>459</v>
       </c>
       <c r="L172" s="6" t="s">
@@ -7449,7 +7484,7 @@
       <c r="I174" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="K174" s="12" t="s">
+      <c r="K174" s="3" t="s">
         <v>437</v>
       </c>
       <c r="L174" s="6" t="s">
@@ -7469,7 +7504,7 @@
       <c r="D175" t="s">
         <v>388</v>
       </c>
-      <c r="F175" s="12">
+      <c r="F175" s="3">
         <v>1</v>
       </c>
       <c r="G175" s="3" t="s">
@@ -7481,7 +7516,7 @@
       <c r="I175" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="K175" s="12" t="s">
+      <c r="K175" s="3" t="s">
         <v>563</v>
       </c>
       <c r="L175" s="7" t="s">
@@ -7513,7 +7548,7 @@
       <c r="I176" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="K176" s="12" t="s">
+      <c r="K176" s="3" t="s">
         <v>483</v>
       </c>
       <c r="L176" s="6" t="s">
@@ -7545,7 +7580,7 @@
       <c r="I177" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="K177" s="12" t="s">
+      <c r="K177" s="3" t="s">
         <v>481</v>
       </c>
       <c r="L177" s="6" t="s">
@@ -7577,7 +7612,7 @@
       <c r="I178" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="K178" s="12" t="s">
+      <c r="K178" s="3" t="s">
         <v>530</v>
       </c>
       <c r="L178" s="6" t="s">
@@ -7597,7 +7632,7 @@
       <c r="D179" t="s">
         <v>388</v>
       </c>
-      <c r="F179" s="12">
+      <c r="F179" s="3">
         <v>2</v>
       </c>
       <c r="G179" s="3" t="s">
@@ -7609,7 +7644,7 @@
       <c r="I179" s="3" t="s">
         <v>544</v>
       </c>
-      <c r="K179" s="12" t="s">
+      <c r="K179" s="3" t="s">
         <v>543</v>
       </c>
       <c r="L179" s="6" t="s">
@@ -7641,7 +7676,7 @@
       <c r="I180" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="K180" s="12" t="s">
+      <c r="K180" s="3" t="s">
         <v>448</v>
       </c>
       <c r="L180" s="6" t="s">
@@ -7661,7 +7696,7 @@
       <c r="D181" t="s">
         <v>388</v>
       </c>
-      <c r="F181" s="12">
+      <c r="F181" s="3">
         <v>2</v>
       </c>
       <c r="G181" s="3" t="s">
@@ -7673,7 +7708,7 @@
       <c r="I181" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="K181" s="12" t="s">
+      <c r="K181" s="3" t="s">
         <v>546</v>
       </c>
       <c r="L181" s="6" t="s">
@@ -7705,7 +7740,7 @@
       <c r="I182" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="K182" s="12" t="s">
+      <c r="K182" s="3" t="s">
         <v>456</v>
       </c>
       <c r="L182" s="6" t="s">
@@ -7737,7 +7772,7 @@
       <c r="I183" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="K183" s="12" t="s">
+      <c r="K183" s="3" t="s">
         <v>496</v>
       </c>
       <c r="L183" s="6" t="s">
@@ -7769,7 +7804,7 @@
       <c r="I184" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="K184" s="12" t="s">
+      <c r="K184" s="3" t="s">
         <v>497</v>
       </c>
       <c r="L184" s="6" t="s">
@@ -7801,7 +7836,7 @@
       <c r="I185" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="K185" s="12" t="s">
+      <c r="K185" s="3" t="s">
         <v>514</v>
       </c>
       <c r="L185" s="6" t="s">
@@ -7865,7 +7900,7 @@
       <c r="I187" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="K187" s="12" t="s">
+      <c r="K187" s="3" t="s">
         <v>478</v>
       </c>
       <c r="L187" s="6" t="s">
@@ -7897,7 +7932,7 @@
       <c r="I188" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="K188" s="12" t="s">
+      <c r="K188" s="3" t="s">
         <v>473</v>
       </c>
       <c r="L188" s="6" t="s">
@@ -7929,7 +7964,7 @@
       <c r="I189" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="K189" s="12" t="s">
+      <c r="K189" s="3" t="s">
         <v>473</v>
       </c>
       <c r="L189" s="6" t="s">
@@ -7961,7 +7996,7 @@
       <c r="I190" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="K190" s="12" t="s">
+      <c r="K190" s="3" t="s">
         <v>425</v>
       </c>
       <c r="L190" s="6" t="s">
@@ -7993,7 +8028,7 @@
       <c r="I191" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="K191" s="12" t="s">
+      <c r="K191" s="3" t="s">
         <v>421</v>
       </c>
       <c r="L191" s="6" t="s">
@@ -8025,7 +8060,7 @@
       <c r="I192" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="K192" s="12" t="s">
+      <c r="K192" s="3" t="s">
         <v>424</v>
       </c>
       <c r="L192" s="6" t="s">
@@ -8045,7 +8080,7 @@
       <c r="D193" t="s">
         <v>388</v>
       </c>
-      <c r="F193" s="12">
+      <c r="F193" s="3">
         <v>1</v>
       </c>
       <c r="G193" s="3" t="s">
@@ -8057,7 +8092,7 @@
       <c r="I193" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="K193" s="12" t="s">
+      <c r="K193" s="3" t="s">
         <v>569</v>
       </c>
       <c r="L193" s="7" t="s">
@@ -8217,7 +8252,7 @@
       <c r="I198" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="K198" s="12" t="s">
+      <c r="K198" s="3" t="s">
         <v>395</v>
       </c>
       <c r="L198" s="6" t="s">
@@ -8249,7 +8284,7 @@
       <c r="I199" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="K199" s="12" t="s">
+      <c r="K199" s="3" t="s">
         <v>416</v>
       </c>
       <c r="L199" s="6" t="s">
@@ -8281,7 +8316,7 @@
       <c r="I200" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="K200" s="12" t="s">
+      <c r="K200" s="3" t="s">
         <v>398</v>
       </c>
       <c r="L200" s="7" t="s">
@@ -8313,7 +8348,7 @@
       <c r="I201" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="K201" s="12" t="s">
+      <c r="K201" s="3" t="s">
         <v>410</v>
       </c>
       <c r="L201" s="6" t="s">
@@ -8377,7 +8412,7 @@
       <c r="I203" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="K203" s="12" t="s">
+      <c r="K203" s="3" t="s">
         <v>503</v>
       </c>
       <c r="L203" s="6" t="s">
@@ -8409,7 +8444,7 @@
       <c r="I204" s="3" t="s">
         <v>537</v>
       </c>
-      <c r="K204" s="12" t="s">
+      <c r="K204" s="3" t="s">
         <v>536</v>
       </c>
       <c r="L204" s="6" t="s">
@@ -8441,7 +8476,7 @@
       <c r="I205" s="3" t="s">
         <v>537</v>
       </c>
-      <c r="K205" s="12" t="s">
+      <c r="K205" s="3" t="s">
         <v>536</v>
       </c>
       <c r="L205" s="6" t="s">
@@ -8473,7 +8508,7 @@
       <c r="I206" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="K206" s="12" t="s">
+      <c r="K206" s="3" t="s">
         <v>508</v>
       </c>
       <c r="L206" s="6" t="s">
@@ -8493,7 +8528,7 @@
       <c r="D207" t="s">
         <v>388</v>
       </c>
-      <c r="F207" s="12">
+      <c r="F207" s="3">
         <v>3</v>
       </c>
       <c r="G207" s="3" t="s">
@@ -8505,7 +8540,7 @@
       <c r="I207" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="K207" s="12" t="s">
+      <c r="K207" s="3" t="s">
         <v>521</v>
       </c>
       <c r="L207" s="6" t="s">
@@ -8525,7 +8560,7 @@
       <c r="D208" t="s">
         <v>388</v>
       </c>
-      <c r="F208" s="12">
+      <c r="F208" s="3">
         <v>2</v>
       </c>
       <c r="G208" s="3" t="s">
@@ -8537,7 +8572,7 @@
       <c r="I208" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="K208" s="12" t="s">
+      <c r="K208" s="3" t="s">
         <v>518</v>
       </c>
       <c r="L208" s="6" t="s">
@@ -8557,7 +8592,7 @@
       <c r="D209" t="s">
         <v>388</v>
       </c>
-      <c r="F209" s="12">
+      <c r="F209" s="3">
         <v>2</v>
       </c>
       <c r="G209" s="3" t="s">
@@ -8569,7 +8604,7 @@
       <c r="I209" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="K209" s="12" t="s">
+      <c r="K209" s="3" t="s">
         <v>533</v>
       </c>
       <c r="L209" s="6" t="s">
@@ -8601,7 +8636,7 @@
       <c r="I210" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="K210" s="12" t="s">
+      <c r="K210" s="3" t="s">
         <v>500</v>
       </c>
       <c r="L210" s="6" t="s">
@@ -8633,7 +8668,7 @@
       <c r="I211" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="K211" s="12" t="s">
+      <c r="K211" s="3" t="s">
         <v>500</v>
       </c>
       <c r="L211" s="6" t="s">
@@ -8665,7 +8700,7 @@
       <c r="I212" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="K212" s="12" t="s">
+      <c r="K212" s="3" t="s">
         <v>500</v>
       </c>
       <c r="L212" s="6" t="s">
@@ -8697,7 +8732,7 @@
       <c r="I213" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="K213" s="12" t="s">
+      <c r="K213" s="3" t="s">
         <v>500</v>
       </c>
       <c r="L213" s="6" t="s">
@@ -8729,7 +8764,7 @@
       <c r="I214" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="K214" s="12" t="s">
+      <c r="K214" s="3" t="s">
         <v>491</v>
       </c>
       <c r="L214" s="6" t="s">
@@ -8761,7 +8796,7 @@
       <c r="I215" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="K215" s="12" t="s">
+      <c r="K215" s="3" t="s">
         <v>491</v>
       </c>
       <c r="L215" s="6" t="s">
@@ -8807,29 +8842,29 @@
       <c r="B217" t="s">
         <v>405</v>
       </c>
-      <c r="C217" t="s">
-        <v>366</v>
+      <c r="C217" s="9" t="s">
+        <v>576</v>
       </c>
       <c r="D217" t="s">
         <v>388</v>
       </c>
-      <c r="F217" s="3">
-        <v>3</v>
+      <c r="F217" s="12">
+        <v>1</v>
       </c>
       <c r="G217" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H217" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I217" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="K217" s="12" t="s">
-        <v>489</v>
+        <v>579</v>
+      </c>
+      <c r="K217" s="3" t="s">
+        <v>580</v>
       </c>
       <c r="L217" s="6" t="s">
-        <v>488</v>
+        <v>581</v>
       </c>
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.2">
@@ -8839,29 +8874,29 @@
       <c r="B218" t="s">
         <v>405</v>
       </c>
-      <c r="C218" t="s">
-        <v>367</v>
+      <c r="C218" s="9" t="s">
+        <v>578</v>
       </c>
       <c r="D218" t="s">
         <v>388</v>
       </c>
-      <c r="F218" s="3">
+      <c r="F218" s="12">
         <v>0</v>
       </c>
       <c r="G218" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H218" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I218" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="K218" s="12" t="s">
-        <v>489</v>
+        <v>579</v>
+      </c>
+      <c r="K218" s="3" t="s">
+        <v>580</v>
       </c>
       <c r="L218" s="6" t="s">
-        <v>488</v>
+        <v>581</v>
       </c>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.2">
@@ -8871,29 +8906,29 @@
       <c r="B219" t="s">
         <v>405</v>
       </c>
-      <c r="C219" t="s">
-        <v>368</v>
+      <c r="C219" s="9" t="s">
+        <v>577</v>
       </c>
       <c r="D219" t="s">
         <v>388</v>
       </c>
-      <c r="F219" s="3">
+      <c r="F219" s="12">
         <v>0</v>
       </c>
       <c r="G219" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H219" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I219" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="K219" s="12" t="s">
-        <v>489</v>
+        <v>579</v>
+      </c>
+      <c r="K219" s="3" t="s">
+        <v>580</v>
       </c>
       <c r="L219" s="6" t="s">
-        <v>488</v>
+        <v>581</v>
       </c>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.2">
@@ -8904,45 +8939,45 @@
         <v>405</v>
       </c>
       <c r="C220" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D220" t="s">
         <v>388</v>
       </c>
-      <c r="F220" s="11">
+      <c r="F220" s="3">
         <v>3</v>
       </c>
       <c r="G220" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H220" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="K220" s="12" t="s">
-        <v>516</v>
+        <v>487</v>
+      </c>
+      <c r="K220" s="3" t="s">
+        <v>489</v>
       </c>
       <c r="L220" s="6" t="s">
-        <v>515</v>
+        <v>488</v>
       </c>
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B221" t="s">
         <v>405</v>
       </c>
       <c r="C221" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D221" t="s">
         <v>388</v>
       </c>
       <c r="F221" s="3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G221" s="3" t="s">
         <v>174</v>
@@ -8951,30 +8986,30 @@
         <v>391</v>
       </c>
       <c r="I221" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="K221" s="12" t="s">
-        <v>462</v>
+        <v>487</v>
+      </c>
+      <c r="K221" s="3" t="s">
+        <v>489</v>
       </c>
       <c r="L221" s="6" t="s">
-        <v>461</v>
+        <v>488</v>
       </c>
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B222" t="s">
         <v>405</v>
       </c>
       <c r="C222" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D222" t="s">
         <v>388</v>
       </c>
       <c r="F222" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G222" s="3" t="s">
         <v>174</v>
@@ -8983,62 +9018,62 @@
         <v>391</v>
       </c>
       <c r="I222" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="K222" s="12" t="s">
-        <v>418</v>
+        <v>487</v>
+      </c>
+      <c r="K222" s="3" t="s">
+        <v>489</v>
       </c>
       <c r="L222" s="6" t="s">
-        <v>417</v>
+        <v>488</v>
       </c>
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B223" t="s">
         <v>405</v>
       </c>
       <c r="C223" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D223" t="s">
         <v>388</v>
       </c>
-      <c r="F223" s="3">
-        <v>18</v>
+      <c r="F223" s="11">
+        <v>3</v>
       </c>
       <c r="G223" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H223" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="K223" s="12" t="s">
-        <v>434</v>
+        <v>396</v>
+      </c>
+      <c r="K223" s="3" t="s">
+        <v>516</v>
       </c>
       <c r="L223" s="6" t="s">
-        <v>433</v>
+        <v>515</v>
       </c>
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B224" t="s">
         <v>405</v>
       </c>
       <c r="C224" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D224" t="s">
         <v>388</v>
       </c>
       <c r="F224" s="3">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G224" s="3" t="s">
         <v>174</v>
@@ -9047,30 +9082,30 @@
         <v>391</v>
       </c>
       <c r="I224" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="K224" s="12" t="s">
-        <v>445</v>
+        <v>463</v>
+      </c>
+      <c r="K224" s="3" t="s">
+        <v>462</v>
       </c>
       <c r="L224" s="6" t="s">
-        <v>444</v>
+        <v>461</v>
       </c>
     </row>
     <row r="225" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B225" t="s">
         <v>405</v>
       </c>
       <c r="C225" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D225" t="s">
         <v>388</v>
       </c>
       <c r="F225" s="3">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G225" s="3" t="s">
         <v>174</v>
@@ -9079,30 +9114,30 @@
         <v>391</v>
       </c>
       <c r="I225" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="K225" s="12" t="s">
-        <v>431</v>
+        <v>419</v>
+      </c>
+      <c r="K225" s="3" t="s">
+        <v>418</v>
       </c>
       <c r="L225" s="6" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B226" t="s">
         <v>405</v>
       </c>
       <c r="C226" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D226" t="s">
         <v>388</v>
       </c>
       <c r="F226" s="3">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G226" s="3" t="s">
         <v>174</v>
@@ -9111,13 +9146,13 @@
         <v>391</v>
       </c>
       <c r="I226" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="K226" s="12" t="s">
-        <v>445</v>
+        <v>435</v>
+      </c>
+      <c r="K226" s="3" t="s">
+        <v>434</v>
       </c>
       <c r="L226" s="6" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.2">
@@ -9128,13 +9163,13 @@
         <v>405</v>
       </c>
       <c r="C227" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D227" t="s">
         <v>388</v>
       </c>
       <c r="F227" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G227" s="3" t="s">
         <v>174</v>
@@ -9143,13 +9178,13 @@
         <v>391</v>
       </c>
       <c r="I227" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="K227" s="12" t="s">
-        <v>453</v>
+        <v>446</v>
+      </c>
+      <c r="K227" s="3" t="s">
+        <v>445</v>
       </c>
       <c r="L227" s="6" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.2">
@@ -9160,13 +9195,13 @@
         <v>405</v>
       </c>
       <c r="C228" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D228" t="s">
         <v>388</v>
       </c>
       <c r="F228" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G228" s="3" t="s">
         <v>174</v>
@@ -9177,11 +9212,11 @@
       <c r="I228" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="K228" s="12" t="s">
-        <v>476</v>
+      <c r="K228" s="3" t="s">
+        <v>431</v>
       </c>
       <c r="L228" s="6" t="s">
-        <v>475</v>
+        <v>430</v>
       </c>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.2">
@@ -9192,13 +9227,13 @@
         <v>405</v>
       </c>
       <c r="C229" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D229" t="s">
         <v>388</v>
       </c>
       <c r="F229" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G229" s="3" t="s">
         <v>174</v>
@@ -9207,13 +9242,13 @@
         <v>391</v>
       </c>
       <c r="I229" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="K229" s="12" t="s">
-        <v>505</v>
+        <v>446</v>
+      </c>
+      <c r="K229" s="3" t="s">
+        <v>445</v>
       </c>
       <c r="L229" s="6" t="s">
-        <v>504</v>
+        <v>444</v>
       </c>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.2">
@@ -9224,13 +9259,13 @@
         <v>405</v>
       </c>
       <c r="C230" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D230" t="s">
         <v>388</v>
       </c>
       <c r="F230" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G230" s="3" t="s">
         <v>174</v>
@@ -9239,13 +9274,13 @@
         <v>391</v>
       </c>
       <c r="I230" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="K230" s="12" t="s">
-        <v>440</v>
+        <v>454</v>
+      </c>
+      <c r="K230" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="L230" s="6" t="s">
-        <v>439</v>
+        <v>452</v>
       </c>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.2">
@@ -9256,13 +9291,13 @@
         <v>405</v>
       </c>
       <c r="C231" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D231" t="s">
         <v>388</v>
       </c>
       <c r="F231" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G231" s="3" t="s">
         <v>174</v>
@@ -9271,13 +9306,13 @@
         <v>391</v>
       </c>
       <c r="I231" s="3" t="s">
-        <v>443</v>
-      </c>
-      <c r="K231" s="12" t="s">
-        <v>440</v>
+        <v>411</v>
+      </c>
+      <c r="K231" s="3" t="s">
+        <v>476</v>
       </c>
       <c r="L231" s="6" t="s">
-        <v>442</v>
+        <v>475</v>
       </c>
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.2">
@@ -9288,7 +9323,7 @@
         <v>405</v>
       </c>
       <c r="C232" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D232" t="s">
         <v>388</v>
@@ -9303,30 +9338,30 @@
         <v>391</v>
       </c>
       <c r="I232" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="K232" s="12" t="s">
-        <v>451</v>
+        <v>506</v>
+      </c>
+      <c r="K232" s="3" t="s">
+        <v>505</v>
       </c>
       <c r="L232" s="6" t="s">
-        <v>450</v>
+        <v>504</v>
       </c>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B233" t="s">
         <v>405</v>
       </c>
       <c r="C233" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D233" t="s">
         <v>388</v>
       </c>
       <c r="F233" s="3">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="G233" s="3" t="s">
         <v>174</v>
@@ -9335,13 +9370,13 @@
         <v>391</v>
       </c>
       <c r="I233" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="K233" s="12" t="s">
-        <v>413</v>
+        <v>441</v>
+      </c>
+      <c r="K233" s="3" t="s">
+        <v>440</v>
       </c>
       <c r="L233" s="6" t="s">
-        <v>412</v>
+        <v>439</v>
       </c>
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.2">
@@ -9352,28 +9387,28 @@
         <v>405</v>
       </c>
       <c r="C234" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D234" t="s">
         <v>388</v>
       </c>
-      <c r="F234" s="11">
-        <v>2</v>
+      <c r="F234" s="3">
+        <v>4</v>
       </c>
       <c r="G234" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H234" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I234" s="3" t="s">
-        <v>525</v>
+        <v>443</v>
       </c>
       <c r="K234" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="L234" s="10" t="s">
-        <v>523</v>
+        <v>440</v>
+      </c>
+      <c r="L234" s="6" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.2">
@@ -9384,7 +9419,7 @@
         <v>405</v>
       </c>
       <c r="C235" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D235" t="s">
         <v>388</v>
@@ -9398,32 +9433,31 @@
       <c r="H235" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I235" t="s">
-        <v>573</v>
-      </c>
-      <c r="J235"/>
-      <c r="K235" s="13" t="s">
-        <v>574</v>
+      <c r="I235" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="K235" s="3" t="s">
+        <v>451</v>
       </c>
       <c r="L235" s="6" t="s">
-        <v>575</v>
+        <v>450</v>
       </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B236" t="s">
         <v>405</v>
       </c>
       <c r="C236" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D236" t="s">
         <v>388</v>
       </c>
       <c r="F236" s="3">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="G236" s="3" t="s">
         <v>174</v>
@@ -9431,47 +9465,46 @@
       <c r="H236" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I236" t="s">
-        <v>570</v>
-      </c>
-      <c r="J236"/>
-      <c r="K236" s="13" t="s">
-        <v>571</v>
+      <c r="I236" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="K236" s="3" t="s">
+        <v>413</v>
       </c>
       <c r="L236" s="6" t="s">
-        <v>572</v>
+        <v>412</v>
       </c>
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B237" t="s">
         <v>405</v>
       </c>
       <c r="C237" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D237" t="s">
         <v>388</v>
       </c>
-      <c r="F237" s="3">
-        <v>10</v>
+      <c r="F237" s="11">
+        <v>2</v>
       </c>
       <c r="G237" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H237" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I237" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="K237" s="12" t="s">
-        <v>403</v>
-      </c>
-      <c r="L237" s="7" t="s">
-        <v>404</v>
+        <v>525</v>
+      </c>
+      <c r="K237" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="L237" s="10" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.2">
@@ -9482,7 +9515,7 @@
         <v>405</v>
       </c>
       <c r="C238" t="s">
-        <v>58</v>
+        <v>384</v>
       </c>
       <c r="D238" t="s">
         <v>388</v>
@@ -9496,14 +9529,15 @@
       <c r="H238" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I238" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="K238" s="12" t="s">
-        <v>467</v>
+      <c r="I238" t="s">
+        <v>573</v>
+      </c>
+      <c r="J238"/>
+      <c r="K238" t="s">
+        <v>574</v>
       </c>
       <c r="L238" s="6" t="s">
-        <v>466</v>
+        <v>575</v>
       </c>
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.2">
@@ -9514,7 +9548,7 @@
         <v>405</v>
       </c>
       <c r="C239" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D239" t="s">
         <v>388</v>
@@ -9528,18 +9562,243 @@
       <c r="H239" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I239" s="3" t="s">
+      <c r="I239" t="s">
+        <v>570</v>
+      </c>
+      <c r="J239"/>
+      <c r="K239" t="s">
+        <v>571</v>
+      </c>
+      <c r="L239" s="6" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>401</v>
+      </c>
+      <c r="B240" t="s">
+        <v>405</v>
+      </c>
+      <c r="C240" t="s">
+        <v>386</v>
+      </c>
+      <c r="D240" t="s">
+        <v>388</v>
+      </c>
+      <c r="F240" s="3">
+        <v>10</v>
+      </c>
+      <c r="G240" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H240" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I240" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="K240" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="L240" s="7" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>389</v>
+      </c>
+      <c r="B241" t="s">
+        <v>405</v>
+      </c>
+      <c r="C241" t="s">
+        <v>58</v>
+      </c>
+      <c r="D241" t="s">
+        <v>388</v>
+      </c>
+      <c r="F241" s="3">
+        <v>1</v>
+      </c>
+      <c r="G241" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H241" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I241" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="K241" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="L241" s="6" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>389</v>
+      </c>
+      <c r="B242" t="s">
+        <v>405</v>
+      </c>
+      <c r="C242" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="D242" t="s">
+        <v>388</v>
+      </c>
+      <c r="F242" s="3">
+        <v>1</v>
+      </c>
+      <c r="G242" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="H242" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I242" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="K242" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="L242" s="6" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>389</v>
+      </c>
+      <c r="B243" t="s">
+        <v>405</v>
+      </c>
+      <c r="C243" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="D243" t="s">
+        <v>388</v>
+      </c>
+      <c r="F243" s="3">
+        <v>0</v>
+      </c>
+      <c r="G243" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="H243" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I243" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="K243" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="L243" s="6" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>389</v>
+      </c>
+      <c r="B244" t="s">
+        <v>405</v>
+      </c>
+      <c r="C244" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="D244" t="s">
+        <v>388</v>
+      </c>
+      <c r="F244" s="3">
+        <v>0</v>
+      </c>
+      <c r="G244" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="H244" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I244" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="K244" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="L244" s="6" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>389</v>
+      </c>
+      <c r="B245" t="s">
+        <v>405</v>
+      </c>
+      <c r="C245" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="D245" t="s">
+        <v>388</v>
+      </c>
+      <c r="F245" s="3">
+        <v>1</v>
+      </c>
+      <c r="G245" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="H245" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I245" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="K245" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="L245" s="6" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>389</v>
+      </c>
+      <c r="B246" t="s">
+        <v>405</v>
+      </c>
+      <c r="C246" t="s">
+        <v>387</v>
+      </c>
+      <c r="D246" t="s">
+        <v>388</v>
+      </c>
+      <c r="F246" s="3">
+        <v>1</v>
+      </c>
+      <c r="G246" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H246" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I246" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="K239" s="12" t="s">
+      <c r="K246" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="L239" s="6" t="s">
+      <c r="L246" s="6" t="s">
         <v>469</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L239" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}"/>
+  <autoFilter ref="A1:L246" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}"/>
   <hyperlinks>
     <hyperlink ref="L3" r:id="rId1" location="query=target&amp;position=0&amp;from_view=search&amp;track=sph&amp;uuid=07a631b0-afe2-4d83-9076-a80360e62f2f" xr:uid="{6340FD26-01F6-9246-82E5-C8936FBB7B36}"/>
     <hyperlink ref="L4" r:id="rId2" location="query=spell%20book&amp;position=12&amp;from_view=keyword&amp;track=ais&amp;uuid=3aa8f740-41d0-409e-b03b-268281a69be6" xr:uid="{1A91BF66-CE85-304F-BBE7-7F8EBE53C285}"/>
@@ -9668,13 +9927,13 @@
     <hyperlink ref="L158" r:id="rId125" xr:uid="{F88953B7-468E-C34B-9347-94009F9A78D2}"/>
     <hyperlink ref="L198" r:id="rId126" xr:uid="{1F3BBC8C-29E8-C74A-AB3F-04AE466222EF}"/>
     <hyperlink ref="L200" r:id="rId127" xr:uid="{3C51058F-793C-D34A-8286-18AE4C8EF6CE}"/>
-    <hyperlink ref="L237" r:id="rId128" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
+    <hyperlink ref="L240" r:id="rId128" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
     <hyperlink ref="L155" r:id="rId129" xr:uid="{6A722A1D-2F7B-4242-8134-716EFF33F7D2}"/>
     <hyperlink ref="L156" r:id="rId130" xr:uid="{547CD1A8-1967-1C46-95E3-89E39CD045C2}"/>
     <hyperlink ref="L201" r:id="rId131" xr:uid="{5ACD6BFD-52F0-0940-AA8E-B04F1D397BC7}"/>
-    <hyperlink ref="L233" r:id="rId132" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
+    <hyperlink ref="L236" r:id="rId132" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
     <hyperlink ref="L199" r:id="rId133" xr:uid="{2030AD8C-28A7-544B-92DC-5CBE411DE1C0}"/>
-    <hyperlink ref="L222" r:id="rId134" xr:uid="{05363CA1-BE60-3F42-B56A-1A92A0EDA166}"/>
+    <hyperlink ref="L225" r:id="rId134" xr:uid="{05363CA1-BE60-3F42-B56A-1A92A0EDA166}"/>
     <hyperlink ref="L191" r:id="rId135" xr:uid="{D4C66DCB-D6B4-EC4F-A922-B87887BE6E4A}"/>
     <hyperlink ref="L190" r:id="rId136" xr:uid="{A05D9F8A-ED0A-4143-8920-9422DD4E0BDD}"/>
     <hyperlink ref="L192" r:id="rId137" xr:uid="{83FA4EC1-AB5E-3B43-9476-4CA54526DF8E}"/>
@@ -9683,30 +9942,30 @@
     <hyperlink ref="L168" r:id="rId140" xr:uid="{3AB6BE1F-95C1-A443-B12D-D7A523FAD6C5}"/>
     <hyperlink ref="L169" r:id="rId141" xr:uid="{347BDCC2-5A0C-B249-8CA8-B72D245480FC}"/>
     <hyperlink ref="L170" r:id="rId142" xr:uid="{E58DD28D-BD99-DF44-9E5E-B3D05F881C1F}"/>
-    <hyperlink ref="L225" r:id="rId143" xr:uid="{4F668E79-3664-0547-B3D5-B7724A9D574D}"/>
-    <hyperlink ref="L223" r:id="rId144" xr:uid="{8AB5C10C-8B45-1843-96BD-655A4FA04EFD}"/>
+    <hyperlink ref="L228" r:id="rId143" xr:uid="{4F668E79-3664-0547-B3D5-B7724A9D574D}"/>
+    <hyperlink ref="L226" r:id="rId144" xr:uid="{8AB5C10C-8B45-1843-96BD-655A4FA04EFD}"/>
     <hyperlink ref="L174" r:id="rId145" xr:uid="{EAED74E0-13EE-A046-9ADC-AC8BDE30C3E6}"/>
-    <hyperlink ref="L230" r:id="rId146" xr:uid="{3577256C-215B-134E-B541-B7B77272CD8A}"/>
-    <hyperlink ref="L231" r:id="rId147" xr:uid="{98E325FC-7F95-B44E-98EB-DE0FF53BC89D}"/>
-    <hyperlink ref="L224" r:id="rId148" xr:uid="{5CE3083F-F217-3743-B613-A7DDF354E72D}"/>
-    <hyperlink ref="L226" r:id="rId149" xr:uid="{B81B6B41-2C17-AA48-B730-D906488BA0A0}"/>
+    <hyperlink ref="L233" r:id="rId146" xr:uid="{3577256C-215B-134E-B541-B7B77272CD8A}"/>
+    <hyperlink ref="L234" r:id="rId147" xr:uid="{98E325FC-7F95-B44E-98EB-DE0FF53BC89D}"/>
+    <hyperlink ref="L227" r:id="rId148" xr:uid="{5CE3083F-F217-3743-B613-A7DDF354E72D}"/>
+    <hyperlink ref="L229" r:id="rId149" xr:uid="{B81B6B41-2C17-AA48-B730-D906488BA0A0}"/>
     <hyperlink ref="L180" r:id="rId150" xr:uid="{BA0813A2-2582-7A46-A492-16A943824EE5}"/>
-    <hyperlink ref="L232" r:id="rId151" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
-    <hyperlink ref="L227" r:id="rId152" xr:uid="{C5265333-F7F0-1845-98D7-68E930F9DFAE}"/>
+    <hyperlink ref="L235" r:id="rId151" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
+    <hyperlink ref="L230" r:id="rId152" xr:uid="{C5265333-F7F0-1845-98D7-68E930F9DFAE}"/>
     <hyperlink ref="L182" r:id="rId153" xr:uid="{C0A159CB-3986-1A46-95AD-DCEFF4247697}"/>
     <hyperlink ref="L172" r:id="rId154" xr:uid="{37810A74-E45D-1D46-AEF5-C5FE2F414285}"/>
-    <hyperlink ref="L221" r:id="rId155" xr:uid="{D2906064-B1B8-4648-8201-BEFA97591226}"/>
+    <hyperlink ref="L224" r:id="rId155" xr:uid="{D2906064-B1B8-4648-8201-BEFA97591226}"/>
     <hyperlink ref="L160" r:id="rId156" xr:uid="{1D3CD52E-7AAD-E444-88F4-4BAE6C5B5EB7}"/>
     <hyperlink ref="L161" r:id="rId157" xr:uid="{E6E6DA47-945D-6145-912F-08B17B7BA6AE}"/>
     <hyperlink ref="L162" r:id="rId158" xr:uid="{006B1689-D89A-1E4A-BBC5-E9C9583907F7}"/>
     <hyperlink ref="L163" r:id="rId159" xr:uid="{C3E773B2-D410-AF41-B197-4638485DC8EF}"/>
     <hyperlink ref="L164" r:id="rId160" xr:uid="{A0E8A8E2-4A93-3D42-AF48-81955241A483}"/>
     <hyperlink ref="L165" r:id="rId161" xr:uid="{1B03F18A-8745-AA4F-AA8B-88D65D3B24BC}"/>
-    <hyperlink ref="L238" r:id="rId162" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
-    <hyperlink ref="L239" r:id="rId163" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
+    <hyperlink ref="L241" r:id="rId162" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
+    <hyperlink ref="L246" r:id="rId163" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
     <hyperlink ref="L188" r:id="rId164" xr:uid="{D6B77117-A0D5-9240-8193-0102C36CCE4C}"/>
     <hyperlink ref="L189" r:id="rId165" xr:uid="{79FB1103-88A8-8044-9E2C-4FAEC0906E8E}"/>
-    <hyperlink ref="L228" r:id="rId166" xr:uid="{5BF1C4C9-E63A-4F42-9042-36520975FDFA}"/>
+    <hyperlink ref="L231" r:id="rId166" xr:uid="{5BF1C4C9-E63A-4F42-9042-36520975FDFA}"/>
     <hyperlink ref="L187" r:id="rId167" xr:uid="{21CDF460-9871-0547-AA6B-20304C8DD21D}"/>
     <hyperlink ref="L177" r:id="rId168" xr:uid="{BA1EC844-435A-6C44-87FC-C12B7ECFC55B}"/>
     <hyperlink ref="L176" r:id="rId169" xr:uid="{46D875DC-CDDD-7E4B-88DB-DFC416CF17AB}"/>
@@ -9716,14 +9975,14 @@
     <hyperlink ref="L183" r:id="rId173" xr:uid="{D3BB695A-CBA9-D649-B49D-4CC8D16EFD9B}"/>
     <hyperlink ref="L184" r:id="rId174" xr:uid="{A2922BA8-758D-3149-892C-B7B65B435332}"/>
     <hyperlink ref="L203" r:id="rId175" xr:uid="{BDB09119-6289-4346-BC29-7A54BD393127}"/>
-    <hyperlink ref="L229" r:id="rId176" xr:uid="{5736CAF4-3646-3243-9AEB-4D82B6D0D10A}"/>
+    <hyperlink ref="L232" r:id="rId176" xr:uid="{5736CAF4-3646-3243-9AEB-4D82B6D0D10A}"/>
     <hyperlink ref="L206" r:id="rId177" xr:uid="{60659D55-801C-9A4E-84CA-809884CCBE5C}"/>
     <hyperlink ref="L196" r:id="rId178" xr:uid="{18DDC006-0939-794C-9B5D-10593F8C0973}"/>
     <hyperlink ref="L185" r:id="rId179" xr:uid="{50EA46A5-11DD-0345-ABCA-4206D73C7606}"/>
-    <hyperlink ref="L220" r:id="rId180" xr:uid="{63DDFF3B-E62C-9445-96AD-4BB37ACCD20E}"/>
+    <hyperlink ref="L223" r:id="rId180" xr:uid="{63DDFF3B-E62C-9445-96AD-4BB37ACCD20E}"/>
     <hyperlink ref="L208" r:id="rId181" xr:uid="{05E34BC1-B22F-3E46-8574-E72267507402}"/>
     <hyperlink ref="L207" r:id="rId182" xr:uid="{7125DF67-5A7E-D948-8363-A31AB1EBA44A}"/>
-    <hyperlink ref="L234" r:id="rId183" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
+    <hyperlink ref="L237" r:id="rId183" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
     <hyperlink ref="L197" r:id="rId184" xr:uid="{CCE2D666-E296-D94C-ACE0-791CC746483B}"/>
     <hyperlink ref="L178" r:id="rId185" xr:uid="{E5A2F3EE-A3B1-0842-9364-E4B6EACA9544}"/>
     <hyperlink ref="L209" r:id="rId186" xr:uid="{E08C8BA4-5414-1947-9CA8-45FE0B846CD1}"/>
@@ -9741,9 +10000,16 @@
     <hyperlink ref="L175" r:id="rId198" xr:uid="{927B8B79-A428-2043-9B3B-555F7877CA20}"/>
     <hyperlink ref="L193" r:id="rId199" xr:uid="{6018233D-1425-7148-A608-3B0666055EA2}"/>
     <hyperlink ref="L215" r:id="rId200" xr:uid="{38C9843F-1665-8F46-A66C-287455700886}"/>
-    <hyperlink ref="L235" r:id="rId201" xr:uid="{9E664F43-2A79-3744-BC57-4D11914A4B9C}"/>
-    <hyperlink ref="L236" r:id="rId202" xr:uid="{F55C22EB-ADA4-064F-8C9F-34B8DFB927E8}"/>
+    <hyperlink ref="L238" r:id="rId201" xr:uid="{9E664F43-2A79-3744-BC57-4D11914A4B9C}"/>
+    <hyperlink ref="L239" r:id="rId202" xr:uid="{F55C22EB-ADA4-064F-8C9F-34B8DFB927E8}"/>
     <hyperlink ref="L159" r:id="rId203" xr:uid="{A1B2F4EC-ACE1-B14D-8619-0451D719CFC0}"/>
+    <hyperlink ref="L217" r:id="rId204" xr:uid="{2BF445F0-7B50-5E48-A8E5-4779F07B83CE}"/>
+    <hyperlink ref="L218" r:id="rId205" xr:uid="{6B23A3F9-85DD-4043-853E-3BF95911A2C6}"/>
+    <hyperlink ref="L219" r:id="rId206" xr:uid="{A975FD98-A3FE-5B40-9F31-D14EAE3777F9}"/>
+    <hyperlink ref="L242" r:id="rId207" xr:uid="{F01C8569-23FB-7F4C-A50B-40979911E1B8}"/>
+    <hyperlink ref="L245" r:id="rId208" xr:uid="{B54ABD16-F1A6-DC45-B36E-0CC72B423F70}"/>
+    <hyperlink ref="L243" r:id="rId209" xr:uid="{EBA532A6-AAFD-E54D-BD41-CC4F5F92AF68}"/>
+    <hyperlink ref="L244" r:id="rId210" xr:uid="{0F422DA4-046E-F246-BC4A-695F255E6851}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
AssetsCatalog: update magicheartbeatloop sounds. ChatEngine: update dialogue. GameboardSprite: update heartbeat loop.
</commit_message>
<xml_diff>
--- a/JSON/AssetsCatalog.xlsx
+++ b/JSON/AssetsCatalog.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77466430-B818-1246-82CE-732D0CDDFA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5223B2-23DF-E64D-B913-801AB7EC25D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38760" yWindow="1360" windowWidth="36000" windowHeight="20900" xr2:uid="{E84333C6-E3B6-FB42-AB04-827399F33810}"/>
+    <workbookView xWindow="42040" yWindow="1620" windowWidth="36000" windowHeight="21040" xr2:uid="{E84333C6-E3B6-FB42-AB04-827399F33810}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$246</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$248</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2112" uniqueCount="595">
   <si>
     <t>Filename</t>
   </si>
@@ -1803,6 +1803,27 @@
   </si>
   <si>
     <t>Ocean Waves 4</t>
+  </si>
+  <si>
+    <t>The Heartbeat</t>
+  </si>
+  <si>
+    <t>https://audiojungle.net/item/the-heartbeat/49001977</t>
+  </si>
+  <si>
+    <t>magicheartbeatloop1</t>
+  </si>
+  <si>
+    <t>magicheartbeatloop2</t>
+  </si>
+  <si>
+    <t>https://audiojungle.net/item/heart/19314147</t>
+  </si>
+  <si>
+    <t>Heart</t>
+  </si>
+  <si>
+    <t>AlexM76</t>
   </si>
 </sst>
 </file>
@@ -1837,7 +1858,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1868,6 +1889,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1882,7 +1909,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1896,6 +1923,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2211,13 +2239,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}">
-  <dimension ref="A1:L246"/>
+  <dimension ref="A1:L248"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D214" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D180" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I243" sqref="I243"/>
+      <selection pane="bottomRight" activeCell="L201" sqref="L201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8330,8 +8358,8 @@
       <c r="B201" t="s">
         <v>405</v>
       </c>
-      <c r="C201" t="s">
-        <v>350</v>
+      <c r="C201" s="13" t="s">
+        <v>590</v>
       </c>
       <c r="D201" t="s">
         <v>388</v>
@@ -8339,20 +8367,20 @@
       <c r="F201" s="3">
         <v>1</v>
       </c>
-      <c r="G201" s="3" t="s">
-        <v>174</v>
+      <c r="G201" s="12" t="s">
+        <v>432</v>
       </c>
       <c r="H201" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I201" s="3" t="s">
-        <v>411</v>
+        <v>392</v>
       </c>
       <c r="K201" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="L201" s="6" t="s">
-        <v>409</v>
+        <v>588</v>
+      </c>
+      <c r="L201" s="7" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.2">
@@ -8362,29 +8390,29 @@
       <c r="B202" t="s">
         <v>405</v>
       </c>
-      <c r="C202" t="s">
-        <v>351</v>
+      <c r="C202" s="13" t="s">
+        <v>591</v>
       </c>
       <c r="D202" t="s">
         <v>388</v>
       </c>
-      <c r="F202" s="11">
-        <v>2</v>
-      </c>
-      <c r="G202" s="3" t="s">
+      <c r="F202" s="3">
+        <v>1</v>
+      </c>
+      <c r="G202" s="12" t="s">
         <v>432</v>
       </c>
       <c r="H202" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I202" s="3" t="s">
-        <v>552</v>
+        <v>594</v>
       </c>
       <c r="K202" s="3" t="s">
-        <v>551</v>
-      </c>
-      <c r="L202" s="6" t="s">
-        <v>550</v>
+        <v>593</v>
+      </c>
+      <c r="L202" s="7" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="203" spans="1:12" x14ac:dyDescent="0.2">
@@ -8395,13 +8423,13 @@
         <v>405</v>
       </c>
       <c r="C203" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D203" t="s">
         <v>388</v>
       </c>
       <c r="F203" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G203" s="3" t="s">
         <v>174</v>
@@ -8410,13 +8438,13 @@
         <v>391</v>
       </c>
       <c r="I203" s="3" t="s">
-        <v>501</v>
+        <v>411</v>
       </c>
       <c r="K203" s="3" t="s">
-        <v>503</v>
+        <v>410</v>
       </c>
       <c r="L203" s="6" t="s">
-        <v>502</v>
+        <v>409</v>
       </c>
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.2">
@@ -8427,28 +8455,28 @@
         <v>405</v>
       </c>
       <c r="C204" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D204" t="s">
         <v>388</v>
       </c>
-      <c r="F204" s="3">
+      <c r="F204" s="11">
         <v>2</v>
       </c>
       <c r="G204" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H204" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I204" s="3" t="s">
-        <v>537</v>
+        <v>552</v>
       </c>
       <c r="K204" s="3" t="s">
-        <v>536</v>
+        <v>551</v>
       </c>
       <c r="L204" s="6" t="s">
-        <v>535</v>
+        <v>550</v>
       </c>
     </row>
     <row r="205" spans="1:12" x14ac:dyDescent="0.2">
@@ -8459,13 +8487,13 @@
         <v>405</v>
       </c>
       <c r="C205" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D205" t="s">
         <v>388</v>
       </c>
       <c r="F205" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G205" s="3" t="s">
         <v>174</v>
@@ -8474,13 +8502,13 @@
         <v>391</v>
       </c>
       <c r="I205" s="3" t="s">
-        <v>537</v>
+        <v>501</v>
       </c>
       <c r="K205" s="3" t="s">
-        <v>536</v>
+        <v>503</v>
       </c>
       <c r="L205" s="6" t="s">
-        <v>535</v>
+        <v>502</v>
       </c>
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.2">
@@ -8491,13 +8519,13 @@
         <v>405</v>
       </c>
       <c r="C206" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D206" t="s">
         <v>388</v>
       </c>
       <c r="F206" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G206" s="3" t="s">
         <v>174</v>
@@ -8506,13 +8534,13 @@
         <v>391</v>
       </c>
       <c r="I206" s="3" t="s">
-        <v>509</v>
+        <v>537</v>
       </c>
       <c r="K206" s="3" t="s">
-        <v>508</v>
+        <v>536</v>
       </c>
       <c r="L206" s="6" t="s">
-        <v>507</v>
+        <v>535</v>
       </c>
     </row>
     <row r="207" spans="1:12" x14ac:dyDescent="0.2">
@@ -8523,13 +8551,13 @@
         <v>405</v>
       </c>
       <c r="C207" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D207" t="s">
         <v>388</v>
       </c>
       <c r="F207" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G207" s="3" t="s">
         <v>174</v>
@@ -8538,13 +8566,13 @@
         <v>391</v>
       </c>
       <c r="I207" s="3" t="s">
-        <v>522</v>
+        <v>537</v>
       </c>
       <c r="K207" s="3" t="s">
-        <v>521</v>
+        <v>536</v>
       </c>
       <c r="L207" s="6" t="s">
-        <v>520</v>
+        <v>535</v>
       </c>
     </row>
     <row r="208" spans="1:12" x14ac:dyDescent="0.2">
@@ -8555,13 +8583,13 @@
         <v>405</v>
       </c>
       <c r="C208" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D208" t="s">
         <v>388</v>
       </c>
       <c r="F208" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G208" s="3" t="s">
         <v>174</v>
@@ -8570,13 +8598,13 @@
         <v>391</v>
       </c>
       <c r="I208" s="3" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="K208" s="3" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="L208" s="6" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.2">
@@ -8587,13 +8615,13 @@
         <v>405</v>
       </c>
       <c r="C209" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D209" t="s">
         <v>388</v>
       </c>
       <c r="F209" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G209" s="3" t="s">
         <v>174</v>
@@ -8602,13 +8630,13 @@
         <v>391</v>
       </c>
       <c r="I209" s="3" t="s">
-        <v>534</v>
+        <v>522</v>
       </c>
       <c r="K209" s="3" t="s">
-        <v>533</v>
+        <v>521</v>
       </c>
       <c r="L209" s="6" t="s">
-        <v>532</v>
+        <v>520</v>
       </c>
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.2">
@@ -8619,7 +8647,7 @@
         <v>405</v>
       </c>
       <c r="C210" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D210" t="s">
         <v>388</v>
@@ -8634,13 +8662,13 @@
         <v>391</v>
       </c>
       <c r="I210" s="3" t="s">
-        <v>501</v>
+        <v>519</v>
       </c>
       <c r="K210" s="3" t="s">
-        <v>500</v>
+        <v>518</v>
       </c>
       <c r="L210" s="6" t="s">
-        <v>499</v>
+        <v>517</v>
       </c>
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.2">
@@ -8651,13 +8679,13 @@
         <v>405</v>
       </c>
       <c r="C211" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D211" t="s">
         <v>388</v>
       </c>
       <c r="F211" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G211" s="3" t="s">
         <v>174</v>
@@ -8666,13 +8694,13 @@
         <v>391</v>
       </c>
       <c r="I211" s="3" t="s">
-        <v>501</v>
+        <v>534</v>
       </c>
       <c r="K211" s="3" t="s">
-        <v>500</v>
+        <v>533</v>
       </c>
       <c r="L211" s="6" t="s">
-        <v>499</v>
+        <v>532</v>
       </c>
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.2">
@@ -8683,13 +8711,13 @@
         <v>405</v>
       </c>
       <c r="C212" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D212" t="s">
         <v>388</v>
       </c>
       <c r="F212" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G212" s="3" t="s">
         <v>174</v>
@@ -8715,7 +8743,7 @@
         <v>405</v>
       </c>
       <c r="C213" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D213" t="s">
         <v>388</v>
@@ -8747,13 +8775,13 @@
         <v>405</v>
       </c>
       <c r="C214" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D214" t="s">
         <v>388</v>
       </c>
       <c r="F214" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G214" s="3" t="s">
         <v>174</v>
@@ -8762,13 +8790,13 @@
         <v>391</v>
       </c>
       <c r="I214" s="3" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="K214" s="3" t="s">
-        <v>491</v>
+        <v>500</v>
       </c>
       <c r="L214" s="6" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
     </row>
     <row r="215" spans="1:12" x14ac:dyDescent="0.2">
@@ -8779,7 +8807,7 @@
         <v>405</v>
       </c>
       <c r="C215" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D215" t="s">
         <v>388</v>
@@ -8794,13 +8822,13 @@
         <v>391</v>
       </c>
       <c r="I215" s="3" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="K215" s="3" t="s">
-        <v>491</v>
+        <v>500</v>
       </c>
       <c r="L215" s="6" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
     </row>
     <row r="216" spans="1:12" x14ac:dyDescent="0.2">
@@ -8811,28 +8839,28 @@
         <v>405</v>
       </c>
       <c r="C216" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D216" t="s">
         <v>388</v>
       </c>
-      <c r="F216" s="11">
-        <v>5</v>
+      <c r="F216" s="3">
+        <v>2</v>
       </c>
       <c r="G216" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H216" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I216" s="3" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="K216" s="3" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="L216" s="6" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.2">
@@ -8842,29 +8870,29 @@
       <c r="B217" t="s">
         <v>405</v>
       </c>
-      <c r="C217" s="9" t="s">
-        <v>576</v>
+      <c r="C217" t="s">
+        <v>364</v>
       </c>
       <c r="D217" t="s">
         <v>388</v>
       </c>
-      <c r="F217" s="12">
-        <v>1</v>
+      <c r="F217" s="3">
+        <v>0</v>
       </c>
       <c r="G217" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H217" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I217" s="3" t="s">
-        <v>579</v>
+        <v>487</v>
       </c>
       <c r="K217" s="3" t="s">
-        <v>580</v>
+        <v>491</v>
       </c>
       <c r="L217" s="6" t="s">
-        <v>581</v>
+        <v>490</v>
       </c>
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.2">
@@ -8874,14 +8902,14 @@
       <c r="B218" t="s">
         <v>405</v>
       </c>
-      <c r="C218" s="9" t="s">
-        <v>578</v>
+      <c r="C218" t="s">
+        <v>365</v>
       </c>
       <c r="D218" t="s">
         <v>388</v>
       </c>
-      <c r="F218" s="12">
-        <v>0</v>
+      <c r="F218" s="11">
+        <v>5</v>
       </c>
       <c r="G218" s="3" t="s">
         <v>432</v>
@@ -8890,13 +8918,13 @@
         <v>391</v>
       </c>
       <c r="I218" s="3" t="s">
-        <v>579</v>
+        <v>494</v>
       </c>
       <c r="K218" s="3" t="s">
-        <v>580</v>
+        <v>493</v>
       </c>
       <c r="L218" s="6" t="s">
-        <v>581</v>
+        <v>492</v>
       </c>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.2">
@@ -8907,13 +8935,13 @@
         <v>405</v>
       </c>
       <c r="C219" s="9" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D219" t="s">
         <v>388</v>
       </c>
-      <c r="F219" s="12">
-        <v>0</v>
+      <c r="F219" s="3">
+        <v>1</v>
       </c>
       <c r="G219" s="3" t="s">
         <v>432</v>
@@ -8938,29 +8966,29 @@
       <c r="B220" t="s">
         <v>405</v>
       </c>
-      <c r="C220" t="s">
-        <v>366</v>
+      <c r="C220" s="9" t="s">
+        <v>578</v>
       </c>
       <c r="D220" t="s">
         <v>388</v>
       </c>
       <c r="F220" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G220" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H220" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>487</v>
+        <v>579</v>
       </c>
       <c r="K220" s="3" t="s">
-        <v>489</v>
+        <v>580</v>
       </c>
       <c r="L220" s="6" t="s">
-        <v>488</v>
+        <v>581</v>
       </c>
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.2">
@@ -8970,8 +8998,8 @@
       <c r="B221" t="s">
         <v>405</v>
       </c>
-      <c r="C221" t="s">
-        <v>367</v>
+      <c r="C221" s="9" t="s">
+        <v>577</v>
       </c>
       <c r="D221" t="s">
         <v>388</v>
@@ -8980,19 +9008,19 @@
         <v>0</v>
       </c>
       <c r="G221" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H221" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I221" s="3" t="s">
-        <v>487</v>
+        <v>579</v>
       </c>
       <c r="K221" s="3" t="s">
-        <v>489</v>
+        <v>580</v>
       </c>
       <c r="L221" s="6" t="s">
-        <v>488</v>
+        <v>581</v>
       </c>
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.2">
@@ -9003,13 +9031,13 @@
         <v>405</v>
       </c>
       <c r="C222" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D222" t="s">
         <v>388</v>
       </c>
       <c r="F222" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G222" s="3" t="s">
         <v>174</v>
@@ -9035,45 +9063,45 @@
         <v>405</v>
       </c>
       <c r="C223" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D223" t="s">
         <v>388</v>
       </c>
-      <c r="F223" s="11">
-        <v>3</v>
+      <c r="F223" s="3">
+        <v>0</v>
       </c>
       <c r="G223" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H223" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>396</v>
+        <v>487</v>
       </c>
       <c r="K223" s="3" t="s">
-        <v>516</v>
+        <v>489</v>
       </c>
       <c r="L223" s="6" t="s">
-        <v>515</v>
+        <v>488</v>
       </c>
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B224" t="s">
         <v>405</v>
       </c>
       <c r="C224" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D224" t="s">
         <v>388</v>
       </c>
       <c r="F224" s="3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G224" s="3" t="s">
         <v>174</v>
@@ -9082,45 +9110,45 @@
         <v>391</v>
       </c>
       <c r="I224" s="3" t="s">
-        <v>463</v>
+        <v>487</v>
       </c>
       <c r="K224" s="3" t="s">
-        <v>462</v>
+        <v>489</v>
       </c>
       <c r="L224" s="6" t="s">
-        <v>461</v>
+        <v>488</v>
       </c>
     </row>
     <row r="225" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B225" t="s">
         <v>405</v>
       </c>
       <c r="C225" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D225" t="s">
         <v>388</v>
       </c>
-      <c r="F225" s="3">
-        <v>20</v>
+      <c r="F225" s="11">
+        <v>3</v>
       </c>
       <c r="G225" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H225" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I225" s="3" t="s">
-        <v>419</v>
+        <v>396</v>
       </c>
       <c r="K225" s="3" t="s">
-        <v>418</v>
+        <v>516</v>
       </c>
       <c r="L225" s="6" t="s">
-        <v>417</v>
+        <v>515</v>
       </c>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.2">
@@ -9131,13 +9159,13 @@
         <v>405</v>
       </c>
       <c r="C226" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D226" t="s">
         <v>388</v>
       </c>
       <c r="F226" s="3">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G226" s="3" t="s">
         <v>174</v>
@@ -9146,30 +9174,30 @@
         <v>391</v>
       </c>
       <c r="I226" s="3" t="s">
-        <v>435</v>
+        <v>463</v>
       </c>
       <c r="K226" s="3" t="s">
-        <v>434</v>
+        <v>462</v>
       </c>
       <c r="L226" s="6" t="s">
-        <v>433</v>
+        <v>461</v>
       </c>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B227" t="s">
         <v>405</v>
       </c>
       <c r="C227" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D227" t="s">
         <v>388</v>
       </c>
       <c r="F227" s="3">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="G227" s="3" t="s">
         <v>174</v>
@@ -9178,30 +9206,30 @@
         <v>391</v>
       </c>
       <c r="I227" s="3" t="s">
-        <v>446</v>
+        <v>419</v>
       </c>
       <c r="K227" s="3" t="s">
-        <v>445</v>
+        <v>418</v>
       </c>
       <c r="L227" s="6" t="s">
-        <v>444</v>
+        <v>417</v>
       </c>
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B228" t="s">
         <v>405</v>
       </c>
       <c r="C228" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D228" t="s">
         <v>388</v>
       </c>
       <c r="F228" s="3">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G228" s="3" t="s">
         <v>174</v>
@@ -9210,13 +9238,13 @@
         <v>391</v>
       </c>
       <c r="I228" s="3" t="s">
-        <v>411</v>
+        <v>435</v>
       </c>
       <c r="K228" s="3" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="L228" s="6" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.2">
@@ -9227,13 +9255,13 @@
         <v>405</v>
       </c>
       <c r="C229" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D229" t="s">
         <v>388</v>
       </c>
       <c r="F229" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G229" s="3" t="s">
         <v>174</v>
@@ -9259,13 +9287,13 @@
         <v>405</v>
       </c>
       <c r="C230" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D230" t="s">
         <v>388</v>
       </c>
       <c r="F230" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G230" s="3" t="s">
         <v>174</v>
@@ -9274,13 +9302,13 @@
         <v>391</v>
       </c>
       <c r="I230" s="3" t="s">
-        <v>454</v>
+        <v>411</v>
       </c>
       <c r="K230" s="3" t="s">
-        <v>453</v>
+        <v>431</v>
       </c>
       <c r="L230" s="6" t="s">
-        <v>452</v>
+        <v>430</v>
       </c>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.2">
@@ -9291,13 +9319,13 @@
         <v>405</v>
       </c>
       <c r="C231" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D231" t="s">
         <v>388</v>
       </c>
       <c r="F231" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G231" s="3" t="s">
         <v>174</v>
@@ -9306,13 +9334,13 @@
         <v>391</v>
       </c>
       <c r="I231" s="3" t="s">
-        <v>411</v>
+        <v>446</v>
       </c>
       <c r="K231" s="3" t="s">
-        <v>476</v>
+        <v>445</v>
       </c>
       <c r="L231" s="6" t="s">
-        <v>475</v>
+        <v>444</v>
       </c>
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.2">
@@ -9323,13 +9351,13 @@
         <v>405</v>
       </c>
       <c r="C232" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D232" t="s">
         <v>388</v>
       </c>
       <c r="F232" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G232" s="3" t="s">
         <v>174</v>
@@ -9338,13 +9366,13 @@
         <v>391</v>
       </c>
       <c r="I232" s="3" t="s">
-        <v>506</v>
+        <v>454</v>
       </c>
       <c r="K232" s="3" t="s">
-        <v>505</v>
+        <v>453</v>
       </c>
       <c r="L232" s="6" t="s">
-        <v>504</v>
+        <v>452</v>
       </c>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.2">
@@ -9355,13 +9383,13 @@
         <v>405</v>
       </c>
       <c r="C233" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D233" t="s">
         <v>388</v>
       </c>
       <c r="F233" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G233" s="3" t="s">
         <v>174</v>
@@ -9370,13 +9398,13 @@
         <v>391</v>
       </c>
       <c r="I233" s="3" t="s">
-        <v>441</v>
+        <v>411</v>
       </c>
       <c r="K233" s="3" t="s">
-        <v>440</v>
+        <v>476</v>
       </c>
       <c r="L233" s="6" t="s">
-        <v>439</v>
+        <v>475</v>
       </c>
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.2">
@@ -9387,13 +9415,13 @@
         <v>405</v>
       </c>
       <c r="C234" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D234" t="s">
         <v>388</v>
       </c>
       <c r="F234" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G234" s="3" t="s">
         <v>174</v>
@@ -9402,13 +9430,13 @@
         <v>391</v>
       </c>
       <c r="I234" s="3" t="s">
-        <v>443</v>
+        <v>506</v>
       </c>
       <c r="K234" s="3" t="s">
-        <v>440</v>
+        <v>505</v>
       </c>
       <c r="L234" s="6" t="s">
-        <v>442</v>
+        <v>504</v>
       </c>
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.2">
@@ -9419,7 +9447,7 @@
         <v>405</v>
       </c>
       <c r="C235" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D235" t="s">
         <v>388</v>
@@ -9434,30 +9462,30 @@
         <v>391</v>
       </c>
       <c r="I235" s="3" t="s">
-        <v>411</v>
+        <v>441</v>
       </c>
       <c r="K235" s="3" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="L235" s="6" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B236" t="s">
         <v>405</v>
       </c>
       <c r="C236" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D236" t="s">
         <v>388</v>
       </c>
       <c r="F236" s="3">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="G236" s="3" t="s">
         <v>174</v>
@@ -9466,13 +9494,13 @@
         <v>391</v>
       </c>
       <c r="I236" s="3" t="s">
-        <v>414</v>
+        <v>443</v>
       </c>
       <c r="K236" s="3" t="s">
-        <v>413</v>
+        <v>440</v>
       </c>
       <c r="L236" s="6" t="s">
-        <v>412</v>
+        <v>442</v>
       </c>
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.2">
@@ -9483,45 +9511,45 @@
         <v>405</v>
       </c>
       <c r="C237" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D237" t="s">
         <v>388</v>
       </c>
-      <c r="F237" s="11">
-        <v>2</v>
+      <c r="F237" s="3">
+        <v>1</v>
       </c>
       <c r="G237" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H237" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I237" s="3" t="s">
-        <v>525</v>
+        <v>411</v>
       </c>
       <c r="K237" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="L237" s="10" t="s">
-        <v>523</v>
+        <v>451</v>
+      </c>
+      <c r="L237" s="6" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B238" t="s">
         <v>405</v>
       </c>
       <c r="C238" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D238" t="s">
         <v>388</v>
       </c>
       <c r="F238" s="3">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="G238" s="3" t="s">
         <v>174</v>
@@ -9529,15 +9557,14 @@
       <c r="H238" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I238" t="s">
-        <v>573</v>
-      </c>
-      <c r="J238"/>
-      <c r="K238" t="s">
-        <v>574</v>
+      <c r="I238" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="K238" s="3" t="s">
+        <v>413</v>
       </c>
       <c r="L238" s="6" t="s">
-        <v>575</v>
+        <v>412</v>
       </c>
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.2">
@@ -9548,46 +9575,45 @@
         <v>405</v>
       </c>
       <c r="C239" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D239" t="s">
         <v>388</v>
       </c>
-      <c r="F239" s="3">
-        <v>1</v>
+      <c r="F239" s="11">
+        <v>2</v>
       </c>
       <c r="G239" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H239" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I239" t="s">
-        <v>570</v>
-      </c>
-      <c r="J239"/>
-      <c r="K239" t="s">
-        <v>571</v>
-      </c>
-      <c r="L239" s="6" t="s">
-        <v>572</v>
+      <c r="I239" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="K239" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="L239" s="10" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B240" t="s">
         <v>405</v>
       </c>
       <c r="C240" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D240" t="s">
         <v>388</v>
       </c>
       <c r="F240" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G240" s="3" t="s">
         <v>174</v>
@@ -9595,14 +9621,15 @@
       <c r="H240" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I240" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="K240" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="L240" s="7" t="s">
-        <v>404</v>
+      <c r="I240" t="s">
+        <v>573</v>
+      </c>
+      <c r="J240"/>
+      <c r="K240" t="s">
+        <v>574</v>
+      </c>
+      <c r="L240" s="6" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.2">
@@ -9613,7 +9640,7 @@
         <v>405</v>
       </c>
       <c r="C241" t="s">
-        <v>58</v>
+        <v>385</v>
       </c>
       <c r="D241" t="s">
         <v>388</v>
@@ -9627,46 +9654,47 @@
       <c r="H241" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I241" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="K241" s="3" t="s">
-        <v>467</v>
+      <c r="I241" t="s">
+        <v>570</v>
+      </c>
+      <c r="J241"/>
+      <c r="K241" t="s">
+        <v>571</v>
       </c>
       <c r="L241" s="6" t="s">
-        <v>466</v>
+        <v>572</v>
       </c>
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B242" t="s">
         <v>405</v>
       </c>
-      <c r="C242" s="9" t="s">
-        <v>582</v>
+      <c r="C242" t="s">
+        <v>386</v>
       </c>
       <c r="D242" t="s">
         <v>388</v>
       </c>
       <c r="F242" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G242" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H242" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I242" s="3" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="K242" s="3" t="s">
-        <v>587</v>
-      </c>
-      <c r="L242" s="6" t="s">
-        <v>586</v>
+        <v>403</v>
+      </c>
+      <c r="L242" s="7" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.2">
@@ -9676,29 +9704,29 @@
       <c r="B243" t="s">
         <v>405</v>
       </c>
-      <c r="C243" s="9" t="s">
-        <v>582</v>
+      <c r="C243" t="s">
+        <v>58</v>
       </c>
       <c r="D243" t="s">
         <v>388</v>
       </c>
       <c r="F243" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G243" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H243" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I243" s="3" t="s">
-        <v>392</v>
+        <v>468</v>
       </c>
       <c r="K243" s="3" t="s">
-        <v>587</v>
+        <v>467</v>
       </c>
       <c r="L243" s="6" t="s">
-        <v>586</v>
+        <v>466</v>
       </c>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.2">
@@ -9715,7 +9743,7 @@
         <v>388</v>
       </c>
       <c r="F244" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G244" s="3" t="s">
         <v>432</v>
@@ -9741,13 +9769,13 @@
         <v>405</v>
       </c>
       <c r="C245" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D245" t="s">
         <v>388</v>
       </c>
       <c r="F245" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G245" s="3" t="s">
         <v>432</v>
@@ -9756,13 +9784,13 @@
         <v>391</v>
       </c>
       <c r="I245" s="3" t="s">
-        <v>537</v>
+        <v>392</v>
       </c>
       <c r="K245" s="3" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="L245" s="6" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.2">
@@ -9772,33 +9800,97 @@
       <c r="B246" t="s">
         <v>405</v>
       </c>
-      <c r="C246" t="s">
-        <v>387</v>
+      <c r="C246" s="9" t="s">
+        <v>582</v>
       </c>
       <c r="D246" t="s">
         <v>388</v>
       </c>
       <c r="F246" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G246" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H246" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I246" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="K246" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="L246" s="6" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>389</v>
+      </c>
+      <c r="B247" t="s">
+        <v>405</v>
+      </c>
+      <c r="C247" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="D247" t="s">
+        <v>388</v>
+      </c>
+      <c r="F247" s="3">
+        <v>1</v>
+      </c>
+      <c r="G247" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="H247" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I247" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="K247" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="L247" s="6" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>389</v>
+      </c>
+      <c r="B248" t="s">
+        <v>405</v>
+      </c>
+      <c r="C248" t="s">
+        <v>387</v>
+      </c>
+      <c r="D248" t="s">
+        <v>388</v>
+      </c>
+      <c r="F248" s="3">
+        <v>1</v>
+      </c>
+      <c r="G248" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H248" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I248" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="K246" s="3" t="s">
+      <c r="K248" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="L246" s="6" t="s">
+      <c r="L248" s="6" t="s">
         <v>469</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L246" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}"/>
+  <autoFilter ref="A1:L248" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}"/>
   <hyperlinks>
     <hyperlink ref="L3" r:id="rId1" location="query=target&amp;position=0&amp;from_view=search&amp;track=sph&amp;uuid=07a631b0-afe2-4d83-9076-a80360e62f2f" xr:uid="{6340FD26-01F6-9246-82E5-C8936FBB7B36}"/>
     <hyperlink ref="L4" r:id="rId2" location="query=spell%20book&amp;position=12&amp;from_view=keyword&amp;track=ais&amp;uuid=3aa8f740-41d0-409e-b03b-268281a69be6" xr:uid="{1A91BF66-CE85-304F-BBE7-7F8EBE53C285}"/>
@@ -9927,13 +10019,13 @@
     <hyperlink ref="L158" r:id="rId125" xr:uid="{F88953B7-468E-C34B-9347-94009F9A78D2}"/>
     <hyperlink ref="L198" r:id="rId126" xr:uid="{1F3BBC8C-29E8-C74A-AB3F-04AE466222EF}"/>
     <hyperlink ref="L200" r:id="rId127" xr:uid="{3C51058F-793C-D34A-8286-18AE4C8EF6CE}"/>
-    <hyperlink ref="L240" r:id="rId128" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
+    <hyperlink ref="L242" r:id="rId128" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
     <hyperlink ref="L155" r:id="rId129" xr:uid="{6A722A1D-2F7B-4242-8134-716EFF33F7D2}"/>
     <hyperlink ref="L156" r:id="rId130" xr:uid="{547CD1A8-1967-1C46-95E3-89E39CD045C2}"/>
-    <hyperlink ref="L201" r:id="rId131" xr:uid="{5ACD6BFD-52F0-0940-AA8E-B04F1D397BC7}"/>
-    <hyperlink ref="L236" r:id="rId132" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
+    <hyperlink ref="L203" r:id="rId131" xr:uid="{5ACD6BFD-52F0-0940-AA8E-B04F1D397BC7}"/>
+    <hyperlink ref="L238" r:id="rId132" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
     <hyperlink ref="L199" r:id="rId133" xr:uid="{2030AD8C-28A7-544B-92DC-5CBE411DE1C0}"/>
-    <hyperlink ref="L225" r:id="rId134" xr:uid="{05363CA1-BE60-3F42-B56A-1A92A0EDA166}"/>
+    <hyperlink ref="L227" r:id="rId134" xr:uid="{05363CA1-BE60-3F42-B56A-1A92A0EDA166}"/>
     <hyperlink ref="L191" r:id="rId135" xr:uid="{D4C66DCB-D6B4-EC4F-A922-B87887BE6E4A}"/>
     <hyperlink ref="L190" r:id="rId136" xr:uid="{A05D9F8A-ED0A-4143-8920-9422DD4E0BDD}"/>
     <hyperlink ref="L192" r:id="rId137" xr:uid="{83FA4EC1-AB5E-3B43-9476-4CA54526DF8E}"/>
@@ -9942,74 +10034,76 @@
     <hyperlink ref="L168" r:id="rId140" xr:uid="{3AB6BE1F-95C1-A443-B12D-D7A523FAD6C5}"/>
     <hyperlink ref="L169" r:id="rId141" xr:uid="{347BDCC2-5A0C-B249-8CA8-B72D245480FC}"/>
     <hyperlink ref="L170" r:id="rId142" xr:uid="{E58DD28D-BD99-DF44-9E5E-B3D05F881C1F}"/>
-    <hyperlink ref="L228" r:id="rId143" xr:uid="{4F668E79-3664-0547-B3D5-B7724A9D574D}"/>
-    <hyperlink ref="L226" r:id="rId144" xr:uid="{8AB5C10C-8B45-1843-96BD-655A4FA04EFD}"/>
+    <hyperlink ref="L230" r:id="rId143" xr:uid="{4F668E79-3664-0547-B3D5-B7724A9D574D}"/>
+    <hyperlink ref="L228" r:id="rId144" xr:uid="{8AB5C10C-8B45-1843-96BD-655A4FA04EFD}"/>
     <hyperlink ref="L174" r:id="rId145" xr:uid="{EAED74E0-13EE-A046-9ADC-AC8BDE30C3E6}"/>
-    <hyperlink ref="L233" r:id="rId146" xr:uid="{3577256C-215B-134E-B541-B7B77272CD8A}"/>
-    <hyperlink ref="L234" r:id="rId147" xr:uid="{98E325FC-7F95-B44E-98EB-DE0FF53BC89D}"/>
-    <hyperlink ref="L227" r:id="rId148" xr:uid="{5CE3083F-F217-3743-B613-A7DDF354E72D}"/>
-    <hyperlink ref="L229" r:id="rId149" xr:uid="{B81B6B41-2C17-AA48-B730-D906488BA0A0}"/>
+    <hyperlink ref="L235" r:id="rId146" xr:uid="{3577256C-215B-134E-B541-B7B77272CD8A}"/>
+    <hyperlink ref="L236" r:id="rId147" xr:uid="{98E325FC-7F95-B44E-98EB-DE0FF53BC89D}"/>
+    <hyperlink ref="L229" r:id="rId148" xr:uid="{5CE3083F-F217-3743-B613-A7DDF354E72D}"/>
+    <hyperlink ref="L231" r:id="rId149" xr:uid="{B81B6B41-2C17-AA48-B730-D906488BA0A0}"/>
     <hyperlink ref="L180" r:id="rId150" xr:uid="{BA0813A2-2582-7A46-A492-16A943824EE5}"/>
-    <hyperlink ref="L235" r:id="rId151" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
-    <hyperlink ref="L230" r:id="rId152" xr:uid="{C5265333-F7F0-1845-98D7-68E930F9DFAE}"/>
+    <hyperlink ref="L237" r:id="rId151" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
+    <hyperlink ref="L232" r:id="rId152" xr:uid="{C5265333-F7F0-1845-98D7-68E930F9DFAE}"/>
     <hyperlink ref="L182" r:id="rId153" xr:uid="{C0A159CB-3986-1A46-95AD-DCEFF4247697}"/>
     <hyperlink ref="L172" r:id="rId154" xr:uid="{37810A74-E45D-1D46-AEF5-C5FE2F414285}"/>
-    <hyperlink ref="L224" r:id="rId155" xr:uid="{D2906064-B1B8-4648-8201-BEFA97591226}"/>
+    <hyperlink ref="L226" r:id="rId155" xr:uid="{D2906064-B1B8-4648-8201-BEFA97591226}"/>
     <hyperlink ref="L160" r:id="rId156" xr:uid="{1D3CD52E-7AAD-E444-88F4-4BAE6C5B5EB7}"/>
     <hyperlink ref="L161" r:id="rId157" xr:uid="{E6E6DA47-945D-6145-912F-08B17B7BA6AE}"/>
     <hyperlink ref="L162" r:id="rId158" xr:uid="{006B1689-D89A-1E4A-BBC5-E9C9583907F7}"/>
     <hyperlink ref="L163" r:id="rId159" xr:uid="{C3E773B2-D410-AF41-B197-4638485DC8EF}"/>
     <hyperlink ref="L164" r:id="rId160" xr:uid="{A0E8A8E2-4A93-3D42-AF48-81955241A483}"/>
     <hyperlink ref="L165" r:id="rId161" xr:uid="{1B03F18A-8745-AA4F-AA8B-88D65D3B24BC}"/>
-    <hyperlink ref="L241" r:id="rId162" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
-    <hyperlink ref="L246" r:id="rId163" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
+    <hyperlink ref="L243" r:id="rId162" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
+    <hyperlink ref="L248" r:id="rId163" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
     <hyperlink ref="L188" r:id="rId164" xr:uid="{D6B77117-A0D5-9240-8193-0102C36CCE4C}"/>
     <hyperlink ref="L189" r:id="rId165" xr:uid="{79FB1103-88A8-8044-9E2C-4FAEC0906E8E}"/>
-    <hyperlink ref="L231" r:id="rId166" xr:uid="{5BF1C4C9-E63A-4F42-9042-36520975FDFA}"/>
+    <hyperlink ref="L233" r:id="rId166" xr:uid="{5BF1C4C9-E63A-4F42-9042-36520975FDFA}"/>
     <hyperlink ref="L187" r:id="rId167" xr:uid="{21CDF460-9871-0547-AA6B-20304C8DD21D}"/>
     <hyperlink ref="L177" r:id="rId168" xr:uid="{BA1EC844-435A-6C44-87FC-C12B7ECFC55B}"/>
     <hyperlink ref="L176" r:id="rId169" xr:uid="{46D875DC-CDDD-7E4B-88DB-DFC416CF17AB}"/>
     <hyperlink ref="L166" r:id="rId170" xr:uid="{7D2FF6AE-1C67-9D4A-A760-7E3745DD9EA6}"/>
-    <hyperlink ref="L214" r:id="rId171" xr:uid="{B5E5E388-8F37-414E-A0C6-1DC58E77628C}"/>
-    <hyperlink ref="L216" r:id="rId172" xr:uid="{A96B1ACF-D982-9240-BB1C-69459154AE5A}"/>
+    <hyperlink ref="L216" r:id="rId171" xr:uid="{B5E5E388-8F37-414E-A0C6-1DC58E77628C}"/>
+    <hyperlink ref="L218" r:id="rId172" xr:uid="{A96B1ACF-D982-9240-BB1C-69459154AE5A}"/>
     <hyperlink ref="L183" r:id="rId173" xr:uid="{D3BB695A-CBA9-D649-B49D-4CC8D16EFD9B}"/>
     <hyperlink ref="L184" r:id="rId174" xr:uid="{A2922BA8-758D-3149-892C-B7B65B435332}"/>
-    <hyperlink ref="L203" r:id="rId175" xr:uid="{BDB09119-6289-4346-BC29-7A54BD393127}"/>
-    <hyperlink ref="L232" r:id="rId176" xr:uid="{5736CAF4-3646-3243-9AEB-4D82B6D0D10A}"/>
-    <hyperlink ref="L206" r:id="rId177" xr:uid="{60659D55-801C-9A4E-84CA-809884CCBE5C}"/>
+    <hyperlink ref="L205" r:id="rId175" xr:uid="{BDB09119-6289-4346-BC29-7A54BD393127}"/>
+    <hyperlink ref="L234" r:id="rId176" xr:uid="{5736CAF4-3646-3243-9AEB-4D82B6D0D10A}"/>
+    <hyperlink ref="L208" r:id="rId177" xr:uid="{60659D55-801C-9A4E-84CA-809884CCBE5C}"/>
     <hyperlink ref="L196" r:id="rId178" xr:uid="{18DDC006-0939-794C-9B5D-10593F8C0973}"/>
     <hyperlink ref="L185" r:id="rId179" xr:uid="{50EA46A5-11DD-0345-ABCA-4206D73C7606}"/>
-    <hyperlink ref="L223" r:id="rId180" xr:uid="{63DDFF3B-E62C-9445-96AD-4BB37ACCD20E}"/>
-    <hyperlink ref="L208" r:id="rId181" xr:uid="{05E34BC1-B22F-3E46-8574-E72267507402}"/>
-    <hyperlink ref="L207" r:id="rId182" xr:uid="{7125DF67-5A7E-D948-8363-A31AB1EBA44A}"/>
-    <hyperlink ref="L237" r:id="rId183" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
+    <hyperlink ref="L225" r:id="rId180" xr:uid="{63DDFF3B-E62C-9445-96AD-4BB37ACCD20E}"/>
+    <hyperlink ref="L210" r:id="rId181" xr:uid="{05E34BC1-B22F-3E46-8574-E72267507402}"/>
+    <hyperlink ref="L209" r:id="rId182" xr:uid="{7125DF67-5A7E-D948-8363-A31AB1EBA44A}"/>
+    <hyperlink ref="L239" r:id="rId183" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
     <hyperlink ref="L197" r:id="rId184" xr:uid="{CCE2D666-E296-D94C-ACE0-791CC746483B}"/>
     <hyperlink ref="L178" r:id="rId185" xr:uid="{E5A2F3EE-A3B1-0842-9364-E4B6EACA9544}"/>
-    <hyperlink ref="L209" r:id="rId186" xr:uid="{E08C8BA4-5414-1947-9CA8-45FE0B846CD1}"/>
-    <hyperlink ref="L205" r:id="rId187" xr:uid="{F1A64091-5BF7-8243-B7A0-F4C13B8B0ABB}"/>
+    <hyperlink ref="L211" r:id="rId186" xr:uid="{E08C8BA4-5414-1947-9CA8-45FE0B846CD1}"/>
+    <hyperlink ref="L207" r:id="rId187" xr:uid="{F1A64091-5BF7-8243-B7A0-F4C13B8B0ABB}"/>
     <hyperlink ref="L194" r:id="rId188" xr:uid="{745AEF03-3150-C54B-800A-696460474256}"/>
     <hyperlink ref="L195" r:id="rId189" xr:uid="{9C078FBA-3B11-8049-9187-5BC86D78EA09}"/>
     <hyperlink ref="L179" r:id="rId190" xr:uid="{BF9A6A48-C664-FA4B-A769-D87460BB9387}"/>
     <hyperlink ref="L181" r:id="rId191" xr:uid="{11E0C06F-BBA9-B446-A3A4-5862C893161B}"/>
-    <hyperlink ref="L204" r:id="rId192" xr:uid="{D5E45024-1B58-714D-9576-1FA969BDADD9}"/>
+    <hyperlink ref="L206" r:id="rId192" xr:uid="{D5E45024-1B58-714D-9576-1FA969BDADD9}"/>
     <hyperlink ref="L186" r:id="rId193" xr:uid="{D160676D-AC82-D243-B9A9-56033B0A6EFE}"/>
-    <hyperlink ref="L202" r:id="rId194" xr:uid="{3DB54A74-68B7-734A-BC3C-BFE4E2E4103E}"/>
+    <hyperlink ref="L204" r:id="rId194" xr:uid="{3DB54A74-68B7-734A-BC3C-BFE4E2E4103E}"/>
     <hyperlink ref="L103" r:id="rId195" xr:uid="{4686296B-C235-4048-A384-BE461895E2AC}"/>
     <hyperlink ref="L105" r:id="rId196" location="page=2&amp;query=gold%20badge%20sprite&amp;position=49&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{061AB839-ADB1-BA47-A152-68CDFE8A1979}"/>
     <hyperlink ref="L106" r:id="rId197" location="page=4&amp;query=gold%20badge%20sprite&amp;position=9&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{138577BB-7F7D-D64A-806E-567F3970D250}"/>
     <hyperlink ref="L175" r:id="rId198" xr:uid="{927B8B79-A428-2043-9B3B-555F7877CA20}"/>
     <hyperlink ref="L193" r:id="rId199" xr:uid="{6018233D-1425-7148-A608-3B0666055EA2}"/>
-    <hyperlink ref="L215" r:id="rId200" xr:uid="{38C9843F-1665-8F46-A66C-287455700886}"/>
-    <hyperlink ref="L238" r:id="rId201" xr:uid="{9E664F43-2A79-3744-BC57-4D11914A4B9C}"/>
-    <hyperlink ref="L239" r:id="rId202" xr:uid="{F55C22EB-ADA4-064F-8C9F-34B8DFB927E8}"/>
+    <hyperlink ref="L217" r:id="rId200" xr:uid="{38C9843F-1665-8F46-A66C-287455700886}"/>
+    <hyperlink ref="L240" r:id="rId201" xr:uid="{9E664F43-2A79-3744-BC57-4D11914A4B9C}"/>
+    <hyperlink ref="L241" r:id="rId202" xr:uid="{F55C22EB-ADA4-064F-8C9F-34B8DFB927E8}"/>
     <hyperlink ref="L159" r:id="rId203" xr:uid="{A1B2F4EC-ACE1-B14D-8619-0451D719CFC0}"/>
-    <hyperlink ref="L217" r:id="rId204" xr:uid="{2BF445F0-7B50-5E48-A8E5-4779F07B83CE}"/>
-    <hyperlink ref="L218" r:id="rId205" xr:uid="{6B23A3F9-85DD-4043-853E-3BF95911A2C6}"/>
-    <hyperlink ref="L219" r:id="rId206" xr:uid="{A975FD98-A3FE-5B40-9F31-D14EAE3777F9}"/>
-    <hyperlink ref="L242" r:id="rId207" xr:uid="{F01C8569-23FB-7F4C-A50B-40979911E1B8}"/>
-    <hyperlink ref="L245" r:id="rId208" xr:uid="{B54ABD16-F1A6-DC45-B36E-0CC72B423F70}"/>
-    <hyperlink ref="L243" r:id="rId209" xr:uid="{EBA532A6-AAFD-E54D-BD41-CC4F5F92AF68}"/>
-    <hyperlink ref="L244" r:id="rId210" xr:uid="{0F422DA4-046E-F246-BC4A-695F255E6851}"/>
+    <hyperlink ref="L219" r:id="rId204" xr:uid="{2BF445F0-7B50-5E48-A8E5-4779F07B83CE}"/>
+    <hyperlink ref="L220" r:id="rId205" xr:uid="{6B23A3F9-85DD-4043-853E-3BF95911A2C6}"/>
+    <hyperlink ref="L221" r:id="rId206" xr:uid="{A975FD98-A3FE-5B40-9F31-D14EAE3777F9}"/>
+    <hyperlink ref="L244" r:id="rId207" xr:uid="{F01C8569-23FB-7F4C-A50B-40979911E1B8}"/>
+    <hyperlink ref="L247" r:id="rId208" xr:uid="{B54ABD16-F1A6-DC45-B36E-0CC72B423F70}"/>
+    <hyperlink ref="L245" r:id="rId209" xr:uid="{EBA532A6-AAFD-E54D-BD41-CC4F5F92AF68}"/>
+    <hyperlink ref="L246" r:id="rId210" xr:uid="{0F422DA4-046E-F246-BC4A-695F255E6851}"/>
+    <hyperlink ref="L201" r:id="rId211" xr:uid="{1F9FD82A-7BDA-7143-B89F-0DBBBC864386}"/>
+    <hyperlink ref="L202" r:id="rId212" xr:uid="{7F1F0626-5319-784B-97DE-B956AE96359D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
AssetsCatalog: update with sounds and images Assets: add waterSplash textures PlayerSprite: redo animateExplosion() to make it more universal, so it can be used for any type of explosions. Refactor removeFromParent to eliminate hidden retain cycles!
</commit_message>
<xml_diff>
--- a/JSON/AssetsCatalog.xlsx
+++ b/JSON/AssetsCatalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5223B2-23DF-E64D-B913-801AB7EC25D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4677AC7-8412-0F47-84CF-D50FBBF42C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42040" yWindow="1620" windowWidth="36000" windowHeight="21040" xr2:uid="{E84333C6-E3B6-FB42-AB04-827399F33810}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$248</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$250</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2112" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2129" uniqueCount="601">
   <si>
     <t>Filename</t>
   </si>
@@ -1824,6 +1824,24 @@
   </si>
   <si>
     <t>AlexM76</t>
+  </si>
+  <si>
+    <t>marlinblast</t>
+  </si>
+  <si>
+    <t>Bolt Of Lightning Strikes Close By</t>
+  </si>
+  <si>
+    <t>https://audiojungle.net/item/bolt-of-lighting-strikes-close-by/13482011</t>
+  </si>
+  <si>
+    <t>marlinBlast</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>https://www.freepik.com/free-photo/abstract_12570110.htm#page=2&amp;query=light%20beam&amp;position=25&amp;from_view=search&amp;track=ais&amp;uuid=063fa81a-19de-4aad-b5fc-7caa6fa59141#position=25&amp;page=2&amp;query=light%20beam</t>
   </si>
 </sst>
 </file>
@@ -1909,7 +1927,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1922,8 +1940,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2239,13 +2258,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}">
-  <dimension ref="A1:L248"/>
+  <dimension ref="A1:L250"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D180" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L201" sqref="L201"/>
+      <selection pane="bottomRight" activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4710,10 +4729,10 @@
         <v>4</v>
       </c>
       <c r="B83" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C83" t="s">
-        <v>205</v>
+        <v>598</v>
       </c>
       <c r="D83" t="s">
         <v>6</v>
@@ -4722,19 +4741,16 @@
         <v>0</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>216</v>
+        <v>36</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>554</v>
-      </c>
-      <c r="J83" s="3" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="K83" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="L83" s="3" t="s">
-        <v>553</v>
+        <v>599</v>
+      </c>
+      <c r="L83" s="6" t="s">
+        <v>600</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
@@ -4745,7 +4761,7 @@
         <v>204</v>
       </c>
       <c r="C84" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D84" t="s">
         <v>6</v>
@@ -4777,7 +4793,7 @@
         <v>204</v>
       </c>
       <c r="C85" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D85" t="s">
         <v>6</v>
@@ -4809,7 +4825,7 @@
         <v>204</v>
       </c>
       <c r="C86" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D86" t="s">
         <v>6</v>
@@ -4841,7 +4857,7 @@
         <v>204</v>
       </c>
       <c r="C87" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D87" t="s">
         <v>6</v>
@@ -4873,7 +4889,7 @@
         <v>204</v>
       </c>
       <c r="C88" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D88" t="s">
         <v>6</v>
@@ -4905,7 +4921,7 @@
         <v>204</v>
       </c>
       <c r="C89" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D89" t="s">
         <v>6</v>
@@ -4937,7 +4953,7 @@
         <v>204</v>
       </c>
       <c r="C90" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D90" t="s">
         <v>6</v>
@@ -4969,7 +4985,7 @@
         <v>204</v>
       </c>
       <c r="C91" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D91" t="s">
         <v>6</v>
@@ -5001,7 +5017,7 @@
         <v>204</v>
       </c>
       <c r="C92" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D92" t="s">
         <v>6</v>
@@ -5033,7 +5049,7 @@
         <v>204</v>
       </c>
       <c r="C93" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D93" t="s">
         <v>6</v>
@@ -5062,10 +5078,10 @@
         <v>4</v>
       </c>
       <c r="B94" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="C94" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D94" t="s">
         <v>6</v>
@@ -5074,16 +5090,19 @@
         <v>0</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>36</v>
+        <v>216</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>93</v>
+        <v>554</v>
+      </c>
+      <c r="J94" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="K94" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="L94" s="6" t="s">
-        <v>219</v>
+        <v>553</v>
+      </c>
+      <c r="L94" s="3" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.2">
@@ -5091,10 +5110,10 @@
         <v>4</v>
       </c>
       <c r="B95" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C95" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D95" t="s">
         <v>6</v>
@@ -5106,13 +5125,13 @@
         <v>36</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="K95" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="L95" s="6" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.2">
@@ -5123,7 +5142,7 @@
         <v>221</v>
       </c>
       <c r="C96" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D96" t="s">
         <v>6</v>
@@ -5138,10 +5157,10 @@
         <v>135</v>
       </c>
       <c r="K96" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="L96" s="7" t="s">
-        <v>230</v>
+        <v>224</v>
+      </c>
+      <c r="L96" s="6" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.2">
@@ -5152,7 +5171,7 @@
         <v>221</v>
       </c>
       <c r="C97" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D97" t="s">
         <v>6</v>
@@ -5167,10 +5186,10 @@
         <v>135</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="L97" s="6" t="s">
-        <v>223</v>
+        <v>229</v>
+      </c>
+      <c r="L97" s="7" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.2">
@@ -5181,7 +5200,7 @@
         <v>221</v>
       </c>
       <c r="C98" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D98" t="s">
         <v>6</v>
@@ -5210,7 +5229,7 @@
         <v>221</v>
       </c>
       <c r="C99" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D99" t="s">
         <v>6</v>
@@ -5225,10 +5244,10 @@
         <v>135</v>
       </c>
       <c r="K99" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="L99" s="7" t="s">
-        <v>230</v>
+        <v>224</v>
+      </c>
+      <c r="L99" s="6" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.2">
@@ -5236,10 +5255,10 @@
         <v>4</v>
       </c>
       <c r="B100" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="C100" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D100" t="s">
         <v>6</v>
@@ -5248,19 +5267,16 @@
         <v>0</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>234</v>
+        <v>36</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="J100" s="3" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
       <c r="K100" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="L100" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
+      </c>
+      <c r="L100" s="7" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.2">
@@ -5268,10 +5284,10 @@
         <v>4</v>
       </c>
       <c r="B101" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C101" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D101" t="s">
         <v>6</v>
@@ -5280,19 +5296,19 @@
         <v>0</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>125</v>
+        <v>234</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>125</v>
+        <v>235</v>
       </c>
       <c r="J101" s="3" t="s">
-        <v>174</v>
+        <v>62</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>126</v>
+        <v>236</v>
       </c>
       <c r="L101" s="6" t="s">
-        <v>124</v>
+        <v>233</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.2">
@@ -5300,7 +5316,7 @@
         <v>4</v>
       </c>
       <c r="B102" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C102" t="s">
         <v>238</v>
@@ -5321,10 +5337,10 @@
         <v>174</v>
       </c>
       <c r="K102" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="L102" s="7" t="s">
-        <v>196</v>
+        <v>126</v>
+      </c>
+      <c r="L102" s="6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.2">
@@ -5332,7 +5348,7 @@
         <v>4</v>
       </c>
       <c r="B103" t="s">
-        <v>556</v>
+        <v>239</v>
       </c>
       <c r="C103" t="s">
         <v>238</v>
@@ -5364,16 +5380,13 @@
         <v>4</v>
       </c>
       <c r="B104" t="s">
-        <v>240</v>
+        <v>556</v>
       </c>
       <c r="C104" t="s">
-        <v>557</v>
+        <v>238</v>
       </c>
       <c r="D104" t="s">
         <v>6</v>
-      </c>
-      <c r="E104" t="s">
-        <v>174</v>
       </c>
       <c r="F104" s="3">
         <v>0</v>
@@ -5388,10 +5401,10 @@
         <v>174</v>
       </c>
       <c r="K104" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="L104" s="6" t="s">
-        <v>124</v>
+        <v>195</v>
+      </c>
+      <c r="L104" s="7" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.2">
@@ -5414,16 +5427,19 @@
         <v>0</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
+      </c>
+      <c r="J105" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="K105" s="3" t="s">
-        <v>559</v>
+        <v>126</v>
       </c>
       <c r="L105" s="6" t="s">
-        <v>558</v>
+        <v>124</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.2">
@@ -5452,10 +5468,10 @@
         <v>135</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="L106" s="6" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.2">
@@ -5463,10 +5479,10 @@
         <v>4</v>
       </c>
       <c r="B107" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C107" t="s">
-        <v>244</v>
+        <v>557</v>
       </c>
       <c r="D107" t="s">
         <v>6</v>
@@ -5484,10 +5500,10 @@
         <v>135</v>
       </c>
       <c r="K107" s="3" t="s">
-        <v>224</v>
+        <v>561</v>
       </c>
       <c r="L107" s="6" t="s">
-        <v>223</v>
+        <v>560</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.2">
@@ -5510,19 +5526,16 @@
         <v>0</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>234</v>
+        <v>36</v>
       </c>
       <c r="I108" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="J108" s="3" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
       <c r="K108" s="3" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="L108" s="6" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.2">
@@ -5545,19 +5558,19 @@
         <v>0</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>125</v>
+        <v>234</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>125</v>
+        <v>235</v>
       </c>
       <c r="J109" s="3" t="s">
-        <v>174</v>
+        <v>62</v>
       </c>
       <c r="K109" s="3" t="s">
-        <v>126</v>
+        <v>236</v>
       </c>
       <c r="L109" s="6" t="s">
-        <v>124</v>
+        <v>233</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.2">
@@ -5589,10 +5602,10 @@
         <v>174</v>
       </c>
       <c r="K110" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="L110" s="7" t="s">
-        <v>196</v>
+        <v>126</v>
+      </c>
+      <c r="L110" s="6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.2">
@@ -5603,7 +5616,7 @@
         <v>243</v>
       </c>
       <c r="C111" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D111" t="s">
         <v>6</v>
@@ -5615,16 +5628,19 @@
         <v>0</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
+      </c>
+      <c r="J111" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="K111" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="L111" s="6" t="s">
-        <v>223</v>
+        <v>195</v>
+      </c>
+      <c r="L111" s="7" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.2">
@@ -5647,19 +5663,16 @@
         <v>0</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>125</v>
+        <v>36</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J112" s="3" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="K112" s="3" t="s">
-        <v>126</v>
+        <v>224</v>
       </c>
       <c r="L112" s="6" t="s">
-        <v>124</v>
+        <v>223</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.2">
@@ -5670,7 +5683,7 @@
         <v>243</v>
       </c>
       <c r="C113" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D113" t="s">
         <v>6</v>
@@ -5682,16 +5695,19 @@
         <v>0</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
+      </c>
+      <c r="J113" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="K113" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="L113" s="7" t="s">
-        <v>230</v>
+        <v>126</v>
+      </c>
+      <c r="L113" s="6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.2">
@@ -5714,19 +5730,16 @@
         <v>0</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>125</v>
+        <v>36</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J114" s="3" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="K114" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="L114" s="6" t="s">
-        <v>124</v>
+        <v>229</v>
+      </c>
+      <c r="L114" s="7" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.2">
@@ -5758,10 +5771,10 @@
         <v>174</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="L115" s="7" t="s">
-        <v>196</v>
+        <v>126</v>
+      </c>
+      <c r="L115" s="6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.2">
@@ -5784,16 +5797,19 @@
         <v>0</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>88</v>
+        <v>125</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="K116" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L116" s="6" t="s">
-        <v>87</v>
+        <v>195</v>
+      </c>
+      <c r="L116" s="7" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.2">
@@ -5804,7 +5820,7 @@
         <v>243</v>
       </c>
       <c r="C117" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D117" t="s">
         <v>6</v>
@@ -5819,13 +5835,13 @@
         <v>36</v>
       </c>
       <c r="I117" s="3" t="s">
-        <v>135</v>
+        <v>88</v>
       </c>
       <c r="K117" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="L117" s="7" t="s">
-        <v>230</v>
+        <v>95</v>
+      </c>
+      <c r="L117" s="6" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.2">
@@ -5848,19 +5864,16 @@
         <v>0</v>
       </c>
       <c r="H118" s="3" t="s">
-        <v>125</v>
+        <v>36</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J118" s="3" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="K118" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="L118" s="6" t="s">
-        <v>124</v>
+        <v>229</v>
+      </c>
+      <c r="L118" s="7" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.2">
@@ -5892,10 +5905,10 @@
         <v>174</v>
       </c>
       <c r="K119" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="L119" s="7" t="s">
-        <v>196</v>
+        <v>126</v>
+      </c>
+      <c r="L119" s="6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.2">
@@ -5918,16 +5931,19 @@
         <v>0</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>93</v>
+        <v>125</v>
+      </c>
+      <c r="J120" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="K120" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="L120" s="6" t="s">
-        <v>106</v>
+        <v>195</v>
+      </c>
+      <c r="L120" s="7" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.2">
@@ -5938,7 +5954,7 @@
         <v>243</v>
       </c>
       <c r="C121" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D121" t="s">
         <v>6</v>
@@ -5953,13 +5969,13 @@
         <v>36</v>
       </c>
       <c r="I121" s="3" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="K121" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="L121" s="7" t="s">
-        <v>230</v>
+        <v>107</v>
+      </c>
+      <c r="L121" s="6" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.2">
@@ -5982,19 +5998,16 @@
         <v>0</v>
       </c>
       <c r="H122" s="3" t="s">
-        <v>125</v>
+        <v>36</v>
       </c>
       <c r="I122" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J122" s="3" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="K122" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="L122" s="6" t="s">
-        <v>124</v>
+        <v>229</v>
+      </c>
+      <c r="L122" s="7" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.2">
@@ -6026,10 +6039,10 @@
         <v>174</v>
       </c>
       <c r="K123" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="L123" s="7" t="s">
-        <v>196</v>
+        <v>126</v>
+      </c>
+      <c r="L123" s="6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.2">
@@ -6040,7 +6053,7 @@
         <v>243</v>
       </c>
       <c r="C124" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D124" t="s">
         <v>6</v>
@@ -6052,16 +6065,19 @@
         <v>0</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
+      </c>
+      <c r="J124" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="K124" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="L124" s="6" t="s">
-        <v>223</v>
+        <v>195</v>
+      </c>
+      <c r="L124" s="7" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.2">
@@ -6084,19 +6100,16 @@
         <v>0</v>
       </c>
       <c r="H125" s="3" t="s">
-        <v>125</v>
+        <v>36</v>
       </c>
       <c r="I125" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J125" s="3" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="K125" s="3" t="s">
-        <v>126</v>
+        <v>224</v>
       </c>
       <c r="L125" s="6" t="s">
-        <v>124</v>
+        <v>223</v>
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.2">
@@ -6119,16 +6132,19 @@
         <v>0</v>
       </c>
       <c r="H126" s="3" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>88</v>
+        <v>125</v>
+      </c>
+      <c r="J126" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="K126" s="3" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="L126" s="6" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.2">
@@ -6136,28 +6152,31 @@
         <v>4</v>
       </c>
       <c r="B127" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C127" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D127" t="s">
         <v>6</v>
       </c>
+      <c r="E127" t="s">
+        <v>174</v>
+      </c>
       <c r="F127" s="3">
         <v>0</v>
       </c>
       <c r="H127" s="3" t="s">
-        <v>111</v>
+        <v>36</v>
       </c>
       <c r="I127" s="3" t="s">
-        <v>257</v>
+        <v>88</v>
       </c>
       <c r="K127" s="3" t="s">
-        <v>258</v>
+        <v>95</v>
       </c>
       <c r="L127" s="6" t="s">
-        <v>256</v>
+        <v>87</v>
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.2">
@@ -6168,7 +6187,7 @@
         <v>250</v>
       </c>
       <c r="C128" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D128" t="s">
         <v>6</v>
@@ -6180,13 +6199,13 @@
         <v>111</v>
       </c>
       <c r="I128" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="K128" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="L128" s="6" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.2">
@@ -6197,7 +6216,7 @@
         <v>250</v>
       </c>
       <c r="C129" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D129" t="s">
         <v>6</v>
@@ -6209,13 +6228,13 @@
         <v>111</v>
       </c>
       <c r="I129" s="3" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="K129" s="3" t="s">
-        <v>301</v>
+        <v>261</v>
       </c>
       <c r="L129" s="6" t="s">
-        <v>300</v>
+        <v>259</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.2">
@@ -6226,7 +6245,7 @@
         <v>250</v>
       </c>
       <c r="C130" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D130" t="s">
         <v>6</v>
@@ -6238,13 +6257,13 @@
         <v>111</v>
       </c>
       <c r="I130" s="3" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="K130" s="3" t="s">
-        <v>263</v>
+        <v>301</v>
       </c>
       <c r="L130" s="6" t="s">
-        <v>262</v>
+        <v>300</v>
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.2">
@@ -6255,7 +6274,7 @@
         <v>250</v>
       </c>
       <c r="C131" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D131" t="s">
         <v>6</v>
@@ -6267,13 +6286,13 @@
         <v>111</v>
       </c>
       <c r="I131" s="3" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="K131" s="3" t="s">
-        <v>303</v>
+        <v>263</v>
       </c>
       <c r="L131" s="6" t="s">
-        <v>302</v>
+        <v>262</v>
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.2">
@@ -6281,10 +6300,10 @@
         <v>4</v>
       </c>
       <c r="B132" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="C132" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="D132" t="s">
         <v>6</v>
@@ -6293,16 +6312,16 @@
         <v>0</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>135</v>
+        <v>257</v>
       </c>
       <c r="K132" s="3" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="L132" s="6" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.2">
@@ -6313,7 +6332,7 @@
         <v>265</v>
       </c>
       <c r="C133" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D133" t="s">
         <v>6</v>
@@ -6342,7 +6361,7 @@
         <v>265</v>
       </c>
       <c r="C134" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D134" t="s">
         <v>6</v>
@@ -6371,7 +6390,7 @@
         <v>265</v>
       </c>
       <c r="C135" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D135" t="s">
         <v>6</v>
@@ -6383,13 +6402,13 @@
         <v>36</v>
       </c>
       <c r="I135" s="3" t="s">
-        <v>36</v>
+        <v>135</v>
       </c>
       <c r="K135" s="3" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="L135" s="6" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.2">
@@ -6400,7 +6419,7 @@
         <v>265</v>
       </c>
       <c r="C136" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D136" t="s">
         <v>6</v>
@@ -6429,20 +6448,26 @@
         <v>265</v>
       </c>
       <c r="C137" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D137" t="s">
         <v>6</v>
       </c>
-      <c r="F137" s="8">
-        <v>0</v>
-      </c>
-      <c r="G137" s="8"/>
-      <c r="H137" s="8"/>
-      <c r="I137" s="8"/>
-      <c r="J137" s="8"/>
-      <c r="K137" s="8"/>
-      <c r="L137" s="9"/>
+      <c r="F137" s="3">
+        <v>0</v>
+      </c>
+      <c r="H137" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I137" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K137" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="L137" s="6" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
@@ -6452,7 +6477,7 @@
         <v>265</v>
       </c>
       <c r="C138" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D138" t="s">
         <v>6</v>
@@ -6475,26 +6500,20 @@
         <v>265</v>
       </c>
       <c r="C139" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D139" t="s">
         <v>6</v>
       </c>
-      <c r="F139" s="3">
-        <v>0</v>
-      </c>
-      <c r="H139" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I139" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="K139" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="L139" s="6" t="s">
-        <v>297</v>
-      </c>
+      <c r="F139" s="8">
+        <v>0</v>
+      </c>
+      <c r="G139" s="8"/>
+      <c r="H139" s="8"/>
+      <c r="I139" s="8"/>
+      <c r="J139" s="8"/>
+      <c r="K139" s="8"/>
+      <c r="L139" s="9"/>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
@@ -6504,7 +6523,7 @@
         <v>265</v>
       </c>
       <c r="C140" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D140" t="s">
         <v>6</v>
@@ -6516,13 +6535,13 @@
         <v>36</v>
       </c>
       <c r="I140" s="3" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="L140" s="6" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.2">
@@ -6533,7 +6552,7 @@
         <v>265</v>
       </c>
       <c r="C141" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D141" t="s">
         <v>6</v>
@@ -6548,10 +6567,10 @@
         <v>135</v>
       </c>
       <c r="K141" s="3" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="L141" s="6" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.2">
@@ -6562,7 +6581,7 @@
         <v>265</v>
       </c>
       <c r="C142" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D142" t="s">
         <v>6</v>
@@ -6591,7 +6610,7 @@
         <v>265</v>
       </c>
       <c r="C143" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="D143" t="s">
         <v>6</v>
@@ -6620,20 +6639,26 @@
         <v>265</v>
       </c>
       <c r="C144" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="D144" t="s">
         <v>6</v>
       </c>
-      <c r="F144" s="8">
-        <v>0</v>
-      </c>
-      <c r="G144" s="8"/>
-      <c r="H144" s="8"/>
-      <c r="I144" s="8"/>
-      <c r="J144" s="8"/>
-      <c r="K144" s="8"/>
-      <c r="L144" s="9"/>
+      <c r="F144" s="3">
+        <v>0</v>
+      </c>
+      <c r="H144" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I144" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K144" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="L144" s="6" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
@@ -6643,7 +6668,7 @@
         <v>265</v>
       </c>
       <c r="C145" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D145" t="s">
         <v>6</v>
@@ -6666,7 +6691,7 @@
         <v>265</v>
       </c>
       <c r="C146" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D146" t="s">
         <v>6</v>
@@ -6689,7 +6714,7 @@
         <v>265</v>
       </c>
       <c r="C147" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D147" t="s">
         <v>6</v>
@@ -6712,26 +6737,20 @@
         <v>265</v>
       </c>
       <c r="C148" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D148" t="s">
         <v>6</v>
       </c>
-      <c r="F148" s="3">
-        <v>0</v>
-      </c>
-      <c r="H148" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I148" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K148" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="L148" s="6" t="s">
-        <v>291</v>
-      </c>
+      <c r="F148" s="8">
+        <v>0</v>
+      </c>
+      <c r="G148" s="8"/>
+      <c r="H148" s="8"/>
+      <c r="I148" s="8"/>
+      <c r="J148" s="8"/>
+      <c r="K148" s="8"/>
+      <c r="L148" s="9"/>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
@@ -6741,7 +6760,7 @@
         <v>265</v>
       </c>
       <c r="C149" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D149" t="s">
         <v>6</v>
@@ -6770,7 +6789,7 @@
         <v>265</v>
       </c>
       <c r="C150" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D150" t="s">
         <v>6</v>
@@ -6799,20 +6818,26 @@
         <v>265</v>
       </c>
       <c r="C151" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D151" t="s">
         <v>6</v>
       </c>
-      <c r="F151" s="8">
-        <v>0</v>
-      </c>
-      <c r="G151" s="8"/>
-      <c r="H151" s="8"/>
-      <c r="I151" s="8"/>
-      <c r="J151" s="8"/>
-      <c r="K151" s="8"/>
-      <c r="L151" s="9"/>
+      <c r="F151" s="3">
+        <v>0</v>
+      </c>
+      <c r="H151" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I151" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K151" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="L151" s="6" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
@@ -6822,26 +6847,20 @@
         <v>265</v>
       </c>
       <c r="C152" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D152" t="s">
         <v>6</v>
       </c>
-      <c r="F152" s="3">
-        <v>0</v>
-      </c>
-      <c r="H152" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I152" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K152" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="L152" s="6" t="s">
-        <v>291</v>
-      </c>
+      <c r="F152" s="8">
+        <v>0</v>
+      </c>
+      <c r="G152" s="8"/>
+      <c r="H152" s="8"/>
+      <c r="I152" s="8"/>
+      <c r="J152" s="8"/>
+      <c r="K152" s="8"/>
+      <c r="L152" s="9"/>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
@@ -6851,7 +6870,7 @@
         <v>265</v>
       </c>
       <c r="C153" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D153" t="s">
         <v>6</v>
@@ -6880,7 +6899,7 @@
         <v>265</v>
       </c>
       <c r="C154" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D154" t="s">
         <v>6</v>
@@ -6903,34 +6922,31 @@
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>401</v>
+        <v>4</v>
       </c>
       <c r="B155" t="s">
-        <v>405</v>
+        <v>265</v>
       </c>
       <c r="C155" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="D155" t="s">
-        <v>388</v>
+        <v>6</v>
       </c>
       <c r="F155" s="3">
-        <v>19</v>
-      </c>
-      <c r="G155" s="3" t="s">
-        <v>174</v>
+        <v>0</v>
       </c>
       <c r="H155" s="3" t="s">
-        <v>391</v>
+        <v>36</v>
       </c>
       <c r="I155" s="3" t="s">
-        <v>406</v>
+        <v>135</v>
       </c>
       <c r="K155" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="L155" s="7" t="s">
-        <v>408</v>
+        <v>292</v>
+      </c>
+      <c r="L155" s="6" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.2">
@@ -6941,13 +6957,13 @@
         <v>405</v>
       </c>
       <c r="C156" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D156" t="s">
         <v>388</v>
       </c>
       <c r="F156" s="3">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G156" s="3" t="s">
         <v>174</v>
@@ -6967,24 +6983,35 @@
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B157" t="s">
         <v>405</v>
       </c>
       <c r="C157" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D157" t="s">
         <v>388</v>
       </c>
-      <c r="F157" s="8"/>
-      <c r="G157" s="8"/>
-      <c r="H157" s="8"/>
-      <c r="I157" s="8"/>
-      <c r="J157" s="8"/>
-      <c r="K157" s="8"/>
-      <c r="L157" s="9"/>
+      <c r="F157" s="3">
+        <v>0</v>
+      </c>
+      <c r="G157" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H157" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I157" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="K157" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="L157" s="7" t="s">
+        <v>408</v>
+      </c>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
@@ -6994,29 +7021,18 @@
         <v>405</v>
       </c>
       <c r="C158" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D158" t="s">
         <v>388</v>
       </c>
-      <c r="F158" s="3">
-        <v>2</v>
-      </c>
-      <c r="G158" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="H158" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="I158" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="K158" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="L158" s="6" t="s">
-        <v>400</v>
-      </c>
+      <c r="F158" s="8"/>
+      <c r="G158" s="8"/>
+      <c r="H158" s="8"/>
+      <c r="I158" s="8"/>
+      <c r="J158" s="8"/>
+      <c r="K158" s="8"/>
+      <c r="L158" s="9"/>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
@@ -7026,13 +7042,13 @@
         <v>405</v>
       </c>
       <c r="C159" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D159" t="s">
         <v>388</v>
       </c>
       <c r="F159" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G159" s="3" t="s">
         <v>174</v>
@@ -7041,13 +7057,13 @@
         <v>391</v>
       </c>
       <c r="I159" s="3" t="s">
-        <v>487</v>
+        <v>392</v>
       </c>
       <c r="K159" s="3" t="s">
-        <v>567</v>
-      </c>
-      <c r="L159" s="7" t="s">
-        <v>566</v>
+        <v>393</v>
+      </c>
+      <c r="L159" s="6" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.2">
@@ -7058,13 +7074,13 @@
         <v>405</v>
       </c>
       <c r="C160" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D160" t="s">
         <v>388</v>
       </c>
       <c r="F160" s="3">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G160" s="3" t="s">
         <v>174</v>
@@ -7073,13 +7089,13 @@
         <v>391</v>
       </c>
       <c r="I160" s="3" t="s">
-        <v>429</v>
+        <v>487</v>
       </c>
       <c r="K160" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="L160" s="6" t="s">
-        <v>464</v>
+        <v>567</v>
+      </c>
+      <c r="L160" s="7" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.2">
@@ -7090,13 +7106,13 @@
         <v>405</v>
       </c>
       <c r="C161" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D161" t="s">
         <v>388</v>
       </c>
       <c r="F161" s="3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G161" s="3" t="s">
         <v>174</v>
@@ -7122,7 +7138,7 @@
         <v>405</v>
       </c>
       <c r="C162" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D162" t="s">
         <v>388</v>
@@ -7154,7 +7170,7 @@
         <v>405</v>
       </c>
       <c r="C163" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D163" t="s">
         <v>388</v>
@@ -7186,7 +7202,7 @@
         <v>405</v>
       </c>
       <c r="C164" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D164" t="s">
         <v>388</v>
@@ -7218,7 +7234,7 @@
         <v>405</v>
       </c>
       <c r="C165" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D165" t="s">
         <v>388</v>
@@ -7250,13 +7266,13 @@
         <v>405</v>
       </c>
       <c r="C166" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D166" t="s">
         <v>388</v>
       </c>
       <c r="F166" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G166" s="3" t="s">
         <v>174</v>
@@ -7265,13 +7281,13 @@
         <v>391</v>
       </c>
       <c r="I166" s="3" t="s">
-        <v>487</v>
+        <v>429</v>
       </c>
       <c r="K166" s="3" t="s">
-        <v>486</v>
+        <v>465</v>
       </c>
       <c r="L166" s="6" t="s">
-        <v>485</v>
+        <v>464</v>
       </c>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.2">
@@ -7282,13 +7298,13 @@
         <v>405</v>
       </c>
       <c r="C167" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D167" t="s">
         <v>388</v>
       </c>
       <c r="F167" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G167" s="3" t="s">
         <v>174</v>
@@ -7297,13 +7313,13 @@
         <v>391</v>
       </c>
       <c r="I167" s="3" t="s">
-        <v>429</v>
+        <v>487</v>
       </c>
       <c r="K167" s="3" t="s">
-        <v>428</v>
+        <v>486</v>
       </c>
       <c r="L167" s="6" t="s">
-        <v>427</v>
+        <v>485</v>
       </c>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.2">
@@ -7314,13 +7330,13 @@
         <v>405</v>
       </c>
       <c r="C168" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D168" t="s">
         <v>388</v>
       </c>
       <c r="F168" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G168" s="3" t="s">
         <v>174</v>
@@ -7346,7 +7362,7 @@
         <v>405</v>
       </c>
       <c r="C169" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D169" t="s">
         <v>388</v>
@@ -7378,7 +7394,7 @@
         <v>405</v>
       </c>
       <c r="C170" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D170" t="s">
         <v>388</v>
@@ -7410,7 +7426,7 @@
         <v>405</v>
       </c>
       <c r="C171" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D171" t="s">
         <v>388</v>
@@ -7442,13 +7458,13 @@
         <v>405</v>
       </c>
       <c r="C172" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D172" t="s">
         <v>388</v>
       </c>
       <c r="F172" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G172" s="3" t="s">
         <v>174</v>
@@ -7457,13 +7473,13 @@
         <v>391</v>
       </c>
       <c r="I172" s="3" t="s">
-        <v>460</v>
+        <v>429</v>
       </c>
       <c r="K172" s="3" t="s">
-        <v>459</v>
+        <v>428</v>
       </c>
       <c r="L172" s="6" t="s">
-        <v>458</v>
+        <v>427</v>
       </c>
     </row>
     <row r="173" spans="1:12" x14ac:dyDescent="0.2">
@@ -7474,18 +7490,29 @@
         <v>405</v>
       </c>
       <c r="C173" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D173" t="s">
         <v>388</v>
       </c>
-      <c r="F173" s="8"/>
-      <c r="G173" s="8"/>
-      <c r="H173" s="8"/>
-      <c r="I173" s="8"/>
-      <c r="J173" s="8"/>
-      <c r="K173" s="8"/>
-      <c r="L173" s="9"/>
+      <c r="F173" s="3">
+        <v>1</v>
+      </c>
+      <c r="G173" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H173" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I173" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K173" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="L173" s="6" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
@@ -7495,29 +7522,18 @@
         <v>405</v>
       </c>
       <c r="C174" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D174" t="s">
         <v>388</v>
       </c>
-      <c r="F174" s="3">
-        <v>2</v>
-      </c>
-      <c r="G174" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="H174" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="I174" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="K174" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="L174" s="6" t="s">
-        <v>436</v>
-      </c>
+      <c r="F174" s="8"/>
+      <c r="G174" s="8"/>
+      <c r="H174" s="8"/>
+      <c r="I174" s="8"/>
+      <c r="J174" s="8"/>
+      <c r="K174" s="8"/>
+      <c r="L174" s="9"/>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
@@ -7527,13 +7543,13 @@
         <v>405</v>
       </c>
       <c r="C175" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D175" t="s">
         <v>388</v>
       </c>
       <c r="F175" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G175" s="3" t="s">
         <v>174</v>
@@ -7542,13 +7558,13 @@
         <v>391</v>
       </c>
       <c r="I175" s="3" t="s">
-        <v>562</v>
+        <v>438</v>
       </c>
       <c r="K175" s="3" t="s">
-        <v>563</v>
-      </c>
-      <c r="L175" s="7" t="s">
-        <v>564</v>
+        <v>437</v>
+      </c>
+      <c r="L175" s="6" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.2">
@@ -7559,28 +7575,28 @@
         <v>405</v>
       </c>
       <c r="C176" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D176" t="s">
         <v>388</v>
       </c>
-      <c r="F176" s="11">
-        <v>5</v>
+      <c r="F176" s="3">
+        <v>1</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H176" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I176" s="3" t="s">
-        <v>484</v>
+        <v>562</v>
       </c>
       <c r="K176" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="L176" s="6" t="s">
-        <v>482</v>
+        <v>563</v>
+      </c>
+      <c r="L176" s="7" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.2">
@@ -7591,16 +7607,16 @@
         <v>405</v>
       </c>
       <c r="C177" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D177" t="s">
         <v>388</v>
       </c>
-      <c r="F177" s="3">
+      <c r="F177" s="11">
         <v>5</v>
       </c>
       <c r="G177" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H177" s="3" t="s">
         <v>391</v>
@@ -7609,10 +7625,10 @@
         <v>484</v>
       </c>
       <c r="K177" s="3" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="L177" s="6" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="178" spans="1:12" x14ac:dyDescent="0.2">
@@ -7623,13 +7639,13 @@
         <v>405</v>
       </c>
       <c r="C178" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D178" t="s">
         <v>388</v>
       </c>
       <c r="F178" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G178" s="3" t="s">
         <v>174</v>
@@ -7638,13 +7654,13 @@
         <v>391</v>
       </c>
       <c r="I178" s="3" t="s">
-        <v>531</v>
+        <v>484</v>
       </c>
       <c r="K178" s="3" t="s">
-        <v>530</v>
+        <v>481</v>
       </c>
       <c r="L178" s="6" t="s">
-        <v>529</v>
+        <v>480</v>
       </c>
     </row>
     <row r="179" spans="1:12" x14ac:dyDescent="0.2">
@@ -7655,13 +7671,13 @@
         <v>405</v>
       </c>
       <c r="C179" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D179" t="s">
         <v>388</v>
       </c>
       <c r="F179" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G179" s="3" t="s">
         <v>174</v>
@@ -7670,13 +7686,13 @@
         <v>391</v>
       </c>
       <c r="I179" s="3" t="s">
-        <v>544</v>
+        <v>531</v>
       </c>
       <c r="K179" s="3" t="s">
-        <v>543</v>
+        <v>530</v>
       </c>
       <c r="L179" s="6" t="s">
-        <v>542</v>
+        <v>529</v>
       </c>
     </row>
     <row r="180" spans="1:12" x14ac:dyDescent="0.2">
@@ -7687,13 +7703,13 @@
         <v>405</v>
       </c>
       <c r="C180" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D180" t="s">
         <v>388</v>
       </c>
       <c r="F180" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G180" s="3" t="s">
         <v>174</v>
@@ -7702,13 +7718,13 @@
         <v>391</v>
       </c>
       <c r="I180" s="3" t="s">
-        <v>449</v>
+        <v>544</v>
       </c>
       <c r="K180" s="3" t="s">
-        <v>448</v>
+        <v>543</v>
       </c>
       <c r="L180" s="6" t="s">
-        <v>447</v>
+        <v>542</v>
       </c>
     </row>
     <row r="181" spans="1:12" x14ac:dyDescent="0.2">
@@ -7719,13 +7735,13 @@
         <v>405</v>
       </c>
       <c r="C181" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D181" t="s">
         <v>388</v>
       </c>
       <c r="F181" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G181" s="3" t="s">
         <v>174</v>
@@ -7734,30 +7750,30 @@
         <v>391</v>
       </c>
       <c r="I181" s="3" t="s">
-        <v>547</v>
+        <v>449</v>
       </c>
       <c r="K181" s="3" t="s">
-        <v>546</v>
+        <v>448</v>
       </c>
       <c r="L181" s="6" t="s">
-        <v>545</v>
+        <v>447</v>
       </c>
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B182" t="s">
         <v>405</v>
       </c>
       <c r="C182" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D182" t="s">
         <v>388</v>
       </c>
       <c r="F182" s="3">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G182" s="3" t="s">
         <v>174</v>
@@ -7766,30 +7782,30 @@
         <v>391</v>
       </c>
       <c r="I182" s="3" t="s">
-        <v>457</v>
+        <v>547</v>
       </c>
       <c r="K182" s="3" t="s">
-        <v>456</v>
+        <v>546</v>
       </c>
       <c r="L182" s="6" t="s">
-        <v>455</v>
+        <v>545</v>
       </c>
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B183" t="s">
         <v>405</v>
       </c>
       <c r="C183" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D183" t="s">
         <v>388</v>
       </c>
       <c r="F183" s="3">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G183" s="3" t="s">
         <v>174</v>
@@ -7798,13 +7814,13 @@
         <v>391</v>
       </c>
       <c r="I183" s="3" t="s">
-        <v>487</v>
+        <v>457</v>
       </c>
       <c r="K183" s="3" t="s">
-        <v>496</v>
+        <v>456</v>
       </c>
       <c r="L183" s="6" t="s">
-        <v>495</v>
+        <v>455</v>
       </c>
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.2">
@@ -7815,7 +7831,7 @@
         <v>405</v>
       </c>
       <c r="C184" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D184" t="s">
         <v>388</v>
@@ -7833,10 +7849,10 @@
         <v>487</v>
       </c>
       <c r="K184" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L184" s="6" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.2">
@@ -7847,7 +7863,7 @@
         <v>405</v>
       </c>
       <c r="C185" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D185" t="s">
         <v>388</v>
@@ -7862,13 +7878,13 @@
         <v>391</v>
       </c>
       <c r="I185" s="3" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="K185" s="3" t="s">
-        <v>514</v>
+        <v>497</v>
       </c>
       <c r="L185" s="6" t="s">
-        <v>513</v>
+        <v>498</v>
       </c>
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.2">
@@ -7879,28 +7895,28 @@
         <v>405</v>
       </c>
       <c r="C186" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D186" t="s">
         <v>388</v>
       </c>
-      <c r="F186" s="11">
-        <v>3</v>
+      <c r="F186" s="3">
+        <v>1</v>
       </c>
       <c r="G186" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H186" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I186" s="3" t="s">
-        <v>522</v>
+        <v>501</v>
       </c>
       <c r="K186" s="3" t="s">
-        <v>549</v>
+        <v>514</v>
       </c>
       <c r="L186" s="6" t="s">
-        <v>548</v>
+        <v>513</v>
       </c>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.2">
@@ -7911,28 +7927,28 @@
         <v>405</v>
       </c>
       <c r="C187" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D187" t="s">
         <v>388</v>
       </c>
-      <c r="F187" s="3">
+      <c r="F187" s="11">
         <v>3</v>
       </c>
       <c r="G187" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H187" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I187" s="3" t="s">
-        <v>479</v>
+        <v>522</v>
       </c>
       <c r="K187" s="3" t="s">
-        <v>478</v>
+        <v>549</v>
       </c>
       <c r="L187" s="6" t="s">
-        <v>477</v>
+        <v>548</v>
       </c>
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.2">
@@ -7943,13 +7959,13 @@
         <v>405</v>
       </c>
       <c r="C188" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D188" t="s">
         <v>388</v>
       </c>
       <c r="F188" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G188" s="3" t="s">
         <v>174</v>
@@ -7958,13 +7974,13 @@
         <v>391</v>
       </c>
       <c r="I188" s="3" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="K188" s="3" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="L188" s="6" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.2">
@@ -7975,13 +7991,13 @@
         <v>405</v>
       </c>
       <c r="C189" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D189" t="s">
         <v>388</v>
       </c>
       <c r="F189" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G189" s="3" t="s">
         <v>174</v>
@@ -8007,13 +8023,13 @@
         <v>405</v>
       </c>
       <c r="C190" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D190" t="s">
         <v>388</v>
       </c>
       <c r="F190" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G190" s="3" t="s">
         <v>174</v>
@@ -8022,13 +8038,13 @@
         <v>391</v>
       </c>
       <c r="I190" s="3" t="s">
-        <v>422</v>
+        <v>474</v>
       </c>
       <c r="K190" s="3" t="s">
-        <v>425</v>
+        <v>473</v>
       </c>
       <c r="L190" s="6" t="s">
-        <v>423</v>
+        <v>472</v>
       </c>
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.2">
@@ -8039,7 +8055,7 @@
         <v>405</v>
       </c>
       <c r="C191" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D191" t="s">
         <v>388</v>
@@ -8057,10 +8073,10 @@
         <v>422</v>
       </c>
       <c r="K191" s="3" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="L191" s="6" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.2">
@@ -8071,7 +8087,7 @@
         <v>405</v>
       </c>
       <c r="C192" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D192" t="s">
         <v>388</v>
@@ -8089,10 +8105,10 @@
         <v>422</v>
       </c>
       <c r="K192" s="3" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="L192" s="6" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.2">
@@ -8103,13 +8119,13 @@
         <v>405</v>
       </c>
       <c r="C193" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D193" t="s">
         <v>388</v>
       </c>
       <c r="F193" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G193" s="3" t="s">
         <v>174</v>
@@ -8118,13 +8134,13 @@
         <v>391</v>
       </c>
       <c r="I193" s="3" t="s">
-        <v>565</v>
+        <v>422</v>
       </c>
       <c r="K193" s="3" t="s">
-        <v>569</v>
-      </c>
-      <c r="L193" s="7" t="s">
-        <v>568</v>
+        <v>424</v>
+      </c>
+      <c r="L193" s="6" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.2">
@@ -8135,28 +8151,28 @@
         <v>405</v>
       </c>
       <c r="C194" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D194" t="s">
         <v>388</v>
       </c>
-      <c r="F194" s="11">
-        <v>2</v>
+      <c r="F194" s="3">
+        <v>1</v>
       </c>
       <c r="G194" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H194" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I194" s="3" t="s">
-        <v>540</v>
+        <v>565</v>
       </c>
       <c r="K194" s="3" t="s">
-        <v>539</v>
-      </c>
-      <c r="L194" s="6" t="s">
-        <v>538</v>
+        <v>569</v>
+      </c>
+      <c r="L194" s="7" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.2">
@@ -8167,13 +8183,13 @@
         <v>405</v>
       </c>
       <c r="C195" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D195" t="s">
         <v>388</v>
       </c>
       <c r="F195" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G195" s="3" t="s">
         <v>432</v>
@@ -8182,13 +8198,13 @@
         <v>391</v>
       </c>
       <c r="I195" s="3" t="s">
-        <v>479</v>
+        <v>540</v>
       </c>
       <c r="K195" s="3" t="s">
         <v>539</v>
       </c>
       <c r="L195" s="6" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.2">
@@ -8199,13 +8215,13 @@
         <v>405</v>
       </c>
       <c r="C196" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D196" t="s">
         <v>388</v>
       </c>
       <c r="F196" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G196" s="3" t="s">
         <v>432</v>
@@ -8214,13 +8230,13 @@
         <v>391</v>
       </c>
       <c r="I196" s="3" t="s">
-        <v>511</v>
+        <v>479</v>
       </c>
       <c r="K196" s="3" t="s">
-        <v>512</v>
+        <v>539</v>
       </c>
       <c r="L196" s="6" t="s">
-        <v>510</v>
+        <v>541</v>
       </c>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.2">
@@ -8231,13 +8247,13 @@
         <v>405</v>
       </c>
       <c r="C197" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D197" t="s">
         <v>388</v>
       </c>
       <c r="F197" s="11">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G197" s="3" t="s">
         <v>432</v>
@@ -8246,13 +8262,13 @@
         <v>391</v>
       </c>
       <c r="I197" s="3" t="s">
-        <v>528</v>
+        <v>511</v>
       </c>
       <c r="K197" s="3" t="s">
-        <v>527</v>
+        <v>512</v>
       </c>
       <c r="L197" s="6" t="s">
-        <v>526</v>
+        <v>510</v>
       </c>
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.2">
@@ -8263,28 +8279,28 @@
         <v>405</v>
       </c>
       <c r="C198" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D198" t="s">
         <v>388</v>
       </c>
-      <c r="F198" s="3">
-        <v>2</v>
+      <c r="F198" s="11">
+        <v>10</v>
       </c>
       <c r="G198" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H198" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I198" s="3" t="s">
-        <v>396</v>
+        <v>528</v>
       </c>
       <c r="K198" s="3" t="s">
-        <v>395</v>
+        <v>527</v>
       </c>
       <c r="L198" s="6" t="s">
-        <v>394</v>
+        <v>526</v>
       </c>
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.2">
@@ -8295,13 +8311,13 @@
         <v>405</v>
       </c>
       <c r="C199" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D199" t="s">
         <v>388</v>
       </c>
       <c r="F199" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G199" s="3" t="s">
         <v>174</v>
@@ -8310,13 +8326,13 @@
         <v>391</v>
       </c>
       <c r="I199" s="3" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="K199" s="3" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
       <c r="L199" s="6" t="s">
-        <v>415</v>
+        <v>394</v>
       </c>
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.2">
@@ -8327,13 +8343,13 @@
         <v>405</v>
       </c>
       <c r="C200" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D200" t="s">
         <v>388</v>
       </c>
       <c r="F200" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G200" s="3" t="s">
         <v>174</v>
@@ -8342,13 +8358,13 @@
         <v>391</v>
       </c>
       <c r="I200" s="3" t="s">
-        <v>397</v>
+        <v>411</v>
       </c>
       <c r="K200" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="L200" s="7" t="s">
-        <v>399</v>
+        <v>416</v>
+      </c>
+      <c r="L200" s="6" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.2">
@@ -8358,29 +8374,29 @@
       <c r="B201" t="s">
         <v>405</v>
       </c>
-      <c r="C201" s="13" t="s">
-        <v>590</v>
+      <c r="C201" t="s">
+        <v>349</v>
       </c>
       <c r="D201" t="s">
         <v>388</v>
       </c>
       <c r="F201" s="3">
-        <v>1</v>
-      </c>
-      <c r="G201" s="12" t="s">
-        <v>432</v>
+        <v>2</v>
+      </c>
+      <c r="G201" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="H201" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I201" s="3" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="K201" s="3" t="s">
-        <v>588</v>
+        <v>398</v>
       </c>
       <c r="L201" s="7" t="s">
-        <v>589</v>
+        <v>399</v>
       </c>
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.2">
@@ -8390,8 +8406,8 @@
       <c r="B202" t="s">
         <v>405</v>
       </c>
-      <c r="C202" s="13" t="s">
-        <v>591</v>
+      <c r="C202" s="12" t="s">
+        <v>590</v>
       </c>
       <c r="D202" t="s">
         <v>388</v>
@@ -8399,20 +8415,20 @@
       <c r="F202" s="3">
         <v>1</v>
       </c>
-      <c r="G202" s="12" t="s">
+      <c r="G202" s="3" t="s">
         <v>432</v>
       </c>
       <c r="H202" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I202" s="3" t="s">
-        <v>594</v>
+        <v>392</v>
       </c>
       <c r="K202" s="3" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="L202" s="7" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="203" spans="1:12" x14ac:dyDescent="0.2">
@@ -8422,8 +8438,8 @@
       <c r="B203" t="s">
         <v>405</v>
       </c>
-      <c r="C203" t="s">
-        <v>350</v>
+      <c r="C203" s="12" t="s">
+        <v>591</v>
       </c>
       <c r="D203" t="s">
         <v>388</v>
@@ -8432,19 +8448,19 @@
         <v>1</v>
       </c>
       <c r="G203" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H203" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I203" s="3" t="s">
-        <v>411</v>
+        <v>594</v>
       </c>
       <c r="K203" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="L203" s="6" t="s">
-        <v>409</v>
+        <v>593</v>
+      </c>
+      <c r="L203" s="7" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.2">
@@ -8455,28 +8471,28 @@
         <v>405</v>
       </c>
       <c r="C204" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D204" t="s">
         <v>388</v>
       </c>
-      <c r="F204" s="11">
-        <v>2</v>
+      <c r="F204" s="3">
+        <v>1</v>
       </c>
       <c r="G204" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H204" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I204" s="3" t="s">
-        <v>552</v>
+        <v>411</v>
       </c>
       <c r="K204" s="3" t="s">
-        <v>551</v>
+        <v>410</v>
       </c>
       <c r="L204" s="6" t="s">
-        <v>550</v>
+        <v>409</v>
       </c>
     </row>
     <row r="205" spans="1:12" x14ac:dyDescent="0.2">
@@ -8487,28 +8503,28 @@
         <v>405</v>
       </c>
       <c r="C205" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D205" t="s">
         <v>388</v>
       </c>
-      <c r="F205" s="3">
+      <c r="F205" s="11">
         <v>2</v>
       </c>
       <c r="G205" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H205" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I205" s="3" t="s">
-        <v>501</v>
+        <v>552</v>
       </c>
       <c r="K205" s="3" t="s">
-        <v>503</v>
+        <v>551</v>
       </c>
       <c r="L205" s="6" t="s">
-        <v>502</v>
+        <v>550</v>
       </c>
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.2">
@@ -8518,29 +8534,30 @@
       <c r="B206" t="s">
         <v>405</v>
       </c>
-      <c r="C206" t="s">
-        <v>353</v>
-      </c>
-      <c r="D206" t="s">
+      <c r="C206" s="12" t="s">
+        <v>595</v>
+      </c>
+      <c r="D206" s="13" t="s">
         <v>388</v>
       </c>
-      <c r="F206" s="3">
-        <v>2</v>
+      <c r="E206" s="13"/>
+      <c r="F206" s="14">
+        <v>1</v>
       </c>
       <c r="G206" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H206" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I206" s="3" t="s">
-        <v>537</v>
+        <v>487</v>
       </c>
       <c r="K206" s="3" t="s">
-        <v>536</v>
+        <v>596</v>
       </c>
       <c r="L206" s="6" t="s">
-        <v>535</v>
+        <v>597</v>
       </c>
     </row>
     <row r="207" spans="1:12" x14ac:dyDescent="0.2">
@@ -8551,13 +8568,13 @@
         <v>405</v>
       </c>
       <c r="C207" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D207" t="s">
         <v>388</v>
       </c>
       <c r="F207" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G207" s="3" t="s">
         <v>174</v>
@@ -8566,13 +8583,13 @@
         <v>391</v>
       </c>
       <c r="I207" s="3" t="s">
-        <v>537</v>
+        <v>501</v>
       </c>
       <c r="K207" s="3" t="s">
-        <v>536</v>
+        <v>503</v>
       </c>
       <c r="L207" s="6" t="s">
-        <v>535</v>
+        <v>502</v>
       </c>
     </row>
     <row r="208" spans="1:12" x14ac:dyDescent="0.2">
@@ -8583,13 +8600,13 @@
         <v>405</v>
       </c>
       <c r="C208" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D208" t="s">
         <v>388</v>
       </c>
       <c r="F208" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G208" s="3" t="s">
         <v>174</v>
@@ -8598,13 +8615,13 @@
         <v>391</v>
       </c>
       <c r="I208" s="3" t="s">
-        <v>509</v>
+        <v>537</v>
       </c>
       <c r="K208" s="3" t="s">
-        <v>508</v>
+        <v>536</v>
       </c>
       <c r="L208" s="6" t="s">
-        <v>507</v>
+        <v>535</v>
       </c>
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.2">
@@ -8615,13 +8632,13 @@
         <v>405</v>
       </c>
       <c r="C209" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D209" t="s">
         <v>388</v>
       </c>
       <c r="F209" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G209" s="3" t="s">
         <v>174</v>
@@ -8630,13 +8647,13 @@
         <v>391</v>
       </c>
       <c r="I209" s="3" t="s">
-        <v>522</v>
+        <v>537</v>
       </c>
       <c r="K209" s="3" t="s">
-        <v>521</v>
+        <v>536</v>
       </c>
       <c r="L209" s="6" t="s">
-        <v>520</v>
+        <v>535</v>
       </c>
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.2">
@@ -8647,13 +8664,13 @@
         <v>405</v>
       </c>
       <c r="C210" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D210" t="s">
         <v>388</v>
       </c>
       <c r="F210" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G210" s="3" t="s">
         <v>174</v>
@@ -8662,13 +8679,13 @@
         <v>391</v>
       </c>
       <c r="I210" s="3" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="K210" s="3" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="L210" s="6" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.2">
@@ -8679,13 +8696,13 @@
         <v>405</v>
       </c>
       <c r="C211" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D211" t="s">
         <v>388</v>
       </c>
       <c r="F211" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G211" s="3" t="s">
         <v>174</v>
@@ -8694,13 +8711,13 @@
         <v>391</v>
       </c>
       <c r="I211" s="3" t="s">
-        <v>534</v>
+        <v>522</v>
       </c>
       <c r="K211" s="3" t="s">
-        <v>533</v>
+        <v>521</v>
       </c>
       <c r="L211" s="6" t="s">
-        <v>532</v>
+        <v>520</v>
       </c>
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.2">
@@ -8711,7 +8728,7 @@
         <v>405</v>
       </c>
       <c r="C212" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D212" t="s">
         <v>388</v>
@@ -8726,13 +8743,13 @@
         <v>391</v>
       </c>
       <c r="I212" s="3" t="s">
-        <v>501</v>
+        <v>519</v>
       </c>
       <c r="K212" s="3" t="s">
-        <v>500</v>
+        <v>518</v>
       </c>
       <c r="L212" s="6" t="s">
-        <v>499</v>
+        <v>517</v>
       </c>
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.2">
@@ -8743,13 +8760,13 @@
         <v>405</v>
       </c>
       <c r="C213" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D213" t="s">
         <v>388</v>
       </c>
       <c r="F213" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G213" s="3" t="s">
         <v>174</v>
@@ -8758,13 +8775,13 @@
         <v>391</v>
       </c>
       <c r="I213" s="3" t="s">
-        <v>501</v>
+        <v>534</v>
       </c>
       <c r="K213" s="3" t="s">
-        <v>500</v>
+        <v>533</v>
       </c>
       <c r="L213" s="6" t="s">
-        <v>499</v>
+        <v>532</v>
       </c>
     </row>
     <row r="214" spans="1:12" x14ac:dyDescent="0.2">
@@ -8775,13 +8792,13 @@
         <v>405</v>
       </c>
       <c r="C214" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D214" t="s">
         <v>388</v>
       </c>
       <c r="F214" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G214" s="3" t="s">
         <v>174</v>
@@ -8807,7 +8824,7 @@
         <v>405</v>
       </c>
       <c r="C215" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D215" t="s">
         <v>388</v>
@@ -8839,13 +8856,13 @@
         <v>405</v>
       </c>
       <c r="C216" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D216" t="s">
         <v>388</v>
       </c>
       <c r="F216" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G216" s="3" t="s">
         <v>174</v>
@@ -8854,13 +8871,13 @@
         <v>391</v>
       </c>
       <c r="I216" s="3" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="K216" s="3" t="s">
-        <v>491</v>
+        <v>500</v>
       </c>
       <c r="L216" s="6" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.2">
@@ -8871,7 +8888,7 @@
         <v>405</v>
       </c>
       <c r="C217" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D217" t="s">
         <v>388</v>
@@ -8886,13 +8903,13 @@
         <v>391</v>
       </c>
       <c r="I217" s="3" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="K217" s="3" t="s">
-        <v>491</v>
+        <v>500</v>
       </c>
       <c r="L217" s="6" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.2">
@@ -8903,28 +8920,28 @@
         <v>405</v>
       </c>
       <c r="C218" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D218" t="s">
         <v>388</v>
       </c>
-      <c r="F218" s="11">
-        <v>5</v>
+      <c r="F218" s="3">
+        <v>2</v>
       </c>
       <c r="G218" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H218" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I218" s="3" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="K218" s="3" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="L218" s="6" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.2">
@@ -8934,29 +8951,29 @@
       <c r="B219" t="s">
         <v>405</v>
       </c>
-      <c r="C219" s="9" t="s">
-        <v>576</v>
+      <c r="C219" t="s">
+        <v>364</v>
       </c>
       <c r="D219" t="s">
         <v>388</v>
       </c>
       <c r="F219" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G219" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H219" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I219" s="3" t="s">
-        <v>579</v>
+        <v>487</v>
       </c>
       <c r="K219" s="3" t="s">
-        <v>580</v>
+        <v>491</v>
       </c>
       <c r="L219" s="6" t="s">
-        <v>581</v>
+        <v>490</v>
       </c>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.2">
@@ -8966,14 +8983,14 @@
       <c r="B220" t="s">
         <v>405</v>
       </c>
-      <c r="C220" s="9" t="s">
-        <v>578</v>
+      <c r="C220" t="s">
+        <v>365</v>
       </c>
       <c r="D220" t="s">
         <v>388</v>
       </c>
-      <c r="F220" s="3">
-        <v>0</v>
+      <c r="F220" s="11">
+        <v>5</v>
       </c>
       <c r="G220" s="3" t="s">
         <v>432</v>
@@ -8982,13 +8999,13 @@
         <v>391</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>579</v>
+        <v>494</v>
       </c>
       <c r="K220" s="3" t="s">
-        <v>580</v>
+        <v>493</v>
       </c>
       <c r="L220" s="6" t="s">
-        <v>581</v>
+        <v>492</v>
       </c>
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.2">
@@ -8999,13 +9016,13 @@
         <v>405</v>
       </c>
       <c r="C221" s="9" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D221" t="s">
         <v>388</v>
       </c>
       <c r="F221" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G221" s="3" t="s">
         <v>432</v>
@@ -9030,29 +9047,29 @@
       <c r="B222" t="s">
         <v>405</v>
       </c>
-      <c r="C222" t="s">
-        <v>366</v>
+      <c r="C222" s="9" t="s">
+        <v>578</v>
       </c>
       <c r="D222" t="s">
         <v>388</v>
       </c>
       <c r="F222" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G222" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H222" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I222" s="3" t="s">
-        <v>487</v>
+        <v>579</v>
       </c>
       <c r="K222" s="3" t="s">
-        <v>489</v>
+        <v>580</v>
       </c>
       <c r="L222" s="6" t="s">
-        <v>488</v>
+        <v>581</v>
       </c>
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.2">
@@ -9062,8 +9079,8 @@
       <c r="B223" t="s">
         <v>405</v>
       </c>
-      <c r="C223" t="s">
-        <v>367</v>
+      <c r="C223" s="9" t="s">
+        <v>577</v>
       </c>
       <c r="D223" t="s">
         <v>388</v>
@@ -9072,19 +9089,19 @@
         <v>0</v>
       </c>
       <c r="G223" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H223" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>487</v>
+        <v>579</v>
       </c>
       <c r="K223" s="3" t="s">
-        <v>489</v>
+        <v>580</v>
       </c>
       <c r="L223" s="6" t="s">
-        <v>488</v>
+        <v>581</v>
       </c>
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.2">
@@ -9095,13 +9112,13 @@
         <v>405</v>
       </c>
       <c r="C224" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D224" t="s">
         <v>388</v>
       </c>
       <c r="F224" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G224" s="3" t="s">
         <v>174</v>
@@ -9127,45 +9144,45 @@
         <v>405</v>
       </c>
       <c r="C225" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D225" t="s">
         <v>388</v>
       </c>
-      <c r="F225" s="11">
-        <v>3</v>
+      <c r="F225" s="3">
+        <v>0</v>
       </c>
       <c r="G225" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H225" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I225" s="3" t="s">
-        <v>396</v>
+        <v>487</v>
       </c>
       <c r="K225" s="3" t="s">
-        <v>516</v>
+        <v>489</v>
       </c>
       <c r="L225" s="6" t="s">
-        <v>515</v>
+        <v>488</v>
       </c>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B226" t="s">
         <v>405</v>
       </c>
       <c r="C226" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D226" t="s">
         <v>388</v>
       </c>
       <c r="F226" s="3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G226" s="3" t="s">
         <v>174</v>
@@ -9174,45 +9191,45 @@
         <v>391</v>
       </c>
       <c r="I226" s="3" t="s">
-        <v>463</v>
+        <v>487</v>
       </c>
       <c r="K226" s="3" t="s">
-        <v>462</v>
+        <v>489</v>
       </c>
       <c r="L226" s="6" t="s">
-        <v>461</v>
+        <v>488</v>
       </c>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B227" t="s">
         <v>405</v>
       </c>
       <c r="C227" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D227" t="s">
         <v>388</v>
       </c>
-      <c r="F227" s="3">
-        <v>20</v>
+      <c r="F227" s="11">
+        <v>3</v>
       </c>
       <c r="G227" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H227" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I227" s="3" t="s">
-        <v>419</v>
+        <v>396</v>
       </c>
       <c r="K227" s="3" t="s">
-        <v>418</v>
+        <v>516</v>
       </c>
       <c r="L227" s="6" t="s">
-        <v>417</v>
+        <v>515</v>
       </c>
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.2">
@@ -9223,13 +9240,13 @@
         <v>405</v>
       </c>
       <c r="C228" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D228" t="s">
         <v>388</v>
       </c>
       <c r="F228" s="3">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G228" s="3" t="s">
         <v>174</v>
@@ -9238,30 +9255,30 @@
         <v>391</v>
       </c>
       <c r="I228" s="3" t="s">
-        <v>435</v>
+        <v>463</v>
       </c>
       <c r="K228" s="3" t="s">
-        <v>434</v>
+        <v>462</v>
       </c>
       <c r="L228" s="6" t="s">
-        <v>433</v>
+        <v>461</v>
       </c>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B229" t="s">
         <v>405</v>
       </c>
       <c r="C229" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D229" t="s">
         <v>388</v>
       </c>
       <c r="F229" s="3">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="G229" s="3" t="s">
         <v>174</v>
@@ -9270,30 +9287,30 @@
         <v>391</v>
       </c>
       <c r="I229" s="3" t="s">
-        <v>446</v>
+        <v>419</v>
       </c>
       <c r="K229" s="3" t="s">
-        <v>445</v>
+        <v>418</v>
       </c>
       <c r="L229" s="6" t="s">
-        <v>444</v>
+        <v>417</v>
       </c>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B230" t="s">
         <v>405</v>
       </c>
       <c r="C230" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D230" t="s">
         <v>388</v>
       </c>
       <c r="F230" s="3">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G230" s="3" t="s">
         <v>174</v>
@@ -9302,13 +9319,13 @@
         <v>391</v>
       </c>
       <c r="I230" s="3" t="s">
-        <v>411</v>
+        <v>435</v>
       </c>
       <c r="K230" s="3" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="L230" s="6" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.2">
@@ -9319,13 +9336,13 @@
         <v>405</v>
       </c>
       <c r="C231" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D231" t="s">
         <v>388</v>
       </c>
       <c r="F231" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G231" s="3" t="s">
         <v>174</v>
@@ -9351,13 +9368,13 @@
         <v>405</v>
       </c>
       <c r="C232" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D232" t="s">
         <v>388</v>
       </c>
       <c r="F232" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G232" s="3" t="s">
         <v>174</v>
@@ -9366,13 +9383,13 @@
         <v>391</v>
       </c>
       <c r="I232" s="3" t="s">
-        <v>454</v>
+        <v>411</v>
       </c>
       <c r="K232" s="3" t="s">
-        <v>453</v>
+        <v>431</v>
       </c>
       <c r="L232" s="6" t="s">
-        <v>452</v>
+        <v>430</v>
       </c>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.2">
@@ -9383,13 +9400,13 @@
         <v>405</v>
       </c>
       <c r="C233" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D233" t="s">
         <v>388</v>
       </c>
       <c r="F233" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G233" s="3" t="s">
         <v>174</v>
@@ -9398,13 +9415,13 @@
         <v>391</v>
       </c>
       <c r="I233" s="3" t="s">
-        <v>411</v>
+        <v>446</v>
       </c>
       <c r="K233" s="3" t="s">
-        <v>476</v>
+        <v>445</v>
       </c>
       <c r="L233" s="6" t="s">
-        <v>475</v>
+        <v>444</v>
       </c>
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.2">
@@ -9415,13 +9432,13 @@
         <v>405</v>
       </c>
       <c r="C234" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D234" t="s">
         <v>388</v>
       </c>
       <c r="F234" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G234" s="3" t="s">
         <v>174</v>
@@ -9430,13 +9447,13 @@
         <v>391</v>
       </c>
       <c r="I234" s="3" t="s">
-        <v>506</v>
+        <v>454</v>
       </c>
       <c r="K234" s="3" t="s">
-        <v>505</v>
+        <v>453</v>
       </c>
       <c r="L234" s="6" t="s">
-        <v>504</v>
+        <v>452</v>
       </c>
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.2">
@@ -9447,13 +9464,13 @@
         <v>405</v>
       </c>
       <c r="C235" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D235" t="s">
         <v>388</v>
       </c>
       <c r="F235" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G235" s="3" t="s">
         <v>174</v>
@@ -9462,13 +9479,13 @@
         <v>391</v>
       </c>
       <c r="I235" s="3" t="s">
-        <v>441</v>
+        <v>411</v>
       </c>
       <c r="K235" s="3" t="s">
-        <v>440</v>
+        <v>476</v>
       </c>
       <c r="L235" s="6" t="s">
-        <v>439</v>
+        <v>475</v>
       </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.2">
@@ -9479,13 +9496,13 @@
         <v>405</v>
       </c>
       <c r="C236" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D236" t="s">
         <v>388</v>
       </c>
       <c r="F236" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G236" s="3" t="s">
         <v>174</v>
@@ -9494,13 +9511,13 @@
         <v>391</v>
       </c>
       <c r="I236" s="3" t="s">
-        <v>443</v>
+        <v>506</v>
       </c>
       <c r="K236" s="3" t="s">
-        <v>440</v>
+        <v>505</v>
       </c>
       <c r="L236" s="6" t="s">
-        <v>442</v>
+        <v>504</v>
       </c>
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.2">
@@ -9511,7 +9528,7 @@
         <v>405</v>
       </c>
       <c r="C237" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D237" t="s">
         <v>388</v>
@@ -9526,30 +9543,30 @@
         <v>391</v>
       </c>
       <c r="I237" s="3" t="s">
-        <v>411</v>
+        <v>441</v>
       </c>
       <c r="K237" s="3" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="L237" s="6" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B238" t="s">
         <v>405</v>
       </c>
       <c r="C238" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D238" t="s">
         <v>388</v>
       </c>
       <c r="F238" s="3">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="G238" s="3" t="s">
         <v>174</v>
@@ -9558,13 +9575,13 @@
         <v>391</v>
       </c>
       <c r="I238" s="3" t="s">
-        <v>414</v>
+        <v>443</v>
       </c>
       <c r="K238" s="3" t="s">
-        <v>413</v>
+        <v>440</v>
       </c>
       <c r="L238" s="6" t="s">
-        <v>412</v>
+        <v>442</v>
       </c>
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.2">
@@ -9575,45 +9592,45 @@
         <v>405</v>
       </c>
       <c r="C239" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D239" t="s">
         <v>388</v>
       </c>
-      <c r="F239" s="11">
-        <v>2</v>
+      <c r="F239" s="3">
+        <v>1</v>
       </c>
       <c r="G239" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H239" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I239" s="3" t="s">
-        <v>525</v>
+        <v>411</v>
       </c>
       <c r="K239" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="L239" s="10" t="s">
-        <v>523</v>
+        <v>451</v>
+      </c>
+      <c r="L239" s="6" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B240" t="s">
         <v>405</v>
       </c>
       <c r="C240" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D240" t="s">
         <v>388</v>
       </c>
       <c r="F240" s="3">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="G240" s="3" t="s">
         <v>174</v>
@@ -9621,15 +9638,14 @@
       <c r="H240" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I240" t="s">
-        <v>573</v>
-      </c>
-      <c r="J240"/>
-      <c r="K240" t="s">
-        <v>574</v>
+      <c r="I240" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="K240" s="3" t="s">
+        <v>413</v>
       </c>
       <c r="L240" s="6" t="s">
-        <v>575</v>
+        <v>412</v>
       </c>
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.2">
@@ -9640,46 +9656,45 @@
         <v>405</v>
       </c>
       <c r="C241" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D241" t="s">
         <v>388</v>
       </c>
-      <c r="F241" s="3">
-        <v>1</v>
+      <c r="F241" s="11">
+        <v>2</v>
       </c>
       <c r="G241" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H241" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I241" t="s">
-        <v>570</v>
-      </c>
-      <c r="J241"/>
-      <c r="K241" t="s">
-        <v>571</v>
-      </c>
-      <c r="L241" s="6" t="s">
-        <v>572</v>
+      <c r="I241" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="K241" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="L241" s="10" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B242" t="s">
         <v>405</v>
       </c>
       <c r="C242" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D242" t="s">
         <v>388</v>
       </c>
       <c r="F242" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G242" s="3" t="s">
         <v>174</v>
@@ -9687,14 +9702,15 @@
       <c r="H242" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I242" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="K242" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="L242" s="7" t="s">
-        <v>404</v>
+      <c r="I242" t="s">
+        <v>573</v>
+      </c>
+      <c r="J242"/>
+      <c r="K242" t="s">
+        <v>574</v>
+      </c>
+      <c r="L242" s="6" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.2">
@@ -9705,7 +9721,7 @@
         <v>405</v>
       </c>
       <c r="C243" t="s">
-        <v>58</v>
+        <v>385</v>
       </c>
       <c r="D243" t="s">
         <v>388</v>
@@ -9719,46 +9735,47 @@
       <c r="H243" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I243" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="K243" s="3" t="s">
-        <v>467</v>
+      <c r="I243" t="s">
+        <v>570</v>
+      </c>
+      <c r="J243"/>
+      <c r="K243" t="s">
+        <v>571</v>
       </c>
       <c r="L243" s="6" t="s">
-        <v>466</v>
+        <v>572</v>
       </c>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B244" t="s">
         <v>405</v>
       </c>
-      <c r="C244" s="9" t="s">
-        <v>582</v>
+      <c r="C244" t="s">
+        <v>386</v>
       </c>
       <c r="D244" t="s">
         <v>388</v>
       </c>
       <c r="F244" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G244" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H244" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I244" s="3" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="K244" s="3" t="s">
-        <v>587</v>
-      </c>
-      <c r="L244" s="6" t="s">
-        <v>586</v>
+        <v>403</v>
+      </c>
+      <c r="L244" s="7" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.2">
@@ -9768,29 +9785,29 @@
       <c r="B245" t="s">
         <v>405</v>
       </c>
-      <c r="C245" s="9" t="s">
-        <v>582</v>
+      <c r="C245" t="s">
+        <v>58</v>
       </c>
       <c r="D245" t="s">
         <v>388</v>
       </c>
       <c r="F245" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G245" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H245" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I245" s="3" t="s">
-        <v>392</v>
+        <v>468</v>
       </c>
       <c r="K245" s="3" t="s">
-        <v>587</v>
+        <v>467</v>
       </c>
       <c r="L245" s="6" t="s">
-        <v>586</v>
+        <v>466</v>
       </c>
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.2">
@@ -9807,7 +9824,7 @@
         <v>388</v>
       </c>
       <c r="F246" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G246" s="3" t="s">
         <v>432</v>
@@ -9833,13 +9850,13 @@
         <v>405</v>
       </c>
       <c r="C247" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D247" t="s">
         <v>388</v>
       </c>
       <c r="F247" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G247" s="3" t="s">
         <v>432</v>
@@ -9848,13 +9865,13 @@
         <v>391</v>
       </c>
       <c r="I247" s="3" t="s">
-        <v>537</v>
+        <v>392</v>
       </c>
       <c r="K247" s="3" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="L247" s="6" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.2">
@@ -9864,33 +9881,97 @@
       <c r="B248" t="s">
         <v>405</v>
       </c>
-      <c r="C248" t="s">
-        <v>387</v>
+      <c r="C248" s="9" t="s">
+        <v>582</v>
       </c>
       <c r="D248" t="s">
         <v>388</v>
       </c>
       <c r="F248" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G248" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H248" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I248" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="K248" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="L248" s="6" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>389</v>
+      </c>
+      <c r="B249" t="s">
+        <v>405</v>
+      </c>
+      <c r="C249" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="D249" t="s">
+        <v>388</v>
+      </c>
+      <c r="F249" s="3">
+        <v>1</v>
+      </c>
+      <c r="G249" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="H249" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I249" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="K249" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="L249" s="6" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>389</v>
+      </c>
+      <c r="B250" t="s">
+        <v>405</v>
+      </c>
+      <c r="C250" t="s">
+        <v>387</v>
+      </c>
+      <c r="D250" t="s">
+        <v>388</v>
+      </c>
+      <c r="F250" s="3">
+        <v>1</v>
+      </c>
+      <c r="G250" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H250" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I250" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="K248" s="3" t="s">
+      <c r="K250" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="L248" s="6" t="s">
+      <c r="L250" s="6" t="s">
         <v>469</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L248" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}"/>
+  <autoFilter ref="A1:L250" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}"/>
   <hyperlinks>
     <hyperlink ref="L3" r:id="rId1" location="query=target&amp;position=0&amp;from_view=search&amp;track=sph&amp;uuid=07a631b0-afe2-4d83-9076-a80360e62f2f" xr:uid="{6340FD26-01F6-9246-82E5-C8936FBB7B36}"/>
     <hyperlink ref="L4" r:id="rId2" location="query=spell%20book&amp;position=12&amp;from_view=keyword&amp;track=ais&amp;uuid=3aa8f740-41d0-409e-b03b-268281a69be6" xr:uid="{1A91BF66-CE85-304F-BBE7-7F8EBE53C285}"/>
@@ -9963,147 +10044,149 @@
     <hyperlink ref="L79" r:id="rId69" location="&amp;position=13&amp;from_view=search&amp;track=ais&amp;uuid=fec8d80b-ddc0-4094-a5d3-12ce905b8324" xr:uid="{EFC3D8D5-193A-7A40-A46E-69D438875999}"/>
     <hyperlink ref="L81" r:id="rId70" location="page=3&amp;query=dragon%20sprite&amp;position=8&amp;from_view=search&amp;track=ais&amp;uuid=a74ae69f-43df-4e46-8d2c-551fbfc06054" xr:uid="{5F5719A4-7B8B-9E45-BEC0-7667F1CB6C28}"/>
     <hyperlink ref="L82" r:id="rId71" location="query=explode%20smoke%20sprite&amp;position=3&amp;from_view=search&amp;track=ais&amp;uuid=d61ee19a-6b7f-4553-a2f8-393d16eb8a74" xr:uid="{4EF9777B-9D84-494F-96A4-7A806036CC03}"/>
-    <hyperlink ref="L94" r:id="rId72" location="query=moon%20sprite%20phase&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=eb51ec8e-6b0f-4dcb-ad91-ebd9a86a89ff" xr:uid="{63C1230E-216D-CF4C-B1AE-0AD16D4C9F4E}"/>
-    <hyperlink ref="L95" r:id="rId73" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{76E2C3CA-7BDA-DB4B-B417-B04F392F2F94}"/>
-    <hyperlink ref="L97" r:id="rId74" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{A08C0C27-1920-5949-B8A9-BC2B98757F1A}"/>
-    <hyperlink ref="L98" r:id="rId75" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{956FB374-FCF8-D845-A6AC-78A383E21E18}"/>
-    <hyperlink ref="L96" r:id="rId76" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{4B9DBD88-1996-F740-AE96-9A4CAFD32458}"/>
-    <hyperlink ref="L99" r:id="rId77" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{F8D6E2FC-7668-7341-AB68-0BAEA695DB1D}"/>
-    <hyperlink ref="L100" r:id="rId78" xr:uid="{875A91BB-08F0-9F41-AA8C-0DA91E9E3433}"/>
-    <hyperlink ref="L101" r:id="rId79" xr:uid="{2358BC99-E6CB-CC40-ADFF-8AC06D23EF07}"/>
-    <hyperlink ref="L102" r:id="rId80" xr:uid="{EE8601B6-0243-2A49-A9C6-75E6146D7CED}"/>
-    <hyperlink ref="L104" r:id="rId81" xr:uid="{11B6F62A-6D9A-614A-B258-D8AA048E0295}"/>
+    <hyperlink ref="L95" r:id="rId72" location="query=moon%20sprite%20phase&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=eb51ec8e-6b0f-4dcb-ad91-ebd9a86a89ff" xr:uid="{63C1230E-216D-CF4C-B1AE-0AD16D4C9F4E}"/>
+    <hyperlink ref="L96" r:id="rId73" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{76E2C3CA-7BDA-DB4B-B417-B04F392F2F94}"/>
+    <hyperlink ref="L98" r:id="rId74" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{A08C0C27-1920-5949-B8A9-BC2B98757F1A}"/>
+    <hyperlink ref="L99" r:id="rId75" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{956FB374-FCF8-D845-A6AC-78A383E21E18}"/>
+    <hyperlink ref="L97" r:id="rId76" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{4B9DBD88-1996-F740-AE96-9A4CAFD32458}"/>
+    <hyperlink ref="L100" r:id="rId77" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{F8D6E2FC-7668-7341-AB68-0BAEA695DB1D}"/>
+    <hyperlink ref="L101" r:id="rId78" xr:uid="{875A91BB-08F0-9F41-AA8C-0DA91E9E3433}"/>
+    <hyperlink ref="L102" r:id="rId79" xr:uid="{2358BC99-E6CB-CC40-ADFF-8AC06D23EF07}"/>
+    <hyperlink ref="L103" r:id="rId80" xr:uid="{EE8601B6-0243-2A49-A9C6-75E6146D7CED}"/>
+    <hyperlink ref="L105" r:id="rId81" xr:uid="{11B6F62A-6D9A-614A-B258-D8AA048E0295}"/>
     <hyperlink ref="L80" r:id="rId82" location="&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=212ca3a5-7aff-48ca-9059-3fd4569bd97d" xr:uid="{5E0BEA94-3C14-624A-B04C-480D52071A59}"/>
-    <hyperlink ref="L107" r:id="rId83" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{62FFBF71-DDCC-FB45-B1A0-5B5743818433}"/>
-    <hyperlink ref="L108" r:id="rId84" xr:uid="{C6D42146-F620-2E4D-A1E8-6C7AB68398A0}"/>
-    <hyperlink ref="L109" r:id="rId85" xr:uid="{69D2711D-2024-4D48-B506-A5426A13437B}"/>
-    <hyperlink ref="L110" r:id="rId86" xr:uid="{D50E3661-FDF1-5C4F-B873-C0CBFBD7EF35}"/>
-    <hyperlink ref="L111" r:id="rId87" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{7D5FDD89-EC51-3648-AED9-53792D3E0C33}"/>
-    <hyperlink ref="L112" r:id="rId88" xr:uid="{152DE699-D73F-EF4E-9197-168BFA94CEA2}"/>
-    <hyperlink ref="L113" r:id="rId89" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{D0737FC4-EBDD-894D-B245-F35B45E2BB9E}"/>
-    <hyperlink ref="L114" r:id="rId90" xr:uid="{F6962BD9-CA67-934F-A5FA-A876F707D991}"/>
-    <hyperlink ref="L115" r:id="rId91" xr:uid="{9FB19C9F-53C1-C14F-B0FB-F6FFC3813A0C}"/>
-    <hyperlink ref="L116" r:id="rId92" location="page=3&amp;query=dragon%20sprite&amp;position=8&amp;from_view=search&amp;track=ais&amp;uuid=a74ae69f-43df-4e46-8d2c-551fbfc06054" xr:uid="{8CF6EC38-B466-5046-9ABB-7B436FB04B00}"/>
-    <hyperlink ref="L117" r:id="rId93" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{0A9F6B86-9F6E-BB4B-A75B-04A9E5D17C6C}"/>
-    <hyperlink ref="L118" r:id="rId94" xr:uid="{5F607910-F685-E446-84A9-7A29F560E55A}"/>
-    <hyperlink ref="L119" r:id="rId95" xr:uid="{578C63E4-A237-DE4B-B0BD-67011C0E3ADD}"/>
-    <hyperlink ref="L120" r:id="rId96" location="page=2&amp;position=43&amp;from_view=search&amp;track=ais&amp;uuid=0f4d7d50-56a5-4394-84f3-725d8c5aaddd" xr:uid="{61842379-CF7B-1241-9EBE-2870DBC6CCF0}"/>
-    <hyperlink ref="L121" r:id="rId97" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{5A8FBE05-CC1C-4445-872A-1F2B5D068722}"/>
-    <hyperlink ref="L122" r:id="rId98" xr:uid="{6C2DDDB8-2819-0F48-9FC2-13E3FD09D89C}"/>
-    <hyperlink ref="L123" r:id="rId99" xr:uid="{FA9A9087-DACC-3348-9590-AF003D7980CD}"/>
-    <hyperlink ref="L124" r:id="rId100" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{13DDFAC9-7E7A-7144-8D4D-5F7238F57C50}"/>
-    <hyperlink ref="L125" r:id="rId101" xr:uid="{536E05BD-607D-8C40-A324-92D273517532}"/>
-    <hyperlink ref="L126" r:id="rId102" location="page=3&amp;query=dragon%20sprite&amp;position=8&amp;from_view=search&amp;track=ais&amp;uuid=a74ae69f-43df-4e46-8d2c-551fbfc06054" xr:uid="{80725854-8C9E-2142-9506-1DAA5EA55E2C}"/>
-    <hyperlink ref="L127" r:id="rId103" xr:uid="{7D317CFF-0421-8240-AC77-11BBCE22AB8E}"/>
-    <hyperlink ref="L128" r:id="rId104" xr:uid="{A2D8E487-AD43-8F4E-A9DE-5869F09C0426}"/>
-    <hyperlink ref="L130" r:id="rId105" xr:uid="{D7E8C3AD-A803-064B-BE47-A4A13A516766}"/>
-    <hyperlink ref="L132" r:id="rId106" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{BDB61EDA-F818-FF45-B87D-6ADEA708FFA7}"/>
-    <hyperlink ref="L133" r:id="rId107" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{253AAE66-6702-8C4F-A846-EBF5AE2F8391}"/>
-    <hyperlink ref="L134" r:id="rId108" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{6939D314-66EF-8D4B-AFF0-C6E403A07A14}"/>
-    <hyperlink ref="L141" r:id="rId109" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{EB09046E-7A86-CA4F-8571-926934A1C16B}"/>
-    <hyperlink ref="L142" r:id="rId110" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{C5A8A89F-FAEB-664B-8EA0-ED39009C9364}"/>
-    <hyperlink ref="L143" r:id="rId111" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{B0D21C11-7039-9747-AFD6-6A560A885C1E}"/>
-    <hyperlink ref="L148" r:id="rId112" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{1565E7C7-B646-D249-BAAB-3FCB7F08DD87}"/>
-    <hyperlink ref="L149" r:id="rId113" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{A8BBBB50-0434-7448-8336-9B7ED86F56E9}"/>
-    <hyperlink ref="L150" r:id="rId114" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{C3D989D9-9B8F-A344-BCD4-784D6E9D731B}"/>
-    <hyperlink ref="L152" r:id="rId115" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{30281897-7108-FC49-9176-CC6B5A425C7A}"/>
-    <hyperlink ref="L153" r:id="rId116" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{A0297FF1-2C4C-E544-B864-7C5A962D424C}"/>
-    <hyperlink ref="L154" r:id="rId117" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{E800482C-5495-E140-9569-17E80FD691E0}"/>
-    <hyperlink ref="L135" r:id="rId118" location="query=discoball%20sprite%20purple&amp;position=5&amp;from_view=search&amp;track=ais&amp;uuid=5e15239d-0812-436d-9e99-3bbe89255301" xr:uid="{6CBD560E-8DE3-AC47-AF1D-9836CBBBCFAF}"/>
-    <hyperlink ref="L136" r:id="rId119" location="query=discoball%20sprite%20purple&amp;position=5&amp;from_view=search&amp;track=ais&amp;uuid=5e15239d-0812-436d-9e99-3bbe89255301" xr:uid="{92122264-574C-904C-AB91-F5AF6D172F32}"/>
-    <hyperlink ref="L140" r:id="rId120" location="&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=3b8eb20b-1ef9-4be4-b972-96b55e0f912c" display="https://www.freepik.com/free-vector/set-square-ui-game-frames-textured-medieval-borders-gold-silver-steel-metal-with-gems-cartoon-empty-metallic-bordering-with-gemstones-isolated-design-gui-elements-vector-illustration_24325879.htm#&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=3b8eb20b-1ef9-4be4-b972-96b55e0f912c" xr:uid="{BA52B0B4-2A86-6842-A815-4370D4A52AF0}"/>
-    <hyperlink ref="L139" r:id="rId121" location="&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=295330cb-9881-4046-9dc8-cb7e28cdaddb" xr:uid="{8F9561E6-335E-E740-8CF3-AF66A1E5C23F}"/>
+    <hyperlink ref="L108" r:id="rId83" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{62FFBF71-DDCC-FB45-B1A0-5B5743818433}"/>
+    <hyperlink ref="L109" r:id="rId84" xr:uid="{C6D42146-F620-2E4D-A1E8-6C7AB68398A0}"/>
+    <hyperlink ref="L110" r:id="rId85" xr:uid="{69D2711D-2024-4D48-B506-A5426A13437B}"/>
+    <hyperlink ref="L111" r:id="rId86" xr:uid="{D50E3661-FDF1-5C4F-B873-C0CBFBD7EF35}"/>
+    <hyperlink ref="L112" r:id="rId87" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{7D5FDD89-EC51-3648-AED9-53792D3E0C33}"/>
+    <hyperlink ref="L113" r:id="rId88" xr:uid="{152DE699-D73F-EF4E-9197-168BFA94CEA2}"/>
+    <hyperlink ref="L114" r:id="rId89" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{D0737FC4-EBDD-894D-B245-F35B45E2BB9E}"/>
+    <hyperlink ref="L115" r:id="rId90" xr:uid="{F6962BD9-CA67-934F-A5FA-A876F707D991}"/>
+    <hyperlink ref="L116" r:id="rId91" xr:uid="{9FB19C9F-53C1-C14F-B0FB-F6FFC3813A0C}"/>
+    <hyperlink ref="L117" r:id="rId92" location="page=3&amp;query=dragon%20sprite&amp;position=8&amp;from_view=search&amp;track=ais&amp;uuid=a74ae69f-43df-4e46-8d2c-551fbfc06054" xr:uid="{8CF6EC38-B466-5046-9ABB-7B436FB04B00}"/>
+    <hyperlink ref="L118" r:id="rId93" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{0A9F6B86-9F6E-BB4B-A75B-04A9E5D17C6C}"/>
+    <hyperlink ref="L119" r:id="rId94" xr:uid="{5F607910-F685-E446-84A9-7A29F560E55A}"/>
+    <hyperlink ref="L120" r:id="rId95" xr:uid="{578C63E4-A237-DE4B-B0BD-67011C0E3ADD}"/>
+    <hyperlink ref="L121" r:id="rId96" location="page=2&amp;position=43&amp;from_view=search&amp;track=ais&amp;uuid=0f4d7d50-56a5-4394-84f3-725d8c5aaddd" xr:uid="{61842379-CF7B-1241-9EBE-2870DBC6CCF0}"/>
+    <hyperlink ref="L122" r:id="rId97" location="&amp;position=1&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{5A8FBE05-CC1C-4445-872A-1F2B5D068722}"/>
+    <hyperlink ref="L123" r:id="rId98" xr:uid="{6C2DDDB8-2819-0F48-9FC2-13E3FD09D89C}"/>
+    <hyperlink ref="L124" r:id="rId99" xr:uid="{FA9A9087-DACC-3348-9590-AF003D7980CD}"/>
+    <hyperlink ref="L125" r:id="rId100" location="&amp;position=2&amp;from_view=search&amp;track=ais&amp;uuid=bc710ade-cbc6-41f0-ac9e-7537aa65a01a" xr:uid="{13DDFAC9-7E7A-7144-8D4D-5F7238F57C50}"/>
+    <hyperlink ref="L126" r:id="rId101" xr:uid="{536E05BD-607D-8C40-A324-92D273517532}"/>
+    <hyperlink ref="L127" r:id="rId102" location="page=3&amp;query=dragon%20sprite&amp;position=8&amp;from_view=search&amp;track=ais&amp;uuid=a74ae69f-43df-4e46-8d2c-551fbfc06054" xr:uid="{80725854-8C9E-2142-9506-1DAA5EA55E2C}"/>
+    <hyperlink ref="L128" r:id="rId103" xr:uid="{7D317CFF-0421-8240-AC77-11BBCE22AB8E}"/>
+    <hyperlink ref="L129" r:id="rId104" xr:uid="{A2D8E487-AD43-8F4E-A9DE-5869F09C0426}"/>
+    <hyperlink ref="L131" r:id="rId105" xr:uid="{D7E8C3AD-A803-064B-BE47-A4A13A516766}"/>
+    <hyperlink ref="L133" r:id="rId106" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{BDB61EDA-F818-FF45-B87D-6ADEA708FFA7}"/>
+    <hyperlink ref="L134" r:id="rId107" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{253AAE66-6702-8C4F-A846-EBF5AE2F8391}"/>
+    <hyperlink ref="L135" r:id="rId108" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{6939D314-66EF-8D4B-AFF0-C6E403A07A14}"/>
+    <hyperlink ref="L142" r:id="rId109" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{EB09046E-7A86-CA4F-8571-926934A1C16B}"/>
+    <hyperlink ref="L143" r:id="rId110" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{C5A8A89F-FAEB-664B-8EA0-ED39009C9364}"/>
+    <hyperlink ref="L144" r:id="rId111" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{B0D21C11-7039-9747-AFD6-6A560A885C1E}"/>
+    <hyperlink ref="L149" r:id="rId112" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{1565E7C7-B646-D249-BAAB-3FCB7F08DD87}"/>
+    <hyperlink ref="L150" r:id="rId113" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{A8BBBB50-0434-7448-8336-9B7ED86F56E9}"/>
+    <hyperlink ref="L151" r:id="rId114" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{C3D989D9-9B8F-A344-BCD4-784D6E9D731B}"/>
+    <hyperlink ref="L153" r:id="rId115" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{30281897-7108-FC49-9176-CC6B5A425C7A}"/>
+    <hyperlink ref="L154" r:id="rId116" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{A0297FF1-2C4C-E544-B864-7C5A962D424C}"/>
+    <hyperlink ref="L155" r:id="rId117" location="query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" display="https://www.freepik.com/free-vector/green-circle-buttons-icons-website-game_27041323.htm#query=green%20buttons%20sprite&amp;position=22&amp;from_view=search&amp;track=ais&amp;uuid=3e99aa9a-d82f-4db3-aefc-313bc75bedcb" xr:uid="{E800482C-5495-E140-9569-17E80FD691E0}"/>
+    <hyperlink ref="L136" r:id="rId118" location="query=discoball%20sprite%20purple&amp;position=5&amp;from_view=search&amp;track=ais&amp;uuid=5e15239d-0812-436d-9e99-3bbe89255301" xr:uid="{6CBD560E-8DE3-AC47-AF1D-9836CBBBCFAF}"/>
+    <hyperlink ref="L137" r:id="rId119" location="query=discoball%20sprite%20purple&amp;position=5&amp;from_view=search&amp;track=ais&amp;uuid=5e15239d-0812-436d-9e99-3bbe89255301" xr:uid="{92122264-574C-904C-AB91-F5AF6D172F32}"/>
+    <hyperlink ref="L141" r:id="rId120" location="&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=3b8eb20b-1ef9-4be4-b972-96b55e0f912c" display="https://www.freepik.com/free-vector/set-square-ui-game-frames-textured-medieval-borders-gold-silver-steel-metal-with-gems-cartoon-empty-metallic-bordering-with-gemstones-isolated-design-gui-elements-vector-illustration_24325879.htm#&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=3b8eb20b-1ef9-4be4-b972-96b55e0f912c" xr:uid="{BA52B0B4-2A86-6842-A815-4370D4A52AF0}"/>
+    <hyperlink ref="L140" r:id="rId121" location="&amp;position=0&amp;from_view=search&amp;track=ais&amp;uuid=295330cb-9881-4046-9dc8-cb7e28cdaddb" xr:uid="{8F9561E6-335E-E740-8CF3-AF66A1E5C23F}"/>
     <hyperlink ref="L2" r:id="rId122" xr:uid="{9DA1D9F2-BD16-914A-B65F-BEFF391AD408}"/>
-    <hyperlink ref="L129" r:id="rId123" xr:uid="{4BFCF1BE-6310-C34B-BA09-218F6A3C75D9}"/>
-    <hyperlink ref="L131" r:id="rId124" xr:uid="{C9C421A7-64D0-5D49-9F28-B71BC19F3239}"/>
-    <hyperlink ref="L158" r:id="rId125" xr:uid="{F88953B7-468E-C34B-9347-94009F9A78D2}"/>
-    <hyperlink ref="L198" r:id="rId126" xr:uid="{1F3BBC8C-29E8-C74A-AB3F-04AE466222EF}"/>
-    <hyperlink ref="L200" r:id="rId127" xr:uid="{3C51058F-793C-D34A-8286-18AE4C8EF6CE}"/>
-    <hyperlink ref="L242" r:id="rId128" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
-    <hyperlink ref="L155" r:id="rId129" xr:uid="{6A722A1D-2F7B-4242-8134-716EFF33F7D2}"/>
-    <hyperlink ref="L156" r:id="rId130" xr:uid="{547CD1A8-1967-1C46-95E3-89E39CD045C2}"/>
-    <hyperlink ref="L203" r:id="rId131" xr:uid="{5ACD6BFD-52F0-0940-AA8E-B04F1D397BC7}"/>
-    <hyperlink ref="L238" r:id="rId132" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
-    <hyperlink ref="L199" r:id="rId133" xr:uid="{2030AD8C-28A7-544B-92DC-5CBE411DE1C0}"/>
-    <hyperlink ref="L227" r:id="rId134" xr:uid="{05363CA1-BE60-3F42-B56A-1A92A0EDA166}"/>
-    <hyperlink ref="L191" r:id="rId135" xr:uid="{D4C66DCB-D6B4-EC4F-A922-B87887BE6E4A}"/>
-    <hyperlink ref="L190" r:id="rId136" xr:uid="{A05D9F8A-ED0A-4143-8920-9422DD4E0BDD}"/>
-    <hyperlink ref="L192" r:id="rId137" xr:uid="{83FA4EC1-AB5E-3B43-9476-4CA54526DF8E}"/>
-    <hyperlink ref="L171" r:id="rId138" xr:uid="{21B7C9CB-274E-C246-8989-83D9E0E7B24F}"/>
-    <hyperlink ref="L167" r:id="rId139" xr:uid="{B5B4FA15-B24C-CE46-9594-7ED28656AA43}"/>
-    <hyperlink ref="L168" r:id="rId140" xr:uid="{3AB6BE1F-95C1-A443-B12D-D7A523FAD6C5}"/>
-    <hyperlink ref="L169" r:id="rId141" xr:uid="{347BDCC2-5A0C-B249-8CA8-B72D245480FC}"/>
-    <hyperlink ref="L170" r:id="rId142" xr:uid="{E58DD28D-BD99-DF44-9E5E-B3D05F881C1F}"/>
-    <hyperlink ref="L230" r:id="rId143" xr:uid="{4F668E79-3664-0547-B3D5-B7724A9D574D}"/>
-    <hyperlink ref="L228" r:id="rId144" xr:uid="{8AB5C10C-8B45-1843-96BD-655A4FA04EFD}"/>
-    <hyperlink ref="L174" r:id="rId145" xr:uid="{EAED74E0-13EE-A046-9ADC-AC8BDE30C3E6}"/>
-    <hyperlink ref="L235" r:id="rId146" xr:uid="{3577256C-215B-134E-B541-B7B77272CD8A}"/>
-    <hyperlink ref="L236" r:id="rId147" xr:uid="{98E325FC-7F95-B44E-98EB-DE0FF53BC89D}"/>
-    <hyperlink ref="L229" r:id="rId148" xr:uid="{5CE3083F-F217-3743-B613-A7DDF354E72D}"/>
-    <hyperlink ref="L231" r:id="rId149" xr:uid="{B81B6B41-2C17-AA48-B730-D906488BA0A0}"/>
-    <hyperlink ref="L180" r:id="rId150" xr:uid="{BA0813A2-2582-7A46-A492-16A943824EE5}"/>
-    <hyperlink ref="L237" r:id="rId151" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
-    <hyperlink ref="L232" r:id="rId152" xr:uid="{C5265333-F7F0-1845-98D7-68E930F9DFAE}"/>
-    <hyperlink ref="L182" r:id="rId153" xr:uid="{C0A159CB-3986-1A46-95AD-DCEFF4247697}"/>
-    <hyperlink ref="L172" r:id="rId154" xr:uid="{37810A74-E45D-1D46-AEF5-C5FE2F414285}"/>
-    <hyperlink ref="L226" r:id="rId155" xr:uid="{D2906064-B1B8-4648-8201-BEFA97591226}"/>
-    <hyperlink ref="L160" r:id="rId156" xr:uid="{1D3CD52E-7AAD-E444-88F4-4BAE6C5B5EB7}"/>
-    <hyperlink ref="L161" r:id="rId157" xr:uid="{E6E6DA47-945D-6145-912F-08B17B7BA6AE}"/>
-    <hyperlink ref="L162" r:id="rId158" xr:uid="{006B1689-D89A-1E4A-BBC5-E9C9583907F7}"/>
-    <hyperlink ref="L163" r:id="rId159" xr:uid="{C3E773B2-D410-AF41-B197-4638485DC8EF}"/>
-    <hyperlink ref="L164" r:id="rId160" xr:uid="{A0E8A8E2-4A93-3D42-AF48-81955241A483}"/>
-    <hyperlink ref="L165" r:id="rId161" xr:uid="{1B03F18A-8745-AA4F-AA8B-88D65D3B24BC}"/>
-    <hyperlink ref="L243" r:id="rId162" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
-    <hyperlink ref="L248" r:id="rId163" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
-    <hyperlink ref="L188" r:id="rId164" xr:uid="{D6B77117-A0D5-9240-8193-0102C36CCE4C}"/>
-    <hyperlink ref="L189" r:id="rId165" xr:uid="{79FB1103-88A8-8044-9E2C-4FAEC0906E8E}"/>
-    <hyperlink ref="L233" r:id="rId166" xr:uid="{5BF1C4C9-E63A-4F42-9042-36520975FDFA}"/>
-    <hyperlink ref="L187" r:id="rId167" xr:uid="{21CDF460-9871-0547-AA6B-20304C8DD21D}"/>
-    <hyperlink ref="L177" r:id="rId168" xr:uid="{BA1EC844-435A-6C44-87FC-C12B7ECFC55B}"/>
-    <hyperlink ref="L176" r:id="rId169" xr:uid="{46D875DC-CDDD-7E4B-88DB-DFC416CF17AB}"/>
-    <hyperlink ref="L166" r:id="rId170" xr:uid="{7D2FF6AE-1C67-9D4A-A760-7E3745DD9EA6}"/>
-    <hyperlink ref="L216" r:id="rId171" xr:uid="{B5E5E388-8F37-414E-A0C6-1DC58E77628C}"/>
-    <hyperlink ref="L218" r:id="rId172" xr:uid="{A96B1ACF-D982-9240-BB1C-69459154AE5A}"/>
-    <hyperlink ref="L183" r:id="rId173" xr:uid="{D3BB695A-CBA9-D649-B49D-4CC8D16EFD9B}"/>
-    <hyperlink ref="L184" r:id="rId174" xr:uid="{A2922BA8-758D-3149-892C-B7B65B435332}"/>
-    <hyperlink ref="L205" r:id="rId175" xr:uid="{BDB09119-6289-4346-BC29-7A54BD393127}"/>
-    <hyperlink ref="L234" r:id="rId176" xr:uid="{5736CAF4-3646-3243-9AEB-4D82B6D0D10A}"/>
-    <hyperlink ref="L208" r:id="rId177" xr:uid="{60659D55-801C-9A4E-84CA-809884CCBE5C}"/>
-    <hyperlink ref="L196" r:id="rId178" xr:uid="{18DDC006-0939-794C-9B5D-10593F8C0973}"/>
-    <hyperlink ref="L185" r:id="rId179" xr:uid="{50EA46A5-11DD-0345-ABCA-4206D73C7606}"/>
-    <hyperlink ref="L225" r:id="rId180" xr:uid="{63DDFF3B-E62C-9445-96AD-4BB37ACCD20E}"/>
-    <hyperlink ref="L210" r:id="rId181" xr:uid="{05E34BC1-B22F-3E46-8574-E72267507402}"/>
-    <hyperlink ref="L209" r:id="rId182" xr:uid="{7125DF67-5A7E-D948-8363-A31AB1EBA44A}"/>
-    <hyperlink ref="L239" r:id="rId183" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
-    <hyperlink ref="L197" r:id="rId184" xr:uid="{CCE2D666-E296-D94C-ACE0-791CC746483B}"/>
-    <hyperlink ref="L178" r:id="rId185" xr:uid="{E5A2F3EE-A3B1-0842-9364-E4B6EACA9544}"/>
-    <hyperlink ref="L211" r:id="rId186" xr:uid="{E08C8BA4-5414-1947-9CA8-45FE0B846CD1}"/>
-    <hyperlink ref="L207" r:id="rId187" xr:uid="{F1A64091-5BF7-8243-B7A0-F4C13B8B0ABB}"/>
-    <hyperlink ref="L194" r:id="rId188" xr:uid="{745AEF03-3150-C54B-800A-696460474256}"/>
-    <hyperlink ref="L195" r:id="rId189" xr:uid="{9C078FBA-3B11-8049-9187-5BC86D78EA09}"/>
-    <hyperlink ref="L179" r:id="rId190" xr:uid="{BF9A6A48-C664-FA4B-A769-D87460BB9387}"/>
-    <hyperlink ref="L181" r:id="rId191" xr:uid="{11E0C06F-BBA9-B446-A3A4-5862C893161B}"/>
-    <hyperlink ref="L206" r:id="rId192" xr:uid="{D5E45024-1B58-714D-9576-1FA969BDADD9}"/>
-    <hyperlink ref="L186" r:id="rId193" xr:uid="{D160676D-AC82-D243-B9A9-56033B0A6EFE}"/>
-    <hyperlink ref="L204" r:id="rId194" xr:uid="{3DB54A74-68B7-734A-BC3C-BFE4E2E4103E}"/>
-    <hyperlink ref="L103" r:id="rId195" xr:uid="{4686296B-C235-4048-A384-BE461895E2AC}"/>
-    <hyperlink ref="L105" r:id="rId196" location="page=2&amp;query=gold%20badge%20sprite&amp;position=49&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{061AB839-ADB1-BA47-A152-68CDFE8A1979}"/>
-    <hyperlink ref="L106" r:id="rId197" location="page=4&amp;query=gold%20badge%20sprite&amp;position=9&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{138577BB-7F7D-D64A-806E-567F3970D250}"/>
-    <hyperlink ref="L175" r:id="rId198" xr:uid="{927B8B79-A428-2043-9B3B-555F7877CA20}"/>
-    <hyperlink ref="L193" r:id="rId199" xr:uid="{6018233D-1425-7148-A608-3B0666055EA2}"/>
-    <hyperlink ref="L217" r:id="rId200" xr:uid="{38C9843F-1665-8F46-A66C-287455700886}"/>
-    <hyperlink ref="L240" r:id="rId201" xr:uid="{9E664F43-2A79-3744-BC57-4D11914A4B9C}"/>
-    <hyperlink ref="L241" r:id="rId202" xr:uid="{F55C22EB-ADA4-064F-8C9F-34B8DFB927E8}"/>
-    <hyperlink ref="L159" r:id="rId203" xr:uid="{A1B2F4EC-ACE1-B14D-8619-0451D719CFC0}"/>
-    <hyperlink ref="L219" r:id="rId204" xr:uid="{2BF445F0-7B50-5E48-A8E5-4779F07B83CE}"/>
-    <hyperlink ref="L220" r:id="rId205" xr:uid="{6B23A3F9-85DD-4043-853E-3BF95911A2C6}"/>
-    <hyperlink ref="L221" r:id="rId206" xr:uid="{A975FD98-A3FE-5B40-9F31-D14EAE3777F9}"/>
-    <hyperlink ref="L244" r:id="rId207" xr:uid="{F01C8569-23FB-7F4C-A50B-40979911E1B8}"/>
-    <hyperlink ref="L247" r:id="rId208" xr:uid="{B54ABD16-F1A6-DC45-B36E-0CC72B423F70}"/>
-    <hyperlink ref="L245" r:id="rId209" xr:uid="{EBA532A6-AAFD-E54D-BD41-CC4F5F92AF68}"/>
-    <hyperlink ref="L246" r:id="rId210" xr:uid="{0F422DA4-046E-F246-BC4A-695F255E6851}"/>
-    <hyperlink ref="L201" r:id="rId211" xr:uid="{1F9FD82A-7BDA-7143-B89F-0DBBBC864386}"/>
-    <hyperlink ref="L202" r:id="rId212" xr:uid="{7F1F0626-5319-784B-97DE-B956AE96359D}"/>
+    <hyperlink ref="L130" r:id="rId123" xr:uid="{4BFCF1BE-6310-C34B-BA09-218F6A3C75D9}"/>
+    <hyperlink ref="L132" r:id="rId124" xr:uid="{C9C421A7-64D0-5D49-9F28-B71BC19F3239}"/>
+    <hyperlink ref="L159" r:id="rId125" xr:uid="{F88953B7-468E-C34B-9347-94009F9A78D2}"/>
+    <hyperlink ref="L199" r:id="rId126" xr:uid="{1F3BBC8C-29E8-C74A-AB3F-04AE466222EF}"/>
+    <hyperlink ref="L201" r:id="rId127" xr:uid="{3C51058F-793C-D34A-8286-18AE4C8EF6CE}"/>
+    <hyperlink ref="L244" r:id="rId128" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
+    <hyperlink ref="L156" r:id="rId129" xr:uid="{6A722A1D-2F7B-4242-8134-716EFF33F7D2}"/>
+    <hyperlink ref="L157" r:id="rId130" xr:uid="{547CD1A8-1967-1C46-95E3-89E39CD045C2}"/>
+    <hyperlink ref="L204" r:id="rId131" xr:uid="{5ACD6BFD-52F0-0940-AA8E-B04F1D397BC7}"/>
+    <hyperlink ref="L240" r:id="rId132" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
+    <hyperlink ref="L200" r:id="rId133" xr:uid="{2030AD8C-28A7-544B-92DC-5CBE411DE1C0}"/>
+    <hyperlink ref="L229" r:id="rId134" xr:uid="{05363CA1-BE60-3F42-B56A-1A92A0EDA166}"/>
+    <hyperlink ref="L192" r:id="rId135" xr:uid="{D4C66DCB-D6B4-EC4F-A922-B87887BE6E4A}"/>
+    <hyperlink ref="L191" r:id="rId136" xr:uid="{A05D9F8A-ED0A-4143-8920-9422DD4E0BDD}"/>
+    <hyperlink ref="L193" r:id="rId137" xr:uid="{83FA4EC1-AB5E-3B43-9476-4CA54526DF8E}"/>
+    <hyperlink ref="L172" r:id="rId138" xr:uid="{21B7C9CB-274E-C246-8989-83D9E0E7B24F}"/>
+    <hyperlink ref="L168" r:id="rId139" xr:uid="{B5B4FA15-B24C-CE46-9594-7ED28656AA43}"/>
+    <hyperlink ref="L169" r:id="rId140" xr:uid="{3AB6BE1F-95C1-A443-B12D-D7A523FAD6C5}"/>
+    <hyperlink ref="L170" r:id="rId141" xr:uid="{347BDCC2-5A0C-B249-8CA8-B72D245480FC}"/>
+    <hyperlink ref="L171" r:id="rId142" xr:uid="{E58DD28D-BD99-DF44-9E5E-B3D05F881C1F}"/>
+    <hyperlink ref="L232" r:id="rId143" xr:uid="{4F668E79-3664-0547-B3D5-B7724A9D574D}"/>
+    <hyperlink ref="L230" r:id="rId144" xr:uid="{8AB5C10C-8B45-1843-96BD-655A4FA04EFD}"/>
+    <hyperlink ref="L175" r:id="rId145" xr:uid="{EAED74E0-13EE-A046-9ADC-AC8BDE30C3E6}"/>
+    <hyperlink ref="L237" r:id="rId146" xr:uid="{3577256C-215B-134E-B541-B7B77272CD8A}"/>
+    <hyperlink ref="L238" r:id="rId147" xr:uid="{98E325FC-7F95-B44E-98EB-DE0FF53BC89D}"/>
+    <hyperlink ref="L231" r:id="rId148" xr:uid="{5CE3083F-F217-3743-B613-A7DDF354E72D}"/>
+    <hyperlink ref="L233" r:id="rId149" xr:uid="{B81B6B41-2C17-AA48-B730-D906488BA0A0}"/>
+    <hyperlink ref="L181" r:id="rId150" xr:uid="{BA0813A2-2582-7A46-A492-16A943824EE5}"/>
+    <hyperlink ref="L239" r:id="rId151" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
+    <hyperlink ref="L234" r:id="rId152" xr:uid="{C5265333-F7F0-1845-98D7-68E930F9DFAE}"/>
+    <hyperlink ref="L183" r:id="rId153" xr:uid="{C0A159CB-3986-1A46-95AD-DCEFF4247697}"/>
+    <hyperlink ref="L173" r:id="rId154" xr:uid="{37810A74-E45D-1D46-AEF5-C5FE2F414285}"/>
+    <hyperlink ref="L228" r:id="rId155" xr:uid="{D2906064-B1B8-4648-8201-BEFA97591226}"/>
+    <hyperlink ref="L161" r:id="rId156" xr:uid="{1D3CD52E-7AAD-E444-88F4-4BAE6C5B5EB7}"/>
+    <hyperlink ref="L162" r:id="rId157" xr:uid="{E6E6DA47-945D-6145-912F-08B17B7BA6AE}"/>
+    <hyperlink ref="L163" r:id="rId158" xr:uid="{006B1689-D89A-1E4A-BBC5-E9C9583907F7}"/>
+    <hyperlink ref="L164" r:id="rId159" xr:uid="{C3E773B2-D410-AF41-B197-4638485DC8EF}"/>
+    <hyperlink ref="L165" r:id="rId160" xr:uid="{A0E8A8E2-4A93-3D42-AF48-81955241A483}"/>
+    <hyperlink ref="L166" r:id="rId161" xr:uid="{1B03F18A-8745-AA4F-AA8B-88D65D3B24BC}"/>
+    <hyperlink ref="L245" r:id="rId162" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
+    <hyperlink ref="L250" r:id="rId163" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
+    <hyperlink ref="L189" r:id="rId164" xr:uid="{D6B77117-A0D5-9240-8193-0102C36CCE4C}"/>
+    <hyperlink ref="L190" r:id="rId165" xr:uid="{79FB1103-88A8-8044-9E2C-4FAEC0906E8E}"/>
+    <hyperlink ref="L235" r:id="rId166" xr:uid="{5BF1C4C9-E63A-4F42-9042-36520975FDFA}"/>
+    <hyperlink ref="L188" r:id="rId167" xr:uid="{21CDF460-9871-0547-AA6B-20304C8DD21D}"/>
+    <hyperlink ref="L178" r:id="rId168" xr:uid="{BA1EC844-435A-6C44-87FC-C12B7ECFC55B}"/>
+    <hyperlink ref="L177" r:id="rId169" xr:uid="{46D875DC-CDDD-7E4B-88DB-DFC416CF17AB}"/>
+    <hyperlink ref="L167" r:id="rId170" xr:uid="{7D2FF6AE-1C67-9D4A-A760-7E3745DD9EA6}"/>
+    <hyperlink ref="L218" r:id="rId171" xr:uid="{B5E5E388-8F37-414E-A0C6-1DC58E77628C}"/>
+    <hyperlink ref="L220" r:id="rId172" xr:uid="{A96B1ACF-D982-9240-BB1C-69459154AE5A}"/>
+    <hyperlink ref="L184" r:id="rId173" xr:uid="{D3BB695A-CBA9-D649-B49D-4CC8D16EFD9B}"/>
+    <hyperlink ref="L185" r:id="rId174" xr:uid="{A2922BA8-758D-3149-892C-B7B65B435332}"/>
+    <hyperlink ref="L207" r:id="rId175" xr:uid="{BDB09119-6289-4346-BC29-7A54BD393127}"/>
+    <hyperlink ref="L236" r:id="rId176" xr:uid="{5736CAF4-3646-3243-9AEB-4D82B6D0D10A}"/>
+    <hyperlink ref="L210" r:id="rId177" xr:uid="{60659D55-801C-9A4E-84CA-809884CCBE5C}"/>
+    <hyperlink ref="L197" r:id="rId178" xr:uid="{18DDC006-0939-794C-9B5D-10593F8C0973}"/>
+    <hyperlink ref="L186" r:id="rId179" xr:uid="{50EA46A5-11DD-0345-ABCA-4206D73C7606}"/>
+    <hyperlink ref="L227" r:id="rId180" xr:uid="{63DDFF3B-E62C-9445-96AD-4BB37ACCD20E}"/>
+    <hyperlink ref="L212" r:id="rId181" xr:uid="{05E34BC1-B22F-3E46-8574-E72267507402}"/>
+    <hyperlink ref="L211" r:id="rId182" xr:uid="{7125DF67-5A7E-D948-8363-A31AB1EBA44A}"/>
+    <hyperlink ref="L241" r:id="rId183" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
+    <hyperlink ref="L198" r:id="rId184" xr:uid="{CCE2D666-E296-D94C-ACE0-791CC746483B}"/>
+    <hyperlink ref="L179" r:id="rId185" xr:uid="{E5A2F3EE-A3B1-0842-9364-E4B6EACA9544}"/>
+    <hyperlink ref="L213" r:id="rId186" xr:uid="{E08C8BA4-5414-1947-9CA8-45FE0B846CD1}"/>
+    <hyperlink ref="L209" r:id="rId187" xr:uid="{F1A64091-5BF7-8243-B7A0-F4C13B8B0ABB}"/>
+    <hyperlink ref="L195" r:id="rId188" xr:uid="{745AEF03-3150-C54B-800A-696460474256}"/>
+    <hyperlink ref="L196" r:id="rId189" xr:uid="{9C078FBA-3B11-8049-9187-5BC86D78EA09}"/>
+    <hyperlink ref="L180" r:id="rId190" xr:uid="{BF9A6A48-C664-FA4B-A769-D87460BB9387}"/>
+    <hyperlink ref="L182" r:id="rId191" xr:uid="{11E0C06F-BBA9-B446-A3A4-5862C893161B}"/>
+    <hyperlink ref="L208" r:id="rId192" xr:uid="{D5E45024-1B58-714D-9576-1FA969BDADD9}"/>
+    <hyperlink ref="L187" r:id="rId193" xr:uid="{D160676D-AC82-D243-B9A9-56033B0A6EFE}"/>
+    <hyperlink ref="L205" r:id="rId194" xr:uid="{3DB54A74-68B7-734A-BC3C-BFE4E2E4103E}"/>
+    <hyperlink ref="L104" r:id="rId195" xr:uid="{4686296B-C235-4048-A384-BE461895E2AC}"/>
+    <hyperlink ref="L106" r:id="rId196" location="page=2&amp;query=gold%20badge%20sprite&amp;position=49&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{061AB839-ADB1-BA47-A152-68CDFE8A1979}"/>
+    <hyperlink ref="L107" r:id="rId197" location="page=4&amp;query=gold%20badge%20sprite&amp;position=9&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{138577BB-7F7D-D64A-806E-567F3970D250}"/>
+    <hyperlink ref="L176" r:id="rId198" xr:uid="{927B8B79-A428-2043-9B3B-555F7877CA20}"/>
+    <hyperlink ref="L194" r:id="rId199" xr:uid="{6018233D-1425-7148-A608-3B0666055EA2}"/>
+    <hyperlink ref="L219" r:id="rId200" xr:uid="{38C9843F-1665-8F46-A66C-287455700886}"/>
+    <hyperlink ref="L242" r:id="rId201" xr:uid="{9E664F43-2A79-3744-BC57-4D11914A4B9C}"/>
+    <hyperlink ref="L243" r:id="rId202" xr:uid="{F55C22EB-ADA4-064F-8C9F-34B8DFB927E8}"/>
+    <hyperlink ref="L160" r:id="rId203" xr:uid="{A1B2F4EC-ACE1-B14D-8619-0451D719CFC0}"/>
+    <hyperlink ref="L221" r:id="rId204" xr:uid="{2BF445F0-7B50-5E48-A8E5-4779F07B83CE}"/>
+    <hyperlink ref="L222" r:id="rId205" xr:uid="{6B23A3F9-85DD-4043-853E-3BF95911A2C6}"/>
+    <hyperlink ref="L223" r:id="rId206" xr:uid="{A975FD98-A3FE-5B40-9F31-D14EAE3777F9}"/>
+    <hyperlink ref="L246" r:id="rId207" xr:uid="{F01C8569-23FB-7F4C-A50B-40979911E1B8}"/>
+    <hyperlink ref="L249" r:id="rId208" xr:uid="{B54ABD16-F1A6-DC45-B36E-0CC72B423F70}"/>
+    <hyperlink ref="L247" r:id="rId209" xr:uid="{EBA532A6-AAFD-E54D-BD41-CC4F5F92AF68}"/>
+    <hyperlink ref="L248" r:id="rId210" xr:uid="{0F422DA4-046E-F246-BC4A-695F255E6851}"/>
+    <hyperlink ref="L202" r:id="rId211" xr:uid="{1F9FD82A-7BDA-7143-B89F-0DBBBC864386}"/>
+    <hyperlink ref="L203" r:id="rId212" xr:uid="{7F1F0626-5319-784B-97DE-B956AE96359D}"/>
+    <hyperlink ref="L206" r:id="rId213" xr:uid="{B2599288-37DA-884B-A5E6-897FBCE08F4D}"/>
+    <hyperlink ref="L83" r:id="rId214" location="page=2&amp;query=light%20beam&amp;position=25&amp;from_view=search&amp;track=ais&amp;uuid=063fa81a-19de-4aad-b5fc-7caa6fa59141#position=25&amp;page=2&amp;query=light%20beam" xr:uid="{F7D7C1C4-CC10-FA4D-8194-8E6ECD655D52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Minor Bug Fixes and New Sounds, Version 1.22 (24) Update build to 1.22 (24) AssetsCatalog: update chatopentrainer, add winlevelice, gameoverice. Levels17MoveList: update 204. Sounds: update chatopentrainer, add gameoverice.mp3, winlevelice.mp3. ChatEngine: use AudioManager.shared.playSoundThenStop() for littlegirllaugh instead of 2 lines - playSound(), stopSound() which bypasses the sound off settings toggle. GameEngine: use new FireIceTheme.soundWinLevel and .musicGameOver sounds. FireIceTheme: add soundWinLevel and musicGameOver properties. AudioManager: add winlevelice and gameoverice sound items GameboardSprite: use playSoundThenStop() for waterappear...
</commit_message>
<xml_diff>
--- a/JSON/AssetsCatalog.xlsx
+++ b/JSON/AssetsCatalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D529BA-B70F-1146-9A16-CBD093A562CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCAD26A-9869-834B-8DD2-372B19B07E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42040" yWindow="1620" windowWidth="36000" windowHeight="21040" xr2:uid="{E84333C6-E3B6-FB42-AB04-827399F33810}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$259</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$260</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2208" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="639">
   <si>
     <t>Filename</t>
   </si>
@@ -1859,12 +1859,6 @@
     <t>BackgroundSounds</t>
   </si>
   <si>
-    <t>https://audiojungle.net/item/magical-spell-poof/14123841</t>
-  </si>
-  <si>
-    <t>Magical Spell Poof</t>
-  </si>
-  <si>
     <t>https://audiojungle.net/item/metallic-dark-magic-spell/25707672</t>
   </si>
   <si>
@@ -1929,6 +1923,39 @@
   </si>
   <si>
     <t>https://audiojungle.net/item/winter-dream/46766831</t>
+  </si>
+  <si>
+    <t>Pop Up Bonus</t>
+  </si>
+  <si>
+    <t>back17ground</t>
+  </si>
+  <si>
+    <t>https://audiojungle.net/item/pop-up-bonus/29164837</t>
+  </si>
+  <si>
+    <t>gameoverice</t>
+  </si>
+  <si>
+    <t>https://audiojungle.net/item/fail-game-lose-level-31/19129693</t>
+  </si>
+  <si>
+    <t>ionics</t>
+  </si>
+  <si>
+    <t>Fail Game Lose Level 31</t>
+  </si>
+  <si>
+    <t>winlevelice</t>
+  </si>
+  <si>
+    <t>https://audiojungle.net/item/win-and-level-up-1/15471120</t>
+  </si>
+  <si>
+    <t>Win and Level Up 1</t>
+  </si>
+  <si>
+    <t>BANT</t>
   </si>
 </sst>
 </file>
@@ -2350,13 +2377,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}">
-  <dimension ref="A1:L259"/>
+  <dimension ref="A1:L261"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D190" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D231" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C196" sqref="C196"/>
+      <selection pane="bottomRight" activeCell="I255" sqref="I255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3390,7 +3417,7 @@
         <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
@@ -4824,7 +4851,7 @@
         <v>198</v>
       </c>
       <c r="C83" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D83" t="s">
         <v>6</v>
@@ -7964,13 +7991,13 @@
         <v>391</v>
       </c>
       <c r="I185" s="3" t="s">
-        <v>487</v>
+        <v>629</v>
       </c>
       <c r="K185" s="3" t="s">
-        <v>607</v>
+        <v>628</v>
       </c>
       <c r="L185" s="6" t="s">
-        <v>606</v>
+        <v>630</v>
       </c>
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.2">
@@ -7996,13 +8023,13 @@
         <v>391</v>
       </c>
       <c r="I186" s="3" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="K186" s="3" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L186" s="6" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.2">
@@ -8173,7 +8200,7 @@
         <v>405</v>
       </c>
       <c r="C192" s="12" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D192" t="s">
         <v>388</v>
@@ -8188,13 +8215,13 @@
         <v>391</v>
       </c>
       <c r="I192" s="3" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="K192" s="3" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="L192" s="6" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.2">
@@ -8205,7 +8232,7 @@
         <v>405</v>
       </c>
       <c r="C193" s="13" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D193" t="s">
         <v>388</v>
@@ -8220,13 +8247,13 @@
         <v>391</v>
       </c>
       <c r="I193" s="3" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="K193" s="3" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="L193" s="6" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.2">
@@ -8300,14 +8327,14 @@
       <c r="B196" t="s">
         <v>405</v>
       </c>
-      <c r="C196" t="s">
-        <v>337</v>
+      <c r="C196" s="12" t="s">
+        <v>631</v>
       </c>
       <c r="D196" t="s">
         <v>388</v>
       </c>
       <c r="F196" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G196" s="3" t="s">
         <v>174</v>
@@ -8316,13 +8343,13 @@
         <v>391</v>
       </c>
       <c r="I196" s="3" t="s">
-        <v>474</v>
+        <v>633</v>
       </c>
       <c r="K196" s="3" t="s">
-        <v>473</v>
+        <v>634</v>
       </c>
       <c r="L196" s="6" t="s">
-        <v>472</v>
+        <v>632</v>
       </c>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.2">
@@ -8333,13 +8360,13 @@
         <v>405</v>
       </c>
       <c r="C197" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D197" t="s">
         <v>388</v>
       </c>
       <c r="F197" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G197" s="3" t="s">
         <v>174</v>
@@ -8365,13 +8392,13 @@
         <v>405</v>
       </c>
       <c r="C198" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D198" t="s">
         <v>388</v>
       </c>
       <c r="F198" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G198" s="3" t="s">
         <v>174</v>
@@ -8380,13 +8407,13 @@
         <v>391</v>
       </c>
       <c r="I198" s="3" t="s">
-        <v>422</v>
+        <v>474</v>
       </c>
       <c r="K198" s="3" t="s">
-        <v>425</v>
+        <v>473</v>
       </c>
       <c r="L198" s="6" t="s">
-        <v>423</v>
+        <v>472</v>
       </c>
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.2">
@@ -8397,7 +8424,7 @@
         <v>405</v>
       </c>
       <c r="C199" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D199" t="s">
         <v>388</v>
@@ -8415,10 +8442,10 @@
         <v>422</v>
       </c>
       <c r="K199" s="3" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="L199" s="6" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.2">
@@ -8429,7 +8456,7 @@
         <v>405</v>
       </c>
       <c r="C200" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D200" t="s">
         <v>388</v>
@@ -8447,10 +8474,10 @@
         <v>422</v>
       </c>
       <c r="K200" s="3" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="L200" s="6" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.2">
@@ -8461,13 +8488,13 @@
         <v>405</v>
       </c>
       <c r="C201" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D201" t="s">
         <v>388</v>
       </c>
       <c r="F201" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G201" s="3" t="s">
         <v>174</v>
@@ -8476,13 +8503,13 @@
         <v>391</v>
       </c>
       <c r="I201" s="3" t="s">
-        <v>565</v>
+        <v>422</v>
       </c>
       <c r="K201" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="L201" s="7" t="s">
-        <v>621</v>
+        <v>424</v>
+      </c>
+      <c r="L201" s="6" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.2">
@@ -8493,28 +8520,28 @@
         <v>405</v>
       </c>
       <c r="C202" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D202" t="s">
         <v>388</v>
       </c>
-      <c r="F202" s="11">
-        <v>2</v>
+      <c r="F202" s="3">
+        <v>1</v>
       </c>
       <c r="G202" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H202" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I202" s="3" t="s">
-        <v>540</v>
+        <v>565</v>
       </c>
       <c r="K202" s="3" t="s">
-        <v>539</v>
-      </c>
-      <c r="L202" s="6" t="s">
-        <v>538</v>
+        <v>568</v>
+      </c>
+      <c r="L202" s="7" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="203" spans="1:12" x14ac:dyDescent="0.2">
@@ -8525,13 +8552,13 @@
         <v>405</v>
       </c>
       <c r="C203" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D203" t="s">
         <v>388</v>
       </c>
       <c r="F203" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G203" s="3" t="s">
         <v>432</v>
@@ -8540,13 +8567,13 @@
         <v>391</v>
       </c>
       <c r="I203" s="3" t="s">
-        <v>479</v>
+        <v>540</v>
       </c>
       <c r="K203" s="3" t="s">
         <v>539</v>
       </c>
       <c r="L203" s="6" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.2">
@@ -8557,13 +8584,13 @@
         <v>405</v>
       </c>
       <c r="C204" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D204" t="s">
         <v>388</v>
       </c>
       <c r="F204" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G204" s="3" t="s">
         <v>432</v>
@@ -8572,13 +8599,13 @@
         <v>391</v>
       </c>
       <c r="I204" s="3" t="s">
-        <v>511</v>
+        <v>479</v>
       </c>
       <c r="K204" s="3" t="s">
-        <v>512</v>
+        <v>539</v>
       </c>
       <c r="L204" s="6" t="s">
-        <v>510</v>
+        <v>541</v>
       </c>
     </row>
     <row r="205" spans="1:12" x14ac:dyDescent="0.2">
@@ -8589,13 +8616,13 @@
         <v>405</v>
       </c>
       <c r="C205" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D205" t="s">
         <v>388</v>
       </c>
       <c r="F205" s="11">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G205" s="3" t="s">
         <v>432</v>
@@ -8604,13 +8631,13 @@
         <v>391</v>
       </c>
       <c r="I205" s="3" t="s">
-        <v>528</v>
+        <v>511</v>
       </c>
       <c r="K205" s="3" t="s">
-        <v>527</v>
+        <v>512</v>
       </c>
       <c r="L205" s="6" t="s">
-        <v>526</v>
+        <v>510</v>
       </c>
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.2">
@@ -8621,28 +8648,28 @@
         <v>405</v>
       </c>
       <c r="C206" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D206" t="s">
         <v>388</v>
       </c>
-      <c r="F206" s="3">
-        <v>2</v>
+      <c r="F206" s="11">
+        <v>10</v>
       </c>
       <c r="G206" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H206" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I206" s="3" t="s">
-        <v>396</v>
+        <v>528</v>
       </c>
       <c r="K206" s="3" t="s">
-        <v>395</v>
+        <v>527</v>
       </c>
       <c r="L206" s="6" t="s">
-        <v>394</v>
+        <v>526</v>
       </c>
     </row>
     <row r="207" spans="1:12" x14ac:dyDescent="0.2">
@@ -8653,13 +8680,13 @@
         <v>405</v>
       </c>
       <c r="C207" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D207" t="s">
         <v>388</v>
       </c>
       <c r="F207" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G207" s="3" t="s">
         <v>174</v>
@@ -8668,13 +8695,13 @@
         <v>391</v>
       </c>
       <c r="I207" s="3" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="K207" s="3" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
       <c r="L207" s="6" t="s">
-        <v>415</v>
+        <v>394</v>
       </c>
     </row>
     <row r="208" spans="1:12" x14ac:dyDescent="0.2">
@@ -8685,13 +8712,13 @@
         <v>405</v>
       </c>
       <c r="C208" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D208" t="s">
         <v>388</v>
       </c>
       <c r="F208" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G208" s="3" t="s">
         <v>174</v>
@@ -8700,13 +8727,13 @@
         <v>391</v>
       </c>
       <c r="I208" s="3" t="s">
-        <v>397</v>
+        <v>411</v>
       </c>
       <c r="K208" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="L208" s="7" t="s">
-        <v>399</v>
+        <v>416</v>
+      </c>
+      <c r="L208" s="6" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.2">
@@ -8716,29 +8743,29 @@
       <c r="B209" t="s">
         <v>405</v>
       </c>
-      <c r="C209" s="12" t="s">
-        <v>589</v>
+      <c r="C209" t="s">
+        <v>349</v>
       </c>
       <c r="D209" t="s">
         <v>388</v>
       </c>
       <c r="F209" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G209" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H209" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I209" s="3" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="K209" s="3" t="s">
-        <v>587</v>
+        <v>398</v>
       </c>
       <c r="L209" s="7" t="s">
-        <v>588</v>
+        <v>399</v>
       </c>
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.2">
@@ -8749,7 +8776,7 @@
         <v>405</v>
       </c>
       <c r="C210" s="12" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D210" t="s">
         <v>388</v>
@@ -8764,13 +8791,13 @@
         <v>391</v>
       </c>
       <c r="I210" s="3" t="s">
-        <v>593</v>
+        <v>392</v>
       </c>
       <c r="K210" s="3" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="L210" s="7" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.2">
@@ -8781,7 +8808,7 @@
         <v>405</v>
       </c>
       <c r="C211" s="12" t="s">
-        <v>611</v>
+        <v>590</v>
       </c>
       <c r="D211" t="s">
         <v>388</v>
@@ -8796,13 +8823,13 @@
         <v>391</v>
       </c>
       <c r="I211" s="3" t="s">
-        <v>614</v>
+        <v>593</v>
       </c>
       <c r="K211" s="3" t="s">
-        <v>613</v>
+        <v>592</v>
       </c>
       <c r="L211" s="7" t="s">
-        <v>612</v>
+        <v>591</v>
       </c>
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.2">
@@ -8812,8 +8839,8 @@
       <c r="B212" t="s">
         <v>405</v>
       </c>
-      <c r="C212" t="s">
-        <v>350</v>
+      <c r="C212" s="12" t="s">
+        <v>609</v>
       </c>
       <c r="D212" t="s">
         <v>388</v>
@@ -8822,19 +8849,19 @@
         <v>1</v>
       </c>
       <c r="G212" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H212" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I212" s="3" t="s">
-        <v>411</v>
+        <v>612</v>
       </c>
       <c r="K212" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="L212" s="6" t="s">
-        <v>409</v>
+        <v>611</v>
+      </c>
+      <c r="L212" s="7" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.2">
@@ -8845,28 +8872,28 @@
         <v>405</v>
       </c>
       <c r="C213" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D213" t="s">
         <v>388</v>
       </c>
-      <c r="F213" s="11">
-        <v>2</v>
+      <c r="F213" s="3">
+        <v>1</v>
       </c>
       <c r="G213" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H213" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I213" s="3" t="s">
-        <v>552</v>
+        <v>411</v>
       </c>
       <c r="K213" s="3" t="s">
-        <v>551</v>
+        <v>410</v>
       </c>
       <c r="L213" s="6" t="s">
-        <v>550</v>
+        <v>409</v>
       </c>
     </row>
     <row r="214" spans="1:12" x14ac:dyDescent="0.2">
@@ -8876,14 +8903,14 @@
       <c r="B214" t="s">
         <v>405</v>
       </c>
-      <c r="C214" s="12" t="s">
-        <v>594</v>
+      <c r="C214" t="s">
+        <v>351</v>
       </c>
       <c r="D214" t="s">
         <v>388</v>
       </c>
-      <c r="F214" s="3">
-        <v>1</v>
+      <c r="F214" s="11">
+        <v>2</v>
       </c>
       <c r="G214" s="3" t="s">
         <v>432</v>
@@ -8892,13 +8919,13 @@
         <v>391</v>
       </c>
       <c r="I214" s="3" t="s">
-        <v>487</v>
+        <v>552</v>
       </c>
       <c r="K214" s="3" t="s">
-        <v>595</v>
+        <v>551</v>
       </c>
       <c r="L214" s="6" t="s">
-        <v>596</v>
+        <v>550</v>
       </c>
     </row>
     <row r="215" spans="1:12" x14ac:dyDescent="0.2">
@@ -8908,29 +8935,29 @@
       <c r="B215" t="s">
         <v>405</v>
       </c>
-      <c r="C215" t="s">
-        <v>352</v>
+      <c r="C215" s="12" t="s">
+        <v>594</v>
       </c>
       <c r="D215" t="s">
         <v>388</v>
       </c>
       <c r="F215" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G215" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H215" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I215" s="3" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="K215" s="3" t="s">
-        <v>503</v>
+        <v>595</v>
       </c>
       <c r="L215" s="6" t="s">
-        <v>502</v>
+        <v>596</v>
       </c>
     </row>
     <row r="216" spans="1:12" x14ac:dyDescent="0.2">
@@ -8941,7 +8968,7 @@
         <v>405</v>
       </c>
       <c r="C216" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D216" t="s">
         <v>388</v>
@@ -8956,13 +8983,13 @@
         <v>391</v>
       </c>
       <c r="I216" s="3" t="s">
-        <v>537</v>
+        <v>501</v>
       </c>
       <c r="K216" s="3" t="s">
-        <v>536</v>
+        <v>503</v>
       </c>
       <c r="L216" s="6" t="s">
-        <v>535</v>
+        <v>502</v>
       </c>
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.2">
@@ -8973,13 +9000,13 @@
         <v>405</v>
       </c>
       <c r="C217" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D217" t="s">
         <v>388</v>
       </c>
       <c r="F217" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G217" s="3" t="s">
         <v>174</v>
@@ -9005,13 +9032,13 @@
         <v>405</v>
       </c>
       <c r="C218" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D218" t="s">
         <v>388</v>
       </c>
       <c r="F218" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G218" s="3" t="s">
         <v>174</v>
@@ -9020,13 +9047,13 @@
         <v>391</v>
       </c>
       <c r="I218" s="3" t="s">
-        <v>509</v>
+        <v>537</v>
       </c>
       <c r="K218" s="3" t="s">
-        <v>508</v>
+        <v>536</v>
       </c>
       <c r="L218" s="6" t="s">
-        <v>507</v>
+        <v>535</v>
       </c>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.2">
@@ -9037,13 +9064,13 @@
         <v>405</v>
       </c>
       <c r="C219" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D219" t="s">
         <v>388</v>
       </c>
       <c r="F219" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G219" s="3" t="s">
         <v>174</v>
@@ -9052,13 +9079,13 @@
         <v>391</v>
       </c>
       <c r="I219" s="3" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="K219" s="3" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="L219" s="6" t="s">
-        <v>520</v>
+        <v>507</v>
       </c>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.2">
@@ -9069,13 +9096,13 @@
         <v>405</v>
       </c>
       <c r="C220" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D220" t="s">
         <v>388</v>
       </c>
       <c r="F220" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G220" s="3" t="s">
         <v>174</v>
@@ -9084,13 +9111,13 @@
         <v>391</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="K220" s="3" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="L220" s="6" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.2">
@@ -9101,7 +9128,7 @@
         <v>405</v>
       </c>
       <c r="C221" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D221" t="s">
         <v>388</v>
@@ -9116,13 +9143,13 @@
         <v>391</v>
       </c>
       <c r="I221" s="3" t="s">
-        <v>534</v>
+        <v>519</v>
       </c>
       <c r="K221" s="3" t="s">
-        <v>533</v>
+        <v>518</v>
       </c>
       <c r="L221" s="6" t="s">
-        <v>532</v>
+        <v>517</v>
       </c>
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.2">
@@ -9133,7 +9160,7 @@
         <v>405</v>
       </c>
       <c r="C222" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D222" t="s">
         <v>388</v>
@@ -9148,13 +9175,13 @@
         <v>391</v>
       </c>
       <c r="I222" s="3" t="s">
-        <v>501</v>
+        <v>534</v>
       </c>
       <c r="K222" s="3" t="s">
-        <v>500</v>
+        <v>533</v>
       </c>
       <c r="L222" s="6" t="s">
-        <v>499</v>
+        <v>532</v>
       </c>
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.2">
@@ -9165,13 +9192,13 @@
         <v>405</v>
       </c>
       <c r="C223" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D223" t="s">
         <v>388</v>
       </c>
       <c r="F223" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G223" s="3" t="s">
         <v>174</v>
@@ -9197,7 +9224,7 @@
         <v>405</v>
       </c>
       <c r="C224" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D224" t="s">
         <v>388</v>
@@ -9229,7 +9256,7 @@
         <v>405</v>
       </c>
       <c r="C225" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D225" t="s">
         <v>388</v>
@@ -9261,13 +9288,13 @@
         <v>405</v>
       </c>
       <c r="C226" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D226" t="s">
         <v>388</v>
       </c>
       <c r="F226" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G226" s="3" t="s">
         <v>174</v>
@@ -9276,13 +9303,13 @@
         <v>391</v>
       </c>
       <c r="I226" s="3" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="K226" s="3" t="s">
-        <v>491</v>
+        <v>500</v>
       </c>
       <c r="L226" s="6" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.2">
@@ -9293,13 +9320,13 @@
         <v>405</v>
       </c>
       <c r="C227" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D227" t="s">
         <v>388</v>
       </c>
       <c r="F227" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G227" s="3" t="s">
         <v>174</v>
@@ -9325,28 +9352,28 @@
         <v>405</v>
       </c>
       <c r="C228" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D228" t="s">
         <v>388</v>
       </c>
-      <c r="F228" s="11">
-        <v>5</v>
+      <c r="F228" s="3">
+        <v>0</v>
       </c>
       <c r="G228" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H228" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I228" s="3" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="K228" s="3" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="L228" s="6" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.2">
@@ -9356,14 +9383,14 @@
       <c r="B229" t="s">
         <v>405</v>
       </c>
-      <c r="C229" s="9" t="s">
-        <v>575</v>
+      <c r="C229" t="s">
+        <v>365</v>
       </c>
       <c r="D229" t="s">
         <v>388</v>
       </c>
       <c r="F229" s="11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G229" s="3" t="s">
         <v>432</v>
@@ -9372,13 +9399,13 @@
         <v>391</v>
       </c>
       <c r="I229" s="3" t="s">
-        <v>578</v>
+        <v>494</v>
       </c>
       <c r="K229" s="3" t="s">
-        <v>579</v>
+        <v>493</v>
       </c>
       <c r="L229" s="6" t="s">
-        <v>580</v>
+        <v>492</v>
       </c>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.2">
@@ -9389,13 +9416,13 @@
         <v>405</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D230" t="s">
         <v>388</v>
       </c>
       <c r="F230" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G230" s="3" t="s">
         <v>432</v>
@@ -9421,7 +9448,7 @@
         <v>405</v>
       </c>
       <c r="C231" s="9" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="D231" t="s">
         <v>388</v>
@@ -9452,29 +9479,29 @@
       <c r="B232" t="s">
         <v>405</v>
       </c>
-      <c r="C232" t="s">
-        <v>366</v>
+      <c r="C232" s="9" t="s">
+        <v>576</v>
       </c>
       <c r="D232" t="s">
         <v>388</v>
       </c>
-      <c r="F232" s="3">
-        <v>3</v>
+      <c r="F232" s="11">
+        <v>0</v>
       </c>
       <c r="G232" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H232" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I232" s="3" t="s">
-        <v>487</v>
+        <v>578</v>
       </c>
       <c r="K232" s="3" t="s">
-        <v>489</v>
+        <v>579</v>
       </c>
       <c r="L232" s="6" t="s">
-        <v>488</v>
+        <v>580</v>
       </c>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.2">
@@ -9485,13 +9512,13 @@
         <v>405</v>
       </c>
       <c r="C233" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D233" t="s">
         <v>388</v>
       </c>
       <c r="F233" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G233" s="3" t="s">
         <v>174</v>
@@ -9517,7 +9544,7 @@
         <v>405</v>
       </c>
       <c r="C234" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D234" t="s">
         <v>388</v>
@@ -9549,60 +9576,60 @@
         <v>405</v>
       </c>
       <c r="C235" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D235" t="s">
         <v>388</v>
       </c>
-      <c r="F235" s="11">
-        <v>3</v>
+      <c r="F235" s="3">
+        <v>0</v>
       </c>
       <c r="G235" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H235" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I235" s="3" t="s">
-        <v>396</v>
+        <v>487</v>
       </c>
       <c r="K235" s="3" t="s">
-        <v>516</v>
+        <v>489</v>
       </c>
       <c r="L235" s="6" t="s">
-        <v>515</v>
+        <v>488</v>
       </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B236" t="s">
         <v>405</v>
       </c>
       <c r="C236" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D236" t="s">
         <v>388</v>
       </c>
-      <c r="F236" s="3">
-        <v>15</v>
+      <c r="F236" s="11">
+        <v>3</v>
       </c>
       <c r="G236" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H236" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I236" s="3" t="s">
-        <v>463</v>
+        <v>396</v>
       </c>
       <c r="K236" s="3" t="s">
-        <v>462</v>
+        <v>516</v>
       </c>
       <c r="L236" s="6" t="s">
-        <v>461</v>
+        <v>515</v>
       </c>
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.2">
@@ -9613,13 +9640,13 @@
         <v>405</v>
       </c>
       <c r="C237" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D237" t="s">
         <v>388</v>
       </c>
       <c r="F237" s="3">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G237" s="3" t="s">
         <v>174</v>
@@ -9628,13 +9655,13 @@
         <v>391</v>
       </c>
       <c r="I237" s="3" t="s">
-        <v>419</v>
+        <v>463</v>
       </c>
       <c r="K237" s="3" t="s">
-        <v>418</v>
+        <v>462</v>
       </c>
       <c r="L237" s="6" t="s">
-        <v>417</v>
+        <v>461</v>
       </c>
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.2">
@@ -9644,29 +9671,29 @@
       <c r="B238" t="s">
         <v>405</v>
       </c>
-      <c r="C238" s="13" t="s">
-        <v>626</v>
+      <c r="C238" t="s">
+        <v>371</v>
       </c>
       <c r="D238" t="s">
         <v>388</v>
       </c>
       <c r="F238" s="3">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G238" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H238" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I238" s="3" t="s">
-        <v>627</v>
+        <v>419</v>
       </c>
       <c r="K238" s="3" t="s">
-        <v>628</v>
+        <v>418</v>
       </c>
       <c r="L238" s="6" t="s">
-        <v>629</v>
+        <v>417</v>
       </c>
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.2">
@@ -9676,46 +9703,46 @@
       <c r="B239" t="s">
         <v>405</v>
       </c>
-      <c r="C239" t="s">
-        <v>372</v>
+      <c r="C239" s="12" t="s">
+        <v>624</v>
       </c>
       <c r="D239" t="s">
         <v>388</v>
       </c>
       <c r="F239" s="3">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G239" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H239" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I239" s="3" t="s">
-        <v>435</v>
+        <v>625</v>
       </c>
       <c r="K239" s="3" t="s">
-        <v>434</v>
+        <v>626</v>
       </c>
       <c r="L239" s="6" t="s">
-        <v>433</v>
+        <v>627</v>
       </c>
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B240" t="s">
         <v>405</v>
       </c>
       <c r="C240" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D240" t="s">
         <v>388</v>
       </c>
       <c r="F240" s="3">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="G240" s="3" t="s">
         <v>174</v>
@@ -9724,13 +9751,13 @@
         <v>391</v>
       </c>
       <c r="I240" s="3" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="K240" s="3" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
       <c r="L240" s="6" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.2">
@@ -9741,13 +9768,13 @@
         <v>405</v>
       </c>
       <c r="C241" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D241" t="s">
         <v>388</v>
       </c>
       <c r="F241" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G241" s="3" t="s">
         <v>174</v>
@@ -9756,13 +9783,13 @@
         <v>391</v>
       </c>
       <c r="I241" s="3" t="s">
-        <v>411</v>
+        <v>446</v>
       </c>
       <c r="K241" s="3" t="s">
-        <v>431</v>
+        <v>445</v>
       </c>
       <c r="L241" s="6" t="s">
-        <v>430</v>
+        <v>444</v>
       </c>
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.2">
@@ -9773,13 +9800,13 @@
         <v>405</v>
       </c>
       <c r="C242" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D242" t="s">
         <v>388</v>
       </c>
       <c r="F242" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G242" s="3" t="s">
         <v>174</v>
@@ -9788,13 +9815,13 @@
         <v>391</v>
       </c>
       <c r="I242" s="3" t="s">
-        <v>446</v>
+        <v>411</v>
       </c>
       <c r="K242" s="3" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
       <c r="L242" s="6" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.2">
@@ -9805,13 +9832,13 @@
         <v>405</v>
       </c>
       <c r="C243" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D243" t="s">
         <v>388</v>
       </c>
       <c r="F243" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G243" s="3" t="s">
         <v>174</v>
@@ -9820,13 +9847,13 @@
         <v>391</v>
       </c>
       <c r="I243" s="3" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="K243" s="3" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="L243" s="6" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.2">
@@ -9837,7 +9864,7 @@
         <v>405</v>
       </c>
       <c r="C244" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D244" t="s">
         <v>388</v>
@@ -9852,13 +9879,13 @@
         <v>391</v>
       </c>
       <c r="I244" s="3" t="s">
-        <v>411</v>
+        <v>454</v>
       </c>
       <c r="K244" s="3" t="s">
-        <v>476</v>
+        <v>453</v>
       </c>
       <c r="L244" s="6" t="s">
-        <v>475</v>
+        <v>452</v>
       </c>
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.2">
@@ -9869,13 +9896,13 @@
         <v>405</v>
       </c>
       <c r="C245" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D245" t="s">
         <v>388</v>
       </c>
       <c r="F245" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G245" s="3" t="s">
         <v>174</v>
@@ -9884,13 +9911,13 @@
         <v>391</v>
       </c>
       <c r="I245" s="3" t="s">
-        <v>506</v>
+        <v>411</v>
       </c>
       <c r="K245" s="3" t="s">
-        <v>505</v>
+        <v>476</v>
       </c>
       <c r="L245" s="6" t="s">
-        <v>504</v>
+        <v>475</v>
       </c>
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.2">
@@ -9901,7 +9928,7 @@
         <v>405</v>
       </c>
       <c r="C246" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D246" t="s">
         <v>388</v>
@@ -9916,13 +9943,13 @@
         <v>391</v>
       </c>
       <c r="I246" s="3" t="s">
-        <v>441</v>
+        <v>506</v>
       </c>
       <c r="K246" s="3" t="s">
-        <v>440</v>
+        <v>505</v>
       </c>
       <c r="L246" s="6" t="s">
-        <v>439</v>
+        <v>504</v>
       </c>
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.2">
@@ -9933,13 +9960,13 @@
         <v>405</v>
       </c>
       <c r="C247" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D247" t="s">
         <v>388</v>
       </c>
       <c r="F247" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G247" s="3" t="s">
         <v>174</v>
@@ -9948,13 +9975,13 @@
         <v>391</v>
       </c>
       <c r="I247" s="3" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="K247" s="3" t="s">
         <v>440</v>
       </c>
       <c r="L247" s="6" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.2">
@@ -9965,13 +9992,13 @@
         <v>405</v>
       </c>
       <c r="C248" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D248" t="s">
         <v>388</v>
       </c>
       <c r="F248" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G248" s="3" t="s">
         <v>174</v>
@@ -9980,30 +10007,30 @@
         <v>391</v>
       </c>
       <c r="I248" s="3" t="s">
-        <v>411</v>
+        <v>443</v>
       </c>
       <c r="K248" s="3" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="L248" s="6" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B249" t="s">
         <v>405</v>
       </c>
       <c r="C249" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D249" t="s">
         <v>388</v>
       </c>
       <c r="F249" s="3">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="G249" s="3" t="s">
         <v>174</v>
@@ -10012,45 +10039,45 @@
         <v>391</v>
       </c>
       <c r="I249" s="3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="K249" s="3" t="s">
-        <v>413</v>
+        <v>451</v>
       </c>
       <c r="L249" s="6" t="s">
-        <v>412</v>
+        <v>450</v>
       </c>
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B250" t="s">
         <v>405</v>
       </c>
       <c r="C250" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D250" t="s">
         <v>388</v>
       </c>
-      <c r="F250" s="11">
-        <v>2</v>
+      <c r="F250" s="3">
+        <v>21</v>
       </c>
       <c r="G250" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H250" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I250" s="3" t="s">
-        <v>525</v>
+        <v>414</v>
       </c>
       <c r="K250" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="L250" s="10" t="s">
-        <v>523</v>
+        <v>413</v>
+      </c>
+      <c r="L250" s="6" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.2">
@@ -10061,29 +10088,28 @@
         <v>405</v>
       </c>
       <c r="C251" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D251" t="s">
         <v>388</v>
       </c>
-      <c r="F251" s="3">
-        <v>1</v>
+      <c r="F251" s="11">
+        <v>2</v>
       </c>
       <c r="G251" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H251" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I251" t="s">
-        <v>572</v>
-      </c>
-      <c r="J251"/>
-      <c r="K251" t="s">
-        <v>573</v>
-      </c>
-      <c r="L251" s="6" t="s">
-        <v>574</v>
+      <c r="I251" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="K251" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="L251" s="10" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.2">
@@ -10094,7 +10120,7 @@
         <v>405</v>
       </c>
       <c r="C252" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D252" t="s">
         <v>388</v>
@@ -10109,31 +10135,31 @@
         <v>391</v>
       </c>
       <c r="I252" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="J252"/>
       <c r="K252" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="L252" s="6" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B253" t="s">
         <v>405</v>
       </c>
       <c r="C253" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D253" t="s">
         <v>388</v>
       </c>
       <c r="F253" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G253" s="3" t="s">
         <v>174</v>
@@ -10141,31 +10167,32 @@
       <c r="H253" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I253" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="K253" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="L253" s="7" t="s">
-        <v>404</v>
+      <c r="I253" t="s">
+        <v>569</v>
+      </c>
+      <c r="J253"/>
+      <c r="K253" t="s">
+        <v>570</v>
+      </c>
+      <c r="L253" s="6" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B254" t="s">
         <v>405</v>
       </c>
       <c r="C254" t="s">
-        <v>58</v>
+        <v>386</v>
       </c>
       <c r="D254" t="s">
         <v>388</v>
       </c>
       <c r="F254" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G254" s="3" t="s">
         <v>174</v>
@@ -10174,13 +10201,13 @@
         <v>391</v>
       </c>
       <c r="I254" s="3" t="s">
-        <v>468</v>
+        <v>402</v>
       </c>
       <c r="K254" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="L254" s="6" t="s">
-        <v>466</v>
+        <v>403</v>
+      </c>
+      <c r="L254" s="7" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.2">
@@ -10190,29 +10217,29 @@
       <c r="B255" t="s">
         <v>405</v>
       </c>
-      <c r="C255" s="9" t="s">
-        <v>581</v>
+      <c r="C255" t="s">
+        <v>58</v>
       </c>
       <c r="D255" t="s">
         <v>388</v>
       </c>
-      <c r="F255" s="11">
+      <c r="F255" s="3">
         <v>1</v>
       </c>
       <c r="G255" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H255" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I255" s="3" t="s">
-        <v>392</v>
+        <v>468</v>
       </c>
       <c r="K255" s="3" t="s">
-        <v>586</v>
+        <v>467</v>
       </c>
       <c r="L255" s="6" t="s">
-        <v>585</v>
+        <v>466</v>
       </c>
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.2">
@@ -10229,7 +10256,7 @@
         <v>388</v>
       </c>
       <c r="F256" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G256" s="3" t="s">
         <v>432</v>
@@ -10287,13 +10314,13 @@
         <v>405</v>
       </c>
       <c r="C258" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D258" t="s">
         <v>388</v>
       </c>
       <c r="F258" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G258" s="3" t="s">
         <v>432</v>
@@ -10302,13 +10329,13 @@
         <v>391</v>
       </c>
       <c r="I258" s="3" t="s">
-        <v>537</v>
+        <v>392</v>
       </c>
       <c r="K258" s="3" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="L258" s="6" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.2">
@@ -10318,33 +10345,97 @@
       <c r="B259" t="s">
         <v>405</v>
       </c>
-      <c r="C259" t="s">
-        <v>387</v>
+      <c r="C259" s="9" t="s">
+        <v>582</v>
       </c>
       <c r="D259" t="s">
         <v>388</v>
       </c>
-      <c r="F259" s="3">
+      <c r="F259" s="11">
         <v>1</v>
       </c>
       <c r="G259" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H259" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I259" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="K259" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="L259" s="6" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>389</v>
+      </c>
+      <c r="B260" t="s">
+        <v>405</v>
+      </c>
+      <c r="C260" t="s">
+        <v>387</v>
+      </c>
+      <c r="D260" t="s">
+        <v>388</v>
+      </c>
+      <c r="F260" s="3">
+        <v>1</v>
+      </c>
+      <c r="G260" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H260" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I260" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="K259" s="3" t="s">
+      <c r="K260" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="L259" s="6" t="s">
+      <c r="L260" s="6" t="s">
         <v>469</v>
       </c>
     </row>
+    <row r="261" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>389</v>
+      </c>
+      <c r="B261" t="s">
+        <v>405</v>
+      </c>
+      <c r="C261" s="12" t="s">
+        <v>635</v>
+      </c>
+      <c r="D261" t="s">
+        <v>388</v>
+      </c>
+      <c r="F261" s="3">
+        <v>1</v>
+      </c>
+      <c r="G261" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H261" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I261" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="K261" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="L261" s="6" t="s">
+        <v>636</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L259" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}"/>
+  <autoFilter ref="A1:L260" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}"/>
   <hyperlinks>
     <hyperlink ref="L3" r:id="rId1" location="query=target&amp;position=0&amp;from_view=search&amp;track=sph&amp;uuid=07a631b0-afe2-4d83-9076-a80360e62f2f" xr:uid="{6340FD26-01F6-9246-82E5-C8936FBB7B36}"/>
     <hyperlink ref="L4" r:id="rId2" location="query=spell%20book&amp;position=12&amp;from_view=keyword&amp;track=ais&amp;uuid=3aa8f740-41d0-409e-b03b-268281a69be6" xr:uid="{1A91BF66-CE85-304F-BBE7-7F8EBE53C285}"/>
@@ -10471,94 +10562,94 @@
     <hyperlink ref="L132" r:id="rId123" xr:uid="{4BFCF1BE-6310-C34B-BA09-218F6A3C75D9}"/>
     <hyperlink ref="L134" r:id="rId124" xr:uid="{C9C421A7-64D0-5D49-9F28-B71BC19F3239}"/>
     <hyperlink ref="L161" r:id="rId125" xr:uid="{F88953B7-468E-C34B-9347-94009F9A78D2}"/>
-    <hyperlink ref="L206" r:id="rId126" xr:uid="{1F3BBC8C-29E8-C74A-AB3F-04AE466222EF}"/>
-    <hyperlink ref="L208" r:id="rId127" xr:uid="{3C51058F-793C-D34A-8286-18AE4C8EF6CE}"/>
-    <hyperlink ref="L253" r:id="rId128" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
+    <hyperlink ref="L207" r:id="rId126" xr:uid="{1F3BBC8C-29E8-C74A-AB3F-04AE466222EF}"/>
+    <hyperlink ref="L209" r:id="rId127" xr:uid="{3C51058F-793C-D34A-8286-18AE4C8EF6CE}"/>
+    <hyperlink ref="L254" r:id="rId128" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
     <hyperlink ref="L158" r:id="rId129" xr:uid="{6A722A1D-2F7B-4242-8134-716EFF33F7D2}"/>
     <hyperlink ref="L159" r:id="rId130" xr:uid="{547CD1A8-1967-1C46-95E3-89E39CD045C2}"/>
-    <hyperlink ref="L212" r:id="rId131" xr:uid="{5ACD6BFD-52F0-0940-AA8E-B04F1D397BC7}"/>
-    <hyperlink ref="L249" r:id="rId132" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
-    <hyperlink ref="L207" r:id="rId133" xr:uid="{2030AD8C-28A7-544B-92DC-5CBE411DE1C0}"/>
-    <hyperlink ref="L237" r:id="rId134" xr:uid="{05363CA1-BE60-3F42-B56A-1A92A0EDA166}"/>
-    <hyperlink ref="L199" r:id="rId135" xr:uid="{D4C66DCB-D6B4-EC4F-A922-B87887BE6E4A}"/>
-    <hyperlink ref="L198" r:id="rId136" xr:uid="{A05D9F8A-ED0A-4143-8920-9422DD4E0BDD}"/>
-    <hyperlink ref="L200" r:id="rId137" xr:uid="{83FA4EC1-AB5E-3B43-9476-4CA54526DF8E}"/>
+    <hyperlink ref="L213" r:id="rId131" xr:uid="{5ACD6BFD-52F0-0940-AA8E-B04F1D397BC7}"/>
+    <hyperlink ref="L250" r:id="rId132" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
+    <hyperlink ref="L208" r:id="rId133" xr:uid="{2030AD8C-28A7-544B-92DC-5CBE411DE1C0}"/>
+    <hyperlink ref="L238" r:id="rId134" xr:uid="{05363CA1-BE60-3F42-B56A-1A92A0EDA166}"/>
+    <hyperlink ref="L200" r:id="rId135" xr:uid="{D4C66DCB-D6B4-EC4F-A922-B87887BE6E4A}"/>
+    <hyperlink ref="L199" r:id="rId136" xr:uid="{A05D9F8A-ED0A-4143-8920-9422DD4E0BDD}"/>
+    <hyperlink ref="L201" r:id="rId137" xr:uid="{83FA4EC1-AB5E-3B43-9476-4CA54526DF8E}"/>
     <hyperlink ref="L174" r:id="rId138" xr:uid="{21B7C9CB-274E-C246-8989-83D9E0E7B24F}"/>
     <hyperlink ref="L170" r:id="rId139" xr:uid="{B5B4FA15-B24C-CE46-9594-7ED28656AA43}"/>
     <hyperlink ref="L171" r:id="rId140" xr:uid="{3AB6BE1F-95C1-A443-B12D-D7A523FAD6C5}"/>
     <hyperlink ref="L172" r:id="rId141" xr:uid="{347BDCC2-5A0C-B249-8CA8-B72D245480FC}"/>
     <hyperlink ref="L173" r:id="rId142" xr:uid="{E58DD28D-BD99-DF44-9E5E-B3D05F881C1F}"/>
-    <hyperlink ref="L241" r:id="rId143" xr:uid="{4F668E79-3664-0547-B3D5-B7724A9D574D}"/>
-    <hyperlink ref="L239" r:id="rId144" xr:uid="{8AB5C10C-8B45-1843-96BD-655A4FA04EFD}"/>
+    <hyperlink ref="L242" r:id="rId143" xr:uid="{4F668E79-3664-0547-B3D5-B7724A9D574D}"/>
+    <hyperlink ref="L240" r:id="rId144" xr:uid="{8AB5C10C-8B45-1843-96BD-655A4FA04EFD}"/>
     <hyperlink ref="L177" r:id="rId145" xr:uid="{EAED74E0-13EE-A046-9ADC-AC8BDE30C3E6}"/>
-    <hyperlink ref="L246" r:id="rId146" xr:uid="{3577256C-215B-134E-B541-B7B77272CD8A}"/>
-    <hyperlink ref="L247" r:id="rId147" xr:uid="{98E325FC-7F95-B44E-98EB-DE0FF53BC89D}"/>
-    <hyperlink ref="L240" r:id="rId148" xr:uid="{5CE3083F-F217-3743-B613-A7DDF354E72D}"/>
-    <hyperlink ref="L242" r:id="rId149" xr:uid="{B81B6B41-2C17-AA48-B730-D906488BA0A0}"/>
+    <hyperlink ref="L247" r:id="rId146" xr:uid="{3577256C-215B-134E-B541-B7B77272CD8A}"/>
+    <hyperlink ref="L248" r:id="rId147" xr:uid="{98E325FC-7F95-B44E-98EB-DE0FF53BC89D}"/>
+    <hyperlink ref="L241" r:id="rId148" xr:uid="{5CE3083F-F217-3743-B613-A7DDF354E72D}"/>
+    <hyperlink ref="L243" r:id="rId149" xr:uid="{B81B6B41-2C17-AA48-B730-D906488BA0A0}"/>
     <hyperlink ref="L183" r:id="rId150" xr:uid="{BA0813A2-2582-7A46-A492-16A943824EE5}"/>
-    <hyperlink ref="L248" r:id="rId151" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
-    <hyperlink ref="L243" r:id="rId152" xr:uid="{C5265333-F7F0-1845-98D7-68E930F9DFAE}"/>
+    <hyperlink ref="L249" r:id="rId151" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
+    <hyperlink ref="L244" r:id="rId152" xr:uid="{C5265333-F7F0-1845-98D7-68E930F9DFAE}"/>
     <hyperlink ref="L188" r:id="rId153" xr:uid="{C0A159CB-3986-1A46-95AD-DCEFF4247697}"/>
     <hyperlink ref="L175" r:id="rId154" xr:uid="{37810A74-E45D-1D46-AEF5-C5FE2F414285}"/>
-    <hyperlink ref="L236" r:id="rId155" xr:uid="{D2906064-B1B8-4648-8201-BEFA97591226}"/>
+    <hyperlink ref="L237" r:id="rId155" xr:uid="{D2906064-B1B8-4648-8201-BEFA97591226}"/>
     <hyperlink ref="L163" r:id="rId156" xr:uid="{1D3CD52E-7AAD-E444-88F4-4BAE6C5B5EB7}"/>
     <hyperlink ref="L164" r:id="rId157" xr:uid="{E6E6DA47-945D-6145-912F-08B17B7BA6AE}"/>
     <hyperlink ref="L165" r:id="rId158" xr:uid="{006B1689-D89A-1E4A-BBC5-E9C9583907F7}"/>
     <hyperlink ref="L166" r:id="rId159" xr:uid="{C3E773B2-D410-AF41-B197-4638485DC8EF}"/>
     <hyperlink ref="L167" r:id="rId160" xr:uid="{A0E8A8E2-4A93-3D42-AF48-81955241A483}"/>
     <hyperlink ref="L168" r:id="rId161" xr:uid="{1B03F18A-8745-AA4F-AA8B-88D65D3B24BC}"/>
-    <hyperlink ref="L254" r:id="rId162" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
-    <hyperlink ref="L259" r:id="rId163" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
-    <hyperlink ref="L196" r:id="rId164" xr:uid="{D6B77117-A0D5-9240-8193-0102C36CCE4C}"/>
-    <hyperlink ref="L197" r:id="rId165" xr:uid="{79FB1103-88A8-8044-9E2C-4FAEC0906E8E}"/>
-    <hyperlink ref="L244" r:id="rId166" xr:uid="{5BF1C4C9-E63A-4F42-9042-36520975FDFA}"/>
+    <hyperlink ref="L255" r:id="rId162" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
+    <hyperlink ref="L260" r:id="rId163" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
+    <hyperlink ref="L197" r:id="rId164" xr:uid="{D6B77117-A0D5-9240-8193-0102C36CCE4C}"/>
+    <hyperlink ref="L198" r:id="rId165" xr:uid="{79FB1103-88A8-8044-9E2C-4FAEC0906E8E}"/>
+    <hyperlink ref="L245" r:id="rId166" xr:uid="{5BF1C4C9-E63A-4F42-9042-36520975FDFA}"/>
     <hyperlink ref="L195" r:id="rId167" xr:uid="{21CDF460-9871-0547-AA6B-20304C8DD21D}"/>
     <hyperlink ref="L180" r:id="rId168" xr:uid="{BA1EC844-435A-6C44-87FC-C12B7ECFC55B}"/>
     <hyperlink ref="L179" r:id="rId169" xr:uid="{46D875DC-CDDD-7E4B-88DB-DFC416CF17AB}"/>
     <hyperlink ref="L169" r:id="rId170" xr:uid="{7D2FF6AE-1C67-9D4A-A760-7E3745DD9EA6}"/>
-    <hyperlink ref="L226" r:id="rId171" xr:uid="{B5E5E388-8F37-414E-A0C6-1DC58E77628C}"/>
-    <hyperlink ref="L228" r:id="rId172" xr:uid="{A96B1ACF-D982-9240-BB1C-69459154AE5A}"/>
+    <hyperlink ref="L227" r:id="rId171" xr:uid="{B5E5E388-8F37-414E-A0C6-1DC58E77628C}"/>
+    <hyperlink ref="L229" r:id="rId172" xr:uid="{A96B1ACF-D982-9240-BB1C-69459154AE5A}"/>
     <hyperlink ref="L189" r:id="rId173" xr:uid="{D3BB695A-CBA9-D649-B49D-4CC8D16EFD9B}"/>
     <hyperlink ref="L190" r:id="rId174" xr:uid="{A2922BA8-758D-3149-892C-B7B65B435332}"/>
-    <hyperlink ref="L215" r:id="rId175" xr:uid="{BDB09119-6289-4346-BC29-7A54BD393127}"/>
-    <hyperlink ref="L245" r:id="rId176" xr:uid="{5736CAF4-3646-3243-9AEB-4D82B6D0D10A}"/>
-    <hyperlink ref="L218" r:id="rId177" xr:uid="{60659D55-801C-9A4E-84CA-809884CCBE5C}"/>
-    <hyperlink ref="L204" r:id="rId178" xr:uid="{18DDC006-0939-794C-9B5D-10593F8C0973}"/>
+    <hyperlink ref="L216" r:id="rId175" xr:uid="{BDB09119-6289-4346-BC29-7A54BD393127}"/>
+    <hyperlink ref="L246" r:id="rId176" xr:uid="{5736CAF4-3646-3243-9AEB-4D82B6D0D10A}"/>
+    <hyperlink ref="L219" r:id="rId177" xr:uid="{60659D55-801C-9A4E-84CA-809884CCBE5C}"/>
+    <hyperlink ref="L205" r:id="rId178" xr:uid="{18DDC006-0939-794C-9B5D-10593F8C0973}"/>
     <hyperlink ref="L191" r:id="rId179" xr:uid="{50EA46A5-11DD-0345-ABCA-4206D73C7606}"/>
-    <hyperlink ref="L235" r:id="rId180" xr:uid="{63DDFF3B-E62C-9445-96AD-4BB37ACCD20E}"/>
-    <hyperlink ref="L220" r:id="rId181" xr:uid="{05E34BC1-B22F-3E46-8574-E72267507402}"/>
-    <hyperlink ref="L219" r:id="rId182" xr:uid="{7125DF67-5A7E-D948-8363-A31AB1EBA44A}"/>
-    <hyperlink ref="L250" r:id="rId183" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
-    <hyperlink ref="L205" r:id="rId184" xr:uid="{CCE2D666-E296-D94C-ACE0-791CC746483B}"/>
+    <hyperlink ref="L236" r:id="rId180" xr:uid="{63DDFF3B-E62C-9445-96AD-4BB37ACCD20E}"/>
+    <hyperlink ref="L221" r:id="rId181" xr:uid="{05E34BC1-B22F-3E46-8574-E72267507402}"/>
+    <hyperlink ref="L220" r:id="rId182" xr:uid="{7125DF67-5A7E-D948-8363-A31AB1EBA44A}"/>
+    <hyperlink ref="L251" r:id="rId183" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
+    <hyperlink ref="L206" r:id="rId184" xr:uid="{CCE2D666-E296-D94C-ACE0-791CC746483B}"/>
     <hyperlink ref="L181" r:id="rId185" xr:uid="{E5A2F3EE-A3B1-0842-9364-E4B6EACA9544}"/>
-    <hyperlink ref="L221" r:id="rId186" xr:uid="{E08C8BA4-5414-1947-9CA8-45FE0B846CD1}"/>
-    <hyperlink ref="L217" r:id="rId187" xr:uid="{F1A64091-5BF7-8243-B7A0-F4C13B8B0ABB}"/>
-    <hyperlink ref="L202" r:id="rId188" xr:uid="{745AEF03-3150-C54B-800A-696460474256}"/>
-    <hyperlink ref="L203" r:id="rId189" xr:uid="{9C078FBA-3B11-8049-9187-5BC86D78EA09}"/>
+    <hyperlink ref="L222" r:id="rId186" xr:uid="{E08C8BA4-5414-1947-9CA8-45FE0B846CD1}"/>
+    <hyperlink ref="L218" r:id="rId187" xr:uid="{F1A64091-5BF7-8243-B7A0-F4C13B8B0ABB}"/>
+    <hyperlink ref="L203" r:id="rId188" xr:uid="{745AEF03-3150-C54B-800A-696460474256}"/>
+    <hyperlink ref="L204" r:id="rId189" xr:uid="{9C078FBA-3B11-8049-9187-5BC86D78EA09}"/>
     <hyperlink ref="L182" r:id="rId190" xr:uid="{BF9A6A48-C664-FA4B-A769-D87460BB9387}"/>
     <hyperlink ref="L187" r:id="rId191" xr:uid="{11E0C06F-BBA9-B446-A3A4-5862C893161B}"/>
-    <hyperlink ref="L216" r:id="rId192" xr:uid="{D5E45024-1B58-714D-9576-1FA969BDADD9}"/>
+    <hyperlink ref="L217" r:id="rId192" xr:uid="{D5E45024-1B58-714D-9576-1FA969BDADD9}"/>
     <hyperlink ref="L194" r:id="rId193" xr:uid="{D160676D-AC82-D243-B9A9-56033B0A6EFE}"/>
-    <hyperlink ref="L213" r:id="rId194" xr:uid="{3DB54A74-68B7-734A-BC3C-BFE4E2E4103E}"/>
+    <hyperlink ref="L214" r:id="rId194" xr:uid="{3DB54A74-68B7-734A-BC3C-BFE4E2E4103E}"/>
     <hyperlink ref="L106" r:id="rId195" xr:uid="{4686296B-C235-4048-A384-BE461895E2AC}"/>
     <hyperlink ref="L108" r:id="rId196" location="page=2&amp;query=gold%20badge%20sprite&amp;position=49&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{061AB839-ADB1-BA47-A152-68CDFE8A1979}"/>
     <hyperlink ref="L109" r:id="rId197" location="page=4&amp;query=gold%20badge%20sprite&amp;position=9&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{138577BB-7F7D-D64A-806E-567F3970D250}"/>
     <hyperlink ref="L178" r:id="rId198" xr:uid="{927B8B79-A428-2043-9B3B-555F7877CA20}"/>
-    <hyperlink ref="L201" r:id="rId199" xr:uid="{6018233D-1425-7148-A608-3B0666055EA2}"/>
-    <hyperlink ref="L227" r:id="rId200" xr:uid="{38C9843F-1665-8F46-A66C-287455700886}"/>
-    <hyperlink ref="L251" r:id="rId201" xr:uid="{9E664F43-2A79-3744-BC57-4D11914A4B9C}"/>
-    <hyperlink ref="L252" r:id="rId202" xr:uid="{F55C22EB-ADA4-064F-8C9F-34B8DFB927E8}"/>
+    <hyperlink ref="L202" r:id="rId199" xr:uid="{6018233D-1425-7148-A608-3B0666055EA2}"/>
+    <hyperlink ref="L228" r:id="rId200" xr:uid="{38C9843F-1665-8F46-A66C-287455700886}"/>
+    <hyperlink ref="L252" r:id="rId201" xr:uid="{9E664F43-2A79-3744-BC57-4D11914A4B9C}"/>
+    <hyperlink ref="L253" r:id="rId202" xr:uid="{F55C22EB-ADA4-064F-8C9F-34B8DFB927E8}"/>
     <hyperlink ref="L162" r:id="rId203" xr:uid="{A1B2F4EC-ACE1-B14D-8619-0451D719CFC0}"/>
-    <hyperlink ref="L229" r:id="rId204" xr:uid="{2BF445F0-7B50-5E48-A8E5-4779F07B83CE}"/>
-    <hyperlink ref="L230" r:id="rId205" xr:uid="{6B23A3F9-85DD-4043-853E-3BF95911A2C6}"/>
-    <hyperlink ref="L231" r:id="rId206" xr:uid="{A975FD98-A3FE-5B40-9F31-D14EAE3777F9}"/>
-    <hyperlink ref="L255" r:id="rId207" xr:uid="{F01C8569-23FB-7F4C-A50B-40979911E1B8}"/>
-    <hyperlink ref="L258" r:id="rId208" xr:uid="{B54ABD16-F1A6-DC45-B36E-0CC72B423F70}"/>
-    <hyperlink ref="L256" r:id="rId209" xr:uid="{EBA532A6-AAFD-E54D-BD41-CC4F5F92AF68}"/>
-    <hyperlink ref="L257" r:id="rId210" xr:uid="{0F422DA4-046E-F246-BC4A-695F255E6851}"/>
-    <hyperlink ref="L209" r:id="rId211" xr:uid="{1F9FD82A-7BDA-7143-B89F-0DBBBC864386}"/>
-    <hyperlink ref="L210" r:id="rId212" xr:uid="{7F1F0626-5319-784B-97DE-B956AE96359D}"/>
-    <hyperlink ref="L214" r:id="rId213" xr:uid="{B2599288-37DA-884B-A5E6-897FBCE08F4D}"/>
+    <hyperlink ref="L230" r:id="rId204" xr:uid="{2BF445F0-7B50-5E48-A8E5-4779F07B83CE}"/>
+    <hyperlink ref="L231" r:id="rId205" xr:uid="{6B23A3F9-85DD-4043-853E-3BF95911A2C6}"/>
+    <hyperlink ref="L232" r:id="rId206" xr:uid="{A975FD98-A3FE-5B40-9F31-D14EAE3777F9}"/>
+    <hyperlink ref="L256" r:id="rId207" xr:uid="{F01C8569-23FB-7F4C-A50B-40979911E1B8}"/>
+    <hyperlink ref="L259" r:id="rId208" xr:uid="{B54ABD16-F1A6-DC45-B36E-0CC72B423F70}"/>
+    <hyperlink ref="L257" r:id="rId209" xr:uid="{EBA532A6-AAFD-E54D-BD41-CC4F5F92AF68}"/>
+    <hyperlink ref="L258" r:id="rId210" xr:uid="{0F422DA4-046E-F246-BC4A-695F255E6851}"/>
+    <hyperlink ref="L210" r:id="rId211" xr:uid="{1F9FD82A-7BDA-7143-B89F-0DBBBC864386}"/>
+    <hyperlink ref="L211" r:id="rId212" xr:uid="{7F1F0626-5319-784B-97DE-B956AE96359D}"/>
+    <hyperlink ref="L215" r:id="rId213" xr:uid="{B2599288-37DA-884B-A5E6-897FBCE08F4D}"/>
     <hyperlink ref="L85" r:id="rId214" location="page=2&amp;query=light%20beam&amp;position=25&amp;from_view=search&amp;track=ais&amp;uuid=063fa81a-19de-4aad-b5fc-7caa6fa59141#position=25&amp;page=2&amp;query=light%20beam" xr:uid="{F7D7C1C4-CC10-FA4D-8194-8E6ECD655D52}"/>
     <hyperlink ref="L184" r:id="rId215" xr:uid="{D7E66CB2-1636-854A-8F67-24ACB034C7F4}"/>
     <hyperlink ref="L185" r:id="rId216" xr:uid="{D83C0C58-CE24-594B-A33D-B788F11BBF4E}"/>
@@ -10566,7 +10657,8 @@
     <hyperlink ref="L35" r:id="rId218" location="page=3&amp;query=dragon%20sprite&amp;position=8&amp;from_view=search&amp;track=ais&amp;uuid=a74ae69f-43df-4e46-8d2c-551fbfc06054" xr:uid="{B03DA0C1-BC2B-EF47-AC66-221CD4C2D9C5}"/>
     <hyperlink ref="L83" r:id="rId219" location="page=3&amp;query=dragon%20sprite&amp;position=8&amp;from_view=search&amp;track=ais&amp;uuid=a74ae69f-43df-4e46-8d2c-551fbfc06054" xr:uid="{027D9EA3-3F97-BA46-BA51-96E2ED000931}"/>
     <hyperlink ref="L193" r:id="rId220" xr:uid="{8BAF1438-906C-504E-A53D-226576B1A1BC}"/>
-    <hyperlink ref="L238" r:id="rId221" xr:uid="{0345E79A-FDC7-314E-8D2A-45798EF5A1E7}"/>
+    <hyperlink ref="L239" r:id="rId221" xr:uid="{0345E79A-FDC7-314E-8D2A-45798EF5A1E7}"/>
+    <hyperlink ref="L261" r:id="rId222" xr:uid="{5971D630-BDBF-1C4D-A608-817C569DA1F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Minor Updates 1/30/24 ChatEngine: update dialogue and sound timing. CutsceneIntro: Remove FireIceTheme and return to blood overlay/red dragon. Update dialogue. GameScene: move tapPointerEngine outside gameEngine.checkControlGuardsIfPassed() so that it always shows even as controls are disabled. GameboardSprite: Move audio in spawnCapturePrincess. Don't play currentThem after despawn either; handle that in ChatEngine.
</commit_message>
<xml_diff>
--- a/JSON/AssetsCatalog.xlsx
+++ b/JSON/AssetsCatalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCAD26A-9869-834B-8DD2-372B19B07E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C611CE3C-91F3-B445-90D2-76B69D49FBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42040" yWindow="1620" windowWidth="36000" windowHeight="21040" xr2:uid="{E84333C6-E3B6-FB42-AB04-827399F33810}"/>
   </bookViews>
@@ -2380,10 +2380,10 @@
   <dimension ref="A1:L261"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D231" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D186" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I255" sqref="I255"/>
+      <selection pane="bottomRight" activeCell="G197" sqref="G197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8337,7 +8337,7 @@
         <v>1</v>
       </c>
       <c r="G196" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H196" s="3" t="s">
         <v>391</v>
@@ -10419,7 +10419,7 @@
         <v>1</v>
       </c>
       <c r="G261" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H261" s="3" t="s">
         <v>391</v>

</xml_diff>

<commit_message>
AssetsCatalog: add row for realmtransition GameEngine: update inBetweenNode fade durations. Add inbetweenSmoke particle effect AudioManager, Assets: add realmtransition.mp3 InBetweenSmokeParticles: add this new effect node. GameboardSprite: update flipGameboard fade durations. Add realmtransition sound effect when gameboard spins.
</commit_message>
<xml_diff>
--- a/JSON/AssetsCatalog.xlsx
+++ b/JSON/AssetsCatalog.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C611CE3C-91F3-B445-90D2-76B69D49FBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71917C3B-942E-AA4B-B5DF-E20F2CCBC447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42040" yWindow="1620" windowWidth="36000" windowHeight="21040" xr2:uid="{E84333C6-E3B6-FB42-AB04-827399F33810}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{E84333C6-E3B6-FB42-AB04-827399F33810}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$260</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$262</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="643">
   <si>
     <t>Filename</t>
   </si>
@@ -1956,6 +1956,18 @@
   </si>
   <si>
     <t>BANT</t>
+  </si>
+  <si>
+    <t>realmtransition</t>
+  </si>
+  <si>
+    <t>JustinDevern</t>
+  </si>
+  <si>
+    <t>Record Scratch Warp Speed</t>
+  </si>
+  <si>
+    <t>https://audiojungle.net/item/record-scratch-speed-warp/24478696</t>
   </si>
 </sst>
 </file>
@@ -2047,7 +2059,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -2062,6 +2074,7 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2081,9 +2094,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2121,7 +2134,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2227,7 +2240,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2369,7 +2382,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2377,13 +2390,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}">
-  <dimension ref="A1:L261"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L262"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D186" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D179" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G197" sqref="G197"/>
+      <selection pane="bottomRight" activeCell="C249" sqref="C249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2440,7 +2454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2469,7 +2483,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2498,7 +2512,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2527,7 +2541,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2556,7 +2570,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2585,7 +2599,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2614,7 +2628,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2643,7 +2657,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2672,7 +2686,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2701,7 +2715,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2730,7 +2744,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2759,7 +2773,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2788,7 +2802,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2817,7 +2831,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -2849,7 +2863,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2881,7 +2895,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -2910,7 +2924,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2939,7 +2953,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -2968,7 +2982,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -2997,7 +3011,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -3026,7 +3040,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -3055,7 +3069,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -3084,7 +3098,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -3113,7 +3127,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -3145,7 +3159,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -3177,7 +3191,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -3206,7 +3220,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -3235,7 +3249,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -3264,7 +3278,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -3293,7 +3307,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -3322,7 +3336,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -3351,7 +3365,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -3380,7 +3394,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -3409,7 +3423,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -3438,7 +3452,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -3467,7 +3481,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -3496,7 +3510,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -3525,7 +3539,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -3554,7 +3568,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -3583,7 +3597,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -3615,7 +3629,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -3644,7 +3658,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -3673,7 +3687,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -3702,7 +3716,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -3731,7 +3745,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -3760,7 +3774,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -3789,7 +3803,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -3821,7 +3835,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -3853,7 +3867,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -3882,7 +3896,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -3911,7 +3925,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -3940,7 +3954,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -3969,7 +3983,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -3998,7 +4012,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -4027,7 +4041,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -4056,7 +4070,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>4</v>
       </c>
@@ -4088,7 +4102,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -4120,7 +4134,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -4152,7 +4166,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -4184,7 +4198,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -4213,7 +4227,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -4242,7 +4256,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>4</v>
       </c>
@@ -4271,7 +4285,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>4</v>
       </c>
@@ -4300,7 +4314,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -4329,7 +4343,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>4</v>
       </c>
@@ -4358,7 +4372,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>4</v>
       </c>
@@ -4387,7 +4401,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>4</v>
       </c>
@@ -4419,7 +4433,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>4</v>
       </c>
@@ -4451,7 +4465,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>4</v>
       </c>
@@ -4483,7 +4497,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>4</v>
       </c>
@@ -4512,7 +4526,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>4</v>
       </c>
@@ -4544,7 +4558,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>4</v>
       </c>
@@ -4576,7 +4590,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>4</v>
       </c>
@@ -4605,7 +4619,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>4</v>
       </c>
@@ -4634,7 +4648,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>4</v>
       </c>
@@ -4663,7 +4677,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>4</v>
       </c>
@@ -4692,7 +4706,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>4</v>
       </c>
@@ -4724,7 +4738,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>4</v>
       </c>
@@ -4756,7 +4770,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>4</v>
       </c>
@@ -4785,7 +4799,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>4</v>
       </c>
@@ -4814,7 +4828,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>4</v>
       </c>
@@ -4843,7 +4857,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>4</v>
       </c>
@@ -4872,7 +4886,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>4</v>
       </c>
@@ -4901,7 +4915,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>4</v>
       </c>
@@ -4930,7 +4944,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>4</v>
       </c>
@@ -4962,7 +4976,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>4</v>
       </c>
@@ -4994,7 +5008,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>4</v>
       </c>
@@ -5026,7 +5040,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>4</v>
       </c>
@@ -5058,7 +5072,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>4</v>
       </c>
@@ -5090,7 +5104,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>4</v>
       </c>
@@ -5122,7 +5136,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>4</v>
       </c>
@@ -5154,7 +5168,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>4</v>
       </c>
@@ -5186,7 +5200,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>4</v>
       </c>
@@ -5218,7 +5232,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>4</v>
       </c>
@@ -5250,7 +5264,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>4</v>
       </c>
@@ -5282,7 +5296,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>4</v>
       </c>
@@ -5311,7 +5325,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>4</v>
       </c>
@@ -5340,7 +5354,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>4</v>
       </c>
@@ -5369,7 +5383,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>4</v>
       </c>
@@ -5398,7 +5412,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>4</v>
       </c>
@@ -5427,7 +5441,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>4</v>
       </c>
@@ -5456,7 +5470,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>4</v>
       </c>
@@ -5488,7 +5502,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>4</v>
       </c>
@@ -5520,7 +5534,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>4</v>
       </c>
@@ -5552,7 +5566,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>4</v>
       </c>
@@ -5584,7 +5598,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>4</v>
       </c>
@@ -5619,7 +5633,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>4</v>
       </c>
@@ -5651,7 +5665,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>4</v>
       </c>
@@ -5683,7 +5697,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>4</v>
       </c>
@@ -5715,7 +5729,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>4</v>
       </c>
@@ -5750,7 +5764,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>4</v>
       </c>
@@ -5785,7 +5799,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>4</v>
       </c>
@@ -5820,7 +5834,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>4</v>
       </c>
@@ -5852,7 +5866,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>4</v>
       </c>
@@ -5887,7 +5901,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>4</v>
       </c>
@@ -5919,7 +5933,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>4</v>
       </c>
@@ -5954,7 +5968,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>4</v>
       </c>
@@ -5989,7 +6003,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>4</v>
       </c>
@@ -6021,7 +6035,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>4</v>
       </c>
@@ -6053,7 +6067,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>4</v>
       </c>
@@ -6088,7 +6102,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>4</v>
       </c>
@@ -6123,7 +6137,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>4</v>
       </c>
@@ -6155,7 +6169,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>4</v>
       </c>
@@ -6187,7 +6201,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>4</v>
       </c>
@@ -6222,7 +6236,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>4</v>
       </c>
@@ -6257,7 +6271,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>4</v>
       </c>
@@ -6289,7 +6303,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>4</v>
       </c>
@@ -6324,7 +6338,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>4</v>
       </c>
@@ -6356,7 +6370,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>4</v>
       </c>
@@ -6385,7 +6399,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>4</v>
       </c>
@@ -6414,7 +6428,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>4</v>
       </c>
@@ -6443,7 +6457,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>4</v>
       </c>
@@ -6472,7 +6486,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>4</v>
       </c>
@@ -6501,7 +6515,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>4</v>
       </c>
@@ -6530,7 +6544,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>4</v>
       </c>
@@ -6559,7 +6573,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>4</v>
       </c>
@@ -6588,7 +6602,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>4</v>
       </c>
@@ -6617,7 +6631,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>4</v>
       </c>
@@ -6646,7 +6660,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>4</v>
       </c>
@@ -6669,7 +6683,7 @@
       <c r="K140" s="8"/>
       <c r="L140" s="9"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>4</v>
       </c>
@@ -6692,7 +6706,7 @@
       <c r="K141" s="8"/>
       <c r="L141" s="9"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>4</v>
       </c>
@@ -6721,7 +6735,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>4</v>
       </c>
@@ -6750,7 +6764,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>4</v>
       </c>
@@ -6779,7 +6793,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>4</v>
       </c>
@@ -6808,7 +6822,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>4</v>
       </c>
@@ -6837,7 +6851,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>4</v>
       </c>
@@ -6860,7 +6874,7 @@
       <c r="K147" s="8"/>
       <c r="L147" s="9"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>4</v>
       </c>
@@ -6883,7 +6897,7 @@
       <c r="K148" s="8"/>
       <c r="L148" s="9"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>4</v>
       </c>
@@ -6906,7 +6920,7 @@
       <c r="K149" s="8"/>
       <c r="L149" s="9"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>4</v>
       </c>
@@ -6929,7 +6943,7 @@
       <c r="K150" s="8"/>
       <c r="L150" s="9"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>4</v>
       </c>
@@ -6958,7 +6972,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>4</v>
       </c>
@@ -6987,7 +7001,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>4</v>
       </c>
@@ -7016,7 +7030,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>4</v>
       </c>
@@ -7039,7 +7053,7 @@
       <c r="K154" s="8"/>
       <c r="L154" s="9"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>4</v>
       </c>
@@ -7068,7 +7082,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>4</v>
       </c>
@@ -7097,7 +7111,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>4</v>
       </c>
@@ -7126,7 +7140,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>401</v>
       </c>
@@ -7158,7 +7172,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>401</v>
       </c>
@@ -7190,7 +7204,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>389</v>
       </c>
@@ -7211,7 +7225,7 @@
       <c r="K160" s="8"/>
       <c r="L160" s="9"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>389</v>
       </c>
@@ -7243,7 +7257,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>389</v>
       </c>
@@ -7275,7 +7289,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>389</v>
       </c>
@@ -7307,7 +7321,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>389</v>
       </c>
@@ -7339,7 +7353,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>389</v>
       </c>
@@ -7371,7 +7385,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>389</v>
       </c>
@@ -7403,7 +7417,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>389</v>
       </c>
@@ -7435,7 +7449,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>389</v>
       </c>
@@ -7467,7 +7481,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>389</v>
       </c>
@@ -7499,7 +7513,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>389</v>
       </c>
@@ -7531,7 +7545,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>389</v>
       </c>
@@ -7563,7 +7577,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>389</v>
       </c>
@@ -7595,7 +7609,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>389</v>
       </c>
@@ -7627,7 +7641,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>389</v>
       </c>
@@ -7659,7 +7673,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>389</v>
       </c>
@@ -7691,7 +7705,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>389</v>
       </c>
@@ -7712,7 +7726,7 @@
       <c r="K176" s="8"/>
       <c r="L176" s="9"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>389</v>
       </c>
@@ -7744,7 +7758,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>389</v>
       </c>
@@ -7808,7 +7822,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>389</v>
       </c>
@@ -7840,7 +7854,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>389</v>
       </c>
@@ -7872,7 +7886,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>389</v>
       </c>
@@ -7904,7 +7918,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>389</v>
       </c>
@@ -8032,7 +8046,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>389</v>
       </c>
@@ -8064,7 +8078,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>401</v>
       </c>
@@ -8096,7 +8110,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>389</v>
       </c>
@@ -8128,7 +8142,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>389</v>
       </c>
@@ -8160,7 +8174,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>389</v>
       </c>
@@ -8288,7 +8302,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>389</v>
       </c>
@@ -8352,7 +8366,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>389</v>
       </c>
@@ -8384,7 +8398,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>389</v>
       </c>
@@ -8416,7 +8430,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>389</v>
       </c>
@@ -8448,7 +8462,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>389</v>
       </c>
@@ -8480,7 +8494,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>389</v>
       </c>
@@ -8512,7 +8526,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>389</v>
       </c>
@@ -8672,7 +8686,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>389</v>
       </c>
@@ -8704,7 +8718,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>389</v>
       </c>
@@ -8736,7 +8750,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>389</v>
       </c>
@@ -8864,7 +8878,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>389</v>
       </c>
@@ -8960,7 +8974,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>389</v>
       </c>
@@ -8992,7 +9006,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>389</v>
       </c>
@@ -9024,7 +9038,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>389</v>
       </c>
@@ -9056,7 +9070,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>389</v>
       </c>
@@ -9088,7 +9102,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>389</v>
       </c>
@@ -9120,7 +9134,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>389</v>
       </c>
@@ -9152,7 +9166,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>389</v>
       </c>
@@ -9184,7 +9198,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>389</v>
       </c>
@@ -9216,7 +9230,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>389</v>
       </c>
@@ -9248,7 +9262,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>389</v>
       </c>
@@ -9280,7 +9294,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>389</v>
       </c>
@@ -9312,7 +9326,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>389</v>
       </c>
@@ -9344,7 +9358,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>389</v>
       </c>
@@ -9504,7 +9518,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>389</v>
       </c>
@@ -9536,7 +9550,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>389</v>
       </c>
@@ -9568,7 +9582,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>389</v>
       </c>
@@ -9632,7 +9646,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>401</v>
       </c>
@@ -9664,7 +9678,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>401</v>
       </c>
@@ -9728,7 +9742,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>401</v>
       </c>
@@ -9760,7 +9774,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>389</v>
       </c>
@@ -9792,7 +9806,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>389</v>
       </c>
@@ -9824,7 +9838,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>389</v>
       </c>
@@ -9856,7 +9870,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>389</v>
       </c>
@@ -9888,7 +9902,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>389</v>
       </c>
@@ -9920,7 +9934,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>389</v>
       </c>
@@ -9952,7 +9966,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>389</v>
       </c>
@@ -9984,7 +9998,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>389</v>
       </c>
@@ -10023,46 +10037,46 @@
       <c r="B249" t="s">
         <v>405</v>
       </c>
-      <c r="C249" t="s">
-        <v>381</v>
+      <c r="C249" s="12" t="s">
+        <v>639</v>
       </c>
       <c r="D249" t="s">
         <v>388</v>
       </c>
-      <c r="F249" s="3">
+      <c r="F249" s="14">
         <v>1</v>
       </c>
       <c r="G249" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H249" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I249" s="3" t="s">
-        <v>411</v>
+        <v>640</v>
       </c>
       <c r="K249" s="3" t="s">
-        <v>451</v>
+        <v>641</v>
       </c>
       <c r="L249" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.2">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B250" t="s">
         <v>405</v>
       </c>
       <c r="C250" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D250" t="s">
         <v>388</v>
       </c>
       <c r="F250" s="3">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="G250" s="3" t="s">
         <v>174</v>
@@ -10071,45 +10085,45 @@
         <v>391</v>
       </c>
       <c r="I250" s="3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="K250" s="3" t="s">
-        <v>413</v>
+        <v>451</v>
       </c>
       <c r="L250" s="6" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B251" t="s">
         <v>405</v>
       </c>
       <c r="C251" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D251" t="s">
         <v>388</v>
       </c>
-      <c r="F251" s="11">
-        <v>2</v>
+      <c r="F251" s="3">
+        <v>21</v>
       </c>
       <c r="G251" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H251" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I251" s="3" t="s">
-        <v>525</v>
+        <v>414</v>
       </c>
       <c r="K251" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="L251" s="10" t="s">
-        <v>523</v>
+        <v>413</v>
+      </c>
+      <c r="L251" s="6" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.2">
@@ -10120,32 +10134,31 @@
         <v>405</v>
       </c>
       <c r="C252" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D252" t="s">
         <v>388</v>
       </c>
-      <c r="F252" s="3">
-        <v>1</v>
+      <c r="F252" s="11">
+        <v>2</v>
       </c>
       <c r="G252" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H252" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I252" t="s">
-        <v>572</v>
-      </c>
-      <c r="J252"/>
-      <c r="K252" t="s">
-        <v>573</v>
-      </c>
-      <c r="L252" s="6" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I252" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="K252" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="L252" s="10" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>389</v>
       </c>
@@ -10153,7 +10166,7 @@
         <v>405</v>
       </c>
       <c r="C253" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D253" t="s">
         <v>388</v>
@@ -10168,31 +10181,31 @@
         <v>391</v>
       </c>
       <c r="I253" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="J253"/>
       <c r="K253" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="L253" s="6" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.2">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B254" t="s">
         <v>405</v>
       </c>
       <c r="C254" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D254" t="s">
         <v>388</v>
       </c>
       <c r="F254" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G254" s="3" t="s">
         <v>174</v>
@@ -10200,31 +10213,32 @@
       <c r="H254" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I254" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="K254" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="L254" s="7" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I254" t="s">
+        <v>569</v>
+      </c>
+      <c r="J254"/>
+      <c r="K254" t="s">
+        <v>570</v>
+      </c>
+      <c r="L254" s="6" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B255" t="s">
         <v>405</v>
       </c>
       <c r="C255" t="s">
-        <v>58</v>
+        <v>386</v>
       </c>
       <c r="D255" t="s">
         <v>388</v>
       </c>
       <c r="F255" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G255" s="3" t="s">
         <v>174</v>
@@ -10233,45 +10247,45 @@
         <v>391</v>
       </c>
       <c r="I255" s="3" t="s">
-        <v>468</v>
+        <v>402</v>
       </c>
       <c r="K255" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="L255" s="6" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.2">
+        <v>403</v>
+      </c>
+      <c r="L255" s="7" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>389</v>
       </c>
       <c r="B256" t="s">
         <v>405</v>
       </c>
-      <c r="C256" s="9" t="s">
-        <v>581</v>
+      <c r="C256" t="s">
+        <v>58</v>
       </c>
       <c r="D256" t="s">
         <v>388</v>
       </c>
-      <c r="F256" s="11">
+      <c r="F256" s="3">
         <v>1</v>
       </c>
       <c r="G256" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H256" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I256" s="3" t="s">
-        <v>392</v>
+        <v>468</v>
       </c>
       <c r="K256" s="3" t="s">
-        <v>586</v>
+        <v>467</v>
       </c>
       <c r="L256" s="6" t="s">
-        <v>585</v>
+        <v>466</v>
       </c>
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.2">
@@ -10288,7 +10302,7 @@
         <v>388</v>
       </c>
       <c r="F257" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G257" s="3" t="s">
         <v>432</v>
@@ -10346,13 +10360,13 @@
         <v>405</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D259" t="s">
         <v>388</v>
       </c>
       <c r="F259" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G259" s="3" t="s">
         <v>432</v>
@@ -10361,13 +10375,13 @@
         <v>391</v>
       </c>
       <c r="I259" s="3" t="s">
-        <v>537</v>
+        <v>392</v>
       </c>
       <c r="K259" s="3" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="L259" s="6" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.2">
@@ -10377,40 +10391,40 @@
       <c r="B260" t="s">
         <v>405</v>
       </c>
-      <c r="C260" t="s">
-        <v>387</v>
+      <c r="C260" s="9" t="s">
+        <v>582</v>
       </c>
       <c r="D260" t="s">
         <v>388</v>
       </c>
-      <c r="F260" s="3">
+      <c r="F260" s="11">
         <v>1</v>
       </c>
       <c r="G260" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H260" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I260" s="3" t="s">
-        <v>470</v>
+        <v>537</v>
       </c>
       <c r="K260" s="3" t="s">
-        <v>471</v>
+        <v>584</v>
       </c>
       <c r="L260" s="6" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.2">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>389</v>
       </c>
       <c r="B261" t="s">
         <v>405</v>
       </c>
-      <c r="C261" s="12" t="s">
-        <v>635</v>
+      <c r="C261" t="s">
+        <v>387</v>
       </c>
       <c r="D261" t="s">
         <v>388</v>
@@ -10419,23 +10433,61 @@
         <v>1</v>
       </c>
       <c r="G261" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H261" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I261" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="K261" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="L261" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>389</v>
+      </c>
+      <c r="B262" t="s">
+        <v>405</v>
+      </c>
+      <c r="C262" s="12" t="s">
+        <v>635</v>
+      </c>
+      <c r="D262" t="s">
+        <v>388</v>
+      </c>
+      <c r="F262" s="3">
+        <v>1</v>
+      </c>
+      <c r="G262" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="H262" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I262" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="K261" s="3" t="s">
+      <c r="K262" s="3" t="s">
         <v>637</v>
       </c>
-      <c r="L261" s="6" t="s">
+      <c r="L262" s="6" t="s">
         <v>636</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L260" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}"/>
+  <autoFilter ref="A1:L262" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="No"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="L3" r:id="rId1" location="query=target&amp;position=0&amp;from_view=search&amp;track=sph&amp;uuid=07a631b0-afe2-4d83-9076-a80360e62f2f" xr:uid="{6340FD26-01F6-9246-82E5-C8936FBB7B36}"/>
     <hyperlink ref="L4" r:id="rId2" location="query=spell%20book&amp;position=12&amp;from_view=keyword&amp;track=ais&amp;uuid=3aa8f740-41d0-409e-b03b-268281a69be6" xr:uid="{1A91BF66-CE85-304F-BBE7-7F8EBE53C285}"/>
@@ -10564,11 +10616,11 @@
     <hyperlink ref="L161" r:id="rId125" xr:uid="{F88953B7-468E-C34B-9347-94009F9A78D2}"/>
     <hyperlink ref="L207" r:id="rId126" xr:uid="{1F3BBC8C-29E8-C74A-AB3F-04AE466222EF}"/>
     <hyperlink ref="L209" r:id="rId127" xr:uid="{3C51058F-793C-D34A-8286-18AE4C8EF6CE}"/>
-    <hyperlink ref="L254" r:id="rId128" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
+    <hyperlink ref="L255" r:id="rId128" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
     <hyperlink ref="L158" r:id="rId129" xr:uid="{6A722A1D-2F7B-4242-8134-716EFF33F7D2}"/>
     <hyperlink ref="L159" r:id="rId130" xr:uid="{547CD1A8-1967-1C46-95E3-89E39CD045C2}"/>
     <hyperlink ref="L213" r:id="rId131" xr:uid="{5ACD6BFD-52F0-0940-AA8E-B04F1D397BC7}"/>
-    <hyperlink ref="L250" r:id="rId132" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
+    <hyperlink ref="L251" r:id="rId132" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
     <hyperlink ref="L208" r:id="rId133" xr:uid="{2030AD8C-28A7-544B-92DC-5CBE411DE1C0}"/>
     <hyperlink ref="L238" r:id="rId134" xr:uid="{05363CA1-BE60-3F42-B56A-1A92A0EDA166}"/>
     <hyperlink ref="L200" r:id="rId135" xr:uid="{D4C66DCB-D6B4-EC4F-A922-B87887BE6E4A}"/>
@@ -10587,7 +10639,7 @@
     <hyperlink ref="L241" r:id="rId148" xr:uid="{5CE3083F-F217-3743-B613-A7DDF354E72D}"/>
     <hyperlink ref="L243" r:id="rId149" xr:uid="{B81B6B41-2C17-AA48-B730-D906488BA0A0}"/>
     <hyperlink ref="L183" r:id="rId150" xr:uid="{BA0813A2-2582-7A46-A492-16A943824EE5}"/>
-    <hyperlink ref="L249" r:id="rId151" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
+    <hyperlink ref="L250" r:id="rId151" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
     <hyperlink ref="L244" r:id="rId152" xr:uid="{C5265333-F7F0-1845-98D7-68E930F9DFAE}"/>
     <hyperlink ref="L188" r:id="rId153" xr:uid="{C0A159CB-3986-1A46-95AD-DCEFF4247697}"/>
     <hyperlink ref="L175" r:id="rId154" xr:uid="{37810A74-E45D-1D46-AEF5-C5FE2F414285}"/>
@@ -10598,8 +10650,8 @@
     <hyperlink ref="L166" r:id="rId159" xr:uid="{C3E773B2-D410-AF41-B197-4638485DC8EF}"/>
     <hyperlink ref="L167" r:id="rId160" xr:uid="{A0E8A8E2-4A93-3D42-AF48-81955241A483}"/>
     <hyperlink ref="L168" r:id="rId161" xr:uid="{1B03F18A-8745-AA4F-AA8B-88D65D3B24BC}"/>
-    <hyperlink ref="L255" r:id="rId162" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
-    <hyperlink ref="L260" r:id="rId163" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
+    <hyperlink ref="L256" r:id="rId162" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
+    <hyperlink ref="L261" r:id="rId163" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
     <hyperlink ref="L197" r:id="rId164" xr:uid="{D6B77117-A0D5-9240-8193-0102C36CCE4C}"/>
     <hyperlink ref="L198" r:id="rId165" xr:uid="{79FB1103-88A8-8044-9E2C-4FAEC0906E8E}"/>
     <hyperlink ref="L245" r:id="rId166" xr:uid="{5BF1C4C9-E63A-4F42-9042-36520975FDFA}"/>
@@ -10619,7 +10671,7 @@
     <hyperlink ref="L236" r:id="rId180" xr:uid="{63DDFF3B-E62C-9445-96AD-4BB37ACCD20E}"/>
     <hyperlink ref="L221" r:id="rId181" xr:uid="{05E34BC1-B22F-3E46-8574-E72267507402}"/>
     <hyperlink ref="L220" r:id="rId182" xr:uid="{7125DF67-5A7E-D948-8363-A31AB1EBA44A}"/>
-    <hyperlink ref="L251" r:id="rId183" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
+    <hyperlink ref="L252" r:id="rId183" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
     <hyperlink ref="L206" r:id="rId184" xr:uid="{CCE2D666-E296-D94C-ACE0-791CC746483B}"/>
     <hyperlink ref="L181" r:id="rId185" xr:uid="{E5A2F3EE-A3B1-0842-9364-E4B6EACA9544}"/>
     <hyperlink ref="L222" r:id="rId186" xr:uid="{E08C8BA4-5414-1947-9CA8-45FE0B846CD1}"/>
@@ -10637,16 +10689,16 @@
     <hyperlink ref="L178" r:id="rId198" xr:uid="{927B8B79-A428-2043-9B3B-555F7877CA20}"/>
     <hyperlink ref="L202" r:id="rId199" xr:uid="{6018233D-1425-7148-A608-3B0666055EA2}"/>
     <hyperlink ref="L228" r:id="rId200" xr:uid="{38C9843F-1665-8F46-A66C-287455700886}"/>
-    <hyperlink ref="L252" r:id="rId201" xr:uid="{9E664F43-2A79-3744-BC57-4D11914A4B9C}"/>
-    <hyperlink ref="L253" r:id="rId202" xr:uid="{F55C22EB-ADA4-064F-8C9F-34B8DFB927E8}"/>
+    <hyperlink ref="L253" r:id="rId201" xr:uid="{9E664F43-2A79-3744-BC57-4D11914A4B9C}"/>
+    <hyperlink ref="L254" r:id="rId202" xr:uid="{F55C22EB-ADA4-064F-8C9F-34B8DFB927E8}"/>
     <hyperlink ref="L162" r:id="rId203" xr:uid="{A1B2F4EC-ACE1-B14D-8619-0451D719CFC0}"/>
     <hyperlink ref="L230" r:id="rId204" xr:uid="{2BF445F0-7B50-5E48-A8E5-4779F07B83CE}"/>
     <hyperlink ref="L231" r:id="rId205" xr:uid="{6B23A3F9-85DD-4043-853E-3BF95911A2C6}"/>
     <hyperlink ref="L232" r:id="rId206" xr:uid="{A975FD98-A3FE-5B40-9F31-D14EAE3777F9}"/>
-    <hyperlink ref="L256" r:id="rId207" xr:uid="{F01C8569-23FB-7F4C-A50B-40979911E1B8}"/>
-    <hyperlink ref="L259" r:id="rId208" xr:uid="{B54ABD16-F1A6-DC45-B36E-0CC72B423F70}"/>
-    <hyperlink ref="L257" r:id="rId209" xr:uid="{EBA532A6-AAFD-E54D-BD41-CC4F5F92AF68}"/>
-    <hyperlink ref="L258" r:id="rId210" xr:uid="{0F422DA4-046E-F246-BC4A-695F255E6851}"/>
+    <hyperlink ref="L257" r:id="rId207" xr:uid="{F01C8569-23FB-7F4C-A50B-40979911E1B8}"/>
+    <hyperlink ref="L260" r:id="rId208" xr:uid="{B54ABD16-F1A6-DC45-B36E-0CC72B423F70}"/>
+    <hyperlink ref="L258" r:id="rId209" xr:uid="{EBA532A6-AAFD-E54D-BD41-CC4F5F92AF68}"/>
+    <hyperlink ref="L259" r:id="rId210" xr:uid="{0F422DA4-046E-F246-BC4A-695F255E6851}"/>
     <hyperlink ref="L210" r:id="rId211" xr:uid="{1F9FD82A-7BDA-7143-B89F-0DBBBC864386}"/>
     <hyperlink ref="L211" r:id="rId212" xr:uid="{7F1F0626-5319-784B-97DE-B956AE96359D}"/>
     <hyperlink ref="L215" r:id="rId213" xr:uid="{B2599288-37DA-884B-A5E6-897FBCE08F4D}"/>
@@ -10658,7 +10710,8 @@
     <hyperlink ref="L83" r:id="rId219" location="page=3&amp;query=dragon%20sprite&amp;position=8&amp;from_view=search&amp;track=ais&amp;uuid=a74ae69f-43df-4e46-8d2c-551fbfc06054" xr:uid="{027D9EA3-3F97-BA46-BA51-96E2ED000931}"/>
     <hyperlink ref="L193" r:id="rId220" xr:uid="{8BAF1438-906C-504E-A53D-226576B1A1BC}"/>
     <hyperlink ref="L239" r:id="rId221" xr:uid="{0345E79A-FDC7-314E-8D2A-45798EF5A1E7}"/>
-    <hyperlink ref="L261" r:id="rId222" xr:uid="{5971D630-BDBF-1C4D-A608-817C569DA1F0}"/>
+    <hyperlink ref="L262" r:id="rId222" xr:uid="{5971D630-BDBF-1C4D-A608-817C569DA1F0}"/>
+    <hyperlink ref="L249" r:id="rId223" xr:uid="{EE815D9F-FD89-0245-8EBF-03580B54BC84}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Purchase Sounds. Bought chatopenprincess, chatopentrainer, chatopenvillain, enemyice, enemyroar, gameoverice, magicheartbeatloop1, magicheartbeatloop2, magichorrorimpact, marlinblast, overworldice, realmtransition, and winlevelice. ChatEngine: update dialogue. AssetsCatalog: update purchases. AudioManager: udpate purchases.
</commit_message>
<xml_diff>
--- a/JSON/AssetsCatalog.xlsx
+++ b/JSON/AssetsCatalog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F4CEF5-FCCA-5243-BEC2-D583D609A2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B86399-BCFC-4D47-850E-AE1A34865618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38140" yWindow="1340" windowWidth="36000" windowHeight="20900" xr2:uid="{E84333C6-E3B6-FB42-AB04-827399F33810}"/>
   </bookViews>
@@ -2002,7 +2002,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2033,12 +2033,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2066,7 +2060,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2389,7 +2383,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D179" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C193" sqref="C193"/>
+      <selection pane="bottomRight" activeCell="G205" sqref="G205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7942,11 +7936,11 @@
         <v>447</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>389</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B184" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C184" s="12" t="s">
@@ -7959,7 +7953,7 @@
         <v>1</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H184" s="3" t="s">
         <v>391</v>
@@ -7974,11 +7968,11 @@
         <v>603</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>389</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B185" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C185" s="12" t="s">
@@ -7991,7 +7985,7 @@
         <v>1</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H185" s="3" t="s">
         <v>391</v>
@@ -8006,11 +8000,11 @@
         <v>627</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>389</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B186" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C186" s="12" t="s">
@@ -8023,7 +8017,7 @@
         <v>1</v>
       </c>
       <c r="G186" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H186" s="3" t="s">
         <v>391</v>
@@ -8045,7 +8039,7 @@
       <c r="B187" t="s">
         <v>405</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C187" s="12" t="s">
         <v>330</v>
       </c>
       <c r="D187" t="s">
@@ -8077,7 +8071,7 @@
       <c r="B188" t="s">
         <v>405</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C188" s="12" t="s">
         <v>331</v>
       </c>
       <c r="D188" t="s">
@@ -8109,7 +8103,7 @@
       <c r="B189" t="s">
         <v>405</v>
       </c>
-      <c r="C189" t="s">
+      <c r="C189" s="12" t="s">
         <v>332</v>
       </c>
       <c r="D189" t="s">
@@ -8141,7 +8135,7 @@
       <c r="B190" t="s">
         <v>405</v>
       </c>
-      <c r="C190" t="s">
+      <c r="C190" s="12" t="s">
         <v>333</v>
       </c>
       <c r="D190" t="s">
@@ -8173,7 +8167,7 @@
       <c r="B191" t="s">
         <v>405</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C191" s="12" t="s">
         <v>334</v>
       </c>
       <c r="D191" t="s">
@@ -8198,11 +8192,11 @@
         <v>513</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>389</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B192" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C192" s="12" t="s">
@@ -8215,7 +8209,7 @@
         <v>1</v>
       </c>
       <c r="G192" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H192" s="3" t="s">
         <v>391</v>
@@ -8230,11 +8224,11 @@
         <v>614</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>389</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B193" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C193" s="12" t="s">
@@ -8247,7 +8241,7 @@
         <v>1</v>
       </c>
       <c r="G193" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H193" s="3" t="s">
         <v>391</v>
@@ -8266,7 +8260,7 @@
       <c r="A194" t="s">
         <v>389</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B194" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C194" t="s">
@@ -8301,7 +8295,7 @@
       <c r="B195" t="s">
         <v>405</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C195" s="12" t="s">
         <v>336</v>
       </c>
       <c r="D195" t="s">
@@ -8326,11 +8320,11 @@
         <v>477</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>389</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B196" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C196" s="12" t="s">
@@ -8343,7 +8337,7 @@
         <v>1</v>
       </c>
       <c r="G196" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H196" s="3" t="s">
         <v>391</v>
@@ -8365,7 +8359,7 @@
       <c r="B197" t="s">
         <v>405</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C197" s="12" t="s">
         <v>337</v>
       </c>
       <c r="D197" t="s">
@@ -8397,7 +8391,7 @@
       <c r="B198" t="s">
         <v>405</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C198" s="12" t="s">
         <v>338</v>
       </c>
       <c r="D198" t="s">
@@ -8429,7 +8423,7 @@
       <c r="B199" t="s">
         <v>405</v>
       </c>
-      <c r="C199" t="s">
+      <c r="C199" s="12" t="s">
         <v>339</v>
       </c>
       <c r="D199" t="s">
@@ -8461,7 +8455,7 @@
       <c r="B200" t="s">
         <v>405</v>
       </c>
-      <c r="C200" t="s">
+      <c r="C200" s="12" t="s">
         <v>340</v>
       </c>
       <c r="D200" t="s">
@@ -8493,7 +8487,7 @@
       <c r="B201" t="s">
         <v>405</v>
       </c>
-      <c r="C201" t="s">
+      <c r="C201" s="12" t="s">
         <v>341</v>
       </c>
       <c r="D201" t="s">
@@ -8525,7 +8519,7 @@
       <c r="B202" t="s">
         <v>405</v>
       </c>
-      <c r="C202" t="s">
+      <c r="C202" s="12" t="s">
         <v>342</v>
       </c>
       <c r="D202" t="s">
@@ -8554,7 +8548,7 @@
       <c r="A203" t="s">
         <v>389</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B203" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C203" t="s">
@@ -8586,7 +8580,7 @@
       <c r="A204" t="s">
         <v>389</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B204" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C204" t="s">
@@ -8618,7 +8612,7 @@
       <c r="A205" t="s">
         <v>389</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B205" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C205" t="s">
@@ -8650,7 +8644,7 @@
       <c r="A206" t="s">
         <v>389</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B206" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C206" t="s">
@@ -8685,7 +8679,7 @@
       <c r="B207" t="s">
         <v>405</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C207" s="12" t="s">
         <v>347</v>
       </c>
       <c r="D207" t="s">
@@ -8717,7 +8711,7 @@
       <c r="B208" t="s">
         <v>405</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C208" s="12" t="s">
         <v>348</v>
       </c>
       <c r="D208" t="s">
@@ -8749,7 +8743,7 @@
       <c r="B209" t="s">
         <v>405</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C209" s="12" t="s">
         <v>349</v>
       </c>
       <c r="D209" t="s">
@@ -8774,11 +8768,11 @@
         <v>399</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>389</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B210" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C210" s="12" t="s">
@@ -8791,7 +8785,7 @@
         <v>1</v>
       </c>
       <c r="G210" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H210" s="3" t="s">
         <v>391</v>
@@ -8806,11 +8800,11 @@
         <v>588</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>389</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B211" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C211" s="12" t="s">
@@ -8823,7 +8817,7 @@
         <v>1</v>
       </c>
       <c r="G211" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H211" s="3" t="s">
         <v>391</v>
@@ -8838,11 +8832,11 @@
         <v>591</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>389</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B212" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C212" s="12" t="s">
@@ -8855,7 +8849,7 @@
         <v>1</v>
       </c>
       <c r="G212" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H212" s="3" t="s">
         <v>391</v>
@@ -8877,7 +8871,7 @@
       <c r="B213" t="s">
         <v>405</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C213" s="12" t="s">
         <v>350</v>
       </c>
       <c r="D213" t="s">
@@ -8906,7 +8900,7 @@
       <c r="A214" t="s">
         <v>389</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B214" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C214" t="s">
@@ -8934,11 +8928,11 @@
         <v>550</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>389</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B215" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C215" s="12" t="s">
@@ -8951,7 +8945,7 @@
         <v>1</v>
       </c>
       <c r="G215" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H215" s="3" t="s">
         <v>391</v>
@@ -8973,7 +8967,7 @@
       <c r="B216" t="s">
         <v>405</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C216" s="12" t="s">
         <v>352</v>
       </c>
       <c r="D216" t="s">
@@ -9005,7 +8999,7 @@
       <c r="B217" t="s">
         <v>405</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C217" s="12" t="s">
         <v>353</v>
       </c>
       <c r="D217" t="s">
@@ -9037,7 +9031,7 @@
       <c r="B218" t="s">
         <v>405</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C218" s="12" t="s">
         <v>354</v>
       </c>
       <c r="D218" t="s">
@@ -9069,7 +9063,7 @@
       <c r="B219" t="s">
         <v>405</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C219" s="12" t="s">
         <v>355</v>
       </c>
       <c r="D219" t="s">
@@ -9101,7 +9095,7 @@
       <c r="B220" t="s">
         <v>405</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C220" s="12" t="s">
         <v>356</v>
       </c>
       <c r="D220" t="s">
@@ -9133,7 +9127,7 @@
       <c r="B221" t="s">
         <v>405</v>
       </c>
-      <c r="C221" t="s">
+      <c r="C221" s="12" t="s">
         <v>357</v>
       </c>
       <c r="D221" t="s">
@@ -9165,7 +9159,7 @@
       <c r="B222" t="s">
         <v>405</v>
       </c>
-      <c r="C222" t="s">
+      <c r="C222" s="12" t="s">
         <v>358</v>
       </c>
       <c r="D222" t="s">
@@ -9197,7 +9191,7 @@
       <c r="B223" t="s">
         <v>405</v>
       </c>
-      <c r="C223" t="s">
+      <c r="C223" s="12" t="s">
         <v>359</v>
       </c>
       <c r="D223" t="s">
@@ -9229,7 +9223,7 @@
       <c r="B224" t="s">
         <v>405</v>
       </c>
-      <c r="C224" t="s">
+      <c r="C224" s="12" t="s">
         <v>360</v>
       </c>
       <c r="D224" t="s">
@@ -9261,7 +9255,7 @@
       <c r="B225" t="s">
         <v>405</v>
       </c>
-      <c r="C225" t="s">
+      <c r="C225" s="12" t="s">
         <v>361</v>
       </c>
       <c r="D225" t="s">
@@ -9293,7 +9287,7 @@
       <c r="B226" t="s">
         <v>405</v>
       </c>
-      <c r="C226" t="s">
+      <c r="C226" s="12" t="s">
         <v>362</v>
       </c>
       <c r="D226" t="s">
@@ -9325,7 +9319,7 @@
       <c r="B227" t="s">
         <v>405</v>
       </c>
-      <c r="C227" t="s">
+      <c r="C227" s="12" t="s">
         <v>363</v>
       </c>
       <c r="D227" t="s">
@@ -9357,7 +9351,7 @@
       <c r="B228" t="s">
         <v>405</v>
       </c>
-      <c r="C228" t="s">
+      <c r="C228" s="12" t="s">
         <v>364</v>
       </c>
       <c r="D228" t="s">
@@ -9386,7 +9380,7 @@
       <c r="A229" t="s">
         <v>389</v>
       </c>
-      <c r="B229" t="s">
+      <c r="B229" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C229" t="s">
@@ -9418,7 +9412,7 @@
       <c r="A230" t="s">
         <v>389</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B230" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C230" s="9" t="s">
@@ -9450,7 +9444,7 @@
       <c r="A231" t="s">
         <v>389</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B231" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C231" s="9" t="s">
@@ -9482,7 +9476,7 @@
       <c r="A232" t="s">
         <v>389</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B232" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C232" s="9" t="s">
@@ -9517,7 +9511,7 @@
       <c r="B233" t="s">
         <v>405</v>
       </c>
-      <c r="C233" t="s">
+      <c r="C233" s="12" t="s">
         <v>366</v>
       </c>
       <c r="D233" t="s">
@@ -9549,7 +9543,7 @@
       <c r="B234" t="s">
         <v>405</v>
       </c>
-      <c r="C234" t="s">
+      <c r="C234" s="12" t="s">
         <v>367</v>
       </c>
       <c r="D234" t="s">
@@ -9581,7 +9575,7 @@
       <c r="B235" t="s">
         <v>405</v>
       </c>
-      <c r="C235" t="s">
+      <c r="C235" s="12" t="s">
         <v>368</v>
       </c>
       <c r="D235" t="s">
@@ -9610,7 +9604,7 @@
       <c r="A236" t="s">
         <v>389</v>
       </c>
-      <c r="B236" t="s">
+      <c r="B236" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C236" t="s">
@@ -9645,7 +9639,7 @@
       <c r="B237" t="s">
         <v>405</v>
       </c>
-      <c r="C237" t="s">
+      <c r="C237" s="12" t="s">
         <v>370</v>
       </c>
       <c r="D237" t="s">
@@ -9677,7 +9671,7 @@
       <c r="B238" t="s">
         <v>405</v>
       </c>
-      <c r="C238" t="s">
+      <c r="C238" s="12" t="s">
         <v>371</v>
       </c>
       <c r="D238" t="s">
@@ -9702,11 +9696,11 @@
         <v>417</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>401</v>
       </c>
-      <c r="B239" t="s">
+      <c r="B239" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C239" s="12" t="s">
@@ -9719,7 +9713,7 @@
         <v>15</v>
       </c>
       <c r="G239" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H239" s="3" t="s">
         <v>391</v>
@@ -9741,7 +9735,7 @@
       <c r="B240" t="s">
         <v>405</v>
       </c>
-      <c r="C240" t="s">
+      <c r="C240" s="12" t="s">
         <v>372</v>
       </c>
       <c r="D240" t="s">
@@ -9773,7 +9767,7 @@
       <c r="B241" t="s">
         <v>405</v>
       </c>
-      <c r="C241" t="s">
+      <c r="C241" s="12" t="s">
         <v>373</v>
       </c>
       <c r="D241" t="s">
@@ -9805,7 +9799,7 @@
       <c r="B242" t="s">
         <v>405</v>
       </c>
-      <c r="C242" t="s">
+      <c r="C242" s="12" t="s">
         <v>374</v>
       </c>
       <c r="D242" t="s">
@@ -9837,7 +9831,7 @@
       <c r="B243" t="s">
         <v>405</v>
       </c>
-      <c r="C243" t="s">
+      <c r="C243" s="12" t="s">
         <v>375</v>
       </c>
       <c r="D243" t="s">
@@ -9869,7 +9863,7 @@
       <c r="B244" t="s">
         <v>405</v>
       </c>
-      <c r="C244" t="s">
+      <c r="C244" s="12" t="s">
         <v>376</v>
       </c>
       <c r="D244" t="s">
@@ -9901,7 +9895,7 @@
       <c r="B245" t="s">
         <v>405</v>
       </c>
-      <c r="C245" t="s">
+      <c r="C245" s="12" t="s">
         <v>377</v>
       </c>
       <c r="D245" t="s">
@@ -9933,7 +9927,7 @@
       <c r="B246" t="s">
         <v>405</v>
       </c>
-      <c r="C246" t="s">
+      <c r="C246" s="12" t="s">
         <v>378</v>
       </c>
       <c r="D246" t="s">
@@ -9965,7 +9959,7 @@
       <c r="B247" t="s">
         <v>405</v>
       </c>
-      <c r="C247" t="s">
+      <c r="C247" s="12" t="s">
         <v>379</v>
       </c>
       <c r="D247" t="s">
@@ -9997,7 +9991,7 @@
       <c r="B248" t="s">
         <v>405</v>
       </c>
-      <c r="C248" t="s">
+      <c r="C248" s="12" t="s">
         <v>380</v>
       </c>
       <c r="D248" t="s">
@@ -10022,11 +10016,11 @@
         <v>442</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>389</v>
       </c>
-      <c r="B249" t="s">
+      <c r="B249" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C249" s="12" t="s">
@@ -10039,7 +10033,7 @@
         <v>1</v>
       </c>
       <c r="G249" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H249" s="3" t="s">
         <v>391</v>
@@ -10061,7 +10055,7 @@
       <c r="B250" t="s">
         <v>405</v>
       </c>
-      <c r="C250" t="s">
+      <c r="C250" s="12" t="s">
         <v>381</v>
       </c>
       <c r="D250" t="s">
@@ -10093,7 +10087,7 @@
       <c r="B251" t="s">
         <v>405</v>
       </c>
-      <c r="C251" t="s">
+      <c r="C251" s="12" t="s">
         <v>382</v>
       </c>
       <c r="D251" t="s">
@@ -10122,7 +10116,7 @@
       <c r="A252" t="s">
         <v>389</v>
       </c>
-      <c r="B252" t="s">
+      <c r="B252" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C252" t="s">
@@ -10157,7 +10151,7 @@
       <c r="B253" t="s">
         <v>405</v>
       </c>
-      <c r="C253" t="s">
+      <c r="C253" s="12" t="s">
         <v>384</v>
       </c>
       <c r="D253" t="s">
@@ -10190,7 +10184,7 @@
       <c r="B254" t="s">
         <v>405</v>
       </c>
-      <c r="C254" t="s">
+      <c r="C254" s="12" t="s">
         <v>385</v>
       </c>
       <c r="D254" t="s">
@@ -10223,7 +10217,7 @@
       <c r="B255" t="s">
         <v>405</v>
       </c>
-      <c r="C255" t="s">
+      <c r="C255" s="12" t="s">
         <v>386</v>
       </c>
       <c r="D255" t="s">
@@ -10255,7 +10249,7 @@
       <c r="B256" t="s">
         <v>405</v>
       </c>
-      <c r="C256" t="s">
+      <c r="C256" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D256" t="s">
@@ -10284,7 +10278,7 @@
       <c r="A257" t="s">
         <v>389</v>
       </c>
-      <c r="B257" t="s">
+      <c r="B257" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C257" s="9" t="s">
@@ -10316,7 +10310,7 @@
       <c r="A258" t="s">
         <v>389</v>
       </c>
-      <c r="B258" t="s">
+      <c r="B258" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C258" s="9" t="s">
@@ -10348,7 +10342,7 @@
       <c r="A259" t="s">
         <v>389</v>
       </c>
-      <c r="B259" t="s">
+      <c r="B259" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C259" s="9" t="s">
@@ -10380,7 +10374,7 @@
       <c r="A260" t="s">
         <v>389</v>
       </c>
-      <c r="B260" t="s">
+      <c r="B260" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C260" s="9" t="s">
@@ -10415,7 +10409,7 @@
       <c r="B261" t="s">
         <v>405</v>
       </c>
-      <c r="C261" t="s">
+      <c r="C261" s="12" t="s">
         <v>387</v>
       </c>
       <c r="D261" t="s">
@@ -10440,11 +10434,11 @@
         <v>469</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>389</v>
       </c>
-      <c r="B262" t="s">
+      <c r="B262" s="12" t="s">
         <v>405</v>
       </c>
       <c r="C262" s="12" t="s">
@@ -10457,7 +10451,7 @@
         <v>1</v>
       </c>
       <c r="G262" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H262" s="3" t="s">
         <v>391</v>

</xml_diff>

<commit_message>
Add lightson lightsoff sound effect in Party Levels. ChatEngine: update dialogue. AudioManager: add lightsoff, lightson soundFX. ButtonTap: add lightsoff, lightson button tap sounds. Constants: add K.UserDefaults.disableLights property. SettingsPage: didTapRadio() delete code that affects party lights when muting/unmuting music. PauseResetEngine: change K.UserDefaults.muteMusic to .disableLights when dealing with the disco ball button. PartyModeSprite: switch from using old .muteMusic to new .disableLights Constants property.
</commit_message>
<xml_diff>
--- a/JSON/AssetsCatalog.xlsx
+++ b/JSON/AssetsCatalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035151DC-C069-3D44-B3A7-26EBC9B3A0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F17F96E-C4D0-D24F-95EE-B17102CCC291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{E84333C6-E3B6-FB42-AB04-827399F33810}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$262</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$264</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2237" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2247" uniqueCount="647">
   <si>
     <t>Filename</t>
   </si>
@@ -1974,6 +1974,12 @@
   </si>
   <si>
     <t>waterappear3</t>
+  </si>
+  <si>
+    <t>lightsoff</t>
+  </si>
+  <si>
+    <t>lightson</t>
   </si>
 </sst>
 </file>
@@ -2059,7 +2065,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -2072,7 +2078,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -2390,13 +2395,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:L262"/>
+  <dimension ref="A1:L264"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D160" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H205" sqref="H205"/>
+      <selection pane="bottomRight" activeCell="G203" sqref="G203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8689,7 +8694,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>389</v>
       </c>
@@ -8697,31 +8702,22 @@
         <v>405</v>
       </c>
       <c r="C207" t="s">
-        <v>347</v>
+        <v>645</v>
       </c>
       <c r="D207" t="s">
         <v>388</v>
       </c>
-      <c r="F207" s="3">
-        <v>2</v>
-      </c>
-      <c r="G207" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="H207" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="I207" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="K207" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="L207" s="6" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F207" s="11"/>
+      <c r="G207" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="H207" s="8"/>
+      <c r="I207" s="8"/>
+      <c r="J207" s="8"/>
+      <c r="K207" s="8"/>
+      <c r="L207" s="9"/>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>389</v>
       </c>
@@ -8729,29 +8725,20 @@
         <v>405</v>
       </c>
       <c r="C208" t="s">
-        <v>348</v>
+        <v>646</v>
       </c>
       <c r="D208" t="s">
         <v>388</v>
       </c>
-      <c r="F208" s="3">
-        <v>1</v>
-      </c>
-      <c r="G208" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="H208" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="I208" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="K208" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="L208" s="6" t="s">
-        <v>415</v>
-      </c>
+      <c r="F208" s="11"/>
+      <c r="G208" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="H208" s="8"/>
+      <c r="I208" s="8"/>
+      <c r="J208" s="8"/>
+      <c r="K208" s="8"/>
+      <c r="L208" s="9"/>
     </row>
     <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
@@ -8761,7 +8748,7 @@
         <v>405</v>
       </c>
       <c r="C209" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D209" t="s">
         <v>388</v>
@@ -8776,13 +8763,13 @@
         <v>391</v>
       </c>
       <c r="I209" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K209" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="L209" s="7" t="s">
-        <v>399</v>
+        <v>395</v>
+      </c>
+      <c r="L209" s="6" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -8793,7 +8780,7 @@
         <v>405</v>
       </c>
       <c r="C210" t="s">
-        <v>588</v>
+        <v>348</v>
       </c>
       <c r="D210" t="s">
         <v>388</v>
@@ -8808,13 +8795,13 @@
         <v>391</v>
       </c>
       <c r="I210" s="3" t="s">
-        <v>392</v>
+        <v>411</v>
       </c>
       <c r="K210" s="3" t="s">
-        <v>586</v>
-      </c>
-      <c r="L210" s="7" t="s">
-        <v>587</v>
+        <v>416</v>
+      </c>
+      <c r="L210" s="6" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -8825,13 +8812,13 @@
         <v>405</v>
       </c>
       <c r="C211" t="s">
-        <v>589</v>
+        <v>349</v>
       </c>
       <c r="D211" t="s">
         <v>388</v>
       </c>
       <c r="F211" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G211" s="3" t="s">
         <v>174</v>
@@ -8840,13 +8827,13 @@
         <v>391</v>
       </c>
       <c r="I211" s="3" t="s">
-        <v>592</v>
+        <v>397</v>
       </c>
       <c r="K211" s="3" t="s">
-        <v>591</v>
+        <v>398</v>
       </c>
       <c r="L211" s="7" t="s">
-        <v>590</v>
+        <v>399</v>
       </c>
     </row>
     <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -8857,7 +8844,7 @@
         <v>405</v>
       </c>
       <c r="C212" t="s">
-        <v>608</v>
+        <v>588</v>
       </c>
       <c r="D212" t="s">
         <v>388</v>
@@ -8872,13 +8859,13 @@
         <v>391</v>
       </c>
       <c r="I212" s="3" t="s">
-        <v>611</v>
+        <v>392</v>
       </c>
       <c r="K212" s="3" t="s">
-        <v>610</v>
+        <v>586</v>
       </c>
       <c r="L212" s="7" t="s">
-        <v>609</v>
+        <v>587</v>
       </c>
     </row>
     <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -8889,7 +8876,7 @@
         <v>405</v>
       </c>
       <c r="C213" t="s">
-        <v>350</v>
+        <v>589</v>
       </c>
       <c r="D213" t="s">
         <v>388</v>
@@ -8904,16 +8891,16 @@
         <v>391</v>
       </c>
       <c r="I213" s="3" t="s">
-        <v>411</v>
+        <v>592</v>
       </c>
       <c r="K213" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="L213" s="6" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
+        <v>591</v>
+      </c>
+      <c r="L213" s="7" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>389</v>
       </c>
@@ -8921,28 +8908,28 @@
         <v>405</v>
       </c>
       <c r="C214" t="s">
-        <v>351</v>
+        <v>608</v>
       </c>
       <c r="D214" t="s">
         <v>388</v>
       </c>
-      <c r="F214" s="11">
-        <v>2</v>
+      <c r="F214" s="3">
+        <v>1</v>
       </c>
       <c r="G214" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H214" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I214" s="3" t="s">
-        <v>552</v>
+        <v>611</v>
       </c>
       <c r="K214" s="3" t="s">
-        <v>551</v>
-      </c>
-      <c r="L214" s="6" t="s">
-        <v>550</v>
+        <v>610</v>
+      </c>
+      <c r="L214" s="7" t="s">
+        <v>609</v>
       </c>
     </row>
     <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -8953,7 +8940,7 @@
         <v>405</v>
       </c>
       <c r="C215" t="s">
-        <v>593</v>
+        <v>350</v>
       </c>
       <c r="D215" t="s">
         <v>388</v>
@@ -8968,16 +8955,16 @@
         <v>391</v>
       </c>
       <c r="I215" s="3" t="s">
-        <v>487</v>
+        <v>411</v>
       </c>
       <c r="K215" s="3" t="s">
-        <v>594</v>
+        <v>410</v>
       </c>
       <c r="L215" s="6" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>389</v>
       </c>
@@ -8985,28 +8972,28 @@
         <v>405</v>
       </c>
       <c r="C216" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D216" t="s">
         <v>388</v>
       </c>
-      <c r="F216" s="3">
+      <c r="F216" s="11">
         <v>2</v>
       </c>
       <c r="G216" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H216" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I216" s="3" t="s">
-        <v>501</v>
+        <v>552</v>
       </c>
       <c r="K216" s="3" t="s">
-        <v>503</v>
+        <v>551</v>
       </c>
       <c r="L216" s="6" t="s">
-        <v>502</v>
+        <v>550</v>
       </c>
     </row>
     <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9017,13 +9004,13 @@
         <v>405</v>
       </c>
       <c r="C217" t="s">
-        <v>353</v>
+        <v>593</v>
       </c>
       <c r="D217" t="s">
         <v>388</v>
       </c>
       <c r="F217" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G217" s="3" t="s">
         <v>174</v>
@@ -9032,13 +9019,13 @@
         <v>391</v>
       </c>
       <c r="I217" s="3" t="s">
-        <v>537</v>
+        <v>487</v>
       </c>
       <c r="K217" s="3" t="s">
-        <v>536</v>
+        <v>594</v>
       </c>
       <c r="L217" s="6" t="s">
-        <v>535</v>
+        <v>595</v>
       </c>
     </row>
     <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9049,13 +9036,13 @@
         <v>405</v>
       </c>
       <c r="C218" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D218" t="s">
         <v>388</v>
       </c>
       <c r="F218" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G218" s="3" t="s">
         <v>174</v>
@@ -9064,13 +9051,13 @@
         <v>391</v>
       </c>
       <c r="I218" s="3" t="s">
-        <v>537</v>
+        <v>501</v>
       </c>
       <c r="K218" s="3" t="s">
-        <v>536</v>
+        <v>503</v>
       </c>
       <c r="L218" s="6" t="s">
-        <v>535</v>
+        <v>502</v>
       </c>
     </row>
     <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9081,13 +9068,13 @@
         <v>405</v>
       </c>
       <c r="C219" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D219" t="s">
         <v>388</v>
       </c>
       <c r="F219" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G219" s="3" t="s">
         <v>174</v>
@@ -9096,13 +9083,13 @@
         <v>391</v>
       </c>
       <c r="I219" s="3" t="s">
-        <v>509</v>
+        <v>537</v>
       </c>
       <c r="K219" s="3" t="s">
-        <v>508</v>
+        <v>536</v>
       </c>
       <c r="L219" s="6" t="s">
-        <v>507</v>
+        <v>535</v>
       </c>
     </row>
     <row r="220" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9113,13 +9100,13 @@
         <v>405</v>
       </c>
       <c r="C220" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D220" t="s">
         <v>388</v>
       </c>
       <c r="F220" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G220" s="3" t="s">
         <v>174</v>
@@ -9128,13 +9115,13 @@
         <v>391</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>522</v>
+        <v>537</v>
       </c>
       <c r="K220" s="3" t="s">
-        <v>521</v>
+        <v>536</v>
       </c>
       <c r="L220" s="6" t="s">
-        <v>520</v>
+        <v>535</v>
       </c>
     </row>
     <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9145,13 +9132,13 @@
         <v>405</v>
       </c>
       <c r="C221" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D221" t="s">
         <v>388</v>
       </c>
       <c r="F221" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G221" s="3" t="s">
         <v>174</v>
@@ -9160,13 +9147,13 @@
         <v>391</v>
       </c>
       <c r="I221" s="3" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="K221" s="3" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="L221" s="6" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
     </row>
     <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9177,13 +9164,13 @@
         <v>405</v>
       </c>
       <c r="C222" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D222" t="s">
         <v>388</v>
       </c>
       <c r="F222" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G222" s="3" t="s">
         <v>174</v>
@@ -9192,13 +9179,13 @@
         <v>391</v>
       </c>
       <c r="I222" s="3" t="s">
-        <v>534</v>
+        <v>522</v>
       </c>
       <c r="K222" s="3" t="s">
-        <v>533</v>
+        <v>521</v>
       </c>
       <c r="L222" s="6" t="s">
-        <v>532</v>
+        <v>520</v>
       </c>
     </row>
     <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9209,7 +9196,7 @@
         <v>405</v>
       </c>
       <c r="C223" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D223" t="s">
         <v>388</v>
@@ -9224,13 +9211,13 @@
         <v>391</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>501</v>
+        <v>519</v>
       </c>
       <c r="K223" s="3" t="s">
-        <v>500</v>
+        <v>518</v>
       </c>
       <c r="L223" s="6" t="s">
-        <v>499</v>
+        <v>517</v>
       </c>
     </row>
     <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9241,13 +9228,13 @@
         <v>405</v>
       </c>
       <c r="C224" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D224" t="s">
         <v>388</v>
       </c>
       <c r="F224" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G224" s="3" t="s">
         <v>174</v>
@@ -9256,13 +9243,13 @@
         <v>391</v>
       </c>
       <c r="I224" s="3" t="s">
-        <v>501</v>
+        <v>534</v>
       </c>
       <c r="K224" s="3" t="s">
-        <v>500</v>
+        <v>533</v>
       </c>
       <c r="L224" s="6" t="s">
-        <v>499</v>
+        <v>532</v>
       </c>
     </row>
     <row r="225" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9273,13 +9260,13 @@
         <v>405</v>
       </c>
       <c r="C225" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D225" t="s">
         <v>388</v>
       </c>
       <c r="F225" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G225" s="3" t="s">
         <v>174</v>
@@ -9305,7 +9292,7 @@
         <v>405</v>
       </c>
       <c r="C226" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D226" t="s">
         <v>388</v>
@@ -9337,13 +9324,13 @@
         <v>405</v>
       </c>
       <c r="C227" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D227" t="s">
         <v>388</v>
       </c>
       <c r="F227" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G227" s="3" t="s">
         <v>174</v>
@@ -9352,13 +9339,13 @@
         <v>391</v>
       </c>
       <c r="I227" s="3" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="K227" s="3" t="s">
-        <v>491</v>
+        <v>500</v>
       </c>
       <c r="L227" s="6" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
     </row>
     <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9369,7 +9356,7 @@
         <v>405</v>
       </c>
       <c r="C228" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D228" t="s">
         <v>388</v>
@@ -9384,16 +9371,16 @@
         <v>391</v>
       </c>
       <c r="I228" s="3" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="K228" s="3" t="s">
-        <v>491</v>
+        <v>500</v>
       </c>
       <c r="L228" s="6" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.2">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>389</v>
       </c>
@@ -9401,60 +9388,60 @@
         <v>405</v>
       </c>
       <c r="C229" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D229" t="s">
         <v>388</v>
       </c>
-      <c r="F229" s="11">
-        <v>5</v>
+      <c r="F229" s="3">
+        <v>2</v>
       </c>
       <c r="G229" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H229" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I229" s="3" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="K229" s="3" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="L229" s="6" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.2">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>389</v>
       </c>
       <c r="B230" t="s">
         <v>405</v>
       </c>
-      <c r="C230" s="9" t="s">
-        <v>575</v>
+      <c r="C230" t="s">
+        <v>364</v>
       </c>
       <c r="D230" t="s">
         <v>388</v>
       </c>
-      <c r="F230" s="11">
-        <v>1</v>
+      <c r="F230" s="3">
+        <v>0</v>
       </c>
       <c r="G230" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H230" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I230" s="3" t="s">
-        <v>578</v>
+        <v>487</v>
       </c>
       <c r="K230" s="3" t="s">
-        <v>579</v>
+        <v>491</v>
       </c>
       <c r="L230" s="6" t="s">
-        <v>580</v>
+        <v>490</v>
       </c>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.2">
@@ -9464,14 +9451,14 @@
       <c r="B231" t="s">
         <v>405</v>
       </c>
-      <c r="C231" s="9" t="s">
-        <v>577</v>
+      <c r="C231" t="s">
+        <v>365</v>
       </c>
       <c r="D231" t="s">
         <v>388</v>
       </c>
       <c r="F231" s="11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G231" s="3" t="s">
         <v>432</v>
@@ -9480,13 +9467,13 @@
         <v>391</v>
       </c>
       <c r="I231" s="3" t="s">
-        <v>578</v>
+        <v>494</v>
       </c>
       <c r="K231" s="3" t="s">
-        <v>579</v>
+        <v>493</v>
       </c>
       <c r="L231" s="6" t="s">
-        <v>580</v>
+        <v>492</v>
       </c>
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.2">
@@ -9497,13 +9484,13 @@
         <v>405</v>
       </c>
       <c r="C232" s="9" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D232" t="s">
         <v>388</v>
       </c>
       <c r="F232" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G232" s="3" t="s">
         <v>432</v>
@@ -9521,68 +9508,68 @@
         <v>580</v>
       </c>
     </row>
-    <row r="233" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>389</v>
       </c>
       <c r="B233" t="s">
         <v>405</v>
       </c>
-      <c r="C233" t="s">
-        <v>366</v>
+      <c r="C233" s="9" t="s">
+        <v>577</v>
       </c>
       <c r="D233" t="s">
         <v>388</v>
       </c>
-      <c r="F233" s="3">
-        <v>3</v>
+      <c r="F233" s="11">
+        <v>0</v>
       </c>
       <c r="G233" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H233" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I233" s="3" t="s">
-        <v>487</v>
+        <v>578</v>
       </c>
       <c r="K233" s="3" t="s">
-        <v>489</v>
+        <v>579</v>
       </c>
       <c r="L233" s="6" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="234" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>389</v>
       </c>
       <c r="B234" t="s">
         <v>405</v>
       </c>
-      <c r="C234" t="s">
-        <v>367</v>
+      <c r="C234" s="9" t="s">
+        <v>576</v>
       </c>
       <c r="D234" t="s">
         <v>388</v>
       </c>
-      <c r="F234" s="3">
+      <c r="F234" s="11">
         <v>0</v>
       </c>
       <c r="G234" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H234" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I234" s="3" t="s">
-        <v>487</v>
+        <v>578</v>
       </c>
       <c r="K234" s="3" t="s">
-        <v>489</v>
+        <v>579</v>
       </c>
       <c r="L234" s="6" t="s">
-        <v>488</v>
+        <v>580</v>
       </c>
     </row>
     <row r="235" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9593,13 +9580,13 @@
         <v>405</v>
       </c>
       <c r="C235" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D235" t="s">
         <v>388</v>
       </c>
       <c r="F235" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G235" s="3" t="s">
         <v>174</v>
@@ -9617,7 +9604,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>389</v>
       </c>
@@ -9625,45 +9612,45 @@
         <v>405</v>
       </c>
       <c r="C236" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D236" t="s">
         <v>388</v>
       </c>
-      <c r="F236" s="11">
-        <v>3</v>
+      <c r="F236" s="3">
+        <v>0</v>
       </c>
       <c r="G236" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H236" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I236" s="3" t="s">
-        <v>396</v>
+        <v>487</v>
       </c>
       <c r="K236" s="3" t="s">
-        <v>516</v>
+        <v>489</v>
       </c>
       <c r="L236" s="6" t="s">
-        <v>515</v>
+        <v>488</v>
       </c>
     </row>
     <row r="237" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B237" t="s">
         <v>405</v>
       </c>
       <c r="C237" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D237" t="s">
         <v>388</v>
       </c>
       <c r="F237" s="3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G237" s="3" t="s">
         <v>174</v>
@@ -9672,45 +9659,45 @@
         <v>391</v>
       </c>
       <c r="I237" s="3" t="s">
-        <v>463</v>
+        <v>487</v>
       </c>
       <c r="K237" s="3" t="s">
-        <v>462</v>
+        <v>489</v>
       </c>
       <c r="L237" s="6" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="238" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B238" t="s">
         <v>405</v>
       </c>
       <c r="C238" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D238" t="s">
         <v>388</v>
       </c>
-      <c r="F238" s="3">
-        <v>20</v>
+      <c r="F238" s="11">
+        <v>3</v>
       </c>
       <c r="G238" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H238" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I238" s="3" t="s">
-        <v>419</v>
+        <v>396</v>
       </c>
       <c r="K238" s="3" t="s">
-        <v>418</v>
+        <v>516</v>
       </c>
       <c r="L238" s="6" t="s">
-        <v>417</v>
+        <v>515</v>
       </c>
     </row>
     <row r="239" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9721,7 +9708,7 @@
         <v>405</v>
       </c>
       <c r="C239" t="s">
-        <v>620</v>
+        <v>370</v>
       </c>
       <c r="D239" t="s">
         <v>388</v>
@@ -9736,13 +9723,13 @@
         <v>391</v>
       </c>
       <c r="I239" s="3" t="s">
-        <v>621</v>
+        <v>463</v>
       </c>
       <c r="K239" s="3" t="s">
-        <v>622</v>
+        <v>462</v>
       </c>
       <c r="L239" s="6" t="s">
-        <v>623</v>
+        <v>461</v>
       </c>
     </row>
     <row r="240" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9753,13 +9740,13 @@
         <v>405</v>
       </c>
       <c r="C240" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D240" t="s">
         <v>388</v>
       </c>
       <c r="F240" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G240" s="3" t="s">
         <v>174</v>
@@ -9768,30 +9755,30 @@
         <v>391</v>
       </c>
       <c r="I240" s="3" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
       <c r="K240" s="3" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
       <c r="L240" s="6" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
     </row>
     <row r="241" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B241" t="s">
         <v>405</v>
       </c>
       <c r="C241" t="s">
-        <v>373</v>
+        <v>620</v>
       </c>
       <c r="D241" t="s">
         <v>388</v>
       </c>
       <c r="F241" s="3">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G241" s="3" t="s">
         <v>174</v>
@@ -9800,30 +9787,30 @@
         <v>391</v>
       </c>
       <c r="I241" s="3" t="s">
-        <v>446</v>
+        <v>621</v>
       </c>
       <c r="K241" s="3" t="s">
-        <v>445</v>
+        <v>622</v>
       </c>
       <c r="L241" s="6" t="s">
-        <v>444</v>
+        <v>623</v>
       </c>
     </row>
     <row r="242" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B242" t="s">
         <v>405</v>
       </c>
       <c r="C242" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D242" t="s">
         <v>388</v>
       </c>
       <c r="F242" s="3">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G242" s="3" t="s">
         <v>174</v>
@@ -9832,13 +9819,13 @@
         <v>391</v>
       </c>
       <c r="I242" s="3" t="s">
-        <v>411</v>
+        <v>435</v>
       </c>
       <c r="K242" s="3" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="L242" s="6" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="243" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9849,13 +9836,13 @@
         <v>405</v>
       </c>
       <c r="C243" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D243" t="s">
         <v>388</v>
       </c>
       <c r="F243" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G243" s="3" t="s">
         <v>174</v>
@@ -9881,13 +9868,13 @@
         <v>405</v>
       </c>
       <c r="C244" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D244" t="s">
         <v>388</v>
       </c>
       <c r="F244" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G244" s="3" t="s">
         <v>174</v>
@@ -9896,13 +9883,13 @@
         <v>391</v>
       </c>
       <c r="I244" s="3" t="s">
-        <v>454</v>
+        <v>411</v>
       </c>
       <c r="K244" s="3" t="s">
-        <v>453</v>
+        <v>431</v>
       </c>
       <c r="L244" s="6" t="s">
-        <v>452</v>
+        <v>430</v>
       </c>
     </row>
     <row r="245" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9913,13 +9900,13 @@
         <v>405</v>
       </c>
       <c r="C245" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D245" t="s">
         <v>388</v>
       </c>
       <c r="F245" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G245" s="3" t="s">
         <v>174</v>
@@ -9928,13 +9915,13 @@
         <v>391</v>
       </c>
       <c r="I245" s="3" t="s">
-        <v>411</v>
+        <v>446</v>
       </c>
       <c r="K245" s="3" t="s">
-        <v>476</v>
+        <v>445</v>
       </c>
       <c r="L245" s="6" t="s">
-        <v>475</v>
+        <v>444</v>
       </c>
     </row>
     <row r="246" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9945,13 +9932,13 @@
         <v>405</v>
       </c>
       <c r="C246" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D246" t="s">
         <v>388</v>
       </c>
       <c r="F246" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G246" s="3" t="s">
         <v>174</v>
@@ -9960,13 +9947,13 @@
         <v>391</v>
       </c>
       <c r="I246" s="3" t="s">
-        <v>506</v>
+        <v>454</v>
       </c>
       <c r="K246" s="3" t="s">
-        <v>505</v>
+        <v>453</v>
       </c>
       <c r="L246" s="6" t="s">
-        <v>504</v>
+        <v>452</v>
       </c>
     </row>
     <row r="247" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9977,13 +9964,13 @@
         <v>405</v>
       </c>
       <c r="C247" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D247" t="s">
         <v>388</v>
       </c>
       <c r="F247" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G247" s="3" t="s">
         <v>174</v>
@@ -9992,13 +9979,13 @@
         <v>391</v>
       </c>
       <c r="I247" s="3" t="s">
-        <v>441</v>
+        <v>411</v>
       </c>
       <c r="K247" s="3" t="s">
-        <v>440</v>
+        <v>476</v>
       </c>
       <c r="L247" s="6" t="s">
-        <v>439</v>
+        <v>475</v>
       </c>
     </row>
     <row r="248" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -10009,13 +9996,13 @@
         <v>405</v>
       </c>
       <c r="C248" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D248" t="s">
         <v>388</v>
       </c>
       <c r="F248" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G248" s="3" t="s">
         <v>174</v>
@@ -10024,13 +10011,13 @@
         <v>391</v>
       </c>
       <c r="I248" s="3" t="s">
-        <v>443</v>
+        <v>506</v>
       </c>
       <c r="K248" s="3" t="s">
-        <v>440</v>
+        <v>505</v>
       </c>
       <c r="L248" s="6" t="s">
-        <v>442</v>
+        <v>504</v>
       </c>
     </row>
     <row r="249" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -10041,7 +10028,7 @@
         <v>405</v>
       </c>
       <c r="C249" t="s">
-        <v>635</v>
+        <v>379</v>
       </c>
       <c r="D249" t="s">
         <v>388</v>
@@ -10056,13 +10043,13 @@
         <v>391</v>
       </c>
       <c r="I249" s="3" t="s">
-        <v>636</v>
+        <v>441</v>
       </c>
       <c r="K249" s="3" t="s">
-        <v>637</v>
+        <v>440</v>
       </c>
       <c r="L249" s="6" t="s">
-        <v>638</v>
+        <v>439</v>
       </c>
     </row>
     <row r="250" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -10073,13 +10060,13 @@
         <v>405</v>
       </c>
       <c r="C250" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D250" t="s">
         <v>388</v>
       </c>
       <c r="F250" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G250" s="3" t="s">
         <v>174</v>
@@ -10088,30 +10075,30 @@
         <v>391</v>
       </c>
       <c r="I250" s="3" t="s">
-        <v>411</v>
+        <v>443</v>
       </c>
       <c r="K250" s="3" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="L250" s="6" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
     </row>
     <row r="251" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B251" t="s">
         <v>405</v>
       </c>
       <c r="C251" t="s">
-        <v>382</v>
+        <v>635</v>
       </c>
       <c r="D251" t="s">
         <v>388</v>
       </c>
       <c r="F251" s="3">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="G251" s="3" t="s">
         <v>174</v>
@@ -10120,16 +10107,16 @@
         <v>391</v>
       </c>
       <c r="I251" s="3" t="s">
-        <v>414</v>
+        <v>636</v>
       </c>
       <c r="K251" s="3" t="s">
-        <v>413</v>
+        <v>637</v>
       </c>
       <c r="L251" s="6" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.2">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>389</v>
       </c>
@@ -10137,45 +10124,45 @@
         <v>405</v>
       </c>
       <c r="C252" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D252" t="s">
         <v>388</v>
       </c>
-      <c r="F252" s="11">
-        <v>2</v>
+      <c r="F252" s="3">
+        <v>1</v>
       </c>
       <c r="G252" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H252" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I252" s="3" t="s">
-        <v>525</v>
+        <v>411</v>
       </c>
       <c r="K252" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="L252" s="10" t="s">
-        <v>523</v>
+        <v>451</v>
+      </c>
+      <c r="L252" s="6" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="253" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B253" t="s">
         <v>405</v>
       </c>
       <c r="C253" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D253" t="s">
         <v>388</v>
       </c>
       <c r="F253" s="3">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="G253" s="3" t="s">
         <v>174</v>
@@ -10183,18 +10170,17 @@
       <c r="H253" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I253" t="s">
-        <v>572</v>
-      </c>
-      <c r="J253"/>
-      <c r="K253" t="s">
-        <v>573</v>
+      <c r="I253" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="K253" s="3" t="s">
+        <v>413</v>
       </c>
       <c r="L253" s="6" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="254" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>389</v>
       </c>
@@ -10202,46 +10188,45 @@
         <v>405</v>
       </c>
       <c r="C254" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D254" t="s">
         <v>388</v>
       </c>
-      <c r="F254" s="3">
-        <v>1</v>
+      <c r="F254" s="11">
+        <v>2</v>
       </c>
       <c r="G254" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H254" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I254" t="s">
-        <v>569</v>
-      </c>
-      <c r="J254"/>
-      <c r="K254" t="s">
-        <v>570</v>
-      </c>
-      <c r="L254" s="6" t="s">
-        <v>571</v>
+      <c r="I254" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="K254" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="L254" s="10" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="255" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B255" t="s">
         <v>405</v>
       </c>
       <c r="C255" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D255" t="s">
         <v>388</v>
       </c>
       <c r="F255" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G255" s="3" t="s">
         <v>174</v>
@@ -10249,14 +10234,15 @@
       <c r="H255" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I255" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="K255" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="L255" s="7" t="s">
-        <v>404</v>
+      <c r="I255" t="s">
+        <v>572</v>
+      </c>
+      <c r="J255"/>
+      <c r="K255" t="s">
+        <v>573</v>
+      </c>
+      <c r="L255" s="6" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="256" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -10267,7 +10253,7 @@
         <v>405</v>
       </c>
       <c r="C256" t="s">
-        <v>58</v>
+        <v>385</v>
       </c>
       <c r="D256" t="s">
         <v>388</v>
@@ -10281,78 +10267,79 @@
       <c r="H256" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I256" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="K256" s="3" t="s">
-        <v>467</v>
+      <c r="I256" t="s">
+        <v>569</v>
+      </c>
+      <c r="J256"/>
+      <c r="K256" t="s">
+        <v>570</v>
       </c>
       <c r="L256" s="6" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.2">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B257" t="s">
         <v>405</v>
       </c>
-      <c r="C257" s="9" t="s">
-        <v>642</v>
+      <c r="C257" t="s">
+        <v>386</v>
       </c>
       <c r="D257" t="s">
         <v>388</v>
       </c>
-      <c r="F257" s="11">
-        <v>3</v>
+      <c r="F257" s="3">
+        <v>10</v>
       </c>
       <c r="G257" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H257" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I257" s="3" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="K257" s="3" t="s">
-        <v>585</v>
-      </c>
-      <c r="L257" s="6" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.2">
+        <v>403</v>
+      </c>
+      <c r="L257" s="7" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>389</v>
       </c>
       <c r="B258" t="s">
         <v>405</v>
       </c>
-      <c r="C258" s="9" t="s">
-        <v>643</v>
+      <c r="C258" t="s">
+        <v>58</v>
       </c>
       <c r="D258" t="s">
         <v>388</v>
       </c>
-      <c r="F258" s="11">
-        <v>0</v>
+      <c r="F258" s="3">
+        <v>1</v>
       </c>
       <c r="G258" s="3" t="s">
-        <v>432</v>
+        <v>174</v>
       </c>
       <c r="H258" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I258" s="3" t="s">
-        <v>392</v>
+        <v>468</v>
       </c>
       <c r="K258" s="3" t="s">
-        <v>585</v>
+        <v>467</v>
       </c>
       <c r="L258" s="6" t="s">
-        <v>584</v>
+        <v>466</v>
       </c>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.2">
@@ -10363,13 +10350,13 @@
         <v>405</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D259" t="s">
         <v>388</v>
       </c>
       <c r="F259" s="11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G259" s="3" t="s">
         <v>432</v>
@@ -10394,14 +10381,14 @@
       <c r="B260" t="s">
         <v>405</v>
       </c>
-      <c r="C260" s="13" t="s">
-        <v>581</v>
+      <c r="C260" s="9" t="s">
+        <v>643</v>
       </c>
       <c r="D260" t="s">
         <v>388</v>
       </c>
-      <c r="F260" s="12">
-        <v>1</v>
+      <c r="F260" s="11">
+        <v>0</v>
       </c>
       <c r="G260" s="3" t="s">
         <v>432</v>
@@ -10410,56 +10397,56 @@
         <v>391</v>
       </c>
       <c r="I260" s="3" t="s">
-        <v>537</v>
+        <v>392</v>
       </c>
       <c r="K260" s="3" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="L260" s="6" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="261" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>389</v>
       </c>
       <c r="B261" t="s">
         <v>405</v>
       </c>
-      <c r="C261" t="s">
-        <v>387</v>
+      <c r="C261" s="9" t="s">
+        <v>644</v>
       </c>
       <c r="D261" t="s">
         <v>388</v>
       </c>
-      <c r="F261" s="3">
-        <v>1</v>
+      <c r="F261" s="11">
+        <v>0</v>
       </c>
       <c r="G261" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H261" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I261" s="3" t="s">
-        <v>470</v>
+        <v>392</v>
       </c>
       <c r="K261" s="3" t="s">
-        <v>471</v>
+        <v>585</v>
       </c>
       <c r="L261" s="6" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="262" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>389</v>
       </c>
       <c r="B262" t="s">
         <v>405</v>
       </c>
-      <c r="C262" t="s">
-        <v>631</v>
+      <c r="C262" s="12" t="s">
+        <v>581</v>
       </c>
       <c r="D262" t="s">
         <v>388</v>
@@ -10468,23 +10455,87 @@
         <v>1</v>
       </c>
       <c r="G262" s="3" t="s">
-        <v>174</v>
+        <v>432</v>
       </c>
       <c r="H262" s="3" t="s">
         <v>391</v>
       </c>
       <c r="I262" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="K262" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="L262" s="6" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>389</v>
+      </c>
+      <c r="B263" t="s">
+        <v>405</v>
+      </c>
+      <c r="C263" t="s">
+        <v>387</v>
+      </c>
+      <c r="D263" t="s">
+        <v>388</v>
+      </c>
+      <c r="F263" s="3">
+        <v>1</v>
+      </c>
+      <c r="G263" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H263" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I263" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="K263" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="L263" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="264" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>389</v>
+      </c>
+      <c r="B264" t="s">
+        <v>405</v>
+      </c>
+      <c r="C264" t="s">
+        <v>631</v>
+      </c>
+      <c r="D264" t="s">
+        <v>388</v>
+      </c>
+      <c r="F264" s="3">
+        <v>1</v>
+      </c>
+      <c r="G264" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H264" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="I264" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="K262" s="3" t="s">
+      <c r="K264" s="3" t="s">
         <v>633</v>
       </c>
-      <c r="L262" s="6" t="s">
+      <c r="L264" s="6" t="s">
         <v>632</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L262" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}">
+  <autoFilter ref="A1:L264" xr:uid="{E74E2A7A-1C46-1944-BF60-96E88FF431CB}">
     <filterColumn colId="6">
       <filters>
         <filter val="No"/>
@@ -10617,15 +10668,15 @@
     <hyperlink ref="L132" r:id="rId123" xr:uid="{4BFCF1BE-6310-C34B-BA09-218F6A3C75D9}"/>
     <hyperlink ref="L134" r:id="rId124" xr:uid="{C9C421A7-64D0-5D49-9F28-B71BC19F3239}"/>
     <hyperlink ref="L161" r:id="rId125" xr:uid="{F88953B7-468E-C34B-9347-94009F9A78D2}"/>
-    <hyperlink ref="L207" r:id="rId126" xr:uid="{1F3BBC8C-29E8-C74A-AB3F-04AE466222EF}"/>
-    <hyperlink ref="L209" r:id="rId127" xr:uid="{3C51058F-793C-D34A-8286-18AE4C8EF6CE}"/>
-    <hyperlink ref="L255" r:id="rId128" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
+    <hyperlink ref="L209" r:id="rId126" xr:uid="{1F3BBC8C-29E8-C74A-AB3F-04AE466222EF}"/>
+    <hyperlink ref="L211" r:id="rId127" xr:uid="{3C51058F-793C-D34A-8286-18AE4C8EF6CE}"/>
+    <hyperlink ref="L257" r:id="rId128" xr:uid="{BBB8C6C5-F263-6443-81E0-F2DEDD190667}"/>
     <hyperlink ref="L158" r:id="rId129" xr:uid="{6A722A1D-2F7B-4242-8134-716EFF33F7D2}"/>
     <hyperlink ref="L159" r:id="rId130" xr:uid="{547CD1A8-1967-1C46-95E3-89E39CD045C2}"/>
-    <hyperlink ref="L213" r:id="rId131" xr:uid="{5ACD6BFD-52F0-0940-AA8E-B04F1D397BC7}"/>
-    <hyperlink ref="L251" r:id="rId132" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
-    <hyperlink ref="L208" r:id="rId133" xr:uid="{2030AD8C-28A7-544B-92DC-5CBE411DE1C0}"/>
-    <hyperlink ref="L238" r:id="rId134" xr:uid="{05363CA1-BE60-3F42-B56A-1A92A0EDA166}"/>
+    <hyperlink ref="L215" r:id="rId131" xr:uid="{5ACD6BFD-52F0-0940-AA8E-B04F1D397BC7}"/>
+    <hyperlink ref="L253" r:id="rId132" xr:uid="{2936745D-6282-5C47-988B-5E89813F8F0A}"/>
+    <hyperlink ref="L210" r:id="rId133" xr:uid="{2030AD8C-28A7-544B-92DC-5CBE411DE1C0}"/>
+    <hyperlink ref="L240" r:id="rId134" xr:uid="{05363CA1-BE60-3F42-B56A-1A92A0EDA166}"/>
     <hyperlink ref="L200" r:id="rId135" xr:uid="{D4C66DCB-D6B4-EC4F-A922-B87887BE6E4A}"/>
     <hyperlink ref="L199" r:id="rId136" xr:uid="{A05D9F8A-ED0A-4143-8920-9422DD4E0BDD}"/>
     <hyperlink ref="L201" r:id="rId137" xr:uid="{83FA4EC1-AB5E-3B43-9476-4CA54526DF8E}"/>
@@ -10634,77 +10685,77 @@
     <hyperlink ref="L171" r:id="rId140" xr:uid="{3AB6BE1F-95C1-A443-B12D-D7A523FAD6C5}"/>
     <hyperlink ref="L172" r:id="rId141" xr:uid="{347BDCC2-5A0C-B249-8CA8-B72D245480FC}"/>
     <hyperlink ref="L173" r:id="rId142" xr:uid="{E58DD28D-BD99-DF44-9E5E-B3D05F881C1F}"/>
-    <hyperlink ref="L242" r:id="rId143" xr:uid="{4F668E79-3664-0547-B3D5-B7724A9D574D}"/>
-    <hyperlink ref="L240" r:id="rId144" xr:uid="{8AB5C10C-8B45-1843-96BD-655A4FA04EFD}"/>
+    <hyperlink ref="L244" r:id="rId143" xr:uid="{4F668E79-3664-0547-B3D5-B7724A9D574D}"/>
+    <hyperlink ref="L242" r:id="rId144" xr:uid="{8AB5C10C-8B45-1843-96BD-655A4FA04EFD}"/>
     <hyperlink ref="L177" r:id="rId145" xr:uid="{EAED74E0-13EE-A046-9ADC-AC8BDE30C3E6}"/>
-    <hyperlink ref="L247" r:id="rId146" xr:uid="{3577256C-215B-134E-B541-B7B77272CD8A}"/>
-    <hyperlink ref="L248" r:id="rId147" xr:uid="{98E325FC-7F95-B44E-98EB-DE0FF53BC89D}"/>
-    <hyperlink ref="L241" r:id="rId148" xr:uid="{5CE3083F-F217-3743-B613-A7DDF354E72D}"/>
-    <hyperlink ref="L243" r:id="rId149" xr:uid="{B81B6B41-2C17-AA48-B730-D906488BA0A0}"/>
+    <hyperlink ref="L249" r:id="rId146" xr:uid="{3577256C-215B-134E-B541-B7B77272CD8A}"/>
+    <hyperlink ref="L250" r:id="rId147" xr:uid="{98E325FC-7F95-B44E-98EB-DE0FF53BC89D}"/>
+    <hyperlink ref="L243" r:id="rId148" xr:uid="{5CE3083F-F217-3743-B613-A7DDF354E72D}"/>
+    <hyperlink ref="L245" r:id="rId149" xr:uid="{B81B6B41-2C17-AA48-B730-D906488BA0A0}"/>
     <hyperlink ref="L183" r:id="rId150" xr:uid="{BA0813A2-2582-7A46-A492-16A943824EE5}"/>
-    <hyperlink ref="L250" r:id="rId151" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
-    <hyperlink ref="L244" r:id="rId152" xr:uid="{C5265333-F7F0-1845-98D7-68E930F9DFAE}"/>
+    <hyperlink ref="L252" r:id="rId151" xr:uid="{B18426A7-D2C4-B049-BCF7-5C6DD332EC27}"/>
+    <hyperlink ref="L246" r:id="rId152" xr:uid="{C5265333-F7F0-1845-98D7-68E930F9DFAE}"/>
     <hyperlink ref="L188" r:id="rId153" xr:uid="{C0A159CB-3986-1A46-95AD-DCEFF4247697}"/>
     <hyperlink ref="L175" r:id="rId154" xr:uid="{37810A74-E45D-1D46-AEF5-C5FE2F414285}"/>
-    <hyperlink ref="L237" r:id="rId155" xr:uid="{D2906064-B1B8-4648-8201-BEFA97591226}"/>
+    <hyperlink ref="L239" r:id="rId155" xr:uid="{D2906064-B1B8-4648-8201-BEFA97591226}"/>
     <hyperlink ref="L163" r:id="rId156" xr:uid="{1D3CD52E-7AAD-E444-88F4-4BAE6C5B5EB7}"/>
     <hyperlink ref="L164" r:id="rId157" xr:uid="{E6E6DA47-945D-6145-912F-08B17B7BA6AE}"/>
     <hyperlink ref="L165" r:id="rId158" xr:uid="{006B1689-D89A-1E4A-BBC5-E9C9583907F7}"/>
     <hyperlink ref="L166" r:id="rId159" xr:uid="{C3E773B2-D410-AF41-B197-4638485DC8EF}"/>
     <hyperlink ref="L167" r:id="rId160" xr:uid="{A0E8A8E2-4A93-3D42-AF48-81955241A483}"/>
     <hyperlink ref="L168" r:id="rId161" xr:uid="{1B03F18A-8745-AA4F-AA8B-88D65D3B24BC}"/>
-    <hyperlink ref="L256" r:id="rId162" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
-    <hyperlink ref="L261" r:id="rId163" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
+    <hyperlink ref="L258" r:id="rId162" xr:uid="{AB0DD4DA-BD05-1C4A-B5BD-A5AD4DF6529D}"/>
+    <hyperlink ref="L263" r:id="rId163" xr:uid="{4EED275B-A8D1-CD41-BF7D-6273434300CA}"/>
     <hyperlink ref="L197" r:id="rId164" xr:uid="{D6B77117-A0D5-9240-8193-0102C36CCE4C}"/>
     <hyperlink ref="L198" r:id="rId165" xr:uid="{79FB1103-88A8-8044-9E2C-4FAEC0906E8E}"/>
-    <hyperlink ref="L245" r:id="rId166" xr:uid="{5BF1C4C9-E63A-4F42-9042-36520975FDFA}"/>
+    <hyperlink ref="L247" r:id="rId166" xr:uid="{5BF1C4C9-E63A-4F42-9042-36520975FDFA}"/>
     <hyperlink ref="L195" r:id="rId167" xr:uid="{21CDF460-9871-0547-AA6B-20304C8DD21D}"/>
     <hyperlink ref="L180" r:id="rId168" xr:uid="{BA1EC844-435A-6C44-87FC-C12B7ECFC55B}"/>
     <hyperlink ref="L179" r:id="rId169" xr:uid="{46D875DC-CDDD-7E4B-88DB-DFC416CF17AB}"/>
     <hyperlink ref="L169" r:id="rId170" xr:uid="{7D2FF6AE-1C67-9D4A-A760-7E3745DD9EA6}"/>
-    <hyperlink ref="L227" r:id="rId171" xr:uid="{B5E5E388-8F37-414E-A0C6-1DC58E77628C}"/>
-    <hyperlink ref="L229" r:id="rId172" xr:uid="{A96B1ACF-D982-9240-BB1C-69459154AE5A}"/>
+    <hyperlink ref="L229" r:id="rId171" xr:uid="{B5E5E388-8F37-414E-A0C6-1DC58E77628C}"/>
+    <hyperlink ref="L231" r:id="rId172" xr:uid="{A96B1ACF-D982-9240-BB1C-69459154AE5A}"/>
     <hyperlink ref="L189" r:id="rId173" xr:uid="{D3BB695A-CBA9-D649-B49D-4CC8D16EFD9B}"/>
     <hyperlink ref="L190" r:id="rId174" xr:uid="{A2922BA8-758D-3149-892C-B7B65B435332}"/>
-    <hyperlink ref="L216" r:id="rId175" xr:uid="{BDB09119-6289-4346-BC29-7A54BD393127}"/>
-    <hyperlink ref="L246" r:id="rId176" xr:uid="{5736CAF4-3646-3243-9AEB-4D82B6D0D10A}"/>
-    <hyperlink ref="L219" r:id="rId177" xr:uid="{60659D55-801C-9A4E-84CA-809884CCBE5C}"/>
+    <hyperlink ref="L218" r:id="rId175" xr:uid="{BDB09119-6289-4346-BC29-7A54BD393127}"/>
+    <hyperlink ref="L248" r:id="rId176" xr:uid="{5736CAF4-3646-3243-9AEB-4D82B6D0D10A}"/>
+    <hyperlink ref="L221" r:id="rId177" xr:uid="{60659D55-801C-9A4E-84CA-809884CCBE5C}"/>
     <hyperlink ref="L205" r:id="rId178" xr:uid="{18DDC006-0939-794C-9B5D-10593F8C0973}"/>
     <hyperlink ref="L191" r:id="rId179" xr:uid="{50EA46A5-11DD-0345-ABCA-4206D73C7606}"/>
-    <hyperlink ref="L236" r:id="rId180" xr:uid="{63DDFF3B-E62C-9445-96AD-4BB37ACCD20E}"/>
-    <hyperlink ref="L221" r:id="rId181" xr:uid="{05E34BC1-B22F-3E46-8574-E72267507402}"/>
-    <hyperlink ref="L220" r:id="rId182" xr:uid="{7125DF67-5A7E-D948-8363-A31AB1EBA44A}"/>
-    <hyperlink ref="L252" r:id="rId183" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
+    <hyperlink ref="L238" r:id="rId180" xr:uid="{63DDFF3B-E62C-9445-96AD-4BB37ACCD20E}"/>
+    <hyperlink ref="L223" r:id="rId181" xr:uid="{05E34BC1-B22F-3E46-8574-E72267507402}"/>
+    <hyperlink ref="L222" r:id="rId182" xr:uid="{7125DF67-5A7E-D948-8363-A31AB1EBA44A}"/>
+    <hyperlink ref="L254" r:id="rId183" xr:uid="{9A8E5672-7F19-6949-9214-999BD97B6718}"/>
     <hyperlink ref="L206" r:id="rId184" xr:uid="{CCE2D666-E296-D94C-ACE0-791CC746483B}"/>
     <hyperlink ref="L181" r:id="rId185" xr:uid="{E5A2F3EE-A3B1-0842-9364-E4B6EACA9544}"/>
-    <hyperlink ref="L222" r:id="rId186" xr:uid="{E08C8BA4-5414-1947-9CA8-45FE0B846CD1}"/>
-    <hyperlink ref="L218" r:id="rId187" xr:uid="{F1A64091-5BF7-8243-B7A0-F4C13B8B0ABB}"/>
+    <hyperlink ref="L224" r:id="rId186" xr:uid="{E08C8BA4-5414-1947-9CA8-45FE0B846CD1}"/>
+    <hyperlink ref="L220" r:id="rId187" xr:uid="{F1A64091-5BF7-8243-B7A0-F4C13B8B0ABB}"/>
     <hyperlink ref="L203" r:id="rId188" xr:uid="{745AEF03-3150-C54B-800A-696460474256}"/>
     <hyperlink ref="L204" r:id="rId189" xr:uid="{9C078FBA-3B11-8049-9187-5BC86D78EA09}"/>
     <hyperlink ref="L182" r:id="rId190" xr:uid="{BF9A6A48-C664-FA4B-A769-D87460BB9387}"/>
     <hyperlink ref="L187" r:id="rId191" xr:uid="{11E0C06F-BBA9-B446-A3A4-5862C893161B}"/>
-    <hyperlink ref="L217" r:id="rId192" xr:uid="{D5E45024-1B58-714D-9576-1FA969BDADD9}"/>
+    <hyperlink ref="L219" r:id="rId192" xr:uid="{D5E45024-1B58-714D-9576-1FA969BDADD9}"/>
     <hyperlink ref="L194" r:id="rId193" xr:uid="{D160676D-AC82-D243-B9A9-56033B0A6EFE}"/>
-    <hyperlink ref="L214" r:id="rId194" xr:uid="{3DB54A74-68B7-734A-BC3C-BFE4E2E4103E}"/>
+    <hyperlink ref="L216" r:id="rId194" xr:uid="{3DB54A74-68B7-734A-BC3C-BFE4E2E4103E}"/>
     <hyperlink ref="L106" r:id="rId195" xr:uid="{4686296B-C235-4048-A384-BE461895E2AC}"/>
     <hyperlink ref="L108" r:id="rId196" location="page=2&amp;query=gold%20badge%20sprite&amp;position=49&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{061AB839-ADB1-BA47-A152-68CDFE8A1979}"/>
     <hyperlink ref="L109" r:id="rId197" location="page=4&amp;query=gold%20badge%20sprite&amp;position=9&amp;from_view=search&amp;track=ais&amp;uuid=84edebd4-34e9-4ca6-8a45-e1f1ad58800d" xr:uid="{138577BB-7F7D-D64A-806E-567F3970D250}"/>
     <hyperlink ref="L178" r:id="rId198" xr:uid="{927B8B79-A428-2043-9B3B-555F7877CA20}"/>
     <hyperlink ref="L202" r:id="rId199" xr:uid="{6018233D-1425-7148-A608-3B0666055EA2}"/>
-    <hyperlink ref="L228" r:id="rId200" xr:uid="{38C9843F-1665-8F46-A66C-287455700886}"/>
-    <hyperlink ref="L253" r:id="rId201" xr:uid="{9E664F43-2A79-3744-BC57-4D11914A4B9C}"/>
-    <hyperlink ref="L254" r:id="rId202" xr:uid="{F55C22EB-ADA4-064F-8C9F-34B8DFB927E8}"/>
+    <hyperlink ref="L230" r:id="rId200" xr:uid="{38C9843F-1665-8F46-A66C-287455700886}"/>
+    <hyperlink ref="L255" r:id="rId201" xr:uid="{9E664F43-2A79-3744-BC57-4D11914A4B9C}"/>
+    <hyperlink ref="L256" r:id="rId202" xr:uid="{F55C22EB-ADA4-064F-8C9F-34B8DFB927E8}"/>
     <hyperlink ref="L162" r:id="rId203" xr:uid="{A1B2F4EC-ACE1-B14D-8619-0451D719CFC0}"/>
-    <hyperlink ref="L230" r:id="rId204" xr:uid="{2BF445F0-7B50-5E48-A8E5-4779F07B83CE}"/>
-    <hyperlink ref="L231" r:id="rId205" xr:uid="{6B23A3F9-85DD-4043-853E-3BF95911A2C6}"/>
-    <hyperlink ref="L232" r:id="rId206" xr:uid="{A975FD98-A3FE-5B40-9F31-D14EAE3777F9}"/>
-    <hyperlink ref="L257" r:id="rId207" xr:uid="{F01C8569-23FB-7F4C-A50B-40979911E1B8}"/>
-    <hyperlink ref="L260" r:id="rId208" xr:uid="{B54ABD16-F1A6-DC45-B36E-0CC72B423F70}"/>
-    <hyperlink ref="L258" r:id="rId209" xr:uid="{EBA532A6-AAFD-E54D-BD41-CC4F5F92AF68}"/>
-    <hyperlink ref="L259" r:id="rId210" xr:uid="{0F422DA4-046E-F246-BC4A-695F255E6851}"/>
-    <hyperlink ref="L210" r:id="rId211" xr:uid="{1F9FD82A-7BDA-7143-B89F-0DBBBC864386}"/>
-    <hyperlink ref="L211" r:id="rId212" xr:uid="{7F1F0626-5319-784B-97DE-B956AE96359D}"/>
-    <hyperlink ref="L215" r:id="rId213" xr:uid="{B2599288-37DA-884B-A5E6-897FBCE08F4D}"/>
+    <hyperlink ref="L232" r:id="rId204" xr:uid="{2BF445F0-7B50-5E48-A8E5-4779F07B83CE}"/>
+    <hyperlink ref="L233" r:id="rId205" xr:uid="{6B23A3F9-85DD-4043-853E-3BF95911A2C6}"/>
+    <hyperlink ref="L234" r:id="rId206" xr:uid="{A975FD98-A3FE-5B40-9F31-D14EAE3777F9}"/>
+    <hyperlink ref="L259" r:id="rId207" xr:uid="{F01C8569-23FB-7F4C-A50B-40979911E1B8}"/>
+    <hyperlink ref="L262" r:id="rId208" xr:uid="{B54ABD16-F1A6-DC45-B36E-0CC72B423F70}"/>
+    <hyperlink ref="L260" r:id="rId209" xr:uid="{EBA532A6-AAFD-E54D-BD41-CC4F5F92AF68}"/>
+    <hyperlink ref="L261" r:id="rId210" xr:uid="{0F422DA4-046E-F246-BC4A-695F255E6851}"/>
+    <hyperlink ref="L212" r:id="rId211" xr:uid="{1F9FD82A-7BDA-7143-B89F-0DBBBC864386}"/>
+    <hyperlink ref="L213" r:id="rId212" xr:uid="{7F1F0626-5319-784B-97DE-B956AE96359D}"/>
+    <hyperlink ref="L217" r:id="rId213" xr:uid="{B2599288-37DA-884B-A5E6-897FBCE08F4D}"/>
     <hyperlink ref="L85" r:id="rId214" location="page=2&amp;query=light%20beam&amp;position=25&amp;from_view=search&amp;track=ais&amp;uuid=063fa81a-19de-4aad-b5fc-7caa6fa59141#position=25&amp;page=2&amp;query=light%20beam" xr:uid="{F7D7C1C4-CC10-FA4D-8194-8E6ECD655D52}"/>
     <hyperlink ref="L184" r:id="rId215" xr:uid="{D7E66CB2-1636-854A-8F67-24ACB034C7F4}"/>
     <hyperlink ref="L185" r:id="rId216" xr:uid="{D83C0C58-CE24-594B-A33D-B788F11BBF4E}"/>
@@ -10712,9 +10763,9 @@
     <hyperlink ref="L35" r:id="rId218" location="page=3&amp;query=dragon%20sprite&amp;position=8&amp;from_view=search&amp;track=ais&amp;uuid=a74ae69f-43df-4e46-8d2c-551fbfc06054" xr:uid="{B03DA0C1-BC2B-EF47-AC66-221CD4C2D9C5}"/>
     <hyperlink ref="L83" r:id="rId219" location="page=3&amp;query=dragon%20sprite&amp;position=8&amp;from_view=search&amp;track=ais&amp;uuid=a74ae69f-43df-4e46-8d2c-551fbfc06054" xr:uid="{027D9EA3-3F97-BA46-BA51-96E2ED000931}"/>
     <hyperlink ref="L193" r:id="rId220" xr:uid="{8BAF1438-906C-504E-A53D-226576B1A1BC}"/>
-    <hyperlink ref="L239" r:id="rId221" xr:uid="{0345E79A-FDC7-314E-8D2A-45798EF5A1E7}"/>
-    <hyperlink ref="L262" r:id="rId222" xr:uid="{5971D630-BDBF-1C4D-A608-817C569DA1F0}"/>
-    <hyperlink ref="L249" r:id="rId223" xr:uid="{EE815D9F-FD89-0245-8EBF-03580B54BC84}"/>
+    <hyperlink ref="L241" r:id="rId221" xr:uid="{0345E79A-FDC7-314E-8D2A-45798EF5A1E7}"/>
+    <hyperlink ref="L264" r:id="rId222" xr:uid="{5971D630-BDBF-1C4D-A608-817C569DA1F0}"/>
+    <hyperlink ref="L251" r:id="rId223" xr:uid="{EE815D9F-FD89-0245-8EBF-03580B54BC84}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>